<commit_message>
eliminated "step_info", working in limited run through step 1. Utilizing new step 0 habitat values per Jeff Nordin
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -28446,8 +28446,8 @@
   </sheetPr>
   <dimension ref="A1:AH335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="C275" sqref="C275"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="E263" sqref="E263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
output working, added force steps. This is producing output for meeting on July 24.
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235" tabRatio="798" activeTab="5"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235" tabRatio="798" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -5071,11 +5071,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198550528"/>
-        <c:axId val="199226432"/>
+        <c:axId val="198308352"/>
+        <c:axId val="169006720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198550528"/>
+        <c:axId val="198308352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5097,14 +5097,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199226432"/>
+        <c:crossAx val="169006720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5112,7 +5111,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199226432"/>
+        <c:axId val="169006720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5143,21 +5142,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198550528"/>
+        <c:crossAx val="198308352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
@@ -5613,11 +5610,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199410688"/>
-        <c:axId val="201008256"/>
+        <c:axId val="198310400"/>
+        <c:axId val="169008448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199410688"/>
+        <c:axId val="198310400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5639,14 +5636,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201008256"/>
+        <c:crossAx val="169008448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5654,7 +5650,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201008256"/>
+        <c:axId val="169008448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -5683,14 +5679,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199410688"/>
+        <c:crossAx val="198310400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5698,7 +5693,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5826,11 +5820,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199412224"/>
-        <c:axId val="201010560"/>
+        <c:axId val="198311424"/>
+        <c:axId val="198526656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199412224"/>
+        <c:axId val="198311424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5852,14 +5846,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201010560"/>
+        <c:crossAx val="198526656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5867,7 +5860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201010560"/>
+        <c:axId val="198526656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5898,14 +5891,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199412224"/>
+        <c:crossAx val="198311424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5988,52 +5980,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2018</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2019</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2020</c:v>
+                  <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2021</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2022</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2023</c:v>
+                  <c:v>2025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2024</c:v>
+                  <c:v>2026</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2025</c:v>
+                  <c:v>2027</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2026</c:v>
+                  <c:v>2028</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2027</c:v>
+                  <c:v>2029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2028</c:v>
+                  <c:v>2030</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2029</c:v>
+                  <c:v>2031</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2030</c:v>
+                  <c:v>2032</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2031</c:v>
+                  <c:v>2033</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2032</c:v>
+                  <c:v>2034</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2033</c:v>
+                  <c:v>2035</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6107,11 +6099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193586176"/>
-        <c:axId val="201012864"/>
+        <c:axId val="199026176"/>
+        <c:axId val="198528960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193586176"/>
+        <c:axId val="199026176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6122,7 +6114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201012864"/>
+        <c:crossAx val="198528960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6130,7 +6122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201012864"/>
+        <c:axId val="198528960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000000"/>
@@ -6143,7 +6135,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193586176"/>
+        <c:crossAx val="199026176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100000000"/>
@@ -6270,133 +6262,133 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
                 <c:pt idx="0">
-                  <c:v>2018</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2019</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2020</c:v>
+                  <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2021</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2022</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2023</c:v>
+                  <c:v>2025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2024</c:v>
+                  <c:v>2026</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2025</c:v>
+                  <c:v>2027</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2026</c:v>
+                  <c:v>2028</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2027</c:v>
+                  <c:v>2029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2028</c:v>
+                  <c:v>2030</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2029</c:v>
+                  <c:v>2031</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2030</c:v>
+                  <c:v>2032</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2031</c:v>
+                  <c:v>2033</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2032</c:v>
+                  <c:v>2034</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2033</c:v>
+                  <c:v>2035</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2034</c:v>
+                  <c:v>2036</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2035</c:v>
+                  <c:v>2037</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2036</c:v>
+                  <c:v>2038</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2037</c:v>
+                  <c:v>2039</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2038</c:v>
+                  <c:v>2040</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2039</c:v>
+                  <c:v>2041</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2040</c:v>
+                  <c:v>2042</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2041</c:v>
+                  <c:v>2043</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2042</c:v>
+                  <c:v>2044</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2043</c:v>
+                  <c:v>2045</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2044</c:v>
+                  <c:v>2046</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2045</c:v>
+                  <c:v>2047</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2046</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2047</c:v>
+                  <c:v>2049</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2048</c:v>
+                  <c:v>2050</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2049</c:v>
+                  <c:v>2051</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2050</c:v>
+                  <c:v>2052</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2051</c:v>
+                  <c:v>2053</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2052</c:v>
+                  <c:v>2054</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2053</c:v>
+                  <c:v>2055</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2054</c:v>
+                  <c:v>2056</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2055</c:v>
+                  <c:v>2057</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2056</c:v>
+                  <c:v>2058</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2057</c:v>
+                  <c:v>2059</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2058</c:v>
+                  <c:v>2060</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2059</c:v>
+                  <c:v>2061</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2060</c:v>
+                  <c:v>2062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6579,133 +6571,133 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"???_);_(@_)</c:formatCode>
                 <c:ptCount val="43"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.4750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.88</c:v>
+                  <c:v>11.234999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.260000000000002</c:v>
+                  <c:v>19.615000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.126000000000001</c:v>
+                  <c:v>32.481000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.027999999999999</c:v>
+                  <c:v>46.383000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53.637025135563896</c:v>
+                  <c:v>60.9920251355639</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69.555152618833233</c:v>
+                  <c:v>76.910152618833237</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.573483139003955</c:v>
+                  <c:v>93.928483139003959</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104.19065835014631</c:v>
+                  <c:v>111.54565835014631</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>123.43724818556032</c:v>
+                  <c:v>130.79224818556034</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>143.82582092003653</c:v>
+                  <c:v>151.18082092003655</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>164.96643117340736</c:v>
+                  <c:v>172.32143117340738</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>188.2795942591404</c:v>
+                  <c:v>195.63459425914041</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>213.12468562410322</c:v>
+                  <c:v>220.47968562410324</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>238.66610802507955</c:v>
+                  <c:v>246.02110802507957</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>267.22960712235465</c:v>
+                  <c:v>274.58460712235467</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>296.60085022140544</c:v>
+                  <c:v>303.95585022140546</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>325.8467537339738</c:v>
+                  <c:v>333.20175373397382</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>356.98667766449893</c:v>
+                  <c:v>364.34167766449895</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>389.08753842472277</c:v>
+                  <c:v>396.44253842472278</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>421.23017904710741</c:v>
+                  <c:v>428.58517904710743</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>454.97995170061125</c:v>
+                  <c:v>462.33495170061127</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>490.41721298679033</c:v>
+                  <c:v>497.77221298679035</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>527.6263373372783</c:v>
+                  <c:v>534.98133733727832</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>566.69591790529068</c:v>
+                  <c:v>574.0509179052907</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>607.71897750170376</c:v>
+                  <c:v>615.07397750170378</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>650.79319007793742</c:v>
+                  <c:v>658.14819007793744</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>696.02111328298281</c:v>
+                  <c:v>703.37611328298283</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>743.51043264828047</c:v>
+                  <c:v>750.86543264828049</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>793.374217981843</c:v>
+                  <c:v>800.72921798184302</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>845.73119258208362</c:v>
+                  <c:v>853.08619258208364</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>900.70601591233628</c:v>
+                  <c:v>908.0610159123363</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>958.42958040910162</c:v>
+                  <c:v>965.78458040910164</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1019.0393231307053</c:v>
+                  <c:v>1026.3943231307053</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1082.6795529883891</c:v>
+                  <c:v>1090.0345529883891</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1149.5017943389571</c:v>
+                  <c:v>1156.8567943389571</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1219.6651477570535</c:v>
+                  <c:v>1227.0201477570536</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1293.3366688460546</c:v>
+                  <c:v>1300.6916688460547</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1370.6917659895059</c:v>
+                  <c:v>1378.046765989506</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1451.9146179901297</c:v>
+                  <c:v>1459.2696179901297</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1537.1986125907847</c:v>
+                  <c:v>1544.5536125907847</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1626.7468069214724</c:v>
+                  <c:v>1634.1018069214724</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1720.7724109686947</c:v>
+                  <c:v>1728.1274109686947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6722,11 +6714,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="201230336"/>
-        <c:axId val="200532544"/>
+        <c:axId val="199673344"/>
+        <c:axId val="199392576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="201230336"/>
+        <c:axId val="199673344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6747,7 +6739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200532544"/>
+        <c:crossAx val="199392576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6755,7 +6747,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200532544"/>
+        <c:axId val="199392576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6777,7 +6769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201230336"/>
+        <c:crossAx val="199673344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -7366,8 +7358,8 @@
   </sheetPr>
   <dimension ref="A1:CP241"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A241" sqref="A22:A241"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16134,67 +16126,67 @@
       <c r="U4" s="350"/>
       <c r="Y4" s="245">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="Z4" s="245">
         <f t="shared" si="0"/>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="AA4" s="245">
         <f t="shared" si="0"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="AB4" s="245">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="AC4" s="245">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="AD4" s="245">
         <f t="shared" si="0"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="AE4" s="245">
         <f t="shared" si="0"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="AF4" s="245">
         <f t="shared" si="0"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="AG4" s="245">
         <f t="shared" si="0"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="AH4" s="245">
         <f t="shared" si="0"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="AI4" s="245">
         <f t="shared" si="0"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="AJ4" s="245">
         <f t="shared" si="0"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="AK4" s="245">
         <f t="shared" si="0"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="AL4" s="245">
         <f t="shared" si="0"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="AM4" s="245">
         <f t="shared" si="0"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="AN4" s="245">
         <f t="shared" si="0"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -16206,67 +16198,67 @@
       <c r="D5" s="359"/>
       <c r="E5" s="69">
         <f>'Step Analysis'!E5</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F5" s="70">
         <f t="shared" ref="F5:T5" si="1">E5 + 1</f>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G5" s="70">
         <f t="shared" si="1"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="H5" s="70">
         <f t="shared" si="1"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="I5" s="70">
         <f t="shared" si="1"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="J5" s="70">
         <f t="shared" si="1"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="K5" s="70">
         <f t="shared" si="1"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="L5" s="70">
         <f t="shared" si="1"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="M5" s="70">
         <f t="shared" si="1"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="N5" s="70">
         <f t="shared" si="1"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="O5" s="70">
         <f t="shared" si="1"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="P5" s="70">
         <f t="shared" si="1"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="Q5" s="70">
         <f t="shared" si="1"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="R5" s="70">
         <f t="shared" si="1"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="S5" s="70">
         <f t="shared" si="1"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="T5" s="70">
         <f t="shared" si="1"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="U5" s="71" t="s">
         <v>269</v>
@@ -16938,67 +16930,67 @@
       </c>
       <c r="Y12" s="245">
         <f t="shared" ref="Y12:AN12" si="9">E5</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="Z12" s="245">
         <f t="shared" si="9"/>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="AA12" s="245">
         <f t="shared" si="9"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="AB12" s="245">
         <f t="shared" si="9"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="AC12" s="245">
         <f t="shared" si="9"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="AD12" s="245">
         <f t="shared" si="9"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="AE12" s="245">
         <f t="shared" si="9"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="AF12" s="245">
         <f t="shared" si="9"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="AG12" s="245">
         <f t="shared" si="9"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="AH12" s="245">
         <f t="shared" si="9"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="AI12" s="245">
         <f t="shared" si="9"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="AJ12" s="245">
         <f t="shared" si="9"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="AK12" s="245">
         <f t="shared" si="9"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="AL12" s="245">
         <f t="shared" si="9"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="AM12" s="245">
         <f t="shared" si="9"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="AN12" s="245">
         <f t="shared" si="9"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -23841,8 +23833,8 @@
   </sheetPr>
   <dimension ref="A1:L222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24643,7 +24635,7 @@
         <v>108</v>
       </c>
       <c r="K68" s="343" t="s">
-        <v>699</v>
+        <v>57</v>
       </c>
       <c r="L68" s="343">
         <v>2</v>
@@ -25958,7 +25950,7 @@
   </sheetPr>
   <dimension ref="A1:AK193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
@@ -30312,8 +30304,8 @@
   </sheetPr>
   <dimension ref="A1:AG335"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37043,7 +37035,7 @@
         <v>0</v>
       </c>
       <c r="H248" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" ref="H248:H257" si="0">5.38*$K$251</f>
         <v>1.4672727272727271</v>
       </c>
       <c r="I248" s="239" t="s">
@@ -37073,7 +37065,7 @@
         <v>0</v>
       </c>
       <c r="H249" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
       <c r="I249" s="140" t="s">
@@ -37103,7 +37095,7 @@
         <v>0</v>
       </c>
       <c r="H250" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
       <c r="I250" s="140" t="s">
@@ -37133,7 +37125,7 @@
         <v>0</v>
       </c>
       <c r="H251" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
       <c r="I251" s="140" t="s">
@@ -37167,7 +37159,7 @@
         <v>0</v>
       </c>
       <c r="H252" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
     </row>
@@ -37194,7 +37186,7 @@
         <v>0</v>
       </c>
       <c r="H253" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
     </row>
@@ -37221,7 +37213,7 @@
         <v>0</v>
       </c>
       <c r="H254" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
     </row>
@@ -37248,7 +37240,7 @@
         <v>0</v>
       </c>
       <c r="H255" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
     </row>
@@ -37275,7 +37267,7 @@
         <v>0</v>
       </c>
       <c r="H256" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
     </row>
@@ -37302,7 +37294,7 @@
         <v>0</v>
       </c>
       <c r="H257" s="243">
-        <f>5.38*$K$251</f>
+        <f t="shared" si="0"/>
         <v>1.4672727272727271</v>
       </c>
     </row>
@@ -39166,8 +39158,8 @@
   </sheetPr>
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41427,7 +41419,7 @@
       </c>
       <c r="B3" s="161">
         <f>INDEX('10 YEAR PROJECTION'!E5:T5, MATCH(TRUE, INDEX('10 YEAR PROJECTION'!E6:T6&lt;&gt;0, ), 0))</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C3" s="161">
         <v>2023</v>
@@ -41482,7 +41474,7 @@
       </c>
       <c r="B4" s="161">
         <f>INDEX('10 YEAR PROJECTION'!E$5:T$5, MATCH(TRUE, INDEX('10 YEAR PROJECTION'!E14:T14&lt;&gt;0, ), 0))</f>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C4" s="161">
         <v>2026</v>
@@ -41537,7 +41529,7 @@
       </c>
       <c r="B5" s="161">
         <f>INDEX('10 YEAR PROJECTION'!E$5:T$5, MATCH(TRUE, INDEX('10 YEAR PROJECTION'!E22:T22&lt;&gt;0, ), 0))</f>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="C5" s="161">
         <v>2029</v>
@@ -41592,7 +41584,7 @@
       </c>
       <c r="B6" s="161">
         <f>INDEX('10 YEAR PROJECTION'!E$5:T$5, MATCH(TRUE, INDEX('10 YEAR PROJECTION'!E30:T30&lt;&gt;0, ), 0))</f>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="C6" s="161">
         <v>2032</v>
@@ -41647,7 +41639,7 @@
       </c>
       <c r="B7" s="161">
         <f>INDEX('10 YEAR PROJECTION'!E$5:T$5, MATCH(TRUE, INDEX('10 YEAR PROJECTION'!E38:T38&lt;&gt;0, ), 0))</f>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="C7" s="161">
         <v>2035</v>
@@ -42424,23 +42416,23 @@
       </c>
       <c r="C2" s="97">
         <f>'10 YEAR PROJECTION'!I5</f>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="D2" s="97">
         <f>'10 YEAR PROJECTION'!L5</f>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="E2" s="97">
         <f>'10 YEAR PROJECTION'!O5</f>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="F2" s="97">
         <f>'10 YEAR PROJECTION'!R5</f>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="G2" s="97">
         <f>'10 YEAR PROJECTION'!T5</f>
-        <v>2033</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -43686,7 +43678,7 @@
   <dimension ref="A1:BZ83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43881,24 +43873,24 @@
     <row r="5" spans="1:78" s="20" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="335">
         <f>MAX(AA9:AA51)</f>
-        <v>2032</v>
+        <v>2021</v>
       </c>
       <c r="B5" s="329">
         <f>Y52-Q52</f>
-        <v>347.11185534234727</v>
+        <v>354.30867788431379</v>
       </c>
       <c r="C5" s="329">
         <f>MAX(R9:R51)*1000000/U52</f>
-        <v>687.22378750697419</v>
+        <v>675.42010990222207</v>
       </c>
       <c r="D5" s="193">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="E5" s="193">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F5" s="194">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="G5" s="195">
         <v>4.2500000000000003E-2</v>
@@ -43978,7 +43970,7 @@
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
         <v>Projected Annual Cost
-2018 Dollar Year
+2020 Dollar Year
 ($Million)</v>
       </c>
       <c r="D7" s="428"/>
@@ -44007,7 +43999,7 @@
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
- ($Million; NPV=$589.534)</v>
+ ($Million; NPV=$596.731)</v>
       </c>
       <c r="T7" s="428"/>
       <c r="U7" s="428"/>
@@ -44228,7 +44220,7 @@
       </c>
       <c r="B9" s="41">
         <f>$E$5</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C9" s="216">
         <f>IF(B9&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -44312,14 +44304,14 @@
              INDEX(MP_new!$A$4:$J$9, INDEX('Cost Analysis Input'!$B$2:$D$7, IF(MATCH(B9, 'Cost Analysis Input'!$C$2:$C$7, 1)&gt;$I$1, $I$1, MATCH(B9, 'Cost Analysis Input'!$C$2:$C$7, 1)), 3)+1, 7)-5000),
         INDEX(MP_new!$A$4:$J$9, $I$1+1, 7)),
     0)</f>
-        <v>64619.055153407739</v>
+        <v>59619.055153407739</v>
       </c>
       <c r="T9" s="154">
         <v>0</v>
       </c>
       <c r="U9" s="1">
         <f>IF(A9, (MP_new!$G$4-S9)+T9, 0)</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="V9" s="1">
         <f t="shared" ref="V9:V51" si="13">IF(A9, IF(EXACT($Q$5,"Treated"),AM9,AN9), 0)</f>
@@ -44327,11 +44319,11 @@
       </c>
       <c r="W9" s="220">
         <f t="shared" ref="W9:W51" si="14">(U9*V9)/1000000</f>
-        <v>0</v>
+        <v>3.4750000000000001</v>
       </c>
       <c r="X9" s="221">
         <f>W9</f>
-        <v>0</v>
+        <v>3.4750000000000001</v>
       </c>
       <c r="Y9" s="221">
         <v>0</v>
@@ -44364,7 +44356,7 @@
       </c>
       <c r="AP9" s="5">
         <f t="shared" ref="AP9:AP50" si="15">AS9</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="AQ9" s="28">
         <f t="shared" si="0"/>
@@ -44372,7 +44364,7 @@
       </c>
       <c r="AS9" s="57">
         <f t="shared" ref="AS9:AS50" si="16">B9</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="AT9" s="28">
         <v>0</v>
@@ -44403,7 +44395,7 @@
       </c>
       <c r="BD9" s="5">
         <f t="shared" ref="BD9:BD50" si="17">BG9</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="BE9" s="28">
         <f t="shared" ref="BE9:BE50" si="18">IF($P$5=15,BH9,IF($P$5=25,BI9,))</f>
@@ -44412,7 +44404,7 @@
       <c r="BF9" s="190"/>
       <c r="BG9" s="5">
         <f t="shared" ref="BG9:BG50" si="19">B9</f>
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="BH9" s="28">
         <v>0</v>
@@ -44431,7 +44423,7 @@
       </c>
       <c r="B10" s="40">
         <f t="shared" ref="B10:B51" si="20">B9+1</f>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C10" s="216">
         <f>IF(B10&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -44515,7 +44507,7 @@
              INDEX(MP_new!$A$4:$J$9, INDEX('Cost Analysis Input'!$B$2:$D$7, IF(MATCH(B10, 'Cost Analysis Input'!$C$2:$C$7, 1)&gt;$I$1, $I$1, MATCH(B10, 'Cost Analysis Input'!$C$2:$C$7, 1)), 3)+1, 7)-5000),
         INDEX(MP_new!$A$4:$J$9, $I$1+1, 7)),
     0)</f>
-        <v>64619.055153407739</v>
+        <v>59619.055153407739</v>
       </c>
       <c r="T10" s="154">
         <f>IF(A10, IF(EXACT($S$5, "Yes"),
@@ -44527,7 +44519,7 @@
       </c>
       <c r="U10" s="1">
         <f>IF(A10, (MP_new!$G$4-S10)+T10, 0)</f>
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="V10" s="1">
         <f t="shared" si="13"/>
@@ -44535,27 +44527,27 @@
       </c>
       <c r="W10" s="227">
         <f t="shared" si="14"/>
-        <v>3.88</v>
+        <v>7.76</v>
       </c>
       <c r="X10" s="224">
         <f t="shared" ref="X10:X51" si="23">IF(A10, X9+W10, 0)</f>
-        <v>3.88</v>
+        <v>11.234999999999999</v>
       </c>
       <c r="Y10" s="224">
         <f t="shared" ref="Y10:Y51" si="24">W10-Q10</f>
-        <v>-0.42910609799999921</v>
+        <v>3.4508939020000007</v>
       </c>
       <c r="Z10" s="224">
         <f t="shared" ref="Z10:Z51" si="25">X10-R10</f>
-        <v>-1.9291060979999992</v>
+        <v>5.4258939020000003</v>
       </c>
       <c r="AA10" s="224">
         <f>IF(SUM(AA$9:AA9)&gt;0,0,IF(SUM(X10-R10)&gt;0,B10,0))</f>
-        <v>0</v>
+        <v>2021</v>
       </c>
       <c r="AB10" s="224">
         <f>ABS(Z10)*1000000/SUM(U$9:U10)</f>
-        <v>385.82121959999984</v>
+        <v>361.72626013333337</v>
       </c>
       <c r="AH10" s="19">
         <f t="shared" ref="AH10:AH51" si="26">AH9+1</f>
@@ -44580,7 +44572,7 @@
       <c r="AO10" s="14"/>
       <c r="AP10" s="15">
         <f t="shared" si="15"/>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="AQ10" s="29">
         <f t="shared" si="0"/>
@@ -44589,7 +44581,7 @@
       <c r="AR10" s="14"/>
       <c r="AS10" s="54">
         <f t="shared" si="16"/>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="AT10" s="29">
         <f t="shared" ref="AT10:BB10" si="29">$M$9</f>
@@ -44630,7 +44622,7 @@
       <c r="BC10" s="14"/>
       <c r="BD10" s="15">
         <f t="shared" si="17"/>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="BE10" s="29">
         <f t="shared" si="18"/>
@@ -44639,7 +44631,7 @@
       <c r="BF10" s="14"/>
       <c r="BG10" s="15">
         <f t="shared" si="19"/>
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="BH10" s="29">
         <f>SUM($O$9)</f>
@@ -44659,7 +44651,7 @@
       </c>
       <c r="B11" s="41">
         <f t="shared" si="20"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="C11" s="216">
         <f>IF(B11&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -44767,7 +44759,7 @@
       </c>
       <c r="X11" s="217">
         <f t="shared" si="23"/>
-        <v>12.260000000000002</v>
+        <v>19.615000000000002</v>
       </c>
       <c r="Y11" s="217">
         <f t="shared" si="24"/>
@@ -44775,7 +44767,7 @@
       </c>
       <c r="Z11" s="217">
         <f t="shared" si="25"/>
-        <v>-18.02607027094599</v>
+        <v>-10.671070270945989</v>
       </c>
       <c r="AA11" s="217">
         <f>IF(SUM(AA$9:AA10)&gt;0,0,IF(SUM(X11-R11)&gt;0,B11,0))</f>
@@ -44783,7 +44775,7 @@
       </c>
       <c r="AB11" s="217">
         <f>ABS(Z11)*1000000/SUM(U$9:U11)</f>
-        <v>1201.738018063066</v>
+        <v>426.84281083783952</v>
       </c>
       <c r="AH11" s="17">
         <f t="shared" si="26"/>
@@ -44807,7 +44799,7 @@
       </c>
       <c r="AP11" s="5">
         <f t="shared" si="15"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="AQ11" s="28">
         <f t="shared" si="0"/>
@@ -44815,7 +44807,7 @@
       </c>
       <c r="AS11" s="57">
         <f t="shared" si="16"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="AT11" s="28">
         <f>SUM($M$9:$M10)</f>
@@ -44855,7 +44847,7 @@
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="17"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="BE11" s="28">
         <f t="shared" si="18"/>
@@ -44864,7 +44856,7 @@
       <c r="BF11" s="190"/>
       <c r="BG11" s="5">
         <f t="shared" si="19"/>
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="BH11" s="28">
         <f>SUM($O$9:O10)</f>
@@ -44882,7 +44874,7 @@
       </c>
       <c r="B12" s="40">
         <f t="shared" si="20"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C12" s="216">
         <f>IF(B12&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -44990,7 +44982,7 @@
       </c>
       <c r="X12" s="224">
         <f t="shared" si="23"/>
-        <v>25.126000000000001</v>
+        <v>32.481000000000002</v>
       </c>
       <c r="Y12" s="224">
         <f t="shared" si="24"/>
@@ -44998,7 +44990,7 @@
       </c>
       <c r="Z12" s="224">
         <f t="shared" si="25"/>
-        <v>-120.60209636659036</v>
+        <v>-113.24709636659037</v>
       </c>
       <c r="AA12" s="224">
         <f>IF(SUM(AA$9:AA11)&gt;0,0,IF(SUM(X12-R12)&gt;0,B12,0))</f>
@@ -45006,7 +44998,7 @@
       </c>
       <c r="AB12" s="224">
         <f>ABS(Z12)*1000000/SUM(U$9:U12)</f>
-        <v>4158.6929781582885</v>
+        <v>2903.7717017074451</v>
       </c>
       <c r="AH12" s="19">
         <f t="shared" si="26"/>
@@ -45031,7 +45023,7 @@
       <c r="AO12" s="14"/>
       <c r="AP12" s="15">
         <f t="shared" si="15"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="AQ12" s="29">
         <f t="shared" si="0"/>
@@ -45040,7 +45032,7 @@
       <c r="AR12" s="14"/>
       <c r="AS12" s="54">
         <f t="shared" si="16"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="AT12" s="29">
         <f>SUM($M$9:$M11)</f>
@@ -45081,7 +45073,7 @@
       <c r="BC12" s="14"/>
       <c r="BD12" s="15">
         <f t="shared" si="17"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="BE12" s="29">
         <f t="shared" si="18"/>
@@ -45090,7 +45082,7 @@
       <c r="BF12" s="14"/>
       <c r="BG12" s="15">
         <f t="shared" si="19"/>
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="BH12" s="29">
         <f>SUM($O$9:O11)</f>
@@ -45110,7 +45102,7 @@
       </c>
       <c r="B13" s="41">
         <f t="shared" si="20"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C13" s="216">
         <f>IF(B13&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -45218,7 +45210,7 @@
       </c>
       <c r="X13" s="217">
         <f t="shared" si="23"/>
-        <v>39.027999999999999</v>
+        <v>46.383000000000003</v>
       </c>
       <c r="Y13" s="217">
         <f t="shared" si="24"/>
@@ -45226,7 +45218,7 @@
       </c>
       <c r="Z13" s="217">
         <f t="shared" si="25"/>
-        <v>-156.82744633592884</v>
+        <v>-149.47244633592882</v>
       </c>
       <c r="AA13" s="217">
         <f>IF(SUM(AA$9:AA12)&gt;0,0,IF(SUM(X13-R13)&gt;0,B13,0))</f>
@@ -45234,7 +45226,7 @@
       </c>
       <c r="AB13" s="217">
         <f>ABS(Z13)*1000000/SUM(U$9:U13)</f>
-        <v>3647.1499147890427</v>
+        <v>2820.234836526959</v>
       </c>
       <c r="AH13" s="17">
         <f t="shared" si="26"/>
@@ -45258,7 +45250,7 @@
       </c>
       <c r="AP13" s="5">
         <f t="shared" si="15"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="AQ13" s="28">
         <f t="shared" si="0"/>
@@ -45266,7 +45258,7 @@
       </c>
       <c r="AS13" s="57">
         <f t="shared" si="16"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="AT13" s="28">
         <f>SUM($M$9:$M12)</f>
@@ -45306,7 +45298,7 @@
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="17"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="BE13" s="28">
         <f t="shared" si="18"/>
@@ -45315,7 +45307,7 @@
       <c r="BF13" s="190"/>
       <c r="BG13" s="5">
         <f t="shared" si="19"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="BH13" s="28">
         <f>SUM($O$9:O12)</f>
@@ -45333,7 +45325,7 @@
       </c>
       <c r="B14" s="40">
         <f t="shared" si="20"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="C14" s="216">
         <f>IF(B14&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -45441,7 +45433,7 @@
       </c>
       <c r="X14" s="224">
         <f t="shared" si="23"/>
-        <v>53.637025135563896</v>
+        <v>60.9920251355639</v>
       </c>
       <c r="Y14" s="224">
         <f t="shared" si="24"/>
@@ -45449,7 +45441,7 @@
       </c>
       <c r="Z14" s="224">
         <f t="shared" si="25"/>
-        <v>-144.87813494066461</v>
+        <v>-137.52313494066462</v>
       </c>
       <c r="AA14" s="224">
         <f>IF(SUM(AA$9:AA13)&gt;0,0,IF(SUM(X14-R14)&gt;0,B14,0))</f>
@@ -45457,7 +45449,7 @@
       </c>
       <c r="AB14" s="224">
         <f>ABS(Z14)*1000000/SUM(U$9:U14)</f>
-        <v>2544.9979835018717</v>
+        <v>2054.8345854105228</v>
       </c>
       <c r="AH14" s="19">
         <f t="shared" si="26"/>
@@ -45482,7 +45474,7 @@
       <c r="AO14" s="14"/>
       <c r="AP14" s="15">
         <f t="shared" si="15"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="AQ14" s="29">
         <f t="shared" si="0"/>
@@ -45491,7 +45483,7 @@
       <c r="AR14" s="14"/>
       <c r="AS14" s="54">
         <f t="shared" si="16"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="AT14" s="29">
         <f>SUM($M$9:$M13)</f>
@@ -45532,7 +45524,7 @@
       <c r="BC14" s="14"/>
       <c r="BD14" s="15">
         <f t="shared" si="17"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="BE14" s="29">
         <f t="shared" si="18"/>
@@ -45541,7 +45533,7 @@
       <c r="BF14" s="14"/>
       <c r="BG14" s="15">
         <f t="shared" si="19"/>
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="BH14" s="29">
         <f>SUM($O$9:O13)</f>
@@ -45561,7 +45553,7 @@
       </c>
       <c r="B15" s="41">
         <f t="shared" si="20"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="C15" s="216">
         <f>IF(B15&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -45669,7 +45661,7 @@
       </c>
       <c r="X15" s="217">
         <f t="shared" si="23"/>
-        <v>69.555152618833233</v>
+        <v>76.910152618833237</v>
       </c>
       <c r="Y15" s="217">
         <f t="shared" si="24"/>
@@ -45677,7 +45669,7 @@
       </c>
       <c r="Z15" s="217">
         <f t="shared" si="25"/>
-        <v>-131.7075060194727</v>
+        <v>-124.3525060194727</v>
       </c>
       <c r="AA15" s="217">
         <f>IF(SUM(AA$9:AA14)&gt;0,0,IF(SUM(X15-R15)&gt;0,B15,0))</f>
@@ -45685,7 +45677,7 @@
       </c>
       <c r="AB15" s="217">
         <f>ABS(Z15)*1000000/SUM(U$9:U15)</f>
-        <v>1858.8776369532677</v>
+        <v>1538.0027294381312</v>
       </c>
       <c r="AH15" s="17">
         <f t="shared" si="26"/>
@@ -45709,7 +45701,7 @@
       </c>
       <c r="AP15" s="5">
         <f t="shared" si="15"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="AQ15" s="28">
         <f t="shared" si="0"/>
@@ -45717,7 +45709,7 @@
       </c>
       <c r="AS15" s="57">
         <f t="shared" si="16"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="AT15" s="28">
         <f t="shared" ref="AT15:AT50" si="30">SUM(M10:M14)</f>
@@ -45757,7 +45749,7 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="17"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="BE15" s="28">
         <f t="shared" si="18"/>
@@ -45766,7 +45758,7 @@
       <c r="BF15" s="190"/>
       <c r="BG15" s="5">
         <f t="shared" si="19"/>
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="BH15" s="28">
         <f>SUM($O$9:O14)</f>
@@ -45784,7 +45776,7 @@
       </c>
       <c r="B16" s="40">
         <f t="shared" si="20"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="C16" s="216">
         <f>IF(B16&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -45892,7 +45884,7 @@
       </c>
       <c r="X16" s="224">
         <f t="shared" si="23"/>
-        <v>86.573483139003955</v>
+        <v>93.928483139003959</v>
       </c>
       <c r="Y16" s="224">
         <f t="shared" si="24"/>
@@ -45900,7 +45892,7 @@
       </c>
       <c r="Z16" s="224">
         <f t="shared" si="25"/>
-        <v>-117.52741216419325</v>
+        <v>-110.17241216419325</v>
       </c>
       <c r="AA16" s="224">
         <f>IF(SUM(AA$9:AA15)&gt;0,0,IF(SUM(X16-R16)&gt;0,B16,0))</f>
@@ -45908,7 +45900,7 @@
       </c>
       <c r="AB16" s="224">
         <f>ABS(Z16)*1000000/SUM(U$9:U16)</f>
-        <v>1386.2656669724852</v>
+        <v>1162.4031693279417</v>
       </c>
       <c r="AH16" s="19">
         <f t="shared" si="26"/>
@@ -45933,7 +45925,7 @@
       <c r="AO16" s="14"/>
       <c r="AP16" s="15">
         <f t="shared" si="15"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="AQ16" s="29">
         <f t="shared" si="0"/>
@@ -45942,7 +45934,7 @@
       <c r="AR16" s="14"/>
       <c r="AS16" s="54">
         <f t="shared" si="16"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="AT16" s="29">
         <f t="shared" si="30"/>
@@ -45983,7 +45975,7 @@
       <c r="BC16" s="14"/>
       <c r="BD16" s="15">
         <f t="shared" si="17"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="BE16" s="29">
         <f t="shared" si="18"/>
@@ -45992,7 +45984,7 @@
       <c r="BF16" s="14"/>
       <c r="BG16" s="15">
         <f t="shared" si="19"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="BH16" s="29">
         <f>SUM($O$9:O15)</f>
@@ -46012,7 +46004,7 @@
       </c>
       <c r="B17" s="41">
         <f t="shared" si="20"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="C17" s="216">
         <f>IF(B17&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -46120,7 +46112,7 @@
       </c>
       <c r="X17" s="217">
         <f t="shared" si="23"/>
-        <v>104.19065835014631</v>
+        <v>111.54565835014631</v>
       </c>
       <c r="Y17" s="217">
         <f t="shared" si="24"/>
@@ -46128,7 +46120,7 @@
       </c>
       <c r="Z17" s="217">
         <f t="shared" si="25"/>
-        <v>-102.8422663896785</v>
+        <v>-95.487266389678496</v>
       </c>
       <c r="AA17" s="217">
         <f>IF(SUM(AA$9:AA16)&gt;0,0,IF(SUM(X17-R17)&gt;0,B17,0))</f>
@@ -46136,7 +46128,7 @@
       </c>
       <c r="AB17" s="217">
         <f>ABS(Z17)*1000000/SUM(U$9:U17)</f>
-        <v>1041.8998163836773</v>
+        <v>878.39532527360859</v>
       </c>
       <c r="AH17" s="17">
         <f t="shared" si="26"/>
@@ -46160,7 +46152,7 @@
       </c>
       <c r="AP17" s="5">
         <f t="shared" si="15"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="AQ17" s="28">
         <f t="shared" si="0"/>
@@ -46168,7 +46160,7 @@
       </c>
       <c r="AS17" s="57">
         <f t="shared" si="16"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="AT17" s="28">
         <f t="shared" si="30"/>
@@ -46208,7 +46200,7 @@
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="17"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="BE17" s="28">
         <f t="shared" si="18"/>
@@ -46217,7 +46209,7 @@
       <c r="BF17" s="190"/>
       <c r="BG17" s="5">
         <f t="shared" si="19"/>
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="BH17" s="28">
         <f>SUM($O$9:O16)</f>
@@ -46235,7 +46227,7 @@
       </c>
       <c r="B18" s="40">
         <f t="shared" si="20"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="C18" s="216">
         <f>IF(B18&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -46343,7 +46335,7 @@
       </c>
       <c r="X18" s="224">
         <f t="shared" si="23"/>
-        <v>123.43724818556032</v>
+        <v>130.79224818556034</v>
       </c>
       <c r="Y18" s="224">
         <f t="shared" si="24"/>
@@ -46351,7 +46343,7 @@
       </c>
       <c r="Z18" s="224">
         <f t="shared" si="25"/>
-        <v>-86.624658372652078</v>
+        <v>-79.26965837265206</v>
       </c>
       <c r="AA18" s="224">
         <f>IF(SUM(AA$9:AA17)&gt;0,0,IF(SUM(X18-R18)&gt;0,B18,0))</f>
@@ -46359,7 +46351,7 @@
       </c>
       <c r="AB18" s="224">
         <f>ABS(Z18)*1000000/SUM(U$9:U18)</f>
-        <v>769.08702328976187</v>
+        <v>646.39690299559004</v>
       </c>
       <c r="AH18" s="19">
         <f t="shared" si="26"/>
@@ -46384,7 +46376,7 @@
       <c r="AO18" s="16"/>
       <c r="AP18" s="15">
         <f t="shared" si="15"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="AQ18" s="29">
         <f t="shared" si="0"/>
@@ -46393,7 +46385,7 @@
       <c r="AR18" s="16"/>
       <c r="AS18" s="55">
         <f t="shared" si="16"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="AT18" s="29">
         <f t="shared" si="30"/>
@@ -46434,7 +46426,7 @@
       <c r="BC18" s="16"/>
       <c r="BD18" s="15">
         <f t="shared" si="17"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="BE18" s="29">
         <f t="shared" si="18"/>
@@ -46443,7 +46435,7 @@
       <c r="BF18" s="16"/>
       <c r="BG18" s="15">
         <f t="shared" si="19"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="BH18" s="29">
         <f>SUM($O$9:O17)</f>
@@ -46463,7 +46455,7 @@
       </c>
       <c r="B19" s="41">
         <f t="shared" si="20"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="C19" s="216">
         <f>IF(B19&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -46571,7 +46563,7 @@
       </c>
       <c r="X19" s="217">
         <f t="shared" si="23"/>
-        <v>143.82582092003653</v>
+        <v>151.18082092003655</v>
       </c>
       <c r="Y19" s="217">
         <f t="shared" si="24"/>
@@ -46579,7 +46571,7 @@
       </c>
       <c r="Z19" s="217">
         <f t="shared" si="25"/>
-        <v>-69.365288069722681</v>
+        <v>-62.010288069722662</v>
       </c>
       <c r="AA19" s="217">
         <f>IF(SUM(AA$9:AA18)&gt;0,0,IF(SUM(X19-R19)&gt;0,B19,0))</f>
@@ -46587,7 +46579,7 @@
       </c>
       <c r="AB19" s="217">
         <f>ABS(Z19)*1000000/SUM(U$9:U19)</f>
-        <v>548.08343208338533</v>
+        <v>454.08914215202105</v>
       </c>
       <c r="AH19" s="17">
         <f t="shared" si="26"/>
@@ -46612,7 +46604,7 @@
       <c r="AO19" s="2"/>
       <c r="AP19" s="5">
         <f t="shared" si="15"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="AQ19" s="28">
         <f t="shared" si="0"/>
@@ -46621,7 +46613,7 @@
       <c r="AR19" s="2"/>
       <c r="AS19" s="56">
         <f t="shared" si="16"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="AT19" s="28">
         <f t="shared" si="30"/>
@@ -46662,7 +46654,7 @@
       <c r="BC19" s="2"/>
       <c r="BD19" s="5">
         <f t="shared" si="17"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="BE19" s="28">
         <f t="shared" si="18"/>
@@ -46671,7 +46663,7 @@
       <c r="BF19" s="2"/>
       <c r="BG19" s="5">
         <f t="shared" si="19"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="BH19" s="28">
         <f>SUM($O$9:O18)</f>
@@ -46689,7 +46681,7 @@
       </c>
       <c r="B20" s="40">
         <f t="shared" si="20"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="C20" s="216">
         <f>IF(B20&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -46797,7 +46789,7 @@
       </c>
       <c r="X20" s="224">
         <f t="shared" si="23"/>
-        <v>164.96643117340736</v>
+        <v>172.32143117340738</v>
       </c>
       <c r="Y20" s="224">
         <f t="shared" si="24"/>
@@ -46805,7 +46797,7 @@
       </c>
       <c r="Z20" s="224">
         <f t="shared" si="25"/>
-        <v>-51.457481525796993</v>
+        <v>-44.102481525796975</v>
       </c>
       <c r="AA20" s="224">
         <f>IF(SUM(AA$9:AA19)&gt;0,0,IF(SUM(X20-R20)&gt;0,B20,0))</f>
@@ -46813,7 +46805,7 @@
       </c>
       <c r="AB20" s="224">
         <f>ABS(Z20)*1000000/SUM(U$9:U20)</f>
-        <v>366.28101834702755</v>
+        <v>293.06633444728226</v>
       </c>
       <c r="AH20" s="19">
         <f t="shared" si="26"/>
@@ -46838,7 +46830,7 @@
       <c r="AO20" s="14"/>
       <c r="AP20" s="15">
         <f t="shared" si="15"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="AQ20" s="29">
         <f t="shared" si="0"/>
@@ -46847,7 +46839,7 @@
       <c r="AR20" s="14"/>
       <c r="AS20" s="54">
         <f t="shared" si="16"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="AT20" s="29">
         <f t="shared" si="30"/>
@@ -46888,7 +46880,7 @@
       <c r="BC20" s="14"/>
       <c r="BD20" s="15">
         <f t="shared" si="17"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="BE20" s="29">
         <f t="shared" si="18"/>
@@ -46897,7 +46889,7 @@
       <c r="BF20" s="14"/>
       <c r="BG20" s="15">
         <f t="shared" si="19"/>
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="BH20" s="29">
         <f>SUM($O$9:O19)</f>
@@ -46915,7 +46907,7 @@
       </c>
       <c r="B21" s="41">
         <f t="shared" si="20"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="C21" s="216">
         <f>IF(B21&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -47023,7 +47015,7 @@
       </c>
       <c r="X21" s="217">
         <f t="shared" si="23"/>
-        <v>188.2795942591404</v>
+        <v>195.63459425914041</v>
       </c>
       <c r="Y21" s="217">
         <f t="shared" si="24"/>
@@ -47031,7 +47023,7 @@
       </c>
       <c r="Z21" s="217">
         <f t="shared" si="25"/>
-        <v>-31.484220473942457</v>
+        <v>-24.129220473942439</v>
       </c>
       <c r="AA21" s="217">
         <f>IF(SUM(AA$9:AA20)&gt;0,0,IF(SUM(X21-R21)&gt;0,B21,0))</f>
@@ -47039,7 +47031,7 @@
       </c>
       <c r="AB21" s="217">
         <f>ABS(Z21)*1000000/SUM(U$9:U21)</f>
-        <v>203.89622282390516</v>
+        <v>146.75983954238163</v>
       </c>
       <c r="AH21" s="17">
         <f t="shared" si="26"/>
@@ -47063,7 +47055,7 @@
       </c>
       <c r="AP21" s="5">
         <f t="shared" si="15"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="AQ21" s="28">
         <f t="shared" si="0"/>
@@ -47071,7 +47063,7 @@
       </c>
       <c r="AS21" s="57">
         <f t="shared" si="16"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="AT21" s="28">
         <f t="shared" si="30"/>
@@ -47111,7 +47103,7 @@
       </c>
       <c r="BD21" s="5">
         <f t="shared" si="17"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="BE21" s="28">
         <f t="shared" si="18"/>
@@ -47120,7 +47112,7 @@
       <c r="BF21" s="190"/>
       <c r="BG21" s="5">
         <f t="shared" si="19"/>
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="BH21" s="28">
         <f>SUM($O$9:O20)</f>
@@ -47138,7 +47130,7 @@
       </c>
       <c r="B22" s="40">
         <f t="shared" si="20"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="C22" s="216">
         <f>IF(B22&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -47246,7 +47238,7 @@
       </c>
       <c r="X22" s="224">
         <f t="shared" si="23"/>
-        <v>213.12468562410322</v>
+        <v>220.47968562410324</v>
       </c>
       <c r="Y22" s="224">
         <f t="shared" si="24"/>
@@ -47254,7 +47246,7 @@
       </c>
       <c r="Z22" s="224">
         <f t="shared" si="25"/>
-        <v>-10.089746985550477</v>
+        <v>-2.7347469855504585</v>
       </c>
       <c r="AA22" s="224">
         <f>IF(SUM(AA$9:AA21)&gt;0,0,IF(SUM(X22-R22)&gt;0,B22,0))</f>
@@ -47262,7 +47254,7 @@
       </c>
       <c r="AB22" s="224">
         <f>ABS(Z22)*1000000/SUM(U$9:U22)</f>
-        <v>59.936864503366365</v>
+        <v>15.334492130942543</v>
       </c>
       <c r="AH22" s="19">
         <f t="shared" si="26"/>
@@ -47287,7 +47279,7 @@
       <c r="AO22" s="14"/>
       <c r="AP22" s="15">
         <f t="shared" si="15"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="AQ22" s="29">
         <f t="shared" si="0"/>
@@ -47296,7 +47288,7 @@
       <c r="AR22" s="14"/>
       <c r="AS22" s="54">
         <f t="shared" si="16"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="AT22" s="29">
         <f t="shared" si="30"/>
@@ -47337,7 +47329,7 @@
       <c r="BC22" s="14"/>
       <c r="BD22" s="15">
         <f t="shared" si="17"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="BE22" s="29">
         <f t="shared" si="18"/>
@@ -47346,7 +47338,7 @@
       <c r="BF22" s="14"/>
       <c r="BG22" s="15">
         <f t="shared" si="19"/>
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="BH22" s="29">
         <f>SUM($O$9:O21)</f>
@@ -47366,7 +47358,7 @@
       </c>
       <c r="B23" s="41">
         <f t="shared" si="20"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="C23" s="216">
         <f>IF(B23&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -47474,7 +47466,7 @@
       </c>
       <c r="X23" s="217">
         <f t="shared" si="23"/>
-        <v>238.66610802507955</v>
+        <v>246.02110802507957</v>
       </c>
       <c r="Y23" s="217">
         <f t="shared" si="24"/>
@@ -47482,15 +47474,15 @@
       </c>
       <c r="Z23" s="217">
         <f t="shared" si="25"/>
-        <v>11.886599469614879</v>
+        <v>19.241599469614897</v>
       </c>
       <c r="AA23" s="217">
         <f>IF(SUM(AA$9:AA22)&gt;0,0,IF(SUM(X23-R23)&gt;0,B23,0))</f>
-        <v>2032</v>
+        <v>0</v>
       </c>
       <c r="AB23" s="217">
         <f>ABS(Z23)*1000000/SUM(U$9:U23)</f>
-        <v>65.215596747428108</v>
+        <v>100.0779063027361</v>
       </c>
       <c r="AH23" s="17">
         <f t="shared" si="26"/>
@@ -47514,7 +47506,7 @@
       </c>
       <c r="AP23" s="5">
         <f t="shared" si="15"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="AQ23" s="28">
         <f t="shared" si="0"/>
@@ -47522,7 +47514,7 @@
       </c>
       <c r="AS23" s="57">
         <f t="shared" si="16"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="AT23" s="28">
         <f t="shared" si="30"/>
@@ -47562,7 +47554,7 @@
       </c>
       <c r="BD23" s="5">
         <f t="shared" si="17"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="BE23" s="28">
         <f t="shared" si="18"/>
@@ -47571,7 +47563,7 @@
       <c r="BF23" s="190"/>
       <c r="BG23" s="5">
         <f t="shared" si="19"/>
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="BH23" s="28">
         <f>SUM($O$9:O22)</f>
@@ -47589,7 +47581,7 @@
       </c>
       <c r="B24" s="40">
         <f t="shared" si="20"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="C24" s="216">
         <f>IF(B24&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -47697,7 +47689,7 @@
       </c>
       <c r="X24" s="224">
         <f t="shared" si="23"/>
-        <v>267.22960712235465</v>
+        <v>274.58460712235467</v>
       </c>
       <c r="Y24" s="224">
         <f t="shared" si="24"/>
@@ -47705,7 +47697,7 @@
       </c>
       <c r="Z24" s="224">
         <f t="shared" si="25"/>
-        <v>36.766693228443899</v>
+        <v>44.121693228443917</v>
       </c>
       <c r="AA24" s="224">
         <f>IF(SUM(AA$9:AA23)&gt;0,0,IF(SUM(X24-R24)&gt;0,B24,0))</f>
@@ -47713,7 +47705,7 @@
       </c>
       <c r="AB24" s="224">
         <f>ABS(Z24)*1000000/SUM(U$9:U24)</f>
-        <v>187.40080163826408</v>
+        <v>213.98267666674366</v>
       </c>
       <c r="AH24" s="19">
         <f t="shared" si="26"/>
@@ -47738,7 +47730,7 @@
       <c r="AO24" s="14"/>
       <c r="AP24" s="15">
         <f t="shared" si="15"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="AQ24" s="29">
         <f t="shared" si="0"/>
@@ -47747,7 +47739,7 @@
       <c r="AR24" s="14"/>
       <c r="AS24" s="54">
         <f t="shared" si="16"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="AT24" s="29">
         <f t="shared" si="30"/>
@@ -47788,7 +47780,7 @@
       <c r="BC24" s="14"/>
       <c r="BD24" s="15">
         <f t="shared" si="17"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="BE24" s="29">
         <f t="shared" si="18"/>
@@ -47797,7 +47789,7 @@
       <c r="BF24" s="14"/>
       <c r="BG24" s="15">
         <f t="shared" si="19"/>
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="BH24" s="29">
         <f>SUM($O$9:O23)</f>
@@ -47817,7 +47809,7 @@
       </c>
       <c r="B25" s="41">
         <f t="shared" si="20"/>
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="C25" s="216">
         <f>IF(B25&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -47925,7 +47917,7 @@
       </c>
       <c r="X25" s="217">
         <f t="shared" si="23"/>
-        <v>296.60085022140544</v>
+        <v>303.95585022140546</v>
       </c>
       <c r="Y25" s="217">
         <f t="shared" si="24"/>
@@ -47933,7 +47925,7 @@
       </c>
       <c r="Z25" s="217">
         <f t="shared" si="25"/>
-        <v>62.332196630064061</v>
+        <v>69.687196630064079</v>
       </c>
       <c r="AA25" s="217">
         <f>IF(SUM(AA$9:AA24)&gt;0,0,IF(SUM(X25-R25)&gt;0,B25,0))</f>
@@ -47941,7 +47933,7 @@
       </c>
       <c r="AB25" s="217">
         <f>ABS(Z25)*1000000/SUM(U$9:U25)</f>
-        <v>296.65124781426152</v>
+        <v>316.58809369002017</v>
       </c>
       <c r="AH25" s="17">
         <f t="shared" si="26"/>
@@ -47965,7 +47957,7 @@
       </c>
       <c r="AP25" s="5">
         <f t="shared" si="15"/>
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="AQ25" s="28">
         <f t="shared" si="0"/>
@@ -47973,7 +47965,7 @@
       </c>
       <c r="AS25" s="57">
         <f t="shared" si="16"/>
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="AT25" s="28">
         <f t="shared" si="30"/>
@@ -48013,7 +48005,7 @@
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="17"/>
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="BE25" s="28">
         <f t="shared" si="18"/>
@@ -48022,7 +48014,7 @@
       <c r="BF25" s="190"/>
       <c r="BG25" s="5">
         <f t="shared" si="19"/>
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="BH25" s="28">
         <f t="shared" ref="BH25:BH50" si="33">SUM(O10:O24)</f>
@@ -48040,7 +48032,7 @@
       </c>
       <c r="B26" s="40">
         <f t="shared" si="20"/>
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="C26" s="216">
         <f>IF(B26&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -48148,7 +48140,7 @@
       </c>
       <c r="X26" s="224">
         <f t="shared" si="23"/>
-        <v>325.8467537339738</v>
+        <v>333.20175373397382</v>
       </c>
       <c r="Y26" s="224">
         <f t="shared" si="24"/>
@@ -48156,7 +48148,7 @@
       </c>
       <c r="Z26" s="224">
         <f t="shared" si="25"/>
-        <v>87.645882767494442</v>
+        <v>95.00088276749446</v>
       </c>
       <c r="AA26" s="224">
         <f>IF(SUM(AA$9:AA25)&gt;0,0,IF(SUM(X26-R26)&gt;0,B26,0))</f>
@@ -48164,7 +48156,7 @@
       </c>
       <c r="AB26" s="224">
         <f>ABS(Z26)*1000000/SUM(U$9:U26)</f>
-        <v>391.19580636466151</v>
+        <v>405.90676453506211</v>
       </c>
       <c r="AH26" s="19">
         <f t="shared" si="26"/>
@@ -48189,7 +48181,7 @@
       <c r="AO26" s="14"/>
       <c r="AP26" s="15">
         <f t="shared" si="15"/>
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="AQ26" s="29">
         <f t="shared" si="0"/>
@@ -48198,7 +48190,7 @@
       <c r="AR26" s="14"/>
       <c r="AS26" s="54">
         <f t="shared" si="16"/>
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="AT26" s="29">
         <f t="shared" si="30"/>
@@ -48239,7 +48231,7 @@
       <c r="BC26" s="14"/>
       <c r="BD26" s="15">
         <f t="shared" si="17"/>
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="BE26" s="29">
         <f t="shared" si="18"/>
@@ -48248,7 +48240,7 @@
       <c r="BF26" s="14"/>
       <c r="BG26" s="15">
         <f t="shared" si="19"/>
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="BH26" s="29">
         <f t="shared" si="33"/>
@@ -48268,7 +48260,7 @@
       </c>
       <c r="B27" s="41">
         <f t="shared" si="20"/>
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="C27" s="216">
         <f>IF(B27&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -48376,7 +48368,7 @@
       </c>
       <c r="X27" s="217">
         <f t="shared" si="23"/>
-        <v>356.98667766449893</v>
+        <v>364.34167766449895</v>
       </c>
       <c r="Y27" s="217">
         <f t="shared" si="24"/>
@@ -48384,7 +48376,7 @@
       </c>
       <c r="Z27" s="217">
         <f t="shared" si="25"/>
-        <v>114.72282509537166</v>
+        <v>122.07782509537168</v>
       </c>
       <c r="AA27" s="217">
         <f>IF(SUM(AA$9:AA26)&gt;0,0,IF(SUM(X27-R27)&gt;0,B27,0))</f>
@@ -48392,7 +48384,7 @@
       </c>
       <c r="AB27" s="217">
         <f>ABS(Z27)*1000000/SUM(U$9:U27)</f>
-        <v>482.08399482721461</v>
+        <v>492.30350751174279</v>
       </c>
       <c r="AH27" s="17">
         <f t="shared" si="26"/>
@@ -48416,7 +48408,7 @@
       </c>
       <c r="AP27" s="5">
         <f t="shared" si="15"/>
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="AQ27" s="28">
         <f t="shared" si="0"/>
@@ -48424,7 +48416,7 @@
       </c>
       <c r="AS27" s="57">
         <f t="shared" si="16"/>
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="AT27" s="28">
         <f t="shared" si="30"/>
@@ -48464,7 +48456,7 @@
       </c>
       <c r="BD27" s="5">
         <f t="shared" si="17"/>
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="BE27" s="28">
         <f t="shared" si="18"/>
@@ -48473,7 +48465,7 @@
       <c r="BF27" s="190"/>
       <c r="BG27" s="5">
         <f t="shared" si="19"/>
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="BH27" s="28">
         <f t="shared" si="33"/>
@@ -48491,7 +48483,7 @@
       </c>
       <c r="B28" s="40">
         <f t="shared" si="20"/>
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="C28" s="216">
         <f>IF(B28&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -48599,7 +48591,7 @@
       </c>
       <c r="X28" s="224">
         <f t="shared" si="23"/>
-        <v>389.08753842472277</v>
+        <v>396.44253842472278</v>
       </c>
       <c r="Y28" s="224">
         <f t="shared" si="24"/>
@@ -48607,7 +48599,7 @@
       </c>
       <c r="Z28" s="224">
         <f t="shared" si="25"/>
-        <v>142.62550519036211</v>
+        <v>149.98050519036212</v>
       </c>
       <c r="AA28" s="224">
         <f>IF(SUM(AA$9:AA27)&gt;0,0,IF(SUM(X28-R28)&gt;0,B28,0))</f>
@@ -48615,7 +48607,7 @@
       </c>
       <c r="AB28" s="224">
         <f>ABS(Z28)*1000000/SUM(U$9:U28)</f>
-        <v>566.20045817157325</v>
+        <v>572.66475703928165</v>
       </c>
       <c r="AH28" s="19">
         <f t="shared" si="26"/>
@@ -48640,7 +48632,7 @@
       <c r="AO28" s="14"/>
       <c r="AP28" s="15">
         <f t="shared" si="15"/>
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="AQ28" s="29">
         <f t="shared" si="0"/>
@@ -48649,7 +48641,7 @@
       <c r="AR28" s="14"/>
       <c r="AS28" s="54">
         <f t="shared" si="16"/>
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="AT28" s="29">
         <f t="shared" si="30"/>
@@ -48690,7 +48682,7 @@
       <c r="BC28" s="14"/>
       <c r="BD28" s="15">
         <f t="shared" si="17"/>
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="BE28" s="29">
         <f t="shared" si="18"/>
@@ -48699,7 +48691,7 @@
       <c r="BF28" s="14"/>
       <c r="BG28" s="15">
         <f t="shared" si="19"/>
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="BH28" s="29">
         <f t="shared" si="33"/>
@@ -48719,7 +48711,7 @@
       </c>
       <c r="B29" s="41">
         <f t="shared" si="20"/>
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="C29" s="216">
         <f>IF(B29&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -48827,7 +48819,7 @@
       </c>
       <c r="X29" s="217">
         <f t="shared" si="23"/>
-        <v>421.23017904710741</v>
+        <v>428.58517904710743</v>
       </c>
       <c r="Y29" s="217">
         <f t="shared" si="24"/>
@@ -48835,7 +48827,7 @@
       </c>
       <c r="Z29" s="217">
         <f t="shared" si="25"/>
-        <v>170.43017772847008</v>
+        <v>177.7851777284701</v>
       </c>
       <c r="AA29" s="217">
         <f>IF(SUM(AA$9:AA28)&gt;0,0,IF(SUM(X29-R29)&gt;0,B29,0))</f>
@@ -48843,7 +48835,7 @@
       </c>
       <c r="AB29" s="217">
         <f>ABS(Z29)*1000000/SUM(U$9:U29)</f>
-        <v>641.13450765006019</v>
+        <v>644.55570491851267</v>
       </c>
       <c r="AH29" s="17">
         <f t="shared" si="26"/>
@@ -48867,7 +48859,7 @@
       </c>
       <c r="AP29" s="5">
         <f t="shared" si="15"/>
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="AQ29" s="28">
         <f t="shared" si="0"/>
@@ -48875,7 +48867,7 @@
       </c>
       <c r="AS29" s="57">
         <f t="shared" si="16"/>
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="AT29" s="28">
         <f t="shared" si="30"/>
@@ -48915,7 +48907,7 @@
       </c>
       <c r="BD29" s="5">
         <f t="shared" si="17"/>
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="BE29" s="28">
         <f t="shared" si="18"/>
@@ -48924,7 +48916,7 @@
       <c r="BF29" s="190"/>
       <c r="BG29" s="5">
         <f t="shared" si="19"/>
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="BH29" s="28">
         <f t="shared" si="33"/>
@@ -48942,7 +48934,7 @@
       </c>
       <c r="B30" s="40">
         <f t="shared" si="20"/>
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="C30" s="216">
         <f>IF(B30&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -49050,7 +49042,7 @@
       </c>
       <c r="X30" s="224">
         <f t="shared" si="23"/>
-        <v>454.97995170061125</v>
+        <v>462.33495170061127</v>
       </c>
       <c r="Y30" s="224">
         <f t="shared" si="24"/>
@@ -49058,7 +49050,7 @@
       </c>
       <c r="Z30" s="224">
         <f t="shared" si="25"/>
-        <v>199.69744757611923</v>
+        <v>207.05244757611925</v>
       </c>
       <c r="AA30" s="224">
         <f>IF(SUM(AA$9:AA29)&gt;0,0,IF(SUM(X30-R30)&gt;0,B30,0))</f>
@@ -49066,7 +49058,7 @@
       </c>
       <c r="AB30" s="224">
         <f>ABS(Z30)*1000000/SUM(U$9:U30)</f>
-        <v>713.83601677211641</v>
+        <v>714.58368864109752</v>
       </c>
       <c r="AH30" s="19">
         <f t="shared" si="26"/>
@@ -49096,7 +49088,7 @@
       <c r="AO30" s="14"/>
       <c r="AP30" s="15">
         <f t="shared" si="15"/>
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="AQ30" s="29">
         <f t="shared" si="0"/>
@@ -49105,7 +49097,7 @@
       <c r="AR30" s="14"/>
       <c r="AS30" s="54">
         <f t="shared" si="16"/>
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="AT30" s="29">
         <f t="shared" si="30"/>
@@ -49146,7 +49138,7 @@
       <c r="BC30" s="14"/>
       <c r="BD30" s="15">
         <f t="shared" si="17"/>
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="BE30" s="29">
         <f t="shared" si="18"/>
@@ -49155,7 +49147,7 @@
       <c r="BF30" s="14"/>
       <c r="BG30" s="15">
         <f t="shared" si="19"/>
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="BH30" s="29">
         <f t="shared" si="33"/>
@@ -49175,7 +49167,7 @@
       </c>
       <c r="B31" s="41">
         <f t="shared" si="20"/>
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="C31" s="216">
         <f>IF(B31&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -49283,7 +49275,7 @@
       </c>
       <c r="X31" s="217">
         <f t="shared" si="23"/>
-        <v>490.41721298679033</v>
+        <v>497.77221298679035</v>
       </c>
       <c r="Y31" s="217">
         <f t="shared" si="24"/>
@@ -49291,7 +49283,7 @@
       </c>
       <c r="Z31" s="217">
         <f t="shared" si="25"/>
-        <v>230.50275946605626</v>
+        <v>237.85775946605628</v>
       </c>
       <c r="AA31" s="217">
         <f>IF(SUM(AA$9:AA30)&gt;0,0,IF(SUM(X31-R31)&gt;0,B31,0))</f>
@@ -49299,7 +49291,7 @@
       </c>
       <c r="AB31" s="217">
         <f>ABS(Z31)*1000000/SUM(U$9:U31)</f>
-        <v>784.87948988343112</v>
+        <v>783.25344851215993</v>
       </c>
       <c r="AH31" s="17">
         <f t="shared" si="26"/>
@@ -49328,7 +49320,7 @@
       </c>
       <c r="AP31" s="5">
         <f t="shared" si="15"/>
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="AQ31" s="28">
         <f t="shared" si="0"/>
@@ -49336,7 +49328,7 @@
       </c>
       <c r="AS31" s="57">
         <f t="shared" si="16"/>
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="AT31" s="28">
         <f t="shared" si="30"/>
@@ -49376,7 +49368,7 @@
       </c>
       <c r="BD31" s="5">
         <f t="shared" si="17"/>
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="BE31" s="28">
         <f t="shared" si="18"/>
@@ -49385,7 +49377,7 @@
       <c r="BF31" s="190"/>
       <c r="BG31" s="5">
         <f t="shared" si="19"/>
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="BH31" s="28">
         <f t="shared" si="33"/>
@@ -49403,7 +49395,7 @@
       </c>
       <c r="B32" s="40">
         <f t="shared" si="20"/>
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="C32" s="216">
         <f>IF(B32&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -49511,7 +49503,7 @@
       </c>
       <c r="X32" s="224">
         <f t="shared" si="23"/>
-        <v>527.6263373372783</v>
+        <v>534.98133733727832</v>
       </c>
       <c r="Y32" s="224">
         <f t="shared" si="24"/>
@@ -49519,7 +49511,7 @@
       </c>
       <c r="Z32" s="224">
         <f t="shared" si="25"/>
-        <v>262.92540557195474</v>
+        <v>270.28040557195476</v>
       </c>
       <c r="AA32" s="224">
         <f>IF(SUM(AA$9:AA31)&gt;0,0,IF(SUM(X32-R32)&gt;0,B32,0))</f>
@@ -49527,7 +49519,7 @@
       </c>
       <c r="AB32" s="224">
         <f>ABS(Z32)*1000000/SUM(U$9:U32)</f>
-        <v>854.74789802261944</v>
+        <v>850.9933097753775</v>
       </c>
       <c r="AH32" s="19">
         <f t="shared" si="26"/>
@@ -49557,7 +49549,7 @@
       <c r="AO32" s="14"/>
       <c r="AP32" s="15">
         <f t="shared" si="15"/>
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="AQ32" s="29">
         <f t="shared" si="0"/>
@@ -49566,7 +49558,7 @@
       <c r="AR32" s="14"/>
       <c r="AS32" s="54">
         <f t="shared" si="16"/>
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="AT32" s="29">
         <f t="shared" si="30"/>
@@ -49607,7 +49599,7 @@
       <c r="BC32" s="14"/>
       <c r="BD32" s="15">
         <f t="shared" si="17"/>
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="BE32" s="29">
         <f t="shared" si="18"/>
@@ -49616,7 +49608,7 @@
       <c r="BF32" s="14"/>
       <c r="BG32" s="15">
         <f t="shared" si="19"/>
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="BH32" s="29">
         <f t="shared" si="33"/>
@@ -49636,7 +49628,7 @@
       </c>
       <c r="B33" s="41">
         <f t="shared" si="20"/>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="C33" s="216">
         <f>IF(B33&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -49744,7 +49736,7 @@
       </c>
       <c r="X33" s="217">
         <f t="shared" si="23"/>
-        <v>566.69591790529068</v>
+        <v>574.0509179052907</v>
       </c>
       <c r="Y33" s="217">
         <f t="shared" si="24"/>
@@ -49752,7 +49744,7 @@
       </c>
       <c r="Z33" s="217">
         <f t="shared" si="25"/>
-        <v>297.04872036692132</v>
+        <v>304.40372036692133</v>
       </c>
       <c r="AA33" s="217">
         <f>IF(SUM(AA$9:AA32)&gt;0,0,IF(SUM(X33-R33)&gt;0,B33,0))</f>
@@ -49760,7 +49752,7 @@
       </c>
       <c r="AB33" s="217">
         <f>ABS(Z33)*1000000/SUM(U$9:U33)</f>
-        <v>923.85310798674107</v>
+        <v>918.17182013063359</v>
       </c>
       <c r="AH33" s="17">
         <f t="shared" si="26"/>
@@ -49788,7 +49780,7 @@
       </c>
       <c r="AP33" s="5">
         <f t="shared" si="15"/>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="AQ33" s="28">
         <f t="shared" si="0"/>
@@ -49796,7 +49788,7 @@
       </c>
       <c r="AS33" s="57">
         <f t="shared" si="16"/>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="AT33" s="28">
         <f t="shared" si="30"/>
@@ -49836,7 +49828,7 @@
       </c>
       <c r="BD33" s="5">
         <f t="shared" si="17"/>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="BE33" s="28">
         <f t="shared" si="18"/>
@@ -49845,7 +49837,7 @@
       <c r="BF33" s="190"/>
       <c r="BG33" s="5">
         <f t="shared" si="19"/>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="BH33" s="28">
         <f t="shared" si="33"/>
@@ -49863,7 +49855,7 @@
       </c>
       <c r="B34" s="40">
         <f t="shared" si="20"/>
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="C34" s="216">
         <f>IF(B34&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -49971,7 +49963,7 @@
       </c>
       <c r="X34" s="224">
         <f t="shared" si="23"/>
-        <v>607.71897750170376</v>
+        <v>615.07397750170378</v>
       </c>
       <c r="Y34" s="224">
         <f t="shared" si="24"/>
@@ -49979,7 +49971,7 @@
       </c>
       <c r="Z34" s="224">
         <f t="shared" si="25"/>
-        <v>332.96028530873389</v>
+        <v>340.31528530873391</v>
       </c>
       <c r="AA34" s="224">
         <f>IF(SUM(AA$9:AA33)&gt;0,0,IF(SUM(X34-R34)&gt;0,B34,0))</f>
@@ -49987,7 +49979,7 @@
       </c>
       <c r="AB34" s="224">
         <f>ABS(Z34)*1000000/SUM(U$9:U34)</f>
-        <v>992.55125200007433</v>
+        <v>985.11039140985815</v>
       </c>
       <c r="AH34" s="19">
         <f t="shared" si="26"/>
@@ -50017,7 +50009,7 @@
       <c r="AO34" s="14"/>
       <c r="AP34" s="15">
         <f t="shared" si="15"/>
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="AQ34" s="29">
         <f t="shared" si="0"/>
@@ -50026,7 +50018,7 @@
       <c r="AR34" s="14"/>
       <c r="AS34" s="54">
         <f t="shared" si="16"/>
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="AT34" s="29">
         <f t="shared" si="30"/>
@@ -50067,7 +50059,7 @@
       <c r="BC34" s="14"/>
       <c r="BD34" s="15">
         <f t="shared" si="17"/>
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="BE34" s="29">
         <f t="shared" si="18"/>
@@ -50076,7 +50068,7 @@
       <c r="BF34" s="14"/>
       <c r="BG34" s="15">
         <f t="shared" si="19"/>
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="BH34" s="29">
         <f t="shared" si="33"/>
@@ -50096,7 +50088,7 @@
       </c>
       <c r="B35" s="41">
         <f t="shared" si="20"/>
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="C35" s="216">
         <f>IF(B35&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -50204,7 +50196,7 @@
       </c>
       <c r="X35" s="217">
         <f t="shared" si="23"/>
-        <v>650.79319007793742</v>
+        <v>658.14819007793744</v>
       </c>
       <c r="Y35" s="217">
         <f t="shared" si="24"/>
@@ -50212,7 +50204,7 @@
       </c>
       <c r="Z35" s="217">
         <f t="shared" si="25"/>
-        <v>370.75214384603117</v>
+        <v>378.10714384603119</v>
       </c>
       <c r="AA35" s="217">
         <f>IF(SUM(AA$9:AA34)&gt;0,0,IF(SUM(X35-R35)&gt;0,B35,0))</f>
@@ -50220,7 +50212,7 @@
       </c>
       <c r="AB35" s="217">
         <f>ABS(Z35)*1000000/SUM(U$9:U35)</f>
-        <v>1061.154451084557</v>
+        <v>1052.0930306915252</v>
       </c>
       <c r="AH35" s="17">
         <f t="shared" si="26"/>
@@ -50249,7 +50241,7 @@
       </c>
       <c r="AP35" s="5">
         <f t="shared" si="15"/>
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="AQ35" s="28">
         <f t="shared" si="0"/>
@@ -50257,7 +50249,7 @@
       </c>
       <c r="AS35" s="57">
         <f t="shared" si="16"/>
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="AT35" s="28">
         <f t="shared" si="30"/>
@@ -50297,7 +50289,7 @@
       </c>
       <c r="BD35" s="5">
         <f t="shared" si="17"/>
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="BE35" s="28">
         <f t="shared" si="18"/>
@@ -50306,7 +50298,7 @@
       <c r="BF35" s="190"/>
       <c r="BG35" s="5">
         <f t="shared" si="19"/>
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="BH35" s="28">
         <f t="shared" si="33"/>
@@ -50324,7 +50316,7 @@
       </c>
       <c r="B36" s="40">
         <f t="shared" si="20"/>
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="C36" s="216">
         <f>IF(B36&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -50432,7 +50424,7 @@
       </c>
       <c r="X36" s="224">
         <f t="shared" si="23"/>
-        <v>696.02111328298281</v>
+        <v>703.37611328298283</v>
       </c>
       <c r="Y36" s="224">
         <f t="shared" si="24"/>
@@ -50440,7 +50432,7 @@
       </c>
       <c r="Z36" s="224">
         <f t="shared" si="25"/>
-        <v>410.52102726448629</v>
+        <v>417.87602726448631</v>
       </c>
       <c r="AA36" s="224">
         <f>IF(SUM(AA$9:AA35)&gt;0,0,IF(SUM(X36-R36)&gt;0,B36,0))</f>
@@ -50448,7 +50440,7 @@
       </c>
       <c r="AB36" s="224">
         <f>ABS(Z36)*1000000/SUM(U$9:U36)</f>
-        <v>1129.9398719593132</v>
+        <v>1119.3739223048462</v>
       </c>
       <c r="AH36" s="19">
         <f t="shared" si="26"/>
@@ -50478,7 +50470,7 @@
       <c r="AO36" s="14"/>
       <c r="AP36" s="15">
         <f t="shared" si="15"/>
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="AQ36" s="29">
         <f t="shared" si="0"/>
@@ -50487,7 +50479,7 @@
       <c r="AR36" s="14"/>
       <c r="AS36" s="54">
         <f t="shared" si="16"/>
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="AT36" s="29">
         <f t="shared" si="30"/>
@@ -50528,7 +50520,7 @@
       <c r="BC36" s="14"/>
       <c r="BD36" s="15">
         <f t="shared" si="17"/>
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="BE36" s="29">
         <f t="shared" si="18"/>
@@ -50537,7 +50529,7 @@
       <c r="BF36" s="14"/>
       <c r="BG36" s="15">
         <f t="shared" si="19"/>
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="BH36" s="29">
         <f t="shared" si="33"/>
@@ -50557,7 +50549,7 @@
       </c>
       <c r="B37" s="41">
         <f t="shared" si="20"/>
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="C37" s="216">
         <f>IF(B37&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -50665,7 +50657,7 @@
       </c>
       <c r="X37" s="217">
         <f t="shared" si="23"/>
-        <v>743.51043264828047</v>
+        <v>750.86543264828049</v>
       </c>
       <c r="Y37" s="217">
         <f t="shared" si="24"/>
@@ -50673,7 +50665,7 @@
       </c>
       <c r="Z37" s="217">
         <f t="shared" si="25"/>
-        <v>452.36859191805075</v>
+        <v>459.72359191805077</v>
       </c>
       <c r="AA37" s="217">
         <f>IF(SUM(AA$9:AA36)&gt;0,0,IF(SUM(X37-R37)&gt;0,B37,0))</f>
@@ -50681,7 +50673,7 @@
       </c>
       <c r="AB37" s="217">
         <f>ABS(Z37)*1000000/SUM(U$9:U37)</f>
-        <v>1199.1568079855194</v>
+        <v>1187.1834031639864</v>
       </c>
       <c r="AH37" s="17">
         <f t="shared" si="26"/>
@@ -50711,7 +50703,7 @@
       <c r="AO37" s="190"/>
       <c r="AP37" s="5">
         <f t="shared" si="15"/>
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="AQ37" s="28">
         <f t="shared" si="0"/>
@@ -50720,7 +50712,7 @@
       <c r="AR37" s="190"/>
       <c r="AS37" s="57">
         <f t="shared" si="16"/>
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="AT37" s="28">
         <f t="shared" si="30"/>
@@ -50761,7 +50753,7 @@
       <c r="BC37" s="190"/>
       <c r="BD37" s="5">
         <f t="shared" si="17"/>
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="BE37" s="28">
         <f t="shared" si="18"/>
@@ -50770,7 +50762,7 @@
       <c r="BF37" s="190"/>
       <c r="BG37" s="5">
         <f t="shared" si="19"/>
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="BH37" s="28">
         <f t="shared" si="33"/>
@@ -50788,7 +50780,7 @@
       </c>
       <c r="B38" s="40">
         <f t="shared" si="20"/>
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="C38" s="216">
         <f>IF(B38&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -50896,7 +50888,7 @@
       </c>
       <c r="X38" s="224">
         <f t="shared" si="23"/>
-        <v>793.374217981843</v>
+        <v>800.72921798184302</v>
       </c>
       <c r="Y38" s="224">
         <f t="shared" si="24"/>
@@ -50904,7 +50896,7 @@
       </c>
       <c r="Z38" s="224">
         <f t="shared" si="25"/>
-        <v>496.40166841772105</v>
+        <v>503.75666841772107</v>
       </c>
       <c r="AA38" s="224">
         <f>IF(SUM(AA$9:AA37)&gt;0,0,IF(SUM(X38-R38)&gt;0,B38,0))</f>
@@ -50912,7 +50904,7 @@
       </c>
       <c r="AB38" s="224">
         <f>ABS(Z38)*1000000/SUM(U$9:U38)</f>
-        <v>1269.0322780678614</v>
+        <v>1255.7327232925963</v>
       </c>
       <c r="AC38" s="190"/>
       <c r="AD38" s="190"/>
@@ -50947,7 +50939,7 @@
       <c r="AO38" s="14"/>
       <c r="AP38" s="15">
         <f t="shared" si="15"/>
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="AQ38" s="29">
         <f t="shared" si="0"/>
@@ -50956,7 +50948,7 @@
       <c r="AR38" s="14"/>
       <c r="AS38" s="54">
         <f t="shared" si="16"/>
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="AT38" s="29">
         <f t="shared" si="30"/>
@@ -50997,7 +50989,7 @@
       <c r="BC38" s="14"/>
       <c r="BD38" s="15">
         <f t="shared" si="17"/>
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="BE38" s="29">
         <f t="shared" si="18"/>
@@ -51006,7 +50998,7 @@
       <c r="BF38" s="14"/>
       <c r="BG38" s="15">
         <f t="shared" si="19"/>
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="BH38" s="29">
         <f t="shared" si="33"/>
@@ -51041,7 +51033,7 @@
       </c>
       <c r="B39" s="41">
         <f t="shared" si="20"/>
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="C39" s="216">
         <f>IF(B39&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -51149,7 +51141,7 @@
       </c>
       <c r="X39" s="217">
         <f t="shared" si="23"/>
-        <v>845.73119258208362</v>
+        <v>853.08619258208364</v>
       </c>
       <c r="Y39" s="217">
         <f t="shared" si="24"/>
@@ -51157,7 +51149,7 @@
       </c>
       <c r="Z39" s="217">
         <f t="shared" si="25"/>
-        <v>542.7325233790134</v>
+        <v>550.08752337901342</v>
       </c>
       <c r="AA39" s="217">
         <f>IF(SUM(AA$9:AA38)&gt;0,0,IF(SUM(X39-R39)&gt;0,B39,0))</f>
@@ -51165,7 +51157,7 @@
       </c>
       <c r="AB39" s="217">
         <f>ABS(Z39)*1000000/SUM(U$9:U39)</f>
-        <v>1339.7755016537692</v>
+        <v>1325.2178782907513</v>
       </c>
       <c r="AH39" s="17">
         <f t="shared" si="26"/>
@@ -51194,7 +51186,7 @@
       </c>
       <c r="AP39" s="5">
         <f t="shared" si="15"/>
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="AQ39" s="28">
         <f t="shared" si="0"/>
@@ -51202,7 +51194,7 @@
       </c>
       <c r="AS39" s="57">
         <f t="shared" si="16"/>
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="AT39" s="28">
         <f t="shared" si="30"/>
@@ -51242,7 +51234,7 @@
       </c>
       <c r="BD39" s="5">
         <f t="shared" si="17"/>
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="BE39" s="28">
         <f t="shared" si="18"/>
@@ -51251,7 +51243,7 @@
       <c r="BF39" s="190"/>
       <c r="BG39" s="5">
         <f t="shared" si="19"/>
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="BH39" s="28">
         <f t="shared" si="33"/>
@@ -51269,7 +51261,7 @@
       </c>
       <c r="B40" s="40">
         <f t="shared" si="20"/>
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="C40" s="216">
         <f>IF(B40&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -51377,7 +51369,7 @@
       </c>
       <c r="X40" s="224">
         <f t="shared" si="23"/>
-        <v>900.70601591233628</v>
+        <v>908.0610159123363</v>
       </c>
       <c r="Y40" s="224">
         <f t="shared" si="24"/>
@@ -51385,7 +51377,7 @@
       </c>
       <c r="Z40" s="224">
         <f t="shared" si="25"/>
-        <v>591.47913435950841</v>
+        <v>598.83413435950843</v>
       </c>
       <c r="AA40" s="224">
         <f>IF(SUM(AA$9:AA39)&gt;0,0,IF(SUM(X40-R40)&gt;0,B40,0))</f>
@@ -51393,7 +51385,7 @@
       </c>
       <c r="AB40" s="224">
         <f>ABS(Z40)*1000000/SUM(U$9:U40)</f>
-        <v>1411.5815128174206</v>
+        <v>1395.8227260993663</v>
       </c>
       <c r="AH40" s="17">
         <f t="shared" si="26"/>
@@ -51423,7 +51415,7 @@
       <c r="AO40" s="14"/>
       <c r="AP40" s="15">
         <f t="shared" si="15"/>
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="AQ40" s="29">
         <f t="shared" si="0"/>
@@ -51432,7 +51424,7 @@
       <c r="AR40" s="14"/>
       <c r="AS40" s="54">
         <f t="shared" si="16"/>
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="AT40" s="29">
         <f t="shared" si="30"/>
@@ -51473,7 +51465,7 @@
       <c r="BC40" s="14"/>
       <c r="BD40" s="15">
         <f t="shared" si="17"/>
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="BE40" s="29">
         <f t="shared" si="18"/>
@@ -51482,7 +51474,7 @@
       <c r="BF40" s="14"/>
       <c r="BG40" s="15">
         <f t="shared" si="19"/>
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="BH40" s="29">
         <f t="shared" si="33"/>
@@ -51502,7 +51494,7 @@
       </c>
       <c r="B41" s="41">
         <f t="shared" si="20"/>
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="C41" s="216">
         <f>IF(B41&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -51610,7 +51602,7 @@
       </c>
       <c r="X41" s="217">
         <f t="shared" si="23"/>
-        <v>958.42958040910162</v>
+        <v>965.78458040910164</v>
       </c>
       <c r="Y41" s="217">
         <f t="shared" si="24"/>
@@ -51618,7 +51610,7 @@
       </c>
       <c r="Z41" s="217">
         <f t="shared" si="25"/>
-        <v>642.76547864951681</v>
+        <v>650.12047864951683</v>
       </c>
       <c r="AA41" s="217">
         <f>IF(SUM(AA$9:AA40)&gt;0,0,IF(SUM(X41-R41)&gt;0,B41,0))</f>
@@ -51626,7 +51618,7 @@
       </c>
       <c r="AB41" s="217">
         <f>ABS(Z41)*1000000/SUM(U$9:U41)</f>
-        <v>1484.6341088123527</v>
+        <v>1467.7215470755323</v>
       </c>
       <c r="AH41" s="17">
         <f t="shared" si="26"/>
@@ -51655,7 +51647,7 @@
       </c>
       <c r="AP41" s="5">
         <f t="shared" si="15"/>
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="AQ41" s="28">
         <f t="shared" si="0"/>
@@ -51663,7 +51655,7 @@
       </c>
       <c r="AS41" s="57">
         <f t="shared" si="16"/>
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="AT41" s="28">
         <f t="shared" si="30"/>
@@ -51703,7 +51695,7 @@
       </c>
       <c r="BD41" s="5">
         <f t="shared" si="17"/>
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="BE41" s="28">
         <f t="shared" si="18"/>
@@ -51712,7 +51704,7 @@
       <c r="BF41" s="190"/>
       <c r="BG41" s="5">
         <f t="shared" si="19"/>
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="BH41" s="28">
         <f t="shared" si="33"/>
@@ -51730,7 +51722,7 @@
       </c>
       <c r="B42" s="40">
         <f t="shared" si="20"/>
-        <v>2051</v>
+        <v>2053</v>
       </c>
       <c r="C42" s="216">
         <f>IF(B42&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -51838,7 +51830,7 @@
       </c>
       <c r="X42" s="224">
         <f t="shared" si="23"/>
-        <v>1019.0393231307053</v>
+        <v>1026.3943231307053</v>
       </c>
       <c r="Y42" s="224">
         <f t="shared" si="24"/>
@@ -51846,7 +51838,7 @@
       </c>
       <c r="Z42" s="224">
         <f t="shared" si="25"/>
-        <v>696.72183661219424</v>
+        <v>704.07683661219426</v>
       </c>
       <c r="AA42" s="224">
         <f>IF(SUM(AA$9:AA41)&gt;0,0,IF(SUM(X42-R42)&gt;0,B42,0))</f>
@@ -51854,7 +51846,7 @@
       </c>
       <c r="AB42" s="224">
         <f>ABS(Z42)*1000000/SUM(U$9:U42)</f>
-        <v>1559.1082798383939</v>
+        <v>1541.0811676879914</v>
       </c>
       <c r="AH42" s="17">
         <f t="shared" si="26"/>
@@ -51884,7 +51876,7 @@
       <c r="AO42" s="14"/>
       <c r="AP42" s="15">
         <f t="shared" si="15"/>
-        <v>2051</v>
+        <v>2053</v>
       </c>
       <c r="AQ42" s="29">
         <f t="shared" si="0"/>
@@ -51893,7 +51885,7 @@
       <c r="AR42" s="14"/>
       <c r="AS42" s="54">
         <f t="shared" si="16"/>
-        <v>2051</v>
+        <v>2053</v>
       </c>
       <c r="AT42" s="29">
         <f t="shared" si="30"/>
@@ -51934,7 +51926,7 @@
       <c r="BC42" s="14"/>
       <c r="BD42" s="15">
         <f t="shared" si="17"/>
-        <v>2051</v>
+        <v>2053</v>
       </c>
       <c r="BE42" s="29">
         <f t="shared" si="18"/>
@@ -51943,7 +51935,7 @@
       <c r="BF42" s="14"/>
       <c r="BG42" s="15">
         <f t="shared" si="19"/>
-        <v>2051</v>
+        <v>2053</v>
       </c>
       <c r="BH42" s="29">
         <f t="shared" si="33"/>
@@ -51963,7 +51955,7 @@
       </c>
       <c r="B43" s="41">
         <f t="shared" si="20"/>
-        <v>2052</v>
+        <v>2054</v>
       </c>
       <c r="C43" s="216">
         <f>IF(B43&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -52071,7 +52063,7 @@
       </c>
       <c r="X43" s="217">
         <f t="shared" si="23"/>
-        <v>1082.6795529883891</v>
+        <v>1090.0345529883891</v>
       </c>
       <c r="Y43" s="217">
         <f t="shared" si="24"/>
@@ -52079,7 +52071,7 @@
       </c>
       <c r="Z43" s="217">
         <f t="shared" si="25"/>
-        <v>753.4851103043784</v>
+        <v>760.84011030437841</v>
       </c>
       <c r="AA43" s="217">
         <f>IF(SUM(AA$9:AA42)&gt;0,0,IF(SUM(X43-R43)&gt;0,B43,0))</f>
@@ -52087,7 +52079,7 @@
       </c>
       <c r="AB43" s="217">
         <f>ABS(Z43)*1000000/SUM(U$9:U43)</f>
-        <v>1635.1722313639464</v>
+        <v>1616.0627397454084</v>
       </c>
       <c r="AH43" s="17">
         <f t="shared" si="26"/>
@@ -52116,7 +52108,7 @@
       </c>
       <c r="AP43" s="5">
         <f t="shared" si="15"/>
-        <v>2052</v>
+        <v>2054</v>
       </c>
       <c r="AQ43" s="28">
         <f t="shared" si="0"/>
@@ -52124,7 +52116,7 @@
       </c>
       <c r="AS43" s="57">
         <f t="shared" si="16"/>
-        <v>2052</v>
+        <v>2054</v>
       </c>
       <c r="AT43" s="28">
         <f t="shared" si="30"/>
@@ -52164,7 +52156,7 @@
       </c>
       <c r="BD43" s="5">
         <f t="shared" si="17"/>
-        <v>2052</v>
+        <v>2054</v>
       </c>
       <c r="BE43" s="28">
         <f t="shared" si="18"/>
@@ -52173,7 +52165,7 @@
       <c r="BF43" s="190"/>
       <c r="BG43" s="5">
         <f t="shared" si="19"/>
-        <v>2052</v>
+        <v>2054</v>
       </c>
       <c r="BH43" s="28">
         <f t="shared" si="33"/>
@@ -52191,7 +52183,7 @@
       </c>
       <c r="B44" s="40">
         <f t="shared" si="20"/>
-        <v>2053</v>
+        <v>2055</v>
       </c>
       <c r="C44" s="216">
         <f>IF(B44&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -52299,7 +52291,7 @@
       </c>
       <c r="X44" s="224">
         <f t="shared" si="23"/>
-        <v>1149.5017943389571</v>
+        <v>1156.8567943389571</v>
       </c>
       <c r="Y44" s="224">
         <f t="shared" si="24"/>
@@ -52307,7 +52299,7 @@
       </c>
       <c r="Z44" s="224">
         <f t="shared" si="25"/>
-        <v>813.19915814612409</v>
+        <v>820.55415814612411</v>
       </c>
       <c r="AA44" s="224">
         <f>IF(SUM(AA$9:AA43)&gt;0,0,IF(SUM(X44-R44)&gt;0,B44,0))</f>
@@ -52315,7 +52307,7 @@
       </c>
       <c r="AB44" s="224">
         <f>ABS(Z44)*1000000/SUM(U$9:U44)</f>
-        <v>1712.9890842914072</v>
+        <v>1692.8232460198942</v>
       </c>
       <c r="AH44" s="17">
         <f t="shared" si="26"/>
@@ -52345,7 +52337,7 @@
       <c r="AO44" s="14"/>
       <c r="AP44" s="15">
         <f t="shared" si="15"/>
-        <v>2053</v>
+        <v>2055</v>
       </c>
       <c r="AQ44" s="29">
         <f t="shared" si="0"/>
@@ -52354,7 +52346,7 @@
       <c r="AR44" s="14"/>
       <c r="AS44" s="54">
         <f t="shared" si="16"/>
-        <v>2053</v>
+        <v>2055</v>
       </c>
       <c r="AT44" s="29">
         <f t="shared" si="30"/>
@@ -52395,7 +52387,7 @@
       <c r="BC44" s="14"/>
       <c r="BD44" s="15">
         <f t="shared" si="17"/>
-        <v>2053</v>
+        <v>2055</v>
       </c>
       <c r="BE44" s="29">
         <f t="shared" si="18"/>
@@ -52404,7 +52396,7 @@
       <c r="BF44" s="14"/>
       <c r="BG44" s="15">
         <f t="shared" si="19"/>
-        <v>2053</v>
+        <v>2055</v>
       </c>
       <c r="BH44" s="29">
         <f t="shared" si="33"/>
@@ -52424,7 +52416,7 @@
       </c>
       <c r="B45" s="41">
         <f t="shared" si="20"/>
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="C45" s="216">
         <f>IF(B45&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -52532,7 +52524,7 @@
       </c>
       <c r="X45" s="217">
         <f t="shared" si="23"/>
-        <v>1219.6651477570535</v>
+        <v>1227.0201477570536</v>
       </c>
       <c r="Y45" s="217">
         <f t="shared" si="24"/>
@@ -52540,7 +52532,7 @@
       </c>
       <c r="Z45" s="217">
         <f t="shared" si="25"/>
-        <v>876.0151464454417</v>
+        <v>883.37014644544172</v>
       </c>
       <c r="AA45" s="217">
         <f>IF(SUM(AA$9:AA44)&gt;0,0,IF(SUM(X45-R45)&gt;0,B45,0))</f>
@@ -52548,7 +52540,7 @@
       </c>
       <c r="AB45" s="217">
         <f>ABS(Z45)*1000000/SUM(U$9:U45)</f>
-        <v>1792.7183188866875</v>
+        <v>1771.516787372836</v>
       </c>
       <c r="AH45" s="17">
         <f t="shared" si="26"/>
@@ -52577,7 +52569,7 @@
       </c>
       <c r="AP45" s="5">
         <f t="shared" si="15"/>
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="AQ45" s="28">
         <f t="shared" si="0"/>
@@ -52585,7 +52577,7 @@
       </c>
       <c r="AS45" s="57">
         <f t="shared" si="16"/>
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="AT45" s="28">
         <f t="shared" si="30"/>
@@ -52625,7 +52617,7 @@
       </c>
       <c r="BD45" s="5">
         <f t="shared" si="17"/>
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="BE45" s="28">
         <f t="shared" si="18"/>
@@ -52634,7 +52626,7 @@
       <c r="BF45" s="190"/>
       <c r="BG45" s="5">
         <f t="shared" si="19"/>
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="BH45" s="28">
         <f t="shared" si="33"/>
@@ -52652,7 +52644,7 @@
       </c>
       <c r="B46" s="40">
         <f t="shared" si="20"/>
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="C46" s="216">
         <f>IF(B46&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -52760,7 +52752,7 @@
       </c>
       <c r="X46" s="224">
         <f t="shared" si="23"/>
-        <v>1293.3366688460546</v>
+        <v>1300.6916688460547</v>
       </c>
       <c r="Y46" s="224">
         <f t="shared" si="24"/>
@@ -52768,7 +52760,7 @@
       </c>
       <c r="Z46" s="224">
         <f t="shared" si="25"/>
-        <v>942.09191862522084</v>
+        <v>949.44691862522086</v>
       </c>
       <c r="AA46" s="224">
         <f>IF(SUM(AA$9:AA45)&gt;0,0,IF(SUM(X46-R46)&gt;0,B46,0))</f>
@@ -52776,7 +52768,7 @@
       </c>
       <c r="AB46" s="224">
         <f>ABS(Z46)*1000000/SUM(U$9:U46)</f>
-        <v>1874.517013860793</v>
+        <v>1852.2956945910933</v>
       </c>
       <c r="AH46" s="17">
         <f t="shared" si="26"/>
@@ -52806,7 +52798,7 @@
       <c r="AO46" s="14"/>
       <c r="AP46" s="15">
         <f t="shared" si="15"/>
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="AQ46" s="29">
         <f t="shared" si="0"/>
@@ -52815,7 +52807,7 @@
       <c r="AR46" s="14"/>
       <c r="AS46" s="54">
         <f t="shared" si="16"/>
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="AT46" s="29">
         <f t="shared" si="30"/>
@@ -52856,7 +52848,7 @@
       <c r="BC46" s="14"/>
       <c r="BD46" s="15">
         <f t="shared" si="17"/>
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="BE46" s="29">
         <f t="shared" si="18"/>
@@ -52865,7 +52857,7 @@
       <c r="BF46" s="14"/>
       <c r="BG46" s="15">
         <f t="shared" si="19"/>
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="BH46" s="29">
         <f t="shared" si="33"/>
@@ -52885,7 +52877,7 @@
       </c>
       <c r="B47" s="41">
         <f t="shared" si="20"/>
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="C47" s="216">
         <f>IF(B47&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -52993,7 +52985,7 @@
       </c>
       <c r="X47" s="217">
         <f t="shared" si="23"/>
-        <v>1370.6917659895059</v>
+        <v>1378.046765989506</v>
       </c>
       <c r="Y47" s="217">
         <f t="shared" si="24"/>
@@ -53001,7 +52993,7 @@
       </c>
       <c r="Z47" s="217">
         <f t="shared" si="25"/>
-        <v>1011.5963830418189</v>
+        <v>1018.9513830418189</v>
       </c>
       <c r="AA47" s="217">
         <f>IF(SUM(AA$9:AA46)&gt;0,0,IF(SUM(X47-R47)&gt;0,B47,0))</f>
@@ -53009,7 +53001,7 @@
       </c>
       <c r="AB47" s="217">
         <f>ABS(Z47)*1000000/SUM(U$9:U47)</f>
-        <v>1958.5409209890365</v>
+        <v>1935.3114990791464</v>
       </c>
       <c r="AH47" s="17">
         <f t="shared" si="26"/>
@@ -53038,7 +53030,7 @@
       </c>
       <c r="AP47" s="5">
         <f t="shared" si="15"/>
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="AQ47" s="28">
         <f t="shared" si="0"/>
@@ -53046,7 +53038,7 @@
       </c>
       <c r="AS47" s="57">
         <f t="shared" si="16"/>
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="AT47" s="28">
         <f t="shared" si="30"/>
@@ -53086,7 +53078,7 @@
       </c>
       <c r="BD47" s="5">
         <f t="shared" si="17"/>
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="BE47" s="28">
         <f t="shared" si="18"/>
@@ -53095,7 +53087,7 @@
       <c r="BF47" s="190"/>
       <c r="BG47" s="5">
         <f t="shared" si="19"/>
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="BH47" s="28">
         <f t="shared" si="33"/>
@@ -53113,7 +53105,7 @@
       </c>
       <c r="B48" s="40">
         <f t="shared" si="20"/>
-        <v>2057</v>
+        <v>2059</v>
       </c>
       <c r="C48" s="216">
         <f>IF(B48&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -53221,7 +53213,7 @@
       </c>
       <c r="X48" s="224">
         <f t="shared" si="23"/>
-        <v>1451.9146179901297</v>
+        <v>1459.2696179901297</v>
       </c>
       <c r="Y48" s="224">
         <f t="shared" si="24"/>
@@ -53229,7 +53221,7 @@
       </c>
       <c r="Z48" s="224">
         <f t="shared" si="25"/>
-        <v>1084.7039203294146</v>
+        <v>1092.0589203294146</v>
       </c>
       <c r="AA48" s="224">
         <f>IF(SUM(AA$9:AA47)&gt;0,0,IF(SUM(X48-R48)&gt;0,B48,0))</f>
@@ -53237,7 +53229,7 @@
       </c>
       <c r="AB48" s="224">
         <f>ABS(Z48)*1000000/SUM(U$9:U48)</f>
-        <v>2044.9454072549224</v>
+        <v>2020.7157895960515</v>
       </c>
       <c r="AH48" s="17">
         <f t="shared" si="26"/>
@@ -53267,7 +53259,7 @@
       <c r="AO48" s="14"/>
       <c r="AP48" s="15">
         <f t="shared" si="15"/>
-        <v>2057</v>
+        <v>2059</v>
       </c>
       <c r="AQ48" s="29">
         <f t="shared" si="0"/>
@@ -53276,7 +53268,7 @@
       <c r="AR48" s="14"/>
       <c r="AS48" s="54">
         <f t="shared" si="16"/>
-        <v>2057</v>
+        <v>2059</v>
       </c>
       <c r="AT48" s="29">
         <f t="shared" si="30"/>
@@ -53317,7 +53309,7 @@
       <c r="BC48" s="14"/>
       <c r="BD48" s="15">
         <f t="shared" si="17"/>
-        <v>2057</v>
+        <v>2059</v>
       </c>
       <c r="BE48" s="29">
         <f t="shared" si="18"/>
@@ -53326,7 +53318,7 @@
       <c r="BF48" s="14"/>
       <c r="BG48" s="15">
         <f t="shared" si="19"/>
-        <v>2057</v>
+        <v>2059</v>
       </c>
       <c r="BH48" s="29">
         <f t="shared" si="33"/>
@@ -53346,7 +53338,7 @@
       </c>
       <c r="B49" s="41">
         <f t="shared" si="20"/>
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="C49" s="216">
         <f>IF(B49&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -53454,7 +53446,7 @@
       </c>
       <c r="X49" s="217">
         <f t="shared" si="23"/>
-        <v>1537.1986125907847</v>
+        <v>1544.5536125907847</v>
       </c>
       <c r="Y49" s="217">
         <f t="shared" si="24"/>
@@ -53462,7 +53454,7 @@
       </c>
       <c r="Z49" s="217">
         <f t="shared" si="25"/>
-        <v>1161.5988112511068</v>
+        <v>1168.9538112511068</v>
       </c>
       <c r="AA49" s="217">
         <f>IF(SUM(AA$9:AA48)&gt;0,0,IF(SUM(X49-R49)&gt;0,B49,0))</f>
@@ -53470,7 +53462,7 @@
       </c>
       <c r="AB49" s="217">
         <f>ABS(Z49)*1000000/SUM(U$9:U49)</f>
-        <v>2133.8862900451022</v>
+        <v>2108.6609768462936</v>
       </c>
       <c r="AH49" s="17">
         <f t="shared" si="26"/>
@@ -53499,7 +53491,7 @@
       </c>
       <c r="AP49" s="5">
         <f t="shared" si="15"/>
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="AQ49" s="28">
         <f t="shared" si="0"/>
@@ -53507,7 +53499,7 @@
       </c>
       <c r="AS49" s="57">
         <f t="shared" si="16"/>
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="AT49" s="28">
         <f t="shared" si="30"/>
@@ -53547,7 +53539,7 @@
       </c>
       <c r="BD49" s="5">
         <f t="shared" si="17"/>
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="BE49" s="28">
         <f t="shared" si="18"/>
@@ -53556,7 +53548,7 @@
       <c r="BF49" s="190"/>
       <c r="BG49" s="5">
         <f t="shared" si="19"/>
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="BH49" s="28">
         <f t="shared" si="33"/>
@@ -53574,7 +53566,7 @@
       </c>
       <c r="B50" s="40">
         <f t="shared" si="20"/>
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="C50" s="216">
         <f>IF(B50&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -53682,7 +53674,7 @@
       </c>
       <c r="X50" s="224">
         <f t="shared" si="23"/>
-        <v>1626.7468069214724</v>
+        <v>1634.1018069214724</v>
       </c>
       <c r="Y50" s="224">
         <f t="shared" si="24"/>
@@ -53690,7 +53682,7 @@
       </c>
       <c r="Z50" s="224">
         <f t="shared" si="25"/>
-        <v>1242.4746860869375</v>
+        <v>1249.8296860869375</v>
       </c>
       <c r="AA50" s="224">
         <f>IF(SUM(AA$9:AA49)&gt;0,0,IF(SUM(X50-R50)&gt;0,B50,0))</f>
@@ -53698,7 +53690,7 @@
       </c>
       <c r="AB50" s="224">
         <f>ABS(Z50)*1000000/SUM(U$9:U50)</f>
-        <v>2225.5205859158305</v>
+        <v>2199.3009835445168</v>
       </c>
       <c r="AH50" s="17">
         <f t="shared" si="26"/>
@@ -53728,7 +53720,7 @@
       <c r="AO50" s="14"/>
       <c r="AP50" s="15">
         <f t="shared" si="15"/>
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="AQ50" s="29">
         <f t="shared" si="0"/>
@@ -53737,7 +53729,7 @@
       <c r="AR50" s="14"/>
       <c r="AS50" s="54">
         <f t="shared" si="16"/>
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="AT50" s="29">
         <f t="shared" si="30"/>
@@ -53778,7 +53770,7 @@
       <c r="BC50" s="14"/>
       <c r="BD50" s="15">
         <f t="shared" si="17"/>
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="BE50" s="29">
         <f t="shared" si="18"/>
@@ -53787,7 +53779,7 @@
       <c r="BF50" s="14"/>
       <c r="BG50" s="15">
         <f t="shared" si="19"/>
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="BH50" s="29">
         <f t="shared" si="33"/>
@@ -53807,7 +53799,7 @@
       </c>
       <c r="B51" s="41">
         <f t="shared" si="20"/>
-        <v>2060</v>
+        <v>2062</v>
       </c>
       <c r="C51" s="216">
         <f>IF(B51&gt;MAX('10 YEAR PROJECTION'!$Y$4:$AN$4),
@@ -53915,7 +53907,7 @@
       </c>
       <c r="X51" s="217">
         <f t="shared" si="23"/>
-        <v>1720.7724109686947</v>
+        <v>1728.1274109686947</v>
       </c>
       <c r="Y51" s="217">
         <f t="shared" si="24"/>
@@ -53923,7 +53915,7 @@
       </c>
       <c r="Z51" s="217">
         <f t="shared" si="25"/>
-        <v>1327.5349966407102</v>
+        <v>1334.8899966407103</v>
       </c>
       <c r="AA51" s="217">
         <f>IF(SUM(AA$9:AA50)&gt;0,0,IF(SUM(X51-R51)&gt;0,B51,0))</f>
@@ -53931,7 +53923,7 @@
       </c>
       <c r="AB51" s="217">
         <f>ABS(Z51)*1000000/SUM(U$9:U51)</f>
-        <v>2320.0071895462138</v>
+        <v>2292.7918742911006</v>
       </c>
       <c r="AH51" s="17">
         <f t="shared" si="26"/>
@@ -53973,28 +53965,28 @@
       </c>
       <c r="U52" s="188">
         <f>SUM(U9:U51)</f>
-        <v>572211.5873702839</v>
+        <v>582211.58737028402</v>
       </c>
       <c r="X52" s="65" t="s">
         <v>664</v>
       </c>
       <c r="Y52" s="231">
         <f>NPV($G$5,W9:W51)*(1+$G$5)^($F$5-($E$5-1))</f>
-        <v>589.53389736914983</v>
+        <v>596.73071991111635</v>
       </c>
       <c r="Z52" s="22" t="s">
         <v>665</v>
       </c>
       <c r="AA52" s="23">
         <f>IFERROR(IRR(Y9:Y51), 0)</f>
-        <v>0.1223425781036338</v>
+        <v>0.12509678393325574</v>
       </c>
       <c r="AC52" s="137" t="s">
         <v>666</v>
       </c>
       <c r="AD52" s="232">
         <f>MAX(R9:R51)*1000000/U52</f>
-        <v>687.22378750697419</v>
+        <v>675.42010990222207</v>
       </c>
       <c r="BY52" s="190"/>
       <c r="BZ52" s="190"/>
@@ -54016,7 +54008,7 @@
       </c>
       <c r="AD53" s="233">
         <f>Y52-Q52</f>
-        <v>347.11185534234727</v>
+        <v>354.30867788431379</v>
       </c>
       <c r="BY53" s="190"/>
       <c r="BZ53" s="190"/>

</xml_diff>

<commit_message>
forced changes working, ran scenarios for 07/24 meeting.
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3463" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="700">
   <si>
     <t>Scenario</t>
   </si>
@@ -3664,7 +3664,7 @@
     <xf numFmtId="0" fontId="24" fillId="12" borderId="78"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="432">
+  <cellXfs count="433">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4540,77 +4540,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4631,6 +4571,12 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4645,6 +4591,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4711,6 +4712,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4771,27 +4793,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5071,11 +5072,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198308352"/>
-        <c:axId val="169006720"/>
+        <c:axId val="130741760"/>
+        <c:axId val="126603200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198308352"/>
+        <c:axId val="130741760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5103,7 +5104,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169006720"/>
+        <c:crossAx val="126603200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5111,7 +5112,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169006720"/>
+        <c:axId val="126603200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5148,7 +5149,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198308352"/>
+        <c:crossAx val="130741760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5610,11 +5611,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198310400"/>
-        <c:axId val="169008448"/>
+        <c:axId val="131905536"/>
+        <c:axId val="131848384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198310400"/>
+        <c:axId val="131905536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5642,7 +5643,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169008448"/>
+        <c:crossAx val="131848384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5650,7 +5651,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169008448"/>
+        <c:axId val="131848384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -5685,7 +5686,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198310400"/>
+        <c:crossAx val="131905536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5820,11 +5821,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198311424"/>
-        <c:axId val="198526656"/>
+        <c:axId val="131907072"/>
+        <c:axId val="132646016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198311424"/>
+        <c:axId val="131907072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5852,7 +5853,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198526656"/>
+        <c:crossAx val="132646016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5860,7 +5861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198526656"/>
+        <c:axId val="132646016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5897,7 +5898,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198311424"/>
+        <c:crossAx val="131907072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6099,11 +6100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199026176"/>
-        <c:axId val="198528960"/>
+        <c:axId val="147062272"/>
+        <c:axId val="132648320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199026176"/>
+        <c:axId val="147062272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6114,7 +6115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198528960"/>
+        <c:crossAx val="132648320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6122,7 +6123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198528960"/>
+        <c:axId val="132648320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000000"/>
@@ -6135,7 +6136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199026176"/>
+        <c:crossAx val="147062272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100000000"/>
@@ -6714,11 +6715,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199673344"/>
-        <c:axId val="199392576"/>
+        <c:axId val="151661568"/>
+        <c:axId val="194961408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199673344"/>
+        <c:axId val="151661568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6739,7 +6740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199392576"/>
+        <c:crossAx val="194961408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6747,7 +6748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199392576"/>
+        <c:axId val="194961408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6769,7 +6770,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199673344"/>
+        <c:crossAx val="151661568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -7358,8 +7359,8 @@
   </sheetPr>
   <dimension ref="A1:CP241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9237,7 +9238,7 @@
         <v>42</v>
       </c>
       <c r="F51" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G51" s="130" t="s">
         <v>55</v>
@@ -9247,7 +9248,7 @@
       </c>
       <c r="I51" s="114" t="str">
         <f>IF(EXACT(F51, G51), "none", IF(ISNUMBER(MATCH(G51, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J51" s="123"/>
       <c r="K51" s="242"/>
@@ -9271,7 +9272,7 @@
         <v>42</v>
       </c>
       <c r="F52" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G52" s="130" t="s">
         <v>55</v>
@@ -9281,7 +9282,7 @@
       </c>
       <c r="I52" s="114" t="str">
         <f>IF(EXACT(F52, G52), "none", IF(ISNUMBER(MATCH(G52, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J52" s="123"/>
       <c r="K52" s="242"/>
@@ -9305,7 +9306,7 @@
         <v>42</v>
       </c>
       <c r="F53" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G53" s="130" t="s">
         <v>55</v>
@@ -9315,7 +9316,7 @@
       </c>
       <c r="I53" s="114" t="str">
         <f>IF(EXACT(F53, G53), "none", IF(ISNUMBER(MATCH(G53, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J53" s="123"/>
       <c r="K53" s="242"/>
@@ -9339,7 +9340,7 @@
         <v>42</v>
       </c>
       <c r="F54" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G54" s="130" t="s">
         <v>55</v>
@@ -9349,7 +9350,7 @@
       </c>
       <c r="I54" s="114" t="str">
         <f>IF(EXACT(F54, G54), "none", IF(ISNUMBER(MATCH(G54, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J54" s="123"/>
       <c r="K54" s="242"/>
@@ -9373,7 +9374,7 @@
         <v>42</v>
       </c>
       <c r="F55" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G55" s="130" t="s">
         <v>55</v>
@@ -9383,7 +9384,7 @@
       </c>
       <c r="I55" s="114" t="str">
         <f>IF(EXACT(F55, G55), "none", IF(ISNUMBER(MATCH(G55, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J55" s="123"/>
       <c r="K55" s="242"/>
@@ -9407,7 +9408,7 @@
         <v>42</v>
       </c>
       <c r="F56" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G56" s="130" t="s">
         <v>55</v>
@@ -9417,7 +9418,7 @@
       </c>
       <c r="I56" s="114" t="str">
         <f>IF(EXACT(F56, G56), "none", IF(ISNUMBER(MATCH(G56, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J56" s="123"/>
       <c r="K56" s="242"/>
@@ -9441,7 +9442,7 @@
         <v>42</v>
       </c>
       <c r="F57" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G57" s="130" t="s">
         <v>55</v>
@@ -9451,7 +9452,7 @@
       </c>
       <c r="I57" s="114" t="str">
         <f>IF(EXACT(F57, G57), "none", IF(ISNUMBER(MATCH(G57, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J57" s="123"/>
       <c r="K57" s="242"/>
@@ -9475,7 +9476,7 @@
         <v>42</v>
       </c>
       <c r="F58" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G58" s="130" t="s">
         <v>55</v>
@@ -9485,7 +9486,7 @@
       </c>
       <c r="I58" s="114" t="str">
         <f>IF(EXACT(F58, G58), "none", IF(ISNUMBER(MATCH(G58, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J58" s="123"/>
       <c r="K58" s="242"/>
@@ -9516,7 +9517,7 @@
         <v>42</v>
       </c>
       <c r="F59" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G59" s="130" t="s">
         <v>55</v>
@@ -9526,7 +9527,7 @@
       </c>
       <c r="I59" s="114" t="str">
         <f>IF(EXACT(F59, G59), "none", IF(ISNUMBER(MATCH(G59, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J59" s="123"/>
       <c r="K59" s="242"/>
@@ -9550,7 +9551,7 @@
         <v>42</v>
       </c>
       <c r="F60" s="234" t="s">
-        <v>679</v>
+        <v>55</v>
       </c>
       <c r="G60" s="130" t="s">
         <v>55</v>
@@ -9560,7 +9561,7 @@
       </c>
       <c r="I60" s="114" t="str">
         <f>IF(EXACT(F60, G60), "none", IF(ISNUMBER(MATCH(G60, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>hard</v>
+        <v>none</v>
       </c>
       <c r="J60" s="123"/>
       <c r="K60" s="242"/>
@@ -9852,7 +9853,7 @@
         <v>40</v>
       </c>
       <c r="F67" s="234" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G67" s="130" t="s">
         <v>52</v>
@@ -9862,7 +9863,7 @@
       </c>
       <c r="I67" s="114" t="str">
         <f>IF(EXACT(F67, G67), "none", IF(ISNUMBER(MATCH(G67, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>none</v>
+        <v>hard</v>
       </c>
       <c r="J67" s="123"/>
       <c r="K67" s="242"/>
@@ -9886,7 +9887,7 @@
         <v>40</v>
       </c>
       <c r="F68" s="234" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G68" s="130" t="s">
         <v>52</v>
@@ -9896,7 +9897,7 @@
       </c>
       <c r="I68" s="114" t="str">
         <f>IF(EXACT(F68, G68), "none", IF(ISNUMBER(MATCH(G68, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
-        <v>none</v>
+        <v>hard</v>
       </c>
       <c r="J68" s="123"/>
       <c r="K68" s="242"/>
@@ -16080,16 +16081,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="344" t="s">
+      <c r="A1" s="368" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="345"/>
+      <c r="B1" s="369"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="346" t="s">
+      <c r="A2" s="370" t="s">
         <v>263</v>
       </c>
-      <c r="B2" s="347"/>
+      <c r="B2" s="371"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="X3" s="245" t="s">
@@ -16097,33 +16098,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="354" t="s">
+      <c r="A4" s="375" t="s">
         <v>265</v>
       </c>
-      <c r="B4" s="355"/>
+      <c r="B4" s="376"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="358" t="s">
+      <c r="D4" s="379" t="s">
         <v>266</v>
       </c>
-      <c r="E4" s="348" t="s">
+      <c r="E4" s="372" t="s">
         <v>267</v>
       </c>
-      <c r="F4" s="349"/>
-      <c r="G4" s="349"/>
-      <c r="H4" s="349"/>
-      <c r="I4" s="349"/>
-      <c r="J4" s="349"/>
-      <c r="K4" s="349"/>
-      <c r="L4" s="349"/>
-      <c r="M4" s="349"/>
-      <c r="N4" s="349"/>
-      <c r="O4" s="349"/>
-      <c r="P4" s="349"/>
-      <c r="Q4" s="349"/>
-      <c r="R4" s="349"/>
-      <c r="S4" s="349"/>
-      <c r="T4" s="349"/>
-      <c r="U4" s="350"/>
+      <c r="F4" s="373"/>
+      <c r="G4" s="373"/>
+      <c r="H4" s="373"/>
+      <c r="I4" s="373"/>
+      <c r="J4" s="373"/>
+      <c r="K4" s="373"/>
+      <c r="L4" s="373"/>
+      <c r="M4" s="373"/>
+      <c r="N4" s="373"/>
+      <c r="O4" s="373"/>
+      <c r="P4" s="373"/>
+      <c r="Q4" s="373"/>
+      <c r="R4" s="373"/>
+      <c r="S4" s="373"/>
+      <c r="T4" s="373"/>
+      <c r="U4" s="374"/>
       <c r="Y4" s="245">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -16190,12 +16191,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="356"/>
-      <c r="B5" s="357"/>
+      <c r="A5" s="377"/>
+      <c r="B5" s="378"/>
       <c r="C5" s="68" t="s">
         <v>268</v>
       </c>
-      <c r="D5" s="359"/>
+      <c r="D5" s="380"/>
       <c r="E5" s="69">
         <f>'Step Analysis'!E5</f>
         <v>2020</v>
@@ -16333,10 +16334,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="360" t="s">
+      <c r="A6" s="347" t="s">
         <v>270</v>
       </c>
-      <c r="B6" s="361"/>
+      <c r="B6" s="348"/>
       <c r="C6" s="164">
         <v>10</v>
       </c>
@@ -16854,12 +16855,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="351" t="s">
+      <c r="A12" s="362" t="s">
         <v>281</v>
       </c>
-      <c r="B12" s="352"/>
-      <c r="C12" s="352"/>
-      <c r="D12" s="353"/>
+      <c r="B12" s="363"/>
+      <c r="C12" s="363"/>
+      <c r="D12" s="364"/>
       <c r="E12" s="285">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -16994,12 +16995,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="351" t="s">
+      <c r="A13" s="362" t="s">
         <v>282</v>
       </c>
-      <c r="B13" s="352"/>
-      <c r="C13" s="352"/>
-      <c r="D13" s="353"/>
+      <c r="B13" s="363"/>
+      <c r="C13" s="363"/>
+      <c r="D13" s="364"/>
       <c r="E13" s="285"/>
       <c r="F13" s="285"/>
       <c r="G13" s="285"/>
@@ -17092,10 +17093,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="360" t="s">
+      <c r="A14" s="347" t="s">
         <v>283</v>
       </c>
-      <c r="B14" s="361"/>
+      <c r="B14" s="348"/>
       <c r="C14" s="166">
         <v>10</v>
       </c>
@@ -17610,12 +17611,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="351" t="s">
+      <c r="A20" s="362" t="s">
         <v>286</v>
       </c>
-      <c r="B20" s="352"/>
-      <c r="C20" s="352"/>
-      <c r="D20" s="353"/>
+      <c r="B20" s="363"/>
+      <c r="C20" s="363"/>
+      <c r="D20" s="364"/>
       <c r="E20" s="285">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -17686,12 +17687,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="351" t="s">
+      <c r="A21" s="362" t="s">
         <v>287</v>
       </c>
-      <c r="B21" s="352"/>
-      <c r="C21" s="352"/>
-      <c r="D21" s="353"/>
+      <c r="B21" s="363"/>
+      <c r="C21" s="363"/>
+      <c r="D21" s="364"/>
       <c r="E21" s="285"/>
       <c r="F21" s="285"/>
       <c r="G21" s="285"/>
@@ -17717,10 +17718,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="360" t="s">
+      <c r="A22" s="347" t="s">
         <v>288</v>
       </c>
-      <c r="B22" s="361"/>
+      <c r="B22" s="348"/>
       <c r="C22" s="164">
         <v>10</v>
       </c>
@@ -17967,12 +17968,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="351" t="s">
+      <c r="A28" s="362" t="s">
         <v>289</v>
       </c>
-      <c r="B28" s="352"/>
-      <c r="C28" s="352"/>
-      <c r="D28" s="353"/>
+      <c r="B28" s="363"/>
+      <c r="C28" s="363"/>
+      <c r="D28" s="364"/>
       <c r="E28" s="285">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -18043,12 +18044,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="351" t="s">
+      <c r="A29" s="362" t="s">
         <v>290</v>
       </c>
-      <c r="B29" s="352"/>
-      <c r="C29" s="352"/>
-      <c r="D29" s="353"/>
+      <c r="B29" s="363"/>
+      <c r="C29" s="363"/>
+      <c r="D29" s="364"/>
       <c r="E29" s="285"/>
       <c r="F29" s="285"/>
       <c r="G29" s="285"/>
@@ -18074,10 +18075,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="360" t="s">
+      <c r="A30" s="347" t="s">
         <v>291</v>
       </c>
-      <c r="B30" s="361"/>
+      <c r="B30" s="348"/>
       <c r="C30" s="164">
         <v>10</v>
       </c>
@@ -18324,12 +18325,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="351" t="s">
+      <c r="A36" s="362" t="s">
         <v>292</v>
       </c>
-      <c r="B36" s="352"/>
-      <c r="C36" s="352"/>
-      <c r="D36" s="353"/>
+      <c r="B36" s="363"/>
+      <c r="C36" s="363"/>
+      <c r="D36" s="364"/>
       <c r="E36" s="285">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -18400,12 +18401,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="351" t="s">
+      <c r="A37" s="362" t="s">
         <v>293</v>
       </c>
-      <c r="B37" s="352"/>
-      <c r="C37" s="352"/>
-      <c r="D37" s="353"/>
+      <c r="B37" s="363"/>
+      <c r="C37" s="363"/>
+      <c r="D37" s="364"/>
       <c r="E37" s="285"/>
       <c r="F37" s="285"/>
       <c r="G37" s="285"/>
@@ -18431,10 +18432,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="360" t="s">
+      <c r="A38" s="347" t="s">
         <v>294</v>
       </c>
-      <c r="B38" s="361"/>
+      <c r="B38" s="348"/>
       <c r="C38" s="164">
         <v>10</v>
       </c>
@@ -18681,12 +18682,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="351" t="s">
+      <c r="A44" s="362" t="s">
         <v>295</v>
       </c>
-      <c r="B44" s="352"/>
-      <c r="C44" s="352"/>
-      <c r="D44" s="353"/>
+      <c r="B44" s="363"/>
+      <c r="C44" s="363"/>
+      <c r="D44" s="364"/>
       <c r="E44" s="285">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -18757,12 +18758,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="351" t="s">
+      <c r="A45" s="362" t="s">
         <v>296</v>
       </c>
-      <c r="B45" s="352"/>
-      <c r="C45" s="352"/>
-      <c r="D45" s="353"/>
+      <c r="B45" s="363"/>
+      <c r="C45" s="363"/>
+      <c r="D45" s="364"/>
       <c r="E45" s="285"/>
       <c r="F45" s="285"/>
       <c r="G45" s="285"/>
@@ -18788,11 +18789,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="369" t="s">
+      <c r="A46" s="349" t="s">
         <v>297</v>
       </c>
-      <c r="B46" s="370"/>
-      <c r="C46" s="371"/>
+      <c r="B46" s="350"/>
+      <c r="C46" s="351"/>
       <c r="D46" s="174"/>
       <c r="E46" s="293">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -18865,12 +18866,12 @@
       <c r="V46" s="246"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="375" t="s">
+      <c r="A47" s="357" t="s">
         <v>298</v>
       </c>
-      <c r="B47" s="376"/>
-      <c r="C47" s="376"/>
-      <c r="D47" s="377"/>
+      <c r="B47" s="358"/>
+      <c r="C47" s="358"/>
+      <c r="D47" s="359"/>
       <c r="E47" s="294">
         <f>E46</f>
         <v>1500000</v>
@@ -18941,7 +18942,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="175"/>
       <c r="B48" s="175"/>
-      <c r="C48" s="378" t="s">
+      <c r="C48" s="360" t="s">
         <v>299</v>
       </c>
       <c r="D48" s="176">
@@ -19016,7 +19017,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="175"/>
-      <c r="C49" s="379"/>
+      <c r="C49" s="361"/>
       <c r="D49" s="248">
         <v>37</v>
       </c>
@@ -19087,7 +19088,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="175"/>
-      <c r="C50" s="379"/>
+      <c r="C50" s="361"/>
       <c r="D50" s="248">
         <v>30</v>
       </c>
@@ -19158,7 +19159,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="175"/>
-      <c r="C51" s="379"/>
+      <c r="C51" s="361"/>
       <c r="D51" s="248">
         <v>41</v>
       </c>
@@ -19228,38 +19229,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="372" t="s">
+      <c r="A52" s="352" t="s">
         <v>300</v>
       </c>
-      <c r="B52" s="373"/>
-      <c r="C52" s="373"/>
-      <c r="D52" s="373"/>
-      <c r="E52" s="373"/>
-      <c r="F52" s="373"/>
-      <c r="G52" s="373"/>
-      <c r="H52" s="373"/>
-      <c r="I52" s="373"/>
-      <c r="J52" s="373"/>
-      <c r="K52" s="373"/>
-      <c r="L52" s="373"/>
-      <c r="M52" s="373"/>
-      <c r="N52" s="373"/>
-      <c r="O52" s="373"/>
-      <c r="P52" s="373"/>
-      <c r="Q52" s="373"/>
-      <c r="R52" s="373"/>
-      <c r="S52" s="373"/>
-      <c r="T52" s="373"/>
-      <c r="U52" s="373"/>
-      <c r="V52" s="373"/>
-      <c r="W52" s="374"/>
+      <c r="B52" s="353"/>
+      <c r="C52" s="353"/>
+      <c r="D52" s="353"/>
+      <c r="E52" s="353"/>
+      <c r="F52" s="353"/>
+      <c r="G52" s="353"/>
+      <c r="H52" s="353"/>
+      <c r="I52" s="353"/>
+      <c r="J52" s="353"/>
+      <c r="K52" s="353"/>
+      <c r="L52" s="353"/>
+      <c r="M52" s="353"/>
+      <c r="N52" s="353"/>
+      <c r="O52" s="353"/>
+      <c r="P52" s="353"/>
+      <c r="Q52" s="353"/>
+      <c r="R52" s="353"/>
+      <c r="S52" s="353"/>
+      <c r="T52" s="353"/>
+      <c r="U52" s="353"/>
+      <c r="V52" s="353"/>
+      <c r="W52" s="354"/>
       <c r="X52" s="246"/>
     </row>
     <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="364" t="s">
+      <c r="A53" s="355" t="s">
         <v>301</v>
       </c>
-      <c r="B53" s="365"/>
+      <c r="B53" s="356"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -19436,10 +19437,10 @@
       <c r="X57" s="246"/>
     </row>
     <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="362" t="s">
+      <c r="A58" s="345" t="s">
         <v>303</v>
       </c>
-      <c r="B58" s="363"/>
+      <c r="B58" s="346"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -19621,10 +19622,10 @@
       <c r="X62" s="246"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="362" t="s">
+      <c r="A63" s="345" t="s">
         <v>304</v>
       </c>
-      <c r="B63" s="363"/>
+      <c r="B63" s="346"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -19814,10 +19815,10 @@
       <c r="X67" s="246"/>
     </row>
     <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="362" t="s">
+      <c r="A68" s="345" t="s">
         <v>305</v>
       </c>
-      <c r="B68" s="363"/>
+      <c r="B68" s="346"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -19995,10 +19996,10 @@
       <c r="X72" s="246"/>
     </row>
     <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="362" t="s">
+      <c r="A73" s="345" t="s">
         <v>306</v>
       </c>
-      <c r="B73" s="363"/>
+      <c r="B73" s="346"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -20224,10 +20225,10 @@
       <c r="X77" s="246"/>
     </row>
     <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="362" t="s">
+      <c r="A78" s="345" t="s">
         <v>308</v>
       </c>
-      <c r="B78" s="363"/>
+      <c r="B78" s="346"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -20399,10 +20400,10 @@
       <c r="X82" s="246"/>
     </row>
     <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="362" t="s">
+      <c r="A83" s="345" t="s">
         <v>310</v>
       </c>
-      <c r="B83" s="363"/>
+      <c r="B83" s="346"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -20574,10 +20575,10 @@
       <c r="X87" s="246"/>
     </row>
     <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="362" t="s">
+      <c r="A88" s="345" t="s">
         <v>80</v>
       </c>
-      <c r="B88" s="363"/>
+      <c r="B88" s="346"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -20749,10 +20750,10 @@
       <c r="X92" s="246"/>
     </row>
     <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="362" t="s">
+      <c r="A93" s="345" t="s">
         <v>313</v>
       </c>
-      <c r="B93" s="363"/>
+      <c r="B93" s="346"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -20954,10 +20955,10 @@
       <c r="X97" s="246"/>
     </row>
     <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="362" t="s">
+      <c r="A98" s="345" t="s">
         <v>315</v>
       </c>
-      <c r="B98" s="363"/>
+      <c r="B98" s="346"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -21149,10 +21150,10 @@
       <c r="X102" s="246"/>
     </row>
     <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="362" t="s">
+      <c r="A103" s="345" t="s">
         <v>317</v>
       </c>
-      <c r="B103" s="363"/>
+      <c r="B103" s="346"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -21354,10 +21355,10 @@
       <c r="X107" s="246"/>
     </row>
     <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="362" t="s">
+      <c r="A108" s="345" t="s">
         <v>318</v>
       </c>
-      <c r="B108" s="363"/>
+      <c r="B108" s="346"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -21559,10 +21560,10 @@
       <c r="X112" s="246"/>
     </row>
     <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="362" t="s">
+      <c r="A113" s="345" t="s">
         <v>319</v>
       </c>
-      <c r="B113" s="363"/>
+      <c r="B113" s="346"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -21724,10 +21725,10 @@
       <c r="X117" s="246"/>
     </row>
     <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="362" t="s">
+      <c r="A118" s="345" t="s">
         <v>320</v>
       </c>
-      <c r="B118" s="363"/>
+      <c r="B118" s="346"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -21929,10 +21930,10 @@
       <c r="X122" s="246"/>
     </row>
     <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="362" t="s">
+      <c r="A123" s="345" t="s">
         <v>321</v>
       </c>
-      <c r="B123" s="363"/>
+      <c r="B123" s="346"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -22134,10 +22135,10 @@
       <c r="X127" s="246"/>
     </row>
     <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="362" t="s">
+      <c r="A128" s="345" t="s">
         <v>322</v>
       </c>
-      <c r="B128" s="363"/>
+      <c r="B128" s="346"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -22339,10 +22340,10 @@
       <c r="X132" s="246"/>
     </row>
     <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="362" t="s">
+      <c r="A133" s="345" t="s">
         <v>323</v>
       </c>
-      <c r="B133" s="363"/>
+      <c r="B133" s="346"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -22544,10 +22545,10 @@
       <c r="X137" s="246"/>
     </row>
     <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="362" t="s">
+      <c r="A138" s="345" t="s">
         <v>324</v>
       </c>
-      <c r="B138" s="363"/>
+      <c r="B138" s="346"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -22757,10 +22758,10 @@
       <c r="X142" s="246"/>
     </row>
     <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="362" t="s">
+      <c r="A143" s="345" t="s">
         <v>328</v>
       </c>
-      <c r="B143" s="363"/>
+      <c r="B143" s="346"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -22853,10 +22854,10 @@
       <c r="X144" s="246"/>
     </row>
     <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="364" t="s">
+      <c r="A145" s="355" t="s">
         <v>330</v>
       </c>
-      <c r="B145" s="365"/>
+      <c r="B145" s="356"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -22929,10 +22930,10 @@
       <c r="X146" s="246"/>
     </row>
     <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="364" t="s">
+      <c r="A147" s="355" t="s">
         <v>331</v>
       </c>
-      <c r="B147" s="365"/>
+      <c r="B147" s="356"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -23030,10 +23031,10 @@
       <c r="X148" s="246"/>
     </row>
     <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="364" t="s">
+      <c r="A149" s="355" t="s">
         <v>332</v>
       </c>
-      <c r="B149" s="365"/>
+      <c r="B149" s="356"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -23155,12 +23156,12 @@
       <c r="X151" s="246"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="366" t="s">
+      <c r="A152" s="365" t="s">
         <v>333</v>
       </c>
-      <c r="B152" s="367"/>
-      <c r="C152" s="367"/>
-      <c r="D152" s="368"/>
+      <c r="B152" s="366"/>
+      <c r="C152" s="366"/>
+      <c r="D152" s="367"/>
       <c r="E152" s="317">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -23772,6 +23773,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -23788,37 +23820,6 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -23834,7 +23835,7 @@
   <dimension ref="A1:L222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23870,10 +23871,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="380" t="s">
+      <c r="A3" s="381" t="s">
         <v>334</v>
       </c>
-      <c r="B3" s="381"/>
+      <c r="B3" s="382"/>
       <c r="J3" s="234" t="s">
         <v>30</v>
       </c>
@@ -23920,10 +23921,10 @@
       <c r="L6" s="343"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="380" t="s">
+      <c r="A7" s="381" t="s">
         <v>338</v>
       </c>
-      <c r="B7" s="381"/>
+      <c r="B7" s="382"/>
       <c r="C7" s="115" t="s">
         <v>339</v>
       </c>
@@ -23994,7 +23995,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="109">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="C11" s="116" t="s">
         <v>343</v>
@@ -24156,10 +24157,10 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="382" t="s">
+      <c r="A23" s="383" t="s">
         <v>346</v>
       </c>
-      <c r="B23" s="381"/>
+      <c r="B23" s="382"/>
       <c r="C23" t="s">
         <v>347</v>
       </c>
@@ -24240,14 +24241,14 @@
       <c r="B27" s="234" t="s">
         <v>355</v>
       </c>
-      <c r="C27" s="383" t="s">
+      <c r="C27" s="384" t="s">
         <v>356</v>
       </c>
-      <c r="D27" s="383"/>
-      <c r="E27" s="383"/>
-      <c r="F27" s="383"/>
-      <c r="G27" s="383"/>
-      <c r="H27" s="383"/>
+      <c r="D27" s="384"/>
+      <c r="E27" s="384"/>
+      <c r="F27" s="384"/>
+      <c r="G27" s="384"/>
+      <c r="H27" s="384"/>
       <c r="J27" s="234" t="s">
         <v>64</v>
       </c>
@@ -24259,12 +24260,12 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="383"/>
-      <c r="D28" s="383"/>
-      <c r="E28" s="383"/>
-      <c r="F28" s="383"/>
-      <c r="G28" s="383"/>
-      <c r="H28" s="383"/>
+      <c r="C28" s="384"/>
+      <c r="D28" s="384"/>
+      <c r="E28" s="384"/>
+      <c r="F28" s="384"/>
+      <c r="G28" s="384"/>
+      <c r="H28" s="384"/>
       <c r="J28" s="234" t="s">
         <v>65</v>
       </c>
@@ -24276,12 +24277,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="384"/>
-      <c r="D29" s="384"/>
-      <c r="E29" s="384"/>
-      <c r="F29" s="384"/>
-      <c r="G29" s="384"/>
-      <c r="H29" s="384"/>
+      <c r="C29" s="385"/>
+      <c r="D29" s="385"/>
+      <c r="E29" s="385"/>
+      <c r="F29" s="385"/>
+      <c r="G29" s="385"/>
+      <c r="H29" s="385"/>
       <c r="J29" s="234" t="s">
         <v>66</v>
       </c>
@@ -30304,8 +30305,8 @@
   </sheetPr>
   <dimension ref="A1:AG335"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="G331" sqref="G331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30340,14 +30341,14 @@
       <c r="H1" s="238" t="s">
         <v>444</v>
       </c>
-      <c r="I1" s="385" t="s">
+      <c r="I1" s="386" t="s">
         <v>445</v>
       </c>
-      <c r="J1" s="386"/>
-      <c r="K1" s="386"/>
-      <c r="L1" s="386"/>
-      <c r="M1" s="386"/>
-      <c r="N1" s="386"/>
+      <c r="J1" s="387"/>
+      <c r="K1" s="387"/>
+      <c r="L1" s="387"/>
+      <c r="M1" s="387"/>
+      <c r="N1" s="387"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="245" t="s">
@@ -30375,12 +30376,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I2" s="386"/>
-      <c r="J2" s="386"/>
-      <c r="K2" s="386"/>
-      <c r="L2" s="386"/>
-      <c r="M2" s="386"/>
-      <c r="N2" s="386"/>
+      <c r="I2" s="387"/>
+      <c r="J2" s="387"/>
+      <c r="K2" s="387"/>
+      <c r="L2" s="387"/>
+      <c r="M2" s="387"/>
+      <c r="N2" s="387"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="245" t="s">
@@ -30408,12 +30409,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I3" s="386"/>
-      <c r="J3" s="386"/>
-      <c r="K3" s="386"/>
-      <c r="L3" s="386"/>
-      <c r="M3" s="386"/>
-      <c r="N3" s="386"/>
+      <c r="I3" s="387"/>
+      <c r="J3" s="387"/>
+      <c r="K3" s="387"/>
+      <c r="L3" s="387"/>
+      <c r="M3" s="387"/>
+      <c r="N3" s="387"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="245" t="s">
@@ -30441,12 +30442,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I4" s="386"/>
-      <c r="J4" s="386"/>
-      <c r="K4" s="386"/>
-      <c r="L4" s="386"/>
-      <c r="M4" s="386"/>
-      <c r="N4" s="386"/>
+      <c r="I4" s="387"/>
+      <c r="J4" s="387"/>
+      <c r="K4" s="387"/>
+      <c r="L4" s="387"/>
+      <c r="M4" s="387"/>
+      <c r="N4" s="387"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -30474,12 +30475,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="386"/>
-      <c r="J5" s="386"/>
-      <c r="K5" s="386"/>
-      <c r="L5" s="386"/>
-      <c r="M5" s="386"/>
-      <c r="N5" s="386"/>
+      <c r="I5" s="387"/>
+      <c r="J5" s="387"/>
+      <c r="K5" s="387"/>
+      <c r="L5" s="387"/>
+      <c r="M5" s="387"/>
+      <c r="N5" s="387"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -30507,12 +30508,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I6" s="386"/>
-      <c r="J6" s="386"/>
-      <c r="K6" s="386"/>
-      <c r="L6" s="386"/>
-      <c r="M6" s="386"/>
-      <c r="N6" s="386"/>
+      <c r="I6" s="387"/>
+      <c r="J6" s="387"/>
+      <c r="K6" s="387"/>
+      <c r="L6" s="387"/>
+      <c r="M6" s="387"/>
+      <c r="N6" s="387"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -30540,12 +30541,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I7" s="386"/>
-      <c r="J7" s="386"/>
-      <c r="K7" s="386"/>
-      <c r="L7" s="386"/>
-      <c r="M7" s="386"/>
-      <c r="N7" s="386"/>
+      <c r="I7" s="387"/>
+      <c r="J7" s="387"/>
+      <c r="K7" s="387"/>
+      <c r="L7" s="387"/>
+      <c r="M7" s="387"/>
+      <c r="N7" s="387"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -30573,12 +30574,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I8" s="386"/>
-      <c r="J8" s="386"/>
-      <c r="K8" s="386"/>
-      <c r="L8" s="386"/>
-      <c r="M8" s="386"/>
-      <c r="N8" s="386"/>
+      <c r="I8" s="387"/>
+      <c r="J8" s="387"/>
+      <c r="K8" s="387"/>
+      <c r="L8" s="387"/>
+      <c r="M8" s="387"/>
+      <c r="N8" s="387"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -30606,12 +30607,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I9" s="386"/>
-      <c r="J9" s="386"/>
-      <c r="K9" s="386"/>
-      <c r="L9" s="386"/>
-      <c r="M9" s="386"/>
-      <c r="N9" s="386"/>
+      <c r="I9" s="387"/>
+      <c r="J9" s="387"/>
+      <c r="K9" s="387"/>
+      <c r="L9" s="387"/>
+      <c r="M9" s="387"/>
+      <c r="N9" s="387"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="342" t="s">
@@ -30639,12 +30640,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I10" s="386"/>
-      <c r="J10" s="386"/>
-      <c r="K10" s="386"/>
-      <c r="L10" s="386"/>
-      <c r="M10" s="386"/>
-      <c r="N10" s="386"/>
+      <c r="I10" s="387"/>
+      <c r="J10" s="387"/>
+      <c r="K10" s="387"/>
+      <c r="L10" s="387"/>
+      <c r="M10" s="387"/>
+      <c r="N10" s="387"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="342" t="s">
@@ -30672,12 +30673,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I11" s="386"/>
-      <c r="J11" s="386"/>
-      <c r="K11" s="386"/>
-      <c r="L11" s="386"/>
-      <c r="M11" s="386"/>
-      <c r="N11" s="386"/>
+      <c r="I11" s="387"/>
+      <c r="J11" s="387"/>
+      <c r="K11" s="387"/>
+      <c r="L11" s="387"/>
+      <c r="M11" s="387"/>
+      <c r="N11" s="387"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="342" t="s">
@@ -30705,12 +30706,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I12" s="386"/>
-      <c r="J12" s="386"/>
-      <c r="K12" s="386"/>
-      <c r="L12" s="386"/>
-      <c r="M12" s="386"/>
-      <c r="N12" s="386"/>
+      <c r="I12" s="387"/>
+      <c r="J12" s="387"/>
+      <c r="K12" s="387"/>
+      <c r="L12" s="387"/>
+      <c r="M12" s="387"/>
+      <c r="N12" s="387"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="245" t="s">
@@ -38436,18 +38437,18 @@
       <c r="H298" s="342">
         <v>0</v>
       </c>
-      <c r="V298" s="387"/>
-      <c r="W298" s="387"/>
-      <c r="X298" s="387"/>
-      <c r="Y298" s="387"/>
-      <c r="Z298" s="387"/>
-      <c r="AA298" s="387"/>
-      <c r="AB298" s="387"/>
-      <c r="AC298" s="387"/>
-      <c r="AD298" s="387"/>
-      <c r="AE298" s="387"/>
-      <c r="AF298" s="387"/>
-      <c r="AG298" s="387"/>
+      <c r="V298" s="388"/>
+      <c r="W298" s="388"/>
+      <c r="X298" s="388"/>
+      <c r="Y298" s="388"/>
+      <c r="Z298" s="388"/>
+      <c r="AA298" s="388"/>
+      <c r="AB298" s="388"/>
+      <c r="AC298" s="388"/>
+      <c r="AD298" s="388"/>
+      <c r="AE298" s="388"/>
+      <c r="AF298" s="388"/>
+      <c r="AG298" s="388"/>
     </row>
     <row r="299" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A299" s="342" t="s">
@@ -38474,18 +38475,18 @@
       <c r="H299" s="342">
         <v>0</v>
       </c>
-      <c r="V299" s="387"/>
-      <c r="W299" s="387"/>
-      <c r="X299" s="387"/>
-      <c r="Y299" s="387"/>
-      <c r="Z299" s="387"/>
-      <c r="AA299" s="387"/>
-      <c r="AB299" s="387"/>
-      <c r="AC299" s="387"/>
-      <c r="AD299" s="387"/>
-      <c r="AE299" s="387"/>
-      <c r="AF299" s="387"/>
-      <c r="AG299" s="387"/>
+      <c r="V299" s="388"/>
+      <c r="W299" s="388"/>
+      <c r="X299" s="388"/>
+      <c r="Y299" s="388"/>
+      <c r="Z299" s="388"/>
+      <c r="AA299" s="388"/>
+      <c r="AB299" s="388"/>
+      <c r="AC299" s="388"/>
+      <c r="AD299" s="388"/>
+      <c r="AE299" s="388"/>
+      <c r="AF299" s="388"/>
+      <c r="AG299" s="388"/>
     </row>
     <row r="300" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A300" s="241" t="s">
@@ -38994,88 +38995,274 @@
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B319" s="240"/>
-      <c r="C319" s="240"/>
-      <c r="D319" s="240"/>
-      <c r="E319" s="240"/>
-      <c r="F319" s="240"/>
-      <c r="G319" s="240"/>
-      <c r="H319" s="241"/>
+      <c r="A319" s="242" t="s">
+        <v>69</v>
+      </c>
+      <c r="B319" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C319" s="341">
+        <v>0</v>
+      </c>
+      <c r="D319" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E319" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F319" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G319" s="341">
+        <v>0</v>
+      </c>
+      <c r="H319" s="243">
+        <f t="shared" ref="H319:H328" si="1">5.38*$K$251</f>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B320" s="240"/>
-      <c r="C320" s="240"/>
-      <c r="D320" s="240"/>
-      <c r="E320" s="240"/>
-      <c r="F320" s="240"/>
-      <c r="G320" s="240"/>
+      <c r="A320" s="242" t="s">
+        <v>70</v>
+      </c>
+      <c r="B320" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C320" s="341">
+        <v>0</v>
+      </c>
+      <c r="D320" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E320" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F320" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G320" s="341">
+        <v>0</v>
+      </c>
+      <c r="H320" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A321" s="342"/>
-      <c r="B321" s="240"/>
-      <c r="C321" s="240"/>
-      <c r="D321" s="240"/>
-      <c r="E321" s="240"/>
-      <c r="F321" s="240"/>
-      <c r="G321" s="240"/>
+      <c r="A321" s="242" t="s">
+        <v>71</v>
+      </c>
+      <c r="B321" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C321" s="341">
+        <v>0</v>
+      </c>
+      <c r="D321" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E321" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F321" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G321" s="341">
+        <v>0</v>
+      </c>
+      <c r="H321" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A322" s="245"/>
-      <c r="B322" s="240"/>
-      <c r="C322" s="240"/>
-      <c r="D322" s="240"/>
-      <c r="E322" s="240"/>
-      <c r="F322" s="240"/>
-      <c r="G322" s="240"/>
+      <c r="A322" s="242" t="s">
+        <v>72</v>
+      </c>
+      <c r="B322" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C322" s="341">
+        <v>0</v>
+      </c>
+      <c r="D322" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E322" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F322" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G322" s="341">
+        <v>0</v>
+      </c>
+      <c r="H322" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B323" s="240"/>
-      <c r="C323" s="240"/>
-      <c r="D323" s="240"/>
-      <c r="E323" s="240"/>
-      <c r="F323" s="240"/>
-      <c r="G323" s="240"/>
+      <c r="A323" s="242" t="s">
+        <v>73</v>
+      </c>
+      <c r="B323" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C323" s="341">
+        <v>0</v>
+      </c>
+      <c r="D323" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E323" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F323" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G323" s="341">
+        <v>0</v>
+      </c>
+      <c r="H323" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B324" s="240"/>
-      <c r="C324" s="240"/>
-      <c r="D324" s="240"/>
-      <c r="E324" s="240"/>
-      <c r="F324" s="240"/>
-      <c r="G324" s="240"/>
+      <c r="A324" s="242" t="s">
+        <v>74</v>
+      </c>
+      <c r="B324" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C324" s="341">
+        <v>0</v>
+      </c>
+      <c r="D324" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E324" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F324" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G324" s="341">
+        <v>0</v>
+      </c>
+      <c r="H324" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A325" s="342"/>
-      <c r="B325" s="240"/>
-      <c r="C325" s="240"/>
-      <c r="D325" s="240"/>
-      <c r="E325" s="240"/>
-      <c r="F325" s="240"/>
-      <c r="G325" s="240"/>
+      <c r="A325" s="242" t="s">
+        <v>75</v>
+      </c>
+      <c r="B325" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C325" s="341">
+        <v>0</v>
+      </c>
+      <c r="D325" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E325" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F325" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G325" s="341">
+        <v>0</v>
+      </c>
+      <c r="H325" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B326" s="240"/>
-      <c r="C326" s="240"/>
-      <c r="D326" s="240"/>
-      <c r="E326" s="240"/>
-      <c r="F326" s="240"/>
-      <c r="G326" s="240"/>
+      <c r="A326" s="242" t="s">
+        <v>76</v>
+      </c>
+      <c r="B326" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C326" s="341">
+        <v>0</v>
+      </c>
+      <c r="D326" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E326" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F326" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G326" s="341">
+        <v>0</v>
+      </c>
+      <c r="H326" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B327" s="240"/>
-      <c r="C327" s="240"/>
-      <c r="D327" s="240"/>
-      <c r="E327" s="240"/>
-      <c r="F327" s="240"/>
-      <c r="G327" s="240"/>
+      <c r="A327" s="242" t="s">
+        <v>77</v>
+      </c>
+      <c r="B327" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C327" s="341">
+        <v>0</v>
+      </c>
+      <c r="D327" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E327" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F327" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G327" s="341">
+        <v>0</v>
+      </c>
+      <c r="H327" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C328" s="245"/>
-      <c r="D328" s="245"/>
-      <c r="E328" s="245"/>
-      <c r="F328" s="245"/>
-      <c r="G328" s="245"/>
-      <c r="H328" s="342"/>
+      <c r="A328" s="242" t="s">
+        <v>672</v>
+      </c>
+      <c r="B328" s="344" t="s">
+        <v>55</v>
+      </c>
+      <c r="C328" s="341">
+        <v>0</v>
+      </c>
+      <c r="D328" s="341">
+        <v>0.75500000000000012</v>
+      </c>
+      <c r="E328" s="341">
+        <v>0.15838514486573971</v>
+      </c>
+      <c r="F328" s="341">
+        <v>0.73201711496642863</v>
+      </c>
+      <c r="G328" s="341">
+        <v>0</v>
+      </c>
+      <c r="H328" s="243">
+        <f t="shared" si="1"/>
+        <v>1.4672727272727271</v>
+      </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" s="245"/>
@@ -39159,7 +39346,7 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39176,27 +39363,27 @@
       </c>
     </row>
     <row r="2" spans="1:27" s="245" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="388" t="s">
+      <c r="C2" s="389" t="s">
         <v>454</v>
       </c>
-      <c r="D2" s="389"/>
-      <c r="E2" s="389"/>
-      <c r="F2" s="389"/>
-      <c r="G2" s="389"/>
+      <c r="D2" s="390"/>
+      <c r="E2" s="390"/>
+      <c r="F2" s="390"/>
+      <c r="G2" s="390"/>
       <c r="H2" s="247" t="s">
         <v>455</v>
       </c>
-      <c r="J2" s="390" t="s">
+      <c r="J2" s="391" t="s">
         <v>456</v>
       </c>
-      <c r="K2" s="391"/>
-      <c r="L2" s="391"/>
-      <c r="M2" s="391"/>
-      <c r="N2" s="391"/>
-      <c r="R2" s="392" t="s">
+      <c r="K2" s="392"/>
+      <c r="L2" s="392"/>
+      <c r="M2" s="392"/>
+      <c r="N2" s="392"/>
+      <c r="R2" s="393" t="s">
         <v>457</v>
       </c>
-      <c r="S2" s="392"/>
+      <c r="S2" s="393"/>
     </row>
     <row r="3" spans="1:27" s="245" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="141" t="s">
@@ -42436,25 +42623,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="397" t="s">
+      <c r="A3" s="398" t="s">
         <v>515</v>
       </c>
-      <c r="B3" s="395" t="s">
+      <c r="B3" s="396" t="s">
         <v>552</v>
       </c>
-      <c r="C3" s="395" t="s">
+      <c r="C3" s="396" t="s">
         <v>553</v>
       </c>
-      <c r="D3" s="395" t="s">
+      <c r="D3" s="396" t="s">
         <v>554</v>
       </c>
-      <c r="E3" s="395" t="s">
+      <c r="E3" s="396" t="s">
         <v>555</v>
       </c>
-      <c r="F3" s="395" t="s">
+      <c r="F3" s="396" t="s">
         <v>556</v>
       </c>
-      <c r="G3" s="395" t="s">
+      <c r="G3" s="396" t="s">
         <v>557</v>
       </c>
       <c r="J3" s="108" t="s">
@@ -42467,13 +42654,13 @@
       <c r="O3" s="108"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="398"/>
-      <c r="B4" s="396"/>
-      <c r="C4" s="396"/>
-      <c r="D4" s="396"/>
-      <c r="E4" s="396"/>
-      <c r="F4" s="396"/>
-      <c r="G4" s="396"/>
+      <c r="A4" s="399"/>
+      <c r="B4" s="397"/>
+      <c r="C4" s="397"/>
+      <c r="D4" s="397"/>
+      <c r="E4" s="397"/>
+      <c r="F4" s="397"/>
+      <c r="G4" s="397"/>
       <c r="J4" s="113" t="s">
         <v>16</v>
       </c>
@@ -42745,15 +42932,15 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="401" t="s">
+      <c r="A16" s="402" t="s">
         <v>559</v>
       </c>
-      <c r="B16" s="402"/>
-      <c r="C16" s="402"/>
-      <c r="D16" s="402"/>
-      <c r="E16" s="402"/>
-      <c r="F16" s="402"/>
-      <c r="G16" s="402"/>
+      <c r="B16" s="403"/>
+      <c r="C16" s="403"/>
+      <c r="D16" s="403"/>
+      <c r="E16" s="403"/>
+      <c r="F16" s="403"/>
+      <c r="G16" s="403"/>
       <c r="K16" s="59"/>
       <c r="L16" s="59"/>
       <c r="M16" s="59"/>
@@ -43097,10 +43284,10 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="399" t="s">
+      <c r="A28" s="400" t="s">
         <v>567</v>
       </c>
-      <c r="B28" s="400"/>
+      <c r="B28" s="401"/>
       <c r="C28" s="213">
         <f>SUM(C18:C27)</f>
         <v>108.48299999999998</v>
@@ -43123,15 +43310,15 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="401" t="s">
+      <c r="A29" s="402" t="s">
         <v>568</v>
       </c>
-      <c r="B29" s="402"/>
-      <c r="C29" s="402"/>
-      <c r="D29" s="402"/>
-      <c r="E29" s="402"/>
-      <c r="F29" s="402"/>
-      <c r="G29" s="402"/>
+      <c r="B29" s="403"/>
+      <c r="C29" s="403"/>
+      <c r="D29" s="403"/>
+      <c r="E29" s="403"/>
+      <c r="F29" s="403"/>
+      <c r="G29" s="403"/>
     </row>
     <row r="30" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="98"/>
@@ -43503,15 +43690,15 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="393" t="s">
+      <c r="A43" s="394" t="s">
         <v>577</v>
       </c>
-      <c r="B43" s="394"/>
-      <c r="C43" s="394"/>
-      <c r="D43" s="394"/>
-      <c r="E43" s="394"/>
-      <c r="F43" s="394"/>
-      <c r="G43" s="394"/>
+      <c r="B43" s="395"/>
+      <c r="C43" s="395"/>
+      <c r="D43" s="395"/>
+      <c r="E43" s="395"/>
+      <c r="F43" s="395"/>
+      <c r="G43" s="395"/>
     </row>
     <row r="44" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="98"/>
@@ -43739,69 +43926,69 @@
       <c r="BZ1" s="190"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="344" t="s">
+      <c r="A2" s="368" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="403"/>
-      <c r="C2" s="404"/>
-      <c r="D2" s="406" t="s">
+      <c r="B2" s="411"/>
+      <c r="C2" s="412"/>
+      <c r="D2" s="414" t="s">
         <v>582</v>
       </c>
-      <c r="E2" s="407"/>
-      <c r="F2" s="407"/>
-      <c r="G2" s="407"/>
-      <c r="H2" s="407"/>
-      <c r="I2" s="407"/>
-      <c r="J2" s="407"/>
-      <c r="K2" s="407"/>
-      <c r="L2" s="407"/>
-      <c r="M2" s="407"/>
-      <c r="N2" s="407"/>
-      <c r="O2" s="407"/>
-      <c r="P2" s="407"/>
-      <c r="Q2" s="407"/>
-      <c r="R2" s="407"/>
-      <c r="S2" s="407"/>
-      <c r="T2" s="407"/>
+      <c r="E2" s="415"/>
+      <c r="F2" s="415"/>
+      <c r="G2" s="415"/>
+      <c r="H2" s="415"/>
+      <c r="I2" s="415"/>
+      <c r="J2" s="415"/>
+      <c r="K2" s="415"/>
+      <c r="L2" s="415"/>
+      <c r="M2" s="415"/>
+      <c r="N2" s="415"/>
+      <c r="O2" s="415"/>
+      <c r="P2" s="415"/>
+      <c r="Q2" s="415"/>
+      <c r="R2" s="415"/>
+      <c r="S2" s="415"/>
+      <c r="T2" s="415"/>
       <c r="AA2" s="132"/>
       <c r="BY2" s="190"/>
       <c r="BZ2" s="190"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="346" t="s">
+      <c r="A3" s="370" t="s">
         <v>263</v>
       </c>
-      <c r="B3" s="403"/>
-      <c r="C3" s="404"/>
+      <c r="B3" s="411"/>
+      <c r="C3" s="412"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="408" t="s">
+      <c r="F3" s="416" t="s">
         <v>583</v>
       </c>
-      <c r="G3" s="409"/>
-      <c r="H3" s="410" t="s">
+      <c r="G3" s="417"/>
+      <c r="H3" s="418" t="s">
         <v>584</v>
       </c>
-      <c r="I3" s="410"/>
-      <c r="J3" s="411"/>
-      <c r="K3" s="412" t="s">
+      <c r="I3" s="418"/>
+      <c r="J3" s="419"/>
+      <c r="K3" s="420" t="s">
         <v>585</v>
       </c>
-      <c r="L3" s="413"/>
-      <c r="M3" s="414"/>
-      <c r="N3" s="411" t="s">
+      <c r="L3" s="421"/>
+      <c r="M3" s="422"/>
+      <c r="N3" s="419" t="s">
         <v>586</v>
       </c>
-      <c r="O3" s="415"/>
-      <c r="P3" s="416"/>
-      <c r="Q3" s="417" t="s">
+      <c r="O3" s="423"/>
+      <c r="P3" s="424"/>
+      <c r="Q3" s="425" t="s">
         <v>587</v>
       </c>
-      <c r="R3" s="418"/>
-      <c r="S3" s="419" t="s">
+      <c r="R3" s="426"/>
+      <c r="S3" s="427" t="s">
         <v>588</v>
       </c>
-      <c r="T3" s="420"/>
+      <c r="T3" s="428"/>
       <c r="AA3" s="133"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -43965,7 +44152,7 @@
       <c r="AC6" s="134"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="425" t="str">
+      <c r="C7" s="405" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -43973,81 +44160,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="428"/>
-      <c r="E7" s="426"/>
-      <c r="F7" s="428" t="s">
+      <c r="D7" s="406"/>
+      <c r="E7" s="407"/>
+      <c r="F7" s="406" t="s">
         <v>611</v>
       </c>
-      <c r="G7" s="428"/>
-      <c r="H7" s="426"/>
-      <c r="I7" s="429" t="str">
+      <c r="G7" s="406"/>
+      <c r="H7" s="407"/>
+      <c r="I7" s="408" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$242.422)</v>
       </c>
-      <c r="J7" s="430"/>
-      <c r="K7" s="430"/>
-      <c r="L7" s="430"/>
-      <c r="M7" s="430"/>
-      <c r="N7" s="430"/>
-      <c r="O7" s="430"/>
-      <c r="P7" s="430"/>
-      <c r="Q7" s="430"/>
-      <c r="R7" s="431"/>
-      <c r="S7" s="425" t="str">
+      <c r="J7" s="409"/>
+      <c r="K7" s="409"/>
+      <c r="L7" s="409"/>
+      <c r="M7" s="409"/>
+      <c r="N7" s="409"/>
+      <c r="O7" s="409"/>
+      <c r="P7" s="409"/>
+      <c r="Q7" s="409"/>
+      <c r="R7" s="410"/>
+      <c r="S7" s="405" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$596.731)</v>
       </c>
-      <c r="T7" s="428"/>
-      <c r="U7" s="428"/>
-      <c r="V7" s="428"/>
-      <c r="W7" s="428"/>
-      <c r="X7" s="426"/>
-      <c r="Y7" s="425" t="s">
+      <c r="T7" s="406"/>
+      <c r="U7" s="406"/>
+      <c r="V7" s="406"/>
+      <c r="W7" s="406"/>
+      <c r="X7" s="407"/>
+      <c r="Y7" s="405" t="s">
         <v>612</v>
       </c>
-      <c r="Z7" s="426"/>
+      <c r="Z7" s="407"/>
       <c r="AA7" s="135"/>
-      <c r="AH7" s="421" t="s">
+      <c r="AH7" s="429" t="s">
         <v>613</v>
       </c>
-      <c r="AI7" s="422"/>
+      <c r="AI7" s="430"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="423" t="s">
+      <c r="AK7" s="431" t="s">
         <v>614</v>
       </c>
-      <c r="AL7" s="402"/>
-      <c r="AM7" s="402"/>
-      <c r="AN7" s="422"/>
-      <c r="AP7" s="424" t="s">
+      <c r="AL7" s="403"/>
+      <c r="AM7" s="403"/>
+      <c r="AN7" s="430"/>
+      <c r="AP7" s="432" t="s">
         <v>615</v>
       </c>
-      <c r="AQ7" s="350"/>
-      <c r="AS7" s="405" t="s">
+      <c r="AQ7" s="374"/>
+      <c r="AS7" s="413" t="s">
         <v>616</v>
       </c>
-      <c r="AT7" s="349"/>
-      <c r="AU7" s="349"/>
-      <c r="AV7" s="349"/>
-      <c r="AW7" s="349"/>
-      <c r="AX7" s="349"/>
-      <c r="AY7" s="349"/>
-      <c r="AZ7" s="349"/>
-      <c r="BA7" s="349"/>
-      <c r="BB7" s="350"/>
-      <c r="BD7" s="424" t="s">
+      <c r="AT7" s="373"/>
+      <c r="AU7" s="373"/>
+      <c r="AV7" s="373"/>
+      <c r="AW7" s="373"/>
+      <c r="AX7" s="373"/>
+      <c r="AY7" s="373"/>
+      <c r="AZ7" s="373"/>
+      <c r="BA7" s="373"/>
+      <c r="BB7" s="374"/>
+      <c r="BD7" s="432" t="s">
         <v>617</v>
       </c>
-      <c r="BE7" s="350"/>
+      <c r="BE7" s="374"/>
       <c r="BF7" s="190"/>
-      <c r="BG7" s="405" t="s">
+      <c r="BG7" s="413" t="s">
         <v>618</v>
       </c>
-      <c r="BH7" s="349"/>
-      <c r="BI7" s="349"/>
+      <c r="BH7" s="373"/>
+      <c r="BI7" s="373"/>
       <c r="BY7" s="190"/>
       <c r="BZ7" s="190"/>
     </row>
@@ -53992,17 +54179,17 @@
       <c r="BZ52" s="190"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="427"/>
-      <c r="D53" s="427"/>
-      <c r="E53" s="427"/>
-      <c r="F53" s="427"/>
-      <c r="G53" s="427"/>
-      <c r="H53" s="427"/>
-      <c r="I53" s="427"/>
-      <c r="J53" s="427"/>
-      <c r="K53" s="427"/>
-      <c r="L53" s="427"/>
-      <c r="M53" s="427"/>
+      <c r="C53" s="404"/>
+      <c r="D53" s="404"/>
+      <c r="E53" s="404"/>
+      <c r="F53" s="404"/>
+      <c r="G53" s="404"/>
+      <c r="H53" s="404"/>
+      <c r="I53" s="404"/>
+      <c r="J53" s="404"/>
+      <c r="K53" s="404"/>
+      <c r="L53" s="404"/>
+      <c r="M53" s="404"/>
       <c r="AC53" s="137" t="s">
         <v>667</v>
       </c>
@@ -54137,11 +54324,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -54158,6 +54340,11 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6">

</xml_diff>

<commit_message>
commit prior to changing way step constraints are dealt with
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235" tabRatio="725" activeTab="6"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235" tabRatio="725" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3758" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3745" uniqueCount="715">
   <si>
     <t>Scenario</t>
   </si>
@@ -2327,6 +2327,9 @@
   </si>
   <si>
     <t>* These are John D's final recommendations. Can be changed to test other forced changes…</t>
+  </si>
+  <si>
+    <t>only BWF</t>
   </si>
 </sst>
 </file>
@@ -4593,77 +4596,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4684,6 +4626,12 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4698,6 +4646,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4764,6 +4767,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4824,27 +4848,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4936,7 +4939,63 @@
     <cellStyle name="Percent 5" xfId="83"/>
     <cellStyle name="Style 1" xfId="84"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5131,11 +5190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146483200"/>
-        <c:axId val="137379136"/>
+        <c:axId val="193655296"/>
+        <c:axId val="193532992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146483200"/>
+        <c:axId val="193655296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5164,7 +5223,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137379136"/>
+        <c:crossAx val="193532992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5172,7 +5231,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137379136"/>
+        <c:axId val="193532992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5210,7 +5269,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146483200"/>
+        <c:crossAx val="193655296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5673,11 +5732,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146507776"/>
-        <c:axId val="161267712"/>
+        <c:axId val="193657344"/>
+        <c:axId val="193534720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146507776"/>
+        <c:axId val="193657344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5706,7 +5765,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161267712"/>
+        <c:crossAx val="193534720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5714,7 +5773,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161267712"/>
+        <c:axId val="193534720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -5750,7 +5809,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146507776"/>
+        <c:crossAx val="193657344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5886,11 +5945,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="166863360"/>
-        <c:axId val="161274048"/>
+        <c:axId val="193658368"/>
+        <c:axId val="194331776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166863360"/>
+        <c:axId val="193658368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5919,7 +5978,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161274048"/>
+        <c:crossAx val="194331776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5927,7 +5986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161274048"/>
+        <c:axId val="194331776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5965,7 +6024,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166863360"/>
+        <c:crossAx val="193658368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6167,11 +6226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146482688"/>
-        <c:axId val="164766272"/>
+        <c:axId val="194434560"/>
+        <c:axId val="194334080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146482688"/>
+        <c:axId val="194434560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6182,7 +6241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164766272"/>
+        <c:crossAx val="194334080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6190,7 +6249,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164766272"/>
+        <c:axId val="194334080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000000"/>
@@ -6203,7 +6262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146482688"/>
+        <c:crossAx val="194434560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100000000"/>
@@ -6782,11 +6841,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="180039680"/>
-        <c:axId val="207161600"/>
+        <c:axId val="195084288"/>
+        <c:axId val="194820288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180039680"/>
+        <c:axId val="195084288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6807,7 +6866,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207161600"/>
+        <c:crossAx val="194820288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6815,7 +6874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="207161600"/>
+        <c:axId val="194820288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6837,7 +6896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180039680"/>
+        <c:crossAx val="195084288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -7426,8 +7485,8 @@
   </sheetPr>
   <dimension ref="A1:CP243"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16336,16 +16395,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="353" t="s">
+      <c r="A1" s="376" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="354"/>
+      <c r="B1" s="377"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="355" t="s">
+      <c r="A2" s="378" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="356"/>
+      <c r="B2" s="379"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="X3" s="245" t="s">
@@ -16353,33 +16412,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="363" t="s">
+      <c r="A4" s="383" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="364"/>
+      <c r="B4" s="384"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="367" t="s">
+      <c r="D4" s="387" t="s">
         <v>264</v>
       </c>
-      <c r="E4" s="357" t="s">
+      <c r="E4" s="380" t="s">
         <v>265</v>
       </c>
-      <c r="F4" s="358"/>
-      <c r="G4" s="358"/>
-      <c r="H4" s="358"/>
-      <c r="I4" s="358"/>
-      <c r="J4" s="358"/>
-      <c r="K4" s="358"/>
-      <c r="L4" s="358"/>
-      <c r="M4" s="358"/>
-      <c r="N4" s="358"/>
-      <c r="O4" s="358"/>
-      <c r="P4" s="358"/>
-      <c r="Q4" s="358"/>
-      <c r="R4" s="358"/>
-      <c r="S4" s="358"/>
-      <c r="T4" s="358"/>
-      <c r="U4" s="359"/>
+      <c r="F4" s="381"/>
+      <c r="G4" s="381"/>
+      <c r="H4" s="381"/>
+      <c r="I4" s="381"/>
+      <c r="J4" s="381"/>
+      <c r="K4" s="381"/>
+      <c r="L4" s="381"/>
+      <c r="M4" s="381"/>
+      <c r="N4" s="381"/>
+      <c r="O4" s="381"/>
+      <c r="P4" s="381"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="381"/>
+      <c r="S4" s="381"/>
+      <c r="T4" s="381"/>
+      <c r="U4" s="382"/>
       <c r="Y4" s="245">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -16446,12 +16505,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="365"/>
-      <c r="B5" s="366"/>
+      <c r="A5" s="385"/>
+      <c r="B5" s="386"/>
       <c r="C5" s="68" t="s">
         <v>266</v>
       </c>
-      <c r="D5" s="368"/>
+      <c r="D5" s="388"/>
       <c r="E5" s="69">
         <f>'Step Analysis'!E5</f>
         <v>2020</v>
@@ -16589,10 +16648,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="369" t="s">
+      <c r="A6" s="355" t="s">
         <v>268</v>
       </c>
-      <c r="B6" s="370"/>
+      <c r="B6" s="356"/>
       <c r="C6" s="164">
         <v>10</v>
       </c>
@@ -17110,12 +17169,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="360" t="s">
+      <c r="A12" s="370" t="s">
         <v>279</v>
       </c>
-      <c r="B12" s="361"/>
-      <c r="C12" s="361"/>
-      <c r="D12" s="362"/>
+      <c r="B12" s="371"/>
+      <c r="C12" s="371"/>
+      <c r="D12" s="372"/>
       <c r="E12" s="285">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -17250,12 +17309,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="360" t="s">
+      <c r="A13" s="370" t="s">
         <v>280</v>
       </c>
-      <c r="B13" s="361"/>
-      <c r="C13" s="361"/>
-      <c r="D13" s="362"/>
+      <c r="B13" s="371"/>
+      <c r="C13" s="371"/>
+      <c r="D13" s="372"/>
       <c r="E13" s="285"/>
       <c r="F13" s="285"/>
       <c r="G13" s="285"/>
@@ -17348,10 +17407,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="369" t="s">
+      <c r="A14" s="355" t="s">
         <v>281</v>
       </c>
-      <c r="B14" s="370"/>
+      <c r="B14" s="356"/>
       <c r="C14" s="166">
         <v>10</v>
       </c>
@@ -17866,12 +17925,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="360" t="s">
+      <c r="A20" s="370" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="361"/>
-      <c r="C20" s="361"/>
-      <c r="D20" s="362"/>
+      <c r="B20" s="371"/>
+      <c r="C20" s="371"/>
+      <c r="D20" s="372"/>
       <c r="E20" s="285">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -17942,12 +18001,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="360" t="s">
+      <c r="A21" s="370" t="s">
         <v>285</v>
       </c>
-      <c r="B21" s="361"/>
-      <c r="C21" s="361"/>
-      <c r="D21" s="362"/>
+      <c r="B21" s="371"/>
+      <c r="C21" s="371"/>
+      <c r="D21" s="372"/>
       <c r="E21" s="285"/>
       <c r="F21" s="285"/>
       <c r="G21" s="285"/>
@@ -17973,10 +18032,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="369" t="s">
+      <c r="A22" s="355" t="s">
         <v>286</v>
       </c>
-      <c r="B22" s="370"/>
+      <c r="B22" s="356"/>
       <c r="C22" s="164">
         <v>10</v>
       </c>
@@ -18223,12 +18282,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="360" t="s">
+      <c r="A28" s="370" t="s">
         <v>287</v>
       </c>
-      <c r="B28" s="361"/>
-      <c r="C28" s="361"/>
-      <c r="D28" s="362"/>
+      <c r="B28" s="371"/>
+      <c r="C28" s="371"/>
+      <c r="D28" s="372"/>
       <c r="E28" s="285">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -18299,12 +18358,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="360" t="s">
+      <c r="A29" s="370" t="s">
         <v>288</v>
       </c>
-      <c r="B29" s="361"/>
-      <c r="C29" s="361"/>
-      <c r="D29" s="362"/>
+      <c r="B29" s="371"/>
+      <c r="C29" s="371"/>
+      <c r="D29" s="372"/>
       <c r="E29" s="285"/>
       <c r="F29" s="285"/>
       <c r="G29" s="285"/>
@@ -18330,10 +18389,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="369" t="s">
+      <c r="A30" s="355" t="s">
         <v>289</v>
       </c>
-      <c r="B30" s="370"/>
+      <c r="B30" s="356"/>
       <c r="C30" s="164">
         <v>10</v>
       </c>
@@ -18580,12 +18639,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="360" t="s">
+      <c r="A36" s="370" t="s">
         <v>290</v>
       </c>
-      <c r="B36" s="361"/>
-      <c r="C36" s="361"/>
-      <c r="D36" s="362"/>
+      <c r="B36" s="371"/>
+      <c r="C36" s="371"/>
+      <c r="D36" s="372"/>
       <c r="E36" s="285">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -18656,12 +18715,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="360" t="s">
+      <c r="A37" s="370" t="s">
         <v>291</v>
       </c>
-      <c r="B37" s="361"/>
-      <c r="C37" s="361"/>
-      <c r="D37" s="362"/>
+      <c r="B37" s="371"/>
+      <c r="C37" s="371"/>
+      <c r="D37" s="372"/>
       <c r="E37" s="285"/>
       <c r="F37" s="285"/>
       <c r="G37" s="285"/>
@@ -18687,10 +18746,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="369" t="s">
+      <c r="A38" s="355" t="s">
         <v>292</v>
       </c>
-      <c r="B38" s="370"/>
+      <c r="B38" s="356"/>
       <c r="C38" s="164">
         <v>10</v>
       </c>
@@ -18937,12 +18996,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="360" t="s">
+      <c r="A44" s="370" t="s">
         <v>293</v>
       </c>
-      <c r="B44" s="361"/>
-      <c r="C44" s="361"/>
-      <c r="D44" s="362"/>
+      <c r="B44" s="371"/>
+      <c r="C44" s="371"/>
+      <c r="D44" s="372"/>
       <c r="E44" s="285">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -19013,12 +19072,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="360" t="s">
+      <c r="A45" s="370" t="s">
         <v>294</v>
       </c>
-      <c r="B45" s="361"/>
-      <c r="C45" s="361"/>
-      <c r="D45" s="362"/>
+      <c r="B45" s="371"/>
+      <c r="C45" s="371"/>
+      <c r="D45" s="372"/>
       <c r="E45" s="285"/>
       <c r="F45" s="285"/>
       <c r="G45" s="285"/>
@@ -19044,11 +19103,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="378" t="s">
+      <c r="A46" s="357" t="s">
         <v>295</v>
       </c>
-      <c r="B46" s="379"/>
-      <c r="C46" s="380"/>
+      <c r="B46" s="358"/>
+      <c r="C46" s="359"/>
       <c r="D46" s="174"/>
       <c r="E46" s="293">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -19121,12 +19180,12 @@
       <c r="V46" s="246"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="384" t="s">
+      <c r="A47" s="365" t="s">
         <v>296</v>
       </c>
-      <c r="B47" s="385"/>
-      <c r="C47" s="385"/>
-      <c r="D47" s="386"/>
+      <c r="B47" s="366"/>
+      <c r="C47" s="366"/>
+      <c r="D47" s="367"/>
       <c r="E47" s="294">
         <f>E46</f>
         <v>1500000</v>
@@ -19197,7 +19256,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="175"/>
       <c r="B48" s="175"/>
-      <c r="C48" s="387" t="s">
+      <c r="C48" s="368" t="s">
         <v>297</v>
       </c>
       <c r="D48" s="176">
@@ -19272,7 +19331,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="175"/>
-      <c r="C49" s="388"/>
+      <c r="C49" s="369"/>
       <c r="D49" s="248">
         <v>37</v>
       </c>
@@ -19343,7 +19402,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="175"/>
-      <c r="C50" s="388"/>
+      <c r="C50" s="369"/>
       <c r="D50" s="248">
         <v>30</v>
       </c>
@@ -19414,7 +19473,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="175"/>
-      <c r="C51" s="388"/>
+      <c r="C51" s="369"/>
       <c r="D51" s="248">
         <v>41</v>
       </c>
@@ -19484,38 +19543,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="381" t="s">
+      <c r="A52" s="360" t="s">
         <v>298</v>
       </c>
-      <c r="B52" s="382"/>
-      <c r="C52" s="382"/>
-      <c r="D52" s="382"/>
-      <c r="E52" s="382"/>
-      <c r="F52" s="382"/>
-      <c r="G52" s="382"/>
-      <c r="H52" s="382"/>
-      <c r="I52" s="382"/>
-      <c r="J52" s="382"/>
-      <c r="K52" s="382"/>
-      <c r="L52" s="382"/>
-      <c r="M52" s="382"/>
-      <c r="N52" s="382"/>
-      <c r="O52" s="382"/>
-      <c r="P52" s="382"/>
-      <c r="Q52" s="382"/>
-      <c r="R52" s="382"/>
-      <c r="S52" s="382"/>
-      <c r="T52" s="382"/>
-      <c r="U52" s="382"/>
-      <c r="V52" s="382"/>
-      <c r="W52" s="383"/>
+      <c r="B52" s="361"/>
+      <c r="C52" s="361"/>
+      <c r="D52" s="361"/>
+      <c r="E52" s="361"/>
+      <c r="F52" s="361"/>
+      <c r="G52" s="361"/>
+      <c r="H52" s="361"/>
+      <c r="I52" s="361"/>
+      <c r="J52" s="361"/>
+      <c r="K52" s="361"/>
+      <c r="L52" s="361"/>
+      <c r="M52" s="361"/>
+      <c r="N52" s="361"/>
+      <c r="O52" s="361"/>
+      <c r="P52" s="361"/>
+      <c r="Q52" s="361"/>
+      <c r="R52" s="361"/>
+      <c r="S52" s="361"/>
+      <c r="T52" s="361"/>
+      <c r="U52" s="361"/>
+      <c r="V52" s="361"/>
+      <c r="W52" s="362"/>
       <c r="X52" s="246"/>
     </row>
     <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="373" t="s">
+      <c r="A53" s="363" t="s">
         <v>299</v>
       </c>
-      <c r="B53" s="374"/>
+      <c r="B53" s="364"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -19692,10 +19751,10 @@
       <c r="X57" s="246"/>
     </row>
     <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="371" t="s">
+      <c r="A58" s="353" t="s">
         <v>301</v>
       </c>
-      <c r="B58" s="372"/>
+      <c r="B58" s="354"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -19877,10 +19936,10 @@
       <c r="X62" s="246"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="371" t="s">
+      <c r="A63" s="353" t="s">
         <v>302</v>
       </c>
-      <c r="B63" s="372"/>
+      <c r="B63" s="354"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -20070,10 +20129,10 @@
       <c r="X67" s="246"/>
     </row>
     <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="371" t="s">
+      <c r="A68" s="353" t="s">
         <v>303</v>
       </c>
-      <c r="B68" s="372"/>
+      <c r="B68" s="354"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -20251,10 +20310,10 @@
       <c r="X72" s="246"/>
     </row>
     <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="371" t="s">
+      <c r="A73" s="353" t="s">
         <v>304</v>
       </c>
-      <c r="B73" s="372"/>
+      <c r="B73" s="354"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -20480,10 +20539,10 @@
       <c r="X77" s="246"/>
     </row>
     <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="371" t="s">
+      <c r="A78" s="353" t="s">
         <v>306</v>
       </c>
-      <c r="B78" s="372"/>
+      <c r="B78" s="354"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -20655,10 +20714,10 @@
       <c r="X82" s="246"/>
     </row>
     <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="371" t="s">
+      <c r="A83" s="353" t="s">
         <v>308</v>
       </c>
-      <c r="B83" s="372"/>
+      <c r="B83" s="354"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -20830,10 +20889,10 @@
       <c r="X87" s="246"/>
     </row>
     <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="371" t="s">
+      <c r="A88" s="353" t="s">
         <v>80</v>
       </c>
-      <c r="B88" s="372"/>
+      <c r="B88" s="354"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -21005,10 +21064,10 @@
       <c r="X92" s="246"/>
     </row>
     <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="371" t="s">
+      <c r="A93" s="353" t="s">
         <v>311</v>
       </c>
-      <c r="B93" s="372"/>
+      <c r="B93" s="354"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -21210,10 +21269,10 @@
       <c r="X97" s="246"/>
     </row>
     <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="371" t="s">
+      <c r="A98" s="353" t="s">
         <v>313</v>
       </c>
-      <c r="B98" s="372"/>
+      <c r="B98" s="354"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -21405,10 +21464,10 @@
       <c r="X102" s="246"/>
     </row>
     <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="371" t="s">
+      <c r="A103" s="353" t="s">
         <v>315</v>
       </c>
-      <c r="B103" s="372"/>
+      <c r="B103" s="354"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -21610,10 +21669,10 @@
       <c r="X107" s="246"/>
     </row>
     <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="371" t="s">
+      <c r="A108" s="353" t="s">
         <v>316</v>
       </c>
-      <c r="B108" s="372"/>
+      <c r="B108" s="354"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -21815,10 +21874,10 @@
       <c r="X112" s="246"/>
     </row>
     <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="371" t="s">
+      <c r="A113" s="353" t="s">
         <v>317</v>
       </c>
-      <c r="B113" s="372"/>
+      <c r="B113" s="354"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -21980,10 +22039,10 @@
       <c r="X117" s="246"/>
     </row>
     <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="371" t="s">
+      <c r="A118" s="353" t="s">
         <v>318</v>
       </c>
-      <c r="B118" s="372"/>
+      <c r="B118" s="354"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -22185,10 +22244,10 @@
       <c r="X122" s="246"/>
     </row>
     <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="371" t="s">
+      <c r="A123" s="353" t="s">
         <v>319</v>
       </c>
-      <c r="B123" s="372"/>
+      <c r="B123" s="354"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -22390,10 +22449,10 @@
       <c r="X127" s="246"/>
     </row>
     <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="371" t="s">
+      <c r="A128" s="353" t="s">
         <v>320</v>
       </c>
-      <c r="B128" s="372"/>
+      <c r="B128" s="354"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -22595,10 +22654,10 @@
       <c r="X132" s="246"/>
     </row>
     <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="371" t="s">
+      <c r="A133" s="353" t="s">
         <v>321</v>
       </c>
-      <c r="B133" s="372"/>
+      <c r="B133" s="354"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -22800,10 +22859,10 @@
       <c r="X137" s="246"/>
     </row>
     <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="371" t="s">
+      <c r="A138" s="353" t="s">
         <v>322</v>
       </c>
-      <c r="B138" s="372"/>
+      <c r="B138" s="354"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -23013,10 +23072,10 @@
       <c r="X142" s="246"/>
     </row>
     <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="371" t="s">
+      <c r="A143" s="353" t="s">
         <v>326</v>
       </c>
-      <c r="B143" s="372"/>
+      <c r="B143" s="354"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -23109,10 +23168,10 @@
       <c r="X144" s="246"/>
     </row>
     <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="373" t="s">
+      <c r="A145" s="363" t="s">
         <v>328</v>
       </c>
-      <c r="B145" s="374"/>
+      <c r="B145" s="364"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -23185,10 +23244,10 @@
       <c r="X146" s="246"/>
     </row>
     <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="373" t="s">
+      <c r="A147" s="363" t="s">
         <v>329</v>
       </c>
-      <c r="B147" s="374"/>
+      <c r="B147" s="364"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -23286,10 +23345,10 @@
       <c r="X148" s="246"/>
     </row>
     <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="373" t="s">
+      <c r="A149" s="363" t="s">
         <v>330</v>
       </c>
-      <c r="B149" s="374"/>
+      <c r="B149" s="364"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -23411,12 +23470,12 @@
       <c r="X151" s="246"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="375" t="s">
+      <c r="A152" s="373" t="s">
         <v>331</v>
       </c>
-      <c r="B152" s="376"/>
-      <c r="C152" s="376"/>
-      <c r="D152" s="377"/>
+      <c r="B152" s="374"/>
+      <c r="C152" s="374"/>
+      <c r="D152" s="375"/>
       <c r="E152" s="317">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -24028,6 +24087,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -24044,37 +24134,6 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -26312,10 +26371,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AG200"/>
+  <dimension ref="A1:AG201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26833,20 +26892,14 @@
         <v>60</v>
       </c>
       <c r="B22" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C22" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="234" t="s">
-        <v>52</v>
-      </c>
+      <c r="D22" s="234"/>
+      <c r="E22" s="234"/>
+      <c r="F22" s="234"/>
       <c r="G22" s="234"/>
       <c r="H22" s="234"/>
       <c r="I22" s="234"/>
@@ -26873,20 +26926,14 @@
         <v>61</v>
       </c>
       <c r="B23" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C23" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="234" t="s">
-        <v>52</v>
-      </c>
+      <c r="D23" s="234"/>
+      <c r="E23" s="234"/>
+      <c r="F23" s="234"/>
       <c r="G23" s="234"/>
       <c r="H23" s="234"/>
       <c r="I23" s="234"/>
@@ -26903,20 +26950,14 @@
         <v>62</v>
       </c>
       <c r="B24" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C24" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="234" t="s">
-        <v>52</v>
-      </c>
+      <c r="D24" s="234"/>
+      <c r="E24" s="234"/>
+      <c r="F24" s="234"/>
       <c r="G24" s="234"/>
       <c r="H24" s="234"/>
       <c r="I24" s="234"/>
@@ -26933,20 +26974,14 @@
         <v>63</v>
       </c>
       <c r="B25" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C25" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="234" t="s">
-        <v>52</v>
-      </c>
+      <c r="D25" s="234"/>
+      <c r="E25" s="234"/>
+      <c r="F25" s="234"/>
       <c r="G25" s="234"/>
       <c r="H25" s="234"/>
       <c r="I25" s="234"/>
@@ -26963,20 +26998,14 @@
         <v>64</v>
       </c>
       <c r="B26" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C26" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="234" t="s">
-        <v>52</v>
-      </c>
+      <c r="D26" s="234"/>
+      <c r="E26" s="234"/>
+      <c r="F26" s="234"/>
       <c r="G26" s="234"/>
       <c r="H26" s="234"/>
       <c r="I26" s="234"/>
@@ -27477,83 +27506,77 @@
     </row>
     <row r="46" spans="1:33" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="234" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="346" t="s">
+        <v>696</v>
+      </c>
+      <c r="C46" s="346" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="337"/>
+      <c r="E46" s="337"/>
+      <c r="F46" s="337"/>
+      <c r="G46" s="337"/>
+      <c r="H46" s="337"/>
+      <c r="I46" s="337"/>
+      <c r="J46" s="337"/>
+      <c r="L46" s="242" t="s">
+        <v>92</v>
+      </c>
+      <c r="M46" s="242" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="234" t="s">
         <v>108</v>
       </c>
-      <c r="B46" s="242" t="s">
+      <c r="B47" s="242" t="s">
         <v>693</v>
       </c>
-      <c r="C46" s="336" t="s">
+      <c r="C47" s="336" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="336" t="s">
+      <c r="D47" s="336" t="s">
         <v>196</v>
       </c>
-      <c r="E46" s="336" t="s">
+      <c r="E47" s="336" t="s">
         <v>105</v>
       </c>
-      <c r="F46" s="336" t="s">
+      <c r="F47" s="336" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="336" t="s">
+      <c r="G47" s="336" t="s">
         <v>48</v>
       </c>
-      <c r="H46" s="336" t="s">
+      <c r="H47" s="336" t="s">
         <v>42</v>
       </c>
-      <c r="I46" s="336" t="s">
+      <c r="I47" s="336" t="s">
         <v>100</v>
       </c>
-      <c r="J46" s="336" t="s">
+      <c r="J47" s="336" t="s">
         <v>41</v>
       </c>
-      <c r="L46" s="347" t="s">
+      <c r="L47" s="347" t="s">
         <v>691</v>
       </c>
-      <c r="M46" s="347" t="s">
+      <c r="M47" s="347" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="234" t="s">
+    <row r="48" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="234" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="242" t="s">
+      <c r="B48" s="242" t="s">
         <v>696</v>
       </c>
-      <c r="C47" s="234" t="s">
+      <c r="C48" s="234" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="234"/>
-      <c r="E47" s="234"/>
-      <c r="F47" s="234"/>
-      <c r="G47" s="234"/>
-      <c r="H47" s="234"/>
-      <c r="I47" s="234"/>
-      <c r="J47" s="234"/>
-      <c r="L47" t="s">
-        <v>113</v>
-      </c>
-      <c r="M47" t="s">
-        <v>690</v>
-      </c>
-      <c r="AG47" t="str">
-        <f>'Design HV &amp; WD'!A30</f>
-        <v>Till-Brine</v>
-      </c>
-    </row>
-    <row r="48" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" s="242" t="s">
-        <v>693</v>
-      </c>
-      <c r="C48" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="D48" s="234" t="s">
-        <v>105</v>
-      </c>
+      <c r="D48" s="234"/>
       <c r="E48" s="234"/>
       <c r="F48" s="234"/>
       <c r="G48" s="234"/>
@@ -27561,19 +27584,19 @@
       <c r="I48" s="234"/>
       <c r="J48" s="234"/>
       <c r="L48" t="s">
-        <v>383</v>
+        <v>113</v>
       </c>
       <c r="M48" t="s">
-        <v>371</v>
+        <v>690</v>
       </c>
       <c r="AG48" t="str">
-        <f>'Design HV &amp; WD'!A31</f>
-        <v>Sand Fences</v>
+        <f>'Design HV &amp; WD'!A30</f>
+        <v>Till-Brine</v>
       </c>
     </row>
     <row r="49" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" s="242" t="s">
         <v>693</v>
@@ -27590,10 +27613,20 @@
       <c r="H49" s="234"/>
       <c r="I49" s="234"/>
       <c r="J49" s="234"/>
+      <c r="L49" t="s">
+        <v>383</v>
+      </c>
+      <c r="M49" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG49" t="str">
+        <f>'Design HV &amp; WD'!A31</f>
+        <v>Sand Fences</v>
+      </c>
     </row>
     <row r="50" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B50" s="242" t="s">
         <v>693</v>
@@ -27613,7 +27646,7 @@
     </row>
     <row r="51" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B51" s="242" t="s">
         <v>693</v>
@@ -27633,7 +27666,7 @@
     </row>
     <row r="52" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B52" s="242" t="s">
         <v>693</v>
@@ -27653,7 +27686,7 @@
     </row>
     <row r="53" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B53" s="242" t="s">
         <v>693</v>
@@ -27670,20 +27703,10 @@
       <c r="H53" s="234"/>
       <c r="I53" s="234"/>
       <c r="J53" s="234"/>
-      <c r="L53" t="s">
-        <v>384</v>
-      </c>
-      <c r="M53" t="s">
-        <v>371</v>
-      </c>
-      <c r="AG53" t="str">
-        <f>'Design HV &amp; WD'!A32</f>
-        <v>Brine</v>
-      </c>
     </row>
     <row r="54" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="234" t="s">
-        <v>120</v>
+      <c r="A54" t="s">
+        <v>119</v>
       </c>
       <c r="B54" s="242" t="s">
         <v>693</v>
@@ -27700,14 +27723,20 @@
       <c r="H54" s="234"/>
       <c r="I54" s="234"/>
       <c r="J54" s="234"/>
+      <c r="L54" t="s">
+        <v>384</v>
+      </c>
+      <c r="M54" t="s">
+        <v>371</v>
+      </c>
       <c r="AG54" t="str">
-        <f>'Design HV &amp; WD'!A33</f>
-        <v>Breeding Waterfowl &amp; Meadow</v>
+        <f>'Design HV &amp; WD'!A32</f>
+        <v>Brine</v>
       </c>
     </row>
     <row r="55" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="234" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B55" s="242" t="s">
         <v>693</v>
@@ -27725,37 +27754,37 @@
       <c r="I55" s="234"/>
       <c r="J55" s="234"/>
       <c r="AG55" t="str">
-        <f>'Design HV &amp; WD'!A34</f>
-        <v>None</v>
-      </c>
-    </row>
-    <row r="56" spans="1:33" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="346" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" s="346" t="s">
-        <v>696</v>
+        <f>'Design HV &amp; WD'!A33</f>
+        <v>Breeding Waterfowl &amp; Meadow</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="234" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="242" t="s">
+        <v>693</v>
       </c>
       <c r="C56" s="234" t="s">
-        <v>52</v>
-      </c>
-      <c r="D56" s="234"/>
+        <v>196</v>
+      </c>
+      <c r="D56" s="234" t="s">
+        <v>105</v>
+      </c>
       <c r="E56" s="234"/>
       <c r="F56" s="234"/>
       <c r="G56" s="234"/>
       <c r="H56" s="234"/>
       <c r="I56" s="234"/>
       <c r="J56" s="234"/>
-      <c r="L56" s="242" t="s">
-        <v>122</v>
-      </c>
-      <c r="M56" s="242" t="s">
-        <v>701</v>
+      <c r="AG56" t="str">
+        <f>'Design HV &amp; WD'!A34</f>
+        <v>None</v>
       </c>
     </row>
     <row r="57" spans="1:33" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="346" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B57" s="346" t="s">
         <v>696</v>
@@ -27771,14 +27800,14 @@
       <c r="I57" s="234"/>
       <c r="J57" s="234"/>
       <c r="L57" s="242" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M57" s="242" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:33" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="242" t="s">
         <v>124</v>
       </c>
       <c r="B58" s="242" t="s">
@@ -27796,36 +27825,40 @@
       <c r="H58" s="234"/>
       <c r="I58" s="234"/>
       <c r="J58" s="234"/>
-      <c r="L58" t="s">
+      <c r="L58" s="242" t="s">
         <v>385</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M58" s="242" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="59" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>125</v>
-      </c>
-      <c r="B59" s="242" t="s">
-        <v>693</v>
+      <c r="A59" s="346" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="346" t="s">
+        <v>696</v>
       </c>
       <c r="C59" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="D59" s="234" t="s">
-        <v>105</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D59" s="234"/>
       <c r="E59" s="234"/>
       <c r="F59" s="234"/>
       <c r="G59" s="234"/>
       <c r="H59" s="234"/>
       <c r="I59" s="234"/>
       <c r="J59" s="234"/>
+      <c r="L59" t="s">
+        <v>123</v>
+      </c>
+      <c r="M59" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="60" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="242" t="s">
         <v>693</v>
@@ -27844,8 +27877,8 @@
       <c r="J60" s="234"/>
     </row>
     <row r="61" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="234" t="s">
-        <v>128</v>
+      <c r="A61" t="s">
+        <v>126</v>
       </c>
       <c r="B61" s="242" t="s">
         <v>693</v>
@@ -27856,58 +27889,52 @@
       <c r="D61" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="E61" s="234" t="s">
-        <v>57</v>
-      </c>
+      <c r="E61" s="234"/>
       <c r="F61" s="234"/>
       <c r="G61" s="234"/>
       <c r="H61" s="234"/>
       <c r="I61" s="234"/>
       <c r="J61" s="234"/>
-      <c r="L61" t="s">
-        <v>128</v>
-      </c>
-      <c r="M61" t="s">
-        <v>386</v>
-      </c>
     </row>
     <row r="62" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="234" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B62" s="242" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C62" s="234" t="s">
-        <v>52</v>
-      </c>
-      <c r="D62" s="234"/>
-      <c r="E62" s="234"/>
+        <v>196</v>
+      </c>
+      <c r="D62" s="234" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" s="234" t="s">
+        <v>57</v>
+      </c>
       <c r="F62" s="234"/>
       <c r="G62" s="234"/>
       <c r="H62" s="234"/>
       <c r="I62" s="234"/>
       <c r="J62" s="234"/>
       <c r="L62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M62" t="s">
-        <v>690</v>
+        <v>386</v>
       </c>
     </row>
     <row r="63" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="234" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B63" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C63" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="D63" s="234" t="s">
-        <v>105</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D63" s="234"/>
       <c r="E63" s="234"/>
       <c r="F63" s="234"/>
       <c r="G63" s="234"/>
@@ -27915,15 +27942,15 @@
       <c r="I63" s="234"/>
       <c r="J63" s="234"/>
       <c r="L63" t="s">
-        <v>387</v>
+        <v>129</v>
       </c>
       <c r="M63" t="s">
-        <v>371</v>
+        <v>690</v>
       </c>
     </row>
     <row r="64" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="234" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B64" s="242" t="s">
         <v>693</v>
@@ -27940,34 +27967,36 @@
       <c r="H64" s="234"/>
       <c r="I64" s="234"/>
       <c r="J64" s="234"/>
+      <c r="L64" t="s">
+        <v>387</v>
+      </c>
+      <c r="M64" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>132</v>
+      <c r="A65" s="234" t="s">
+        <v>131</v>
       </c>
       <c r="B65" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C65" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="D65" s="234"/>
+        <v>196</v>
+      </c>
+      <c r="D65" s="234" t="s">
+        <v>105</v>
+      </c>
       <c r="E65" s="234"/>
       <c r="F65" s="234"/>
       <c r="G65" s="234"/>
       <c r="H65" s="234"/>
       <c r="I65" s="234"/>
       <c r="J65" s="234"/>
-      <c r="L65" t="s">
-        <v>388</v>
-      </c>
-      <c r="M65" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B66" s="242" t="s">
         <v>693</v>
@@ -27982,44 +28011,34 @@
       <c r="H66" s="234"/>
       <c r="I66" s="234"/>
       <c r="J66" s="234"/>
+      <c r="L66" t="s">
+        <v>388</v>
+      </c>
+      <c r="M66" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="67" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="234" t="s">
-        <v>134</v>
+      <c r="A67" t="s">
+        <v>133</v>
       </c>
       <c r="B67" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C67" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" s="234" t="s">
-        <v>105</v>
-      </c>
-      <c r="E67" s="234" t="s">
-        <v>48</v>
-      </c>
-      <c r="F67" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="G67" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="H67" s="234" t="s">
-        <v>97</v>
-      </c>
+      <c r="D67" s="234"/>
+      <c r="E67" s="234"/>
+      <c r="F67" s="234"/>
+      <c r="G67" s="234"/>
+      <c r="H67" s="234"/>
       <c r="I67" s="234"/>
       <c r="J67" s="234"/>
-      <c r="L67" t="s">
-        <v>390</v>
-      </c>
-      <c r="M67" t="s">
-        <v>391</v>
-      </c>
     </row>
     <row r="68" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="234" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B68" s="242" t="s">
         <v>693</v>
@@ -28030,22 +28049,30 @@
       <c r="D68" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="E68" s="234"/>
-      <c r="F68" s="234"/>
-      <c r="G68" s="234"/>
-      <c r="H68" s="234"/>
+      <c r="E68" s="234" t="s">
+        <v>48</v>
+      </c>
+      <c r="F68" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="G68" s="234" t="s">
+        <v>34</v>
+      </c>
+      <c r="H68" s="234" t="s">
+        <v>97</v>
+      </c>
       <c r="I68" s="234"/>
       <c r="J68" s="234"/>
       <c r="L68" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="M68" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="234" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B69" s="242" t="s">
         <v>693</v>
@@ -28062,34 +28089,36 @@
       <c r="H69" s="234"/>
       <c r="I69" s="234"/>
       <c r="J69" s="234"/>
+      <c r="L69" t="s">
+        <v>392</v>
+      </c>
+      <c r="M69" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>137</v>
+      <c r="A70" s="234" t="s">
+        <v>136</v>
       </c>
       <c r="B70" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C70" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="D70" s="234"/>
+        <v>196</v>
+      </c>
+      <c r="D70" s="234" t="s">
+        <v>105</v>
+      </c>
       <c r="E70" s="234"/>
       <c r="F70" s="234"/>
       <c r="G70" s="234"/>
       <c r="H70" s="234"/>
       <c r="I70" s="234"/>
       <c r="J70" s="234"/>
-      <c r="L70" t="s">
-        <v>393</v>
-      </c>
-      <c r="M70" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" s="242" t="s">
         <v>693</v>
@@ -28104,10 +28133,16 @@
       <c r="H71" s="234"/>
       <c r="I71" s="234"/>
       <c r="J71" s="234"/>
+      <c r="L71" t="s">
+        <v>393</v>
+      </c>
+      <c r="M71" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B72" s="242" t="s">
         <v>693</v>
@@ -28125,7 +28160,7 @@
     </row>
     <row r="73" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B73" s="242" t="s">
         <v>693</v>
@@ -28143,7 +28178,7 @@
     </row>
     <row r="74" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B74" s="242" t="s">
         <v>693</v>
@@ -28161,7 +28196,7 @@
     </row>
     <row r="75" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B75" s="242" t="s">
         <v>693</v>
@@ -28179,7 +28214,7 @@
     </row>
     <row r="76" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B76" s="242" t="s">
         <v>693</v>
@@ -28197,7 +28232,7 @@
     </row>
     <row r="77" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B77" s="242" t="s">
         <v>693</v>
@@ -28215,7 +28250,7 @@
     </row>
     <row r="78" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" s="242" t="s">
         <v>693</v>
@@ -28233,7 +28268,7 @@
     </row>
     <row r="79" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B79" s="242" t="s">
         <v>693</v>
@@ -28248,16 +28283,10 @@
       <c r="H79" s="234"/>
       <c r="I79" s="234"/>
       <c r="J79" s="234"/>
-      <c r="L79" t="s">
-        <v>394</v>
-      </c>
-      <c r="M79" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="80" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B80" s="242" t="s">
         <v>693</v>
@@ -28272,10 +28301,16 @@
       <c r="H80" s="234"/>
       <c r="I80" s="234"/>
       <c r="J80" s="234"/>
+      <c r="L80" t="s">
+        <v>394</v>
+      </c>
+      <c r="M80" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="81" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B81" s="242" t="s">
         <v>693</v>
@@ -28293,7 +28328,7 @@
     </row>
     <row r="82" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="242" t="s">
         <v>693</v>
@@ -28310,8 +28345,8 @@
       <c r="J82" s="234"/>
     </row>
     <row r="83" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="234" t="s">
-        <v>150</v>
+      <c r="A83" t="s">
+        <v>149</v>
       </c>
       <c r="B83" s="242" t="s">
         <v>693</v>
@@ -28326,16 +28361,10 @@
       <c r="H83" s="234"/>
       <c r="I83" s="234"/>
       <c r="J83" s="234"/>
-      <c r="L83" t="s">
+    </row>
+    <row r="84" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="234" t="s">
         <v>150</v>
-      </c>
-      <c r="M83" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>151</v>
       </c>
       <c r="B84" s="242" t="s">
         <v>693</v>
@@ -28351,7 +28380,7 @@
       <c r="I84" s="234"/>
       <c r="J84" s="234"/>
       <c r="L84" t="s">
-        <v>395</v>
+        <v>150</v>
       </c>
       <c r="M84" t="s">
         <v>389</v>
@@ -28359,7 +28388,7 @@
     </row>
     <row r="85" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B85" s="242" t="s">
         <v>693</v>
@@ -28374,10 +28403,16 @@
       <c r="H85" s="234"/>
       <c r="I85" s="234"/>
       <c r="J85" s="234"/>
+      <c r="L85" t="s">
+        <v>395</v>
+      </c>
+      <c r="M85" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="86" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="234" t="s">
-        <v>153</v>
+      <c r="A86" t="s">
+        <v>152</v>
       </c>
       <c r="B86" s="242" t="s">
         <v>693</v>
@@ -28385,27 +28420,17 @@
       <c r="C86" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="D86" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="E86" s="234" t="s">
-        <v>105</v>
-      </c>
+      <c r="D86" s="234"/>
+      <c r="E86" s="234"/>
       <c r="F86" s="234"/>
       <c r="G86" s="234"/>
       <c r="H86" s="234"/>
       <c r="I86" s="234"/>
       <c r="J86" s="234"/>
-      <c r="L86" t="s">
+    </row>
+    <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="234" t="s">
         <v>153</v>
-      </c>
-      <c r="M86" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>154</v>
       </c>
       <c r="B87" s="242" t="s">
         <v>693</v>
@@ -28425,15 +28450,15 @@
       <c r="I87" s="234"/>
       <c r="J87" s="234"/>
       <c r="L87" t="s">
-        <v>397</v>
+        <v>153</v>
       </c>
       <c r="M87" t="s">
-        <v>698</v>
+        <v>396</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B88" s="242" t="s">
         <v>693</v>
@@ -28441,17 +28466,27 @@
       <c r="C88" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="D88" s="234"/>
-      <c r="E88" s="234"/>
+      <c r="D88" s="234" t="s">
+        <v>196</v>
+      </c>
+      <c r="E88" s="234" t="s">
+        <v>105</v>
+      </c>
       <c r="F88" s="234"/>
       <c r="G88" s="234"/>
       <c r="H88" s="234"/>
       <c r="I88" s="234"/>
       <c r="J88" s="234"/>
+      <c r="L88" t="s">
+        <v>397</v>
+      </c>
+      <c r="M88" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="89" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B89" s="242" t="s">
         <v>693</v>
@@ -28466,16 +28501,10 @@
       <c r="H89" s="234"/>
       <c r="I89" s="234"/>
       <c r="J89" s="234"/>
-      <c r="L89" t="s">
-        <v>398</v>
-      </c>
-      <c r="M89" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="90" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B90" s="242" t="s">
         <v>693</v>
@@ -28490,10 +28519,16 @@
       <c r="H90" s="234"/>
       <c r="I90" s="234"/>
       <c r="J90" s="234"/>
+      <c r="L90" t="s">
+        <v>398</v>
+      </c>
+      <c r="M90" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="91" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B91" s="242" t="s">
         <v>693</v>
@@ -28510,8 +28545,8 @@
       <c r="J91" s="234"/>
     </row>
     <row r="92" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="234" t="s">
-        <v>160</v>
+      <c r="A92" t="s">
+        <v>159</v>
       </c>
       <c r="B92" s="242" t="s">
         <v>693</v>
@@ -28526,16 +28561,10 @@
       <c r="H92" s="234"/>
       <c r="I92" s="234"/>
       <c r="J92" s="234"/>
-      <c r="L92" t="s">
-        <v>160</v>
-      </c>
-      <c r="M92" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="93" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="234" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B93" s="242" t="s">
         <v>693</v>
@@ -28551,15 +28580,15 @@
       <c r="I93" s="234"/>
       <c r="J93" s="234"/>
       <c r="L93" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M93" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>168</v>
+      <c r="A94" s="234" t="s">
+        <v>161</v>
       </c>
       <c r="B94" s="242" t="s">
         <v>693</v>
@@ -28575,7 +28604,7 @@
       <c r="I94" s="234"/>
       <c r="J94" s="234"/>
       <c r="L94" t="s">
-        <v>399</v>
+        <v>161</v>
       </c>
       <c r="M94" t="s">
         <v>389</v>
@@ -28583,7 +28612,7 @@
     </row>
     <row r="95" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B95" s="242" t="s">
         <v>693</v>
@@ -28598,10 +28627,16 @@
       <c r="H95" s="234"/>
       <c r="I95" s="234"/>
       <c r="J95" s="234"/>
+      <c r="L95" t="s">
+        <v>399</v>
+      </c>
+      <c r="M95" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="96" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B96" s="242" t="s">
         <v>693</v>
@@ -28616,16 +28651,10 @@
       <c r="H96" s="234"/>
       <c r="I96" s="234"/>
       <c r="J96" s="234"/>
-      <c r="L96" t="s">
-        <v>400</v>
-      </c>
-      <c r="M96" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="97" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B97" s="242" t="s">
         <v>693</v>
@@ -28640,16 +28669,22 @@
       <c r="H97" s="234"/>
       <c r="I97" s="234"/>
       <c r="J97" s="234"/>
+      <c r="L97" t="s">
+        <v>400</v>
+      </c>
+      <c r="M97" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="98" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="234" t="s">
-        <v>172</v>
+      <c r="A98" t="s">
+        <v>171</v>
       </c>
       <c r="B98" s="242" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C98" s="234" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D98" s="234"/>
       <c r="E98" s="234"/>
@@ -28658,46 +28693,34 @@
       <c r="H98" s="234"/>
       <c r="I98" s="234"/>
       <c r="J98" s="234"/>
-      <c r="L98" t="s">
-        <v>401</v>
-      </c>
-      <c r="M98" t="s">
-        <v>690</v>
-      </c>
     </row>
     <row r="99" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>173</v>
+      <c r="A99" s="234" t="s">
+        <v>172</v>
       </c>
       <c r="B99" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C99" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="D99" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="E99" s="234" t="s">
-        <v>105</v>
-      </c>
-      <c r="F99" s="234" t="s">
-        <v>34</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D99" s="234"/>
+      <c r="E99" s="234"/>
+      <c r="F99" s="234"/>
       <c r="G99" s="234"/>
       <c r="H99" s="234"/>
       <c r="I99" s="234"/>
       <c r="J99" s="234"/>
       <c r="L99" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M99" t="s">
-        <v>702</v>
+        <v>690</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" s="242" t="s">
         <v>693</v>
@@ -28718,10 +28741,16 @@
       <c r="H100" s="234"/>
       <c r="I100" s="234"/>
       <c r="J100" s="234"/>
+      <c r="L100" t="s">
+        <v>402</v>
+      </c>
+      <c r="M100" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="101" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="234" t="s">
-        <v>175</v>
+      <c r="A101" t="s">
+        <v>174</v>
       </c>
       <c r="B101" s="242" t="s">
         <v>693</v>
@@ -28742,11 +28771,10 @@
       <c r="H101" s="234"/>
       <c r="I101" s="234"/>
       <c r="J101" s="234"/>
-      <c r="L101"/>
     </row>
     <row r="102" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="234" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B102" s="242" t="s">
         <v>693</v>
@@ -28767,16 +28795,11 @@
       <c r="H102" s="234"/>
       <c r="I102" s="234"/>
       <c r="J102" s="234"/>
-      <c r="L102" s="242" t="s">
-        <v>403</v>
-      </c>
-      <c r="M102" t="s">
-        <v>702</v>
-      </c>
+      <c r="L102"/>
     </row>
     <row r="103" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="234" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B103" s="242" t="s">
         <v>693</v>
@@ -28797,40 +28820,40 @@
       <c r="H103" s="234"/>
       <c r="I103" s="234"/>
       <c r="J103" s="234"/>
+      <c r="L103" s="242" t="s">
+        <v>403</v>
+      </c>
+      <c r="M103" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="104" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>180</v>
+      <c r="A104" s="234" t="s">
+        <v>177</v>
       </c>
       <c r="B104" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C104" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="D104" s="234" t="s">
         <v>196</v>
       </c>
-      <c r="D104" s="234" t="s">
+      <c r="E104" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="E104" s="234" t="s">
-        <v>48</v>
-      </c>
       <c r="F104" s="234" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="G104" s="234"/>
       <c r="H104" s="234"/>
       <c r="I104" s="234"/>
       <c r="J104" s="234"/>
-      <c r="L104" t="s">
-        <v>404</v>
-      </c>
-      <c r="M104" t="s">
-        <v>405</v>
-      </c>
     </row>
     <row r="105" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B105" s="242" t="s">
         <v>693</v>
@@ -28851,10 +28874,16 @@
       <c r="H105" s="234"/>
       <c r="I105" s="234"/>
       <c r="J105" s="234"/>
+      <c r="L105" t="s">
+        <v>404</v>
+      </c>
+      <c r="M105" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="106" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B106" s="242" t="s">
         <v>693</v>
@@ -28877,40 +28906,26 @@
       <c r="J106" s="234"/>
     </row>
     <row r="107" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="234" t="s">
-        <v>662</v>
+      <c r="A107" t="s">
+        <v>182</v>
       </c>
       <c r="B107" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C107" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="D107" s="234" t="s">
-        <v>105</v>
-      </c>
-      <c r="E107" s="234" t="s">
-        <v>48</v>
-      </c>
-      <c r="F107" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="G107" s="234" t="s">
-        <v>34</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D107" s="234"/>
+      <c r="E107" s="234"/>
+      <c r="F107" s="234"/>
+      <c r="G107" s="234"/>
       <c r="H107" s="234"/>
       <c r="I107" s="234"/>
       <c r="J107" s="234"/>
-      <c r="L107" t="s">
-        <v>406</v>
-      </c>
-      <c r="M107" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="234" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B108" s="242" t="s">
         <v>693</v>
@@ -28933,10 +28948,16 @@
       <c r="H108" s="234"/>
       <c r="I108" s="234"/>
       <c r="J108" s="234"/>
-    </row>
-    <row r="109" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L108" t="s">
+        <v>406</v>
+      </c>
+      <c r="M108" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="234" t="s">
-        <v>183</v>
+        <v>663</v>
       </c>
       <c r="B109" s="242" t="s">
         <v>693</v>
@@ -28959,16 +28980,10 @@
       <c r="H109" s="234"/>
       <c r="I109" s="234"/>
       <c r="J109" s="234"/>
-      <c r="L109" t="s">
-        <v>407</v>
-      </c>
-      <c r="M109" t="s">
-        <v>408</v>
-      </c>
     </row>
     <row r="110" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="234" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B110" s="242" t="s">
         <v>693</v>
@@ -28992,7 +29007,7 @@
       <c r="I110" s="234"/>
       <c r="J110" s="234"/>
       <c r="L110" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M110" t="s">
         <v>408</v>
@@ -29000,7 +29015,7 @@
     </row>
     <row r="111" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="234" t="s">
-        <v>664</v>
+        <v>184</v>
       </c>
       <c r="B111" s="242" t="s">
         <v>693</v>
@@ -29024,15 +29039,15 @@
       <c r="I111" s="234"/>
       <c r="J111" s="234"/>
       <c r="L111" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M111" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="234" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B112" s="242" t="s">
         <v>693</v>
@@ -29055,42 +29070,42 @@
       <c r="H112" s="234"/>
       <c r="I112" s="234"/>
       <c r="J112" s="234"/>
-    </row>
-    <row r="113" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L112" t="s">
+        <v>410</v>
+      </c>
+      <c r="M112" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="234" t="s">
-        <v>188</v>
+        <v>665</v>
       </c>
       <c r="B113" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C113" s="234" t="s">
+        <v>196</v>
+      </c>
+      <c r="D113" s="234" t="s">
+        <v>105</v>
+      </c>
+      <c r="E113" s="234" t="s">
+        <v>48</v>
+      </c>
+      <c r="F113" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="G113" s="234" t="s">
         <v>34</v>
-      </c>
-      <c r="D113" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E113" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="F113" s="234" t="s">
-        <v>105</v>
-      </c>
-      <c r="G113" s="234" t="s">
-        <v>52</v>
       </c>
       <c r="H113" s="234"/>
       <c r="I113" s="234"/>
       <c r="J113" s="234"/>
-      <c r="L113" t="s">
-        <v>411</v>
-      </c>
-      <c r="M113" t="s">
-        <v>412</v>
-      </c>
     </row>
     <row r="114" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="234" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B114" s="242" t="s">
         <v>693</v>
@@ -29114,7 +29129,7 @@
       <c r="I114" s="234"/>
       <c r="J114" s="234"/>
       <c r="L114" t="s">
-        <v>190</v>
+        <v>411</v>
       </c>
       <c r="M114" t="s">
         <v>412</v>
@@ -29122,7 +29137,7 @@
     </row>
     <row r="115" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="234" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B115" s="242" t="s">
         <v>693</v>
@@ -29146,7 +29161,7 @@
       <c r="I115" s="234"/>
       <c r="J115" s="234"/>
       <c r="L115" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M115" t="s">
         <v>412</v>
@@ -29154,7 +29169,7 @@
     </row>
     <row r="116" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="234" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B116" s="242" t="s">
         <v>693</v>
@@ -29178,7 +29193,7 @@
       <c r="I116" s="234"/>
       <c r="J116" s="234"/>
       <c r="L116" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M116" t="s">
         <v>412</v>
@@ -29186,93 +29201,99 @@
     </row>
     <row r="117" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="234" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B117" s="242" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C117" s="234" t="s">
+        <v>34</v>
+      </c>
+      <c r="D117" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="E117" s="234" t="s">
+        <v>196</v>
+      </c>
+      <c r="F117" s="234" t="s">
+        <v>105</v>
+      </c>
+      <c r="G117" s="234" t="s">
         <v>52</v>
       </c>
-      <c r="D117" s="234"/>
-      <c r="E117" s="234"/>
-      <c r="F117" s="234"/>
-      <c r="G117" s="234"/>
       <c r="H117" s="234"/>
       <c r="I117" s="234"/>
       <c r="J117" s="234"/>
       <c r="L117" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M117" t="s">
-        <v>690</v>
+        <v>412</v>
       </c>
     </row>
     <row r="118" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="234" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B118" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C118" s="234" t="s">
-        <v>34</v>
-      </c>
-      <c r="D118" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E118" s="234" t="s">
         <v>52</v>
       </c>
+      <c r="D118" s="234"/>
+      <c r="E118" s="234"/>
       <c r="F118" s="234"/>
       <c r="G118" s="234"/>
       <c r="H118" s="234"/>
       <c r="I118" s="234"/>
       <c r="J118" s="234"/>
       <c r="L118" t="s">
-        <v>413</v>
+        <v>193</v>
       </c>
       <c r="M118" t="s">
-        <v>414</v>
+        <v>690</v>
       </c>
     </row>
     <row r="119" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="234" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B119" s="242" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C119" s="234" t="s">
-        <v>5</v>
-      </c>
-      <c r="D119" s="234"/>
-      <c r="E119" s="234"/>
+        <v>34</v>
+      </c>
+      <c r="D119" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="E119" s="234" t="s">
+        <v>52</v>
+      </c>
       <c r="F119" s="234"/>
       <c r="G119" s="234"/>
       <c r="H119" s="234"/>
       <c r="I119" s="234"/>
       <c r="J119" s="234"/>
       <c r="L119" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="M119" t="s">
-        <v>700</v>
+        <v>414</v>
       </c>
     </row>
     <row r="120" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="234" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B120" s="242" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C120" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="D120" s="234" t="s">
-        <v>105</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D120" s="234"/>
       <c r="E120" s="234"/>
       <c r="F120" s="234"/>
       <c r="G120" s="234"/>
@@ -29280,15 +29301,15 @@
       <c r="I120" s="234"/>
       <c r="J120" s="234"/>
       <c r="L120" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M120" t="s">
-        <v>382</v>
+        <v>700</v>
       </c>
     </row>
     <row r="121" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="234" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B121" s="242" t="s">
         <v>693</v>
@@ -29299,24 +29320,22 @@
       <c r="D121" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="E121" s="234" t="s">
-        <v>57</v>
-      </c>
+      <c r="E121" s="234"/>
       <c r="F121" s="234"/>
       <c r="G121" s="234"/>
       <c r="H121" s="234"/>
       <c r="I121" s="234"/>
       <c r="J121" s="234"/>
       <c r="L121" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M121" t="s">
-        <v>418</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="234" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B122" s="242" t="s">
         <v>693</v>
@@ -29335,40 +29354,38 @@
       <c r="H122" s="234"/>
       <c r="I122" s="234"/>
       <c r="J122" s="234"/>
+      <c r="L122" t="s">
+        <v>417</v>
+      </c>
+      <c r="M122" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="123" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="234" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B123" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C123" s="234" t="s">
-        <v>34</v>
+        <v>196</v>
       </c>
       <c r="D123" s="234" t="s">
+        <v>105</v>
+      </c>
+      <c r="E123" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="E123" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="F123" s="234" t="s">
-        <v>105</v>
-      </c>
+      <c r="F123" s="234"/>
       <c r="G123" s="234"/>
       <c r="H123" s="234"/>
       <c r="I123" s="234"/>
       <c r="J123" s="234"/>
-      <c r="L123" t="s">
-        <v>419</v>
-      </c>
-      <c r="M123" t="s">
-        <v>420</v>
-      </c>
     </row>
     <row r="124" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="234" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B124" s="242" t="s">
         <v>693</v>
@@ -29390,7 +29407,7 @@
       <c r="I124" s="234"/>
       <c r="J124" s="234"/>
       <c r="L124" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="M124" t="s">
         <v>420</v>
@@ -29398,108 +29415,127 @@
     </row>
     <row r="125" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="234" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B125" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C125" s="234" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D125" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="E125" s="234" t="s">
         <v>196</v>
       </c>
-      <c r="E125" s="234" t="s">
+      <c r="F125" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="F125" s="234" t="s">
-        <v>31</v>
-      </c>
-      <c r="G125" s="234" t="s">
-        <v>48</v>
-      </c>
-      <c r="H125" s="234" t="s">
-        <v>42</v>
-      </c>
-      <c r="I125" s="234" t="s">
-        <v>100</v>
-      </c>
-      <c r="J125" s="234" t="s">
-        <v>41</v>
-      </c>
+      <c r="G125" s="234"/>
+      <c r="H125" s="234"/>
+      <c r="I125" s="234"/>
+      <c r="J125" s="234"/>
       <c r="L125" t="s">
-        <v>202</v>
+        <v>421</v>
       </c>
       <c r="M125" t="s">
-        <v>690</v>
+        <v>420</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="234" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
       <c r="B126" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C126" s="234" t="s">
+        <v>40</v>
+      </c>
+      <c r="D126" s="234" t="s">
         <v>196</v>
       </c>
-      <c r="D126" s="234" t="s">
+      <c r="E126" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="E126" s="234"/>
-      <c r="F126" s="234"/>
-      <c r="G126" s="234"/>
-      <c r="H126" s="234"/>
-      <c r="I126" s="234"/>
-      <c r="J126" s="234"/>
+      <c r="F126" s="234" t="s">
+        <v>31</v>
+      </c>
+      <c r="G126" s="234" t="s">
+        <v>48</v>
+      </c>
+      <c r="H126" s="234" t="s">
+        <v>42</v>
+      </c>
+      <c r="I126" s="234" t="s">
+        <v>100</v>
+      </c>
+      <c r="J126" s="234" t="s">
+        <v>41</v>
+      </c>
       <c r="L126" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
       <c r="M126" t="s">
-        <v>371</v>
+        <v>690</v>
       </c>
     </row>
     <row r="127" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="234" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B127" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C127" s="234" t="s">
-        <v>34</v>
+        <v>196</v>
       </c>
       <c r="D127" s="234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E127" s="234" t="s">
-        <v>196</v>
-      </c>
-      <c r="F127" s="234" t="s">
         <v>105</v>
       </c>
+      <c r="E127" s="234"/>
+      <c r="F127" s="234"/>
       <c r="G127" s="234"/>
       <c r="H127" s="234"/>
       <c r="I127" s="234"/>
       <c r="J127" s="234"/>
       <c r="L127" t="s">
+        <v>258</v>
+      </c>
+      <c r="M127" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="234" t="s">
         <v>259</v>
       </c>
-      <c r="M127" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="234"/>
-      <c r="C128" s="234"/>
-      <c r="D128" s="234"/>
-      <c r="E128" s="234"/>
-      <c r="F128" s="234"/>
+      <c r="B128" s="242" t="s">
+        <v>693</v>
+      </c>
+      <c r="C128" s="234" t="s">
+        <v>34</v>
+      </c>
+      <c r="D128" s="234" t="s">
+        <v>57</v>
+      </c>
+      <c r="E128" s="234" t="s">
+        <v>196</v>
+      </c>
+      <c r="F128" s="234" t="s">
+        <v>105</v>
+      </c>
       <c r="G128" s="234"/>
       <c r="H128" s="234"/>
       <c r="I128" s="234"/>
       <c r="J128" s="234"/>
+      <c r="L128" t="s">
+        <v>259</v>
+      </c>
+      <c r="M128" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="129" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="234"/>
@@ -29567,38 +29603,30 @@
       <c r="I134" s="234"/>
       <c r="J134" s="234"/>
     </row>
-    <row r="135" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="159" t="s">
+    <row r="135" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="234"/>
+      <c r="C135" s="234"/>
+      <c r="D135" s="234"/>
+      <c r="E135" s="234"/>
+      <c r="F135" s="234"/>
+      <c r="G135" s="234"/>
+      <c r="H135" s="234"/>
+      <c r="I135" s="234"/>
+      <c r="J135" s="234"/>
+    </row>
+    <row r="136" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="159" t="s">
         <v>423</v>
       </c>
-      <c r="B136" s="159"/>
-      <c r="C136" s="159" t="s">
+      <c r="B137" s="159"/>
+      <c r="C137" s="159" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="234" t="s">
-        <v>33</v>
-      </c>
-      <c r="B137" s="242" t="s">
-        <v>693</v>
-      </c>
-      <c r="C137" s="234">
-        <v>1</v>
-      </c>
-      <c r="D137" s="234">
-        <v>2</v>
-      </c>
-      <c r="E137" s="234">
-        <v>3</v>
-      </c>
-      <c r="F137" s="234"/>
-      <c r="G137" s="234"/>
     </row>
     <row r="138" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="234" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B138" s="242" t="s">
         <v>693</v>
@@ -29614,13 +29642,10 @@
       </c>
       <c r="F138" s="234"/>
       <c r="G138" s="234"/>
-      <c r="L138" t="s">
-        <v>424</v>
-      </c>
     </row>
     <row r="139" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="234" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B139" s="242" t="s">
         <v>693</v>
@@ -29637,12 +29662,12 @@
       <c r="F139" s="234"/>
       <c r="G139" s="234"/>
       <c r="L139" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="234" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B140" s="242" t="s">
         <v>693</v>
@@ -29658,10 +29683,13 @@
       </c>
       <c r="F140" s="234"/>
       <c r="G140" s="234"/>
+      <c r="L140" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="141" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="234" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B141" s="242" t="s">
         <v>693</v>
@@ -29679,8 +29707,8 @@
       <c r="G141" s="234"/>
     </row>
     <row r="142" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>61</v>
+      <c r="A142" s="234" t="s">
+        <v>60</v>
       </c>
       <c r="B142" s="242" t="s">
         <v>693</v>
@@ -29694,15 +29722,12 @@
       <c r="E142" s="234">
         <v>3</v>
       </c>
-      <c r="F142" s="337"/>
+      <c r="F142" s="234"/>
       <c r="G142" s="234"/>
-      <c r="L142" t="s">
-        <v>426</v>
-      </c>
     </row>
     <row r="143" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B143" s="242" t="s">
         <v>693</v>
@@ -29716,12 +29741,15 @@
       <c r="E143" s="234">
         <v>3</v>
       </c>
-      <c r="F143" s="234"/>
+      <c r="F143" s="337"/>
       <c r="G143" s="234"/>
+      <c r="L143" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="144" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B144" s="242" t="s">
         <v>693</v>
@@ -29740,7 +29768,7 @@
     </row>
     <row r="145" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B145" s="242" t="s">
         <v>693</v>
@@ -29758,8 +29786,8 @@
       <c r="G145" s="234"/>
     </row>
     <row r="146" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="337" t="s">
-        <v>68</v>
+      <c r="A146" t="s">
+        <v>64</v>
       </c>
       <c r="B146" s="242" t="s">
         <v>693</v>
@@ -29778,7 +29806,7 @@
     </row>
     <row r="147" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="337" t="s">
-        <v>705</v>
+        <v>68</v>
       </c>
       <c r="B147" s="242" t="s">
         <v>693</v>
@@ -29789,13 +29817,15 @@
       <c r="D147" s="234">
         <v>2</v>
       </c>
-      <c r="E147" s="234"/>
+      <c r="E147" s="234">
+        <v>3</v>
+      </c>
       <c r="F147" s="234"/>
       <c r="G147" s="234"/>
     </row>
-    <row r="148" spans="1:7" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="337" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B148" s="242" t="s">
         <v>693</v>
@@ -29810,68 +29840,66 @@
       <c r="F148" s="234"/>
       <c r="G148" s="234"/>
     </row>
-    <row r="149" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>84</v>
+    <row r="149" spans="1:7" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="337" t="s">
+        <v>706</v>
       </c>
       <c r="B149" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C149" s="234">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D149" s="234">
-        <v>4</v>
-      </c>
-      <c r="E149" s="234">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E149" s="234"/>
       <c r="F149" s="234"/>
       <c r="G149" s="234"/>
     </row>
     <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B150" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C150" s="234">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D150" s="234">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E150" s="234">
-        <v>4</v>
-      </c>
-      <c r="F150" s="234">
         <v>5</v>
       </c>
+      <c r="F150" s="234"/>
       <c r="G150" s="234"/>
     </row>
     <row r="151" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B151" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C151" s="234">
+        <v>2</v>
+      </c>
+      <c r="D151" s="234">
         <v>3</v>
       </c>
-      <c r="D151" s="234">
+      <c r="E151" s="234">
         <v>4</v>
       </c>
-      <c r="E151" s="234">
+      <c r="F151" s="234">
         <v>5</v>
       </c>
-      <c r="F151" s="234"/>
       <c r="G151" s="234"/>
     </row>
     <row r="152" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B152" s="242" t="s">
         <v>693</v>
@@ -29889,8 +29917,8 @@
       <c r="G152" s="234"/>
     </row>
     <row r="153" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="234" t="s">
-        <v>90</v>
+      <c r="A153" t="s">
+        <v>89</v>
       </c>
       <c r="B153" s="242" t="s">
         <v>693</v>
@@ -29909,7 +29937,7 @@
     </row>
     <row r="154" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="234" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B154" s="242" t="s">
         <v>693</v>
@@ -29928,7 +29956,7 @@
     </row>
     <row r="155" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="234" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B155" s="242" t="s">
         <v>693</v>
@@ -29947,26 +29975,26 @@
     </row>
     <row r="156" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="234" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B156" s="242" t="s">
         <v>693</v>
       </c>
       <c r="C156" s="234">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D156" s="234">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E156" s="234">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F156" s="234"/>
       <c r="G156" s="234"/>
     </row>
     <row r="157" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="234" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B157" s="242" t="s">
         <v>693</v>
@@ -29985,7 +30013,7 @@
     </row>
     <row r="158" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="234" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B158" s="242" t="s">
         <v>693</v>
@@ -30004,7 +30032,7 @@
     </row>
     <row r="159" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="234" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B159" s="242" t="s">
         <v>693</v>
@@ -30022,8 +30050,8 @@
       <c r="G159" s="234"/>
     </row>
     <row r="160" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="337" t="s">
-        <v>98</v>
+      <c r="A160" s="234" t="s">
+        <v>96</v>
       </c>
       <c r="B160" s="242" t="s">
         <v>693</v>
@@ -30042,7 +30070,7 @@
     </row>
     <row r="161" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="337" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B161" s="242" t="s">
         <v>693</v>
@@ -30061,7 +30089,7 @@
     </row>
     <row r="162" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="337" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B162" s="242" t="s">
         <v>693</v>
@@ -30080,7 +30108,7 @@
     </row>
     <row r="163" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="337" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B163" s="242" t="s">
         <v>693</v>
@@ -30099,7 +30127,7 @@
     </row>
     <row r="164" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="337" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B164" s="242" t="s">
         <v>693</v>
@@ -30118,7 +30146,7 @@
     </row>
     <row r="165" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="337" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B165" s="242" t="s">
         <v>693</v>
@@ -30136,8 +30164,8 @@
       <c r="G165" s="234"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>137</v>
+      <c r="A166" s="337" t="s">
+        <v>109</v>
       </c>
       <c r="B166" s="242" t="s">
         <v>693</v>
@@ -30156,7 +30184,7 @@
     </row>
     <row r="167" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B167" s="242" t="s">
         <v>693</v>
@@ -30175,7 +30203,7 @@
     </row>
     <row r="168" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B168" s="242" t="s">
         <v>693</v>
@@ -30194,7 +30222,7 @@
     </row>
     <row r="169" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B169" s="242" t="s">
         <v>693</v>
@@ -30213,7 +30241,7 @@
     </row>
     <row r="170" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B170" s="242" t="s">
         <v>693</v>
@@ -30232,7 +30260,7 @@
     </row>
     <row r="171" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B171" s="242" t="s">
         <v>693</v>
@@ -30251,7 +30279,7 @@
     </row>
     <row r="172" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B172" s="242" t="s">
         <v>693</v>
@@ -30270,7 +30298,7 @@
     </row>
     <row r="173" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B173" s="242" t="s">
         <v>693</v>
@@ -30289,7 +30317,7 @@
     </row>
     <row r="174" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B174" s="242" t="s">
         <v>693</v>
@@ -30308,7 +30336,7 @@
     </row>
     <row r="175" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B175" s="242" t="s">
         <v>693</v>
@@ -30327,7 +30355,7 @@
     </row>
     <row r="176" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B176" s="242" t="s">
         <v>693</v>
@@ -30346,7 +30374,7 @@
     </row>
     <row r="177" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B177" s="242" t="s">
         <v>693</v>
@@ -30364,8 +30392,8 @@
       <c r="G177" s="234"/>
     </row>
     <row r="178" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="234" t="s">
-        <v>149</v>
+      <c r="A178" t="s">
+        <v>148</v>
       </c>
       <c r="B178" s="242" t="s">
         <v>693</v>
@@ -30384,7 +30412,7 @@
     </row>
     <row r="179" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="234" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B179" s="242" t="s">
         <v>693</v>
@@ -30402,8 +30430,8 @@
       <c r="G179" s="234"/>
     </row>
     <row r="180" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>158</v>
+      <c r="A180" s="234" t="s">
+        <v>156</v>
       </c>
       <c r="B180" s="242" t="s">
         <v>693</v>
@@ -30422,7 +30450,7 @@
     </row>
     <row r="181" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B181" s="242" t="s">
         <v>693</v>
@@ -30441,7 +30469,7 @@
     </row>
     <row r="182" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B182" s="242" t="s">
         <v>693</v>
@@ -30460,7 +30488,7 @@
     </row>
     <row r="183" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B183" s="242" t="s">
         <v>693</v>
@@ -30478,8 +30506,8 @@
       <c r="G183" s="234"/>
     </row>
     <row r="184" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="234" t="s">
-        <v>164</v>
+      <c r="A184" t="s">
+        <v>163</v>
       </c>
       <c r="B184" s="242" t="s">
         <v>693</v>
@@ -30498,7 +30526,7 @@
     </row>
     <row r="185" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="234" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B185" s="242" t="s">
         <v>693</v>
@@ -30516,8 +30544,8 @@
       <c r="G185" s="234"/>
     </row>
     <row r="186" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>168</v>
+      <c r="A186" s="234" t="s">
+        <v>167</v>
       </c>
       <c r="B186" s="242" t="s">
         <v>693</v>
@@ -30536,7 +30564,7 @@
     </row>
     <row r="187" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B187" s="242" t="s">
         <v>693</v>
@@ -30555,7 +30583,7 @@
     </row>
     <row r="188" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B188" s="242" t="s">
         <v>693</v>
@@ -30573,8 +30601,8 @@
       <c r="G188" s="234"/>
     </row>
     <row r="189" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="234" t="s">
-        <v>171</v>
+      <c r="A189" t="s">
+        <v>170</v>
       </c>
       <c r="B189" s="242" t="s">
         <v>693</v>
@@ -30591,9 +30619,9 @@
       <c r="F189" s="234"/>
       <c r="G189" s="234"/>
     </row>
-    <row r="190" spans="1:7" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="234" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B190" s="242" t="s">
         <v>693</v>
@@ -30610,9 +30638,9 @@
       <c r="F190" s="234"/>
       <c r="G190" s="234"/>
     </row>
-    <row r="191" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="234" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B191" s="242" t="s">
         <v>693</v>
@@ -30631,7 +30659,7 @@
     </row>
     <row r="192" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="234" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B192" s="242" t="s">
         <v>693</v>
@@ -30642,13 +30670,15 @@
       <c r="D192" s="234">
         <v>2</v>
       </c>
-      <c r="E192" s="234"/>
+      <c r="E192" s="234">
+        <v>3</v>
+      </c>
       <c r="F192" s="234"/>
       <c r="G192" s="234"/>
     </row>
     <row r="193" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="234" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B193" s="242" t="s">
         <v>693</v>
@@ -30665,7 +30695,7 @@
     </row>
     <row r="194" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="234" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B194" s="242" t="s">
         <v>693</v>
@@ -30681,8 +30711,8 @@
       <c r="G194" s="234"/>
     </row>
     <row r="195" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="337" t="s">
-        <v>662</v>
+      <c r="A195" s="234" t="s">
+        <v>182</v>
       </c>
       <c r="B195" s="242" t="s">
         <v>693</v>
@@ -30699,7 +30729,7 @@
     </row>
     <row r="196" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="337" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B196" s="242" t="s">
         <v>693</v>
@@ -30716,7 +30746,7 @@
     </row>
     <row r="197" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="337" t="s">
-        <v>184</v>
+        <v>663</v>
       </c>
       <c r="B197" s="242" t="s">
         <v>693</v>
@@ -30733,7 +30763,7 @@
     </row>
     <row r="198" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="337" t="s">
-        <v>664</v>
+        <v>184</v>
       </c>
       <c r="B198" s="242" t="s">
         <v>693</v>
@@ -30750,7 +30780,7 @@
     </row>
     <row r="199" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="337" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B199" s="242" t="s">
         <v>693</v>
@@ -30766,8 +30796,8 @@
       <c r="G199" s="234"/>
     </row>
     <row r="200" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="242" t="s">
-        <v>195</v>
+      <c r="A200" s="337" t="s">
+        <v>665</v>
       </c>
       <c r="B200" s="242" t="s">
         <v>693</v>
@@ -30778,37 +30808,74 @@
       <c r="D200" s="234">
         <v>2</v>
       </c>
-      <c r="E200" s="234">
-        <v>4</v>
-      </c>
+      <c r="E200" s="234"/>
       <c r="F200" s="234"/>
       <c r="G200" s="234"/>
     </row>
+    <row r="201" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="242" t="s">
+        <v>195</v>
+      </c>
+      <c r="B201" s="242" t="s">
+        <v>693</v>
+      </c>
+      <c r="C201" s="234">
+        <v>1</v>
+      </c>
+      <c r="D201" s="234">
+        <v>2</v>
+      </c>
+      <c r="E201" s="234">
+        <v>4</v>
+      </c>
+      <c r="F201" s="234"/>
+      <c r="G201" s="234"/>
+    </row>
   </sheetData>
-  <sortState ref="A133:F195">
-    <sortCondition ref="A133:A195"/>
+  <sortState ref="A13:M134">
+    <sortCondition ref="A13:A134"/>
   </sortState>
-  <conditionalFormatting sqref="L83:M83 L87:M98 L110:M110 L113:M114 L116:M117 L119:M119 L121:M127 L101:M108 G142 A13:J13 C45:J45 A14:B134 A137:G137 C138:G141 C143:G147 C142:E142 A138:B147 L13:M78 C47:J134 C14:J43 A149:G200">
-    <cfRule type="expression" dxfId="1" priority="4">
+  <conditionalFormatting sqref="L84:M84 L88:M99 L111:M111 L114:M115 L117:M118 L120:M120 L122:M128 L102:M109 G143 C45:J46 A138:G138 C139:G142 C144:G148 C143:E143 A139:B148 L13:M79 C48:J135 A13:J22 A150:G201 C27:J43 A27:B135 A23:A26 D23:J26">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A148:G148">
+  <conditionalFormatting sqref="A149:G149">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:C23">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:C24">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:C25">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:C26">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I22:J26 E22:F26 C47:J134 E27:J43 C45:J45 C20:J20 C16:C19 D13:J19 E21:J21 C21:D43">
-      <formula1>$AG$2:$AG$62</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I22:J26 C21:D43 E21:J21 D13:J19 C16:C19 C20:J20 C45:J46 E27:J43 C48:J135 E22:F26">
+      <formula1>$AG$2:$AG$63</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C13:C15">
-      <formula1>$AG$2:$AG$55</formula1>
+      <formula1>$AG$2:$AG$56</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C142:E142 C137:G141 G142 C143:G200">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C143:E143 C138:G142 G143 C144:G201">
       <formula1>"1, 2, 3, 4, 5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B134 B137:B200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B138:B201 B13:B135">
       <formula1>"not, only"</formula1>
     </dataValidation>
   </dataValidations>
@@ -42706,7 +42773,7 @@
   </sheetPr>
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45156,69 +45223,69 @@
       <c r="BZ1" s="190"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="353" t="s">
+      <c r="A2" s="376" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="412"/>
-      <c r="C2" s="413"/>
-      <c r="D2" s="415" t="s">
+      <c r="B2" s="419"/>
+      <c r="C2" s="420"/>
+      <c r="D2" s="422" t="s">
         <v>569</v>
       </c>
-      <c r="E2" s="416"/>
-      <c r="F2" s="416"/>
-      <c r="G2" s="416"/>
-      <c r="H2" s="416"/>
-      <c r="I2" s="416"/>
-      <c r="J2" s="416"/>
-      <c r="K2" s="416"/>
-      <c r="L2" s="416"/>
-      <c r="M2" s="416"/>
-      <c r="N2" s="416"/>
-      <c r="O2" s="416"/>
-      <c r="P2" s="416"/>
-      <c r="Q2" s="416"/>
-      <c r="R2" s="416"/>
-      <c r="S2" s="416"/>
-      <c r="T2" s="416"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
+      <c r="I2" s="423"/>
+      <c r="J2" s="423"/>
+      <c r="K2" s="423"/>
+      <c r="L2" s="423"/>
+      <c r="M2" s="423"/>
+      <c r="N2" s="423"/>
+      <c r="O2" s="423"/>
+      <c r="P2" s="423"/>
+      <c r="Q2" s="423"/>
+      <c r="R2" s="423"/>
+      <c r="S2" s="423"/>
+      <c r="T2" s="423"/>
       <c r="AA2" s="132"/>
       <c r="BY2" s="190"/>
       <c r="BZ2" s="190"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="355" t="s">
+      <c r="A3" s="378" t="s">
         <v>261</v>
       </c>
-      <c r="B3" s="412"/>
-      <c r="C3" s="413"/>
+      <c r="B3" s="419"/>
+      <c r="C3" s="420"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="417" t="s">
+      <c r="F3" s="424" t="s">
         <v>570</v>
       </c>
-      <c r="G3" s="418"/>
-      <c r="H3" s="419" t="s">
+      <c r="G3" s="425"/>
+      <c r="H3" s="426" t="s">
         <v>571</v>
       </c>
-      <c r="I3" s="419"/>
-      <c r="J3" s="420"/>
-      <c r="K3" s="421" t="s">
+      <c r="I3" s="426"/>
+      <c r="J3" s="427"/>
+      <c r="K3" s="428" t="s">
         <v>572</v>
       </c>
-      <c r="L3" s="422"/>
-      <c r="M3" s="423"/>
-      <c r="N3" s="420" t="s">
+      <c r="L3" s="429"/>
+      <c r="M3" s="430"/>
+      <c r="N3" s="427" t="s">
         <v>573</v>
       </c>
-      <c r="O3" s="424"/>
-      <c r="P3" s="425"/>
-      <c r="Q3" s="426" t="s">
+      <c r="O3" s="431"/>
+      <c r="P3" s="432"/>
+      <c r="Q3" s="433" t="s">
         <v>574</v>
       </c>
-      <c r="R3" s="427"/>
-      <c r="S3" s="428" t="s">
+      <c r="R3" s="434"/>
+      <c r="S3" s="435" t="s">
         <v>575</v>
       </c>
-      <c r="T3" s="429"/>
+      <c r="T3" s="436"/>
       <c r="AA3" s="133"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -45382,7 +45449,7 @@
       <c r="AC6" s="134"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="434" t="str">
+      <c r="C7" s="413" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -45390,81 +45457,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="437"/>
-      <c r="E7" s="435"/>
-      <c r="F7" s="437" t="s">
+      <c r="D7" s="414"/>
+      <c r="E7" s="415"/>
+      <c r="F7" s="414" t="s">
         <v>598</v>
       </c>
-      <c r="G7" s="437"/>
-      <c r="H7" s="435"/>
-      <c r="I7" s="438" t="str">
+      <c r="G7" s="414"/>
+      <c r="H7" s="415"/>
+      <c r="I7" s="416" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$242.422)</v>
       </c>
-      <c r="J7" s="439"/>
-      <c r="K7" s="439"/>
-      <c r="L7" s="439"/>
-      <c r="M7" s="439"/>
-      <c r="N7" s="439"/>
-      <c r="O7" s="439"/>
-      <c r="P7" s="439"/>
-      <c r="Q7" s="439"/>
-      <c r="R7" s="440"/>
-      <c r="S7" s="434" t="str">
+      <c r="J7" s="417"/>
+      <c r="K7" s="417"/>
+      <c r="L7" s="417"/>
+      <c r="M7" s="417"/>
+      <c r="N7" s="417"/>
+      <c r="O7" s="417"/>
+      <c r="P7" s="417"/>
+      <c r="Q7" s="417"/>
+      <c r="R7" s="418"/>
+      <c r="S7" s="413" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$596.731)</v>
       </c>
-      <c r="T7" s="437"/>
-      <c r="U7" s="437"/>
-      <c r="V7" s="437"/>
-      <c r="W7" s="437"/>
-      <c r="X7" s="435"/>
-      <c r="Y7" s="434" t="s">
+      <c r="T7" s="414"/>
+      <c r="U7" s="414"/>
+      <c r="V7" s="414"/>
+      <c r="W7" s="414"/>
+      <c r="X7" s="415"/>
+      <c r="Y7" s="413" t="s">
         <v>599</v>
       </c>
-      <c r="Z7" s="435"/>
+      <c r="Z7" s="415"/>
       <c r="AA7" s="135"/>
-      <c r="AH7" s="430" t="s">
+      <c r="AH7" s="437" t="s">
         <v>600</v>
       </c>
-      <c r="AI7" s="431"/>
+      <c r="AI7" s="438"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="432" t="s">
+      <c r="AK7" s="439" t="s">
         <v>601</v>
       </c>
       <c r="AL7" s="411"/>
       <c r="AM7" s="411"/>
-      <c r="AN7" s="431"/>
-      <c r="AP7" s="433" t="s">
+      <c r="AN7" s="438"/>
+      <c r="AP7" s="440" t="s">
         <v>602</v>
       </c>
-      <c r="AQ7" s="359"/>
-      <c r="AS7" s="414" t="s">
+      <c r="AQ7" s="382"/>
+      <c r="AS7" s="421" t="s">
         <v>603</v>
       </c>
-      <c r="AT7" s="358"/>
-      <c r="AU7" s="358"/>
-      <c r="AV7" s="358"/>
-      <c r="AW7" s="358"/>
-      <c r="AX7" s="358"/>
-      <c r="AY7" s="358"/>
-      <c r="AZ7" s="358"/>
-      <c r="BA7" s="358"/>
-      <c r="BB7" s="359"/>
-      <c r="BD7" s="433" t="s">
+      <c r="AT7" s="381"/>
+      <c r="AU7" s="381"/>
+      <c r="AV7" s="381"/>
+      <c r="AW7" s="381"/>
+      <c r="AX7" s="381"/>
+      <c r="AY7" s="381"/>
+      <c r="AZ7" s="381"/>
+      <c r="BA7" s="381"/>
+      <c r="BB7" s="382"/>
+      <c r="BD7" s="440" t="s">
         <v>604</v>
       </c>
-      <c r="BE7" s="359"/>
+      <c r="BE7" s="382"/>
       <c r="BF7" s="190"/>
-      <c r="BG7" s="414" t="s">
+      <c r="BG7" s="421" t="s">
         <v>605</v>
       </c>
-      <c r="BH7" s="358"/>
-      <c r="BI7" s="358"/>
+      <c r="BH7" s="381"/>
+      <c r="BI7" s="381"/>
       <c r="BY7" s="190"/>
       <c r="BZ7" s="190"/>
     </row>
@@ -55409,17 +55476,17 @@
       <c r="BZ52" s="190"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="436"/>
-      <c r="D53" s="436"/>
-      <c r="E53" s="436"/>
-      <c r="F53" s="436"/>
-      <c r="G53" s="436"/>
-      <c r="H53" s="436"/>
-      <c r="I53" s="436"/>
-      <c r="J53" s="436"/>
-      <c r="K53" s="436"/>
-      <c r="L53" s="436"/>
-      <c r="M53" s="436"/>
+      <c r="C53" s="412"/>
+      <c r="D53" s="412"/>
+      <c r="E53" s="412"/>
+      <c r="F53" s="412"/>
+      <c r="G53" s="412"/>
+      <c r="H53" s="412"/>
+      <c r="I53" s="412"/>
+      <c r="J53" s="412"/>
+      <c r="K53" s="412"/>
+      <c r="L53" s="412"/>
+      <c r="M53" s="412"/>
       <c r="AC53" s="137" t="s">
         <v>654</v>
       </c>
@@ -55554,11 +55621,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -55575,6 +55637,11 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6">

</xml_diff>

<commit_message>
effecient step change working
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11235" tabRatio="725" activeTab="3"/>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -4946,14 +4946,7 @@
     <cellStyle name="Percent 5" xfId="83"/>
     <cellStyle name="Style 1" xfId="84"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.1498764000366222"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -5169,11 +5162,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193655296"/>
-        <c:axId val="193532992"/>
+        <c:axId val="141975552"/>
+        <c:axId val="159836992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193655296"/>
+        <c:axId val="141975552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5195,14 +5188,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193532992"/>
+        <c:crossAx val="159836992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5210,7 +5202,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193532992"/>
+        <c:axId val="159836992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5241,21 +5233,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193655296"/>
+        <c:crossAx val="141975552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
@@ -5711,11 +5701,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193657344"/>
-        <c:axId val="193534720"/>
+        <c:axId val="141977600"/>
+        <c:axId val="159838720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193657344"/>
+        <c:axId val="141977600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5737,14 +5727,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193534720"/>
+        <c:crossAx val="159838720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5752,7 +5741,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193534720"/>
+        <c:axId val="159838720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -5781,14 +5770,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193657344"/>
+        <c:crossAx val="141977600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5796,7 +5784,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5924,11 +5911,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193658368"/>
-        <c:axId val="194331776"/>
+        <c:axId val="206603776"/>
+        <c:axId val="159841024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193658368"/>
+        <c:axId val="206603776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5950,14 +5937,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194331776"/>
+        <c:crossAx val="159841024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5965,7 +5951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194331776"/>
+        <c:axId val="159841024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5996,14 +5982,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193658368"/>
+        <c:crossAx val="206603776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6205,11 +6190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="194434560"/>
-        <c:axId val="194334080"/>
+        <c:axId val="141976576"/>
+        <c:axId val="162317440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="194434560"/>
+        <c:axId val="141976576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6220,7 +6205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194334080"/>
+        <c:crossAx val="162317440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6228,7 +6213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194334080"/>
+        <c:axId val="162317440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000000"/>
@@ -6241,7 +6226,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194434560"/>
+        <c:crossAx val="141976576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100000000"/>
@@ -6820,11 +6805,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="195084288"/>
-        <c:axId val="194820288"/>
+        <c:axId val="206848512"/>
+        <c:axId val="162369472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195084288"/>
+        <c:axId val="206848512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6845,7 +6830,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194820288"/>
+        <c:crossAx val="162369472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6853,7 +6838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194820288"/>
+        <c:axId val="162369472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6875,7 +6860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195084288"/>
+        <c:crossAx val="206848512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -7467,7 +7452,7 @@
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="1">
+    <sheetView topLeftCell="A56" workbookViewId="1">
       <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
@@ -24588,7 +24573,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30931,27 +30918,27 @@
     <sortCondition ref="A13:A134"/>
   </sortState>
   <conditionalFormatting sqref="L88:M88 L92:M103 L115:M115 L118:M119 L121:M122 L124:M124 L126:M132 L106:M113 C49:J50 L17:M83 C52:J139 A17:J26 C31:J47 A31:B139 A27:A30 D27:J30 A142:G146">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C28">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:C30">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
changed hardwired step constraints for construction phases
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -5,7 +5,6 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11235" tabRatio="725" activeTab="3"/>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="11235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3629" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3632" uniqueCount="718">
   <si>
     <t>Scenario</t>
   </si>
@@ -2336,7 +2335,10 @@
     <t>* Construction Phase 7.1 = 7A, 7.2 = 7B</t>
   </si>
   <si>
-    <t>Phase 1 - 5 areas only allow change in steps 1 - 3</t>
+    <t>Phase 1 - 3 areas only allow change in steps 1 - 2</t>
+  </si>
+  <si>
+    <t>Phase 4 - 5 areas only allow change in steps 1 - 3</t>
   </si>
 </sst>
 </file>
@@ -4603,16 +4605,77 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4633,12 +4696,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4653,61 +4710,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4774,27 +4776,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4855,6 +4836,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4946,7 +4948,14 @@
     <cellStyle name="Percent 5" xfId="83"/>
     <cellStyle name="Style 1" xfId="84"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5162,11 +5171,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141975552"/>
-        <c:axId val="159836992"/>
+        <c:axId val="206093312"/>
+        <c:axId val="239831872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141975552"/>
+        <c:axId val="206093312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5194,7 +5203,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159836992"/>
+        <c:crossAx val="239831872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5202,7 +5211,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159836992"/>
+        <c:axId val="239831872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5239,7 +5248,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141975552"/>
+        <c:crossAx val="206093312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5701,11 +5710,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141977600"/>
-        <c:axId val="159838720"/>
+        <c:axId val="206909440"/>
+        <c:axId val="239833600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141977600"/>
+        <c:axId val="206909440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5733,7 +5742,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159838720"/>
+        <c:crossAx val="239833600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5741,7 +5750,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159838720"/>
+        <c:axId val="239833600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -5776,7 +5785,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141977600"/>
+        <c:crossAx val="206909440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5911,11 +5920,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206603776"/>
-        <c:axId val="159841024"/>
+        <c:axId val="207269376"/>
+        <c:axId val="239835904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206603776"/>
+        <c:axId val="207269376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5943,7 +5952,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159841024"/>
+        <c:crossAx val="239835904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5951,7 +5960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159841024"/>
+        <c:axId val="239835904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5988,7 +5997,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206603776"/>
+        <c:crossAx val="207269376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6190,11 +6199,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141976576"/>
-        <c:axId val="162317440"/>
+        <c:axId val="237098496"/>
+        <c:axId val="255738432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141976576"/>
+        <c:axId val="237098496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6205,7 +6214,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162317440"/>
+        <c:crossAx val="255738432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6213,7 +6222,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162317440"/>
+        <c:axId val="255738432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000000"/>
@@ -6226,7 +6235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141976576"/>
+        <c:crossAx val="237098496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100000000"/>
@@ -6805,11 +6814,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206848512"/>
-        <c:axId val="162369472"/>
+        <c:axId val="239585792"/>
+        <c:axId val="207495168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206848512"/>
+        <c:axId val="239585792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6830,7 +6839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162369472"/>
+        <c:crossAx val="207495168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6838,7 +6847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162369472"/>
+        <c:axId val="207495168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6860,7 +6869,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206848512"/>
+        <c:crossAx val="239585792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -7452,9 +7461,6 @@
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
-    <sheetView topLeftCell="A56" workbookViewId="1">
-      <selection activeCell="C180" sqref="C180"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16796,9 +16802,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:B1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16817,16 +16820,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="376" t="s">
+      <c r="A1" s="353" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="377"/>
+      <c r="B1" s="354"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="378" t="s">
+      <c r="A2" s="355" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="379"/>
+      <c r="B2" s="356"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="X3" s="245" t="s">
@@ -16834,33 +16837,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="383" t="s">
+      <c r="A4" s="363" t="s">
         <v>261</v>
       </c>
-      <c r="B4" s="384"/>
+      <c r="B4" s="364"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="387" t="s">
+      <c r="D4" s="367" t="s">
         <v>262</v>
       </c>
-      <c r="E4" s="380" t="s">
+      <c r="E4" s="357" t="s">
         <v>263</v>
       </c>
-      <c r="F4" s="381"/>
-      <c r="G4" s="381"/>
-      <c r="H4" s="381"/>
-      <c r="I4" s="381"/>
-      <c r="J4" s="381"/>
-      <c r="K4" s="381"/>
-      <c r="L4" s="381"/>
-      <c r="M4" s="381"/>
-      <c r="N4" s="381"/>
-      <c r="O4" s="381"/>
-      <c r="P4" s="381"/>
-      <c r="Q4" s="381"/>
-      <c r="R4" s="381"/>
-      <c r="S4" s="381"/>
-      <c r="T4" s="381"/>
-      <c r="U4" s="382"/>
+      <c r="F4" s="358"/>
+      <c r="G4" s="358"/>
+      <c r="H4" s="358"/>
+      <c r="I4" s="358"/>
+      <c r="J4" s="358"/>
+      <c r="K4" s="358"/>
+      <c r="L4" s="358"/>
+      <c r="M4" s="358"/>
+      <c r="N4" s="358"/>
+      <c r="O4" s="358"/>
+      <c r="P4" s="358"/>
+      <c r="Q4" s="358"/>
+      <c r="R4" s="358"/>
+      <c r="S4" s="358"/>
+      <c r="T4" s="358"/>
+      <c r="U4" s="359"/>
       <c r="Y4" s="245">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -16927,12 +16930,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="385"/>
-      <c r="B5" s="386"/>
+      <c r="A5" s="365"/>
+      <c r="B5" s="366"/>
       <c r="C5" s="68" t="s">
         <v>264</v>
       </c>
-      <c r="D5" s="388"/>
+      <c r="D5" s="368"/>
       <c r="E5" s="69">
         <f>'Step Analysis'!E5</f>
         <v>2020</v>
@@ -17070,10 +17073,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="355" t="s">
+      <c r="A6" s="369" t="s">
         <v>266</v>
       </c>
-      <c r="B6" s="356"/>
+      <c r="B6" s="370"/>
       <c r="C6" s="164">
         <v>10</v>
       </c>
@@ -17591,12 +17594,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="370" t="s">
+      <c r="A12" s="360" t="s">
         <v>277</v>
       </c>
-      <c r="B12" s="371"/>
-      <c r="C12" s="371"/>
-      <c r="D12" s="372"/>
+      <c r="B12" s="361"/>
+      <c r="C12" s="361"/>
+      <c r="D12" s="362"/>
       <c r="E12" s="285">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -17731,12 +17734,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="370" t="s">
+      <c r="A13" s="360" t="s">
         <v>278</v>
       </c>
-      <c r="B13" s="371"/>
-      <c r="C13" s="371"/>
-      <c r="D13" s="372"/>
+      <c r="B13" s="361"/>
+      <c r="C13" s="361"/>
+      <c r="D13" s="362"/>
       <c r="E13" s="285"/>
       <c r="F13" s="285"/>
       <c r="G13" s="285"/>
@@ -17829,10 +17832,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="355" t="s">
+      <c r="A14" s="369" t="s">
         <v>279</v>
       </c>
-      <c r="B14" s="356"/>
+      <c r="B14" s="370"/>
       <c r="C14" s="166">
         <v>10</v>
       </c>
@@ -18347,12 +18350,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="370" t="s">
+      <c r="A20" s="360" t="s">
         <v>282</v>
       </c>
-      <c r="B20" s="371"/>
-      <c r="C20" s="371"/>
-      <c r="D20" s="372"/>
+      <c r="B20" s="361"/>
+      <c r="C20" s="361"/>
+      <c r="D20" s="362"/>
       <c r="E20" s="285">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -18423,12 +18426,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="370" t="s">
+      <c r="A21" s="360" t="s">
         <v>283</v>
       </c>
-      <c r="B21" s="371"/>
-      <c r="C21" s="371"/>
-      <c r="D21" s="372"/>
+      <c r="B21" s="361"/>
+      <c r="C21" s="361"/>
+      <c r="D21" s="362"/>
       <c r="E21" s="285"/>
       <c r="F21" s="285"/>
       <c r="G21" s="285"/>
@@ -18454,10 +18457,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="355" t="s">
+      <c r="A22" s="369" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="356"/>
+      <c r="B22" s="370"/>
       <c r="C22" s="164">
         <v>10</v>
       </c>
@@ -18704,12 +18707,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="370" t="s">
+      <c r="A28" s="360" t="s">
         <v>285</v>
       </c>
-      <c r="B28" s="371"/>
-      <c r="C28" s="371"/>
-      <c r="D28" s="372"/>
+      <c r="B28" s="361"/>
+      <c r="C28" s="361"/>
+      <c r="D28" s="362"/>
       <c r="E28" s="285">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -18780,12 +18783,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="370" t="s">
+      <c r="A29" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="B29" s="371"/>
-      <c r="C29" s="371"/>
-      <c r="D29" s="372"/>
+      <c r="B29" s="361"/>
+      <c r="C29" s="361"/>
+      <c r="D29" s="362"/>
       <c r="E29" s="285"/>
       <c r="F29" s="285"/>
       <c r="G29" s="285"/>
@@ -18811,10 +18814,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="355" t="s">
+      <c r="A30" s="369" t="s">
         <v>287</v>
       </c>
-      <c r="B30" s="356"/>
+      <c r="B30" s="370"/>
       <c r="C30" s="164">
         <v>10</v>
       </c>
@@ -19061,12 +19064,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="370" t="s">
+      <c r="A36" s="360" t="s">
         <v>288</v>
       </c>
-      <c r="B36" s="371"/>
-      <c r="C36" s="371"/>
-      <c r="D36" s="372"/>
+      <c r="B36" s="361"/>
+      <c r="C36" s="361"/>
+      <c r="D36" s="362"/>
       <c r="E36" s="285">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -19137,12 +19140,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="370" t="s">
+      <c r="A37" s="360" t="s">
         <v>289</v>
       </c>
-      <c r="B37" s="371"/>
-      <c r="C37" s="371"/>
-      <c r="D37" s="372"/>
+      <c r="B37" s="361"/>
+      <c r="C37" s="361"/>
+      <c r="D37" s="362"/>
       <c r="E37" s="285"/>
       <c r="F37" s="285"/>
       <c r="G37" s="285"/>
@@ -19168,10 +19171,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="355" t="s">
+      <c r="A38" s="369" t="s">
         <v>290</v>
       </c>
-      <c r="B38" s="356"/>
+      <c r="B38" s="370"/>
       <c r="C38" s="164">
         <v>10</v>
       </c>
@@ -19418,12 +19421,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="370" t="s">
+      <c r="A44" s="360" t="s">
         <v>291</v>
       </c>
-      <c r="B44" s="371"/>
-      <c r="C44" s="371"/>
-      <c r="D44" s="372"/>
+      <c r="B44" s="361"/>
+      <c r="C44" s="361"/>
+      <c r="D44" s="362"/>
       <c r="E44" s="285">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -19494,12 +19497,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="370" t="s">
+      <c r="A45" s="360" t="s">
         <v>292</v>
       </c>
-      <c r="B45" s="371"/>
-      <c r="C45" s="371"/>
-      <c r="D45" s="372"/>
+      <c r="B45" s="361"/>
+      <c r="C45" s="361"/>
+      <c r="D45" s="362"/>
       <c r="E45" s="285"/>
       <c r="F45" s="285"/>
       <c r="G45" s="285"/>
@@ -19525,11 +19528,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="357" t="s">
+      <c r="A46" s="378" t="s">
         <v>293</v>
       </c>
-      <c r="B46" s="358"/>
-      <c r="C46" s="359"/>
+      <c r="B46" s="379"/>
+      <c r="C46" s="380"/>
       <c r="D46" s="174"/>
       <c r="E46" s="293">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -19602,12 +19605,12 @@
       <c r="V46" s="246"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="365" t="s">
+      <c r="A47" s="384" t="s">
         <v>294</v>
       </c>
-      <c r="B47" s="366"/>
-      <c r="C47" s="366"/>
-      <c r="D47" s="367"/>
+      <c r="B47" s="385"/>
+      <c r="C47" s="385"/>
+      <c r="D47" s="386"/>
       <c r="E47" s="294">
         <f>E46</f>
         <v>1500000</v>
@@ -19678,7 +19681,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="175"/>
       <c r="B48" s="175"/>
-      <c r="C48" s="368" t="s">
+      <c r="C48" s="387" t="s">
         <v>295</v>
       </c>
       <c r="D48" s="176">
@@ -19753,7 +19756,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="175"/>
-      <c r="C49" s="369"/>
+      <c r="C49" s="388"/>
       <c r="D49" s="248">
         <v>37</v>
       </c>
@@ -19824,7 +19827,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="175"/>
-      <c r="C50" s="369"/>
+      <c r="C50" s="388"/>
       <c r="D50" s="248">
         <v>30</v>
       </c>
@@ -19895,7 +19898,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="175"/>
-      <c r="C51" s="369"/>
+      <c r="C51" s="388"/>
       <c r="D51" s="248">
         <v>41</v>
       </c>
@@ -19965,38 +19968,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="360" t="s">
+      <c r="A52" s="381" t="s">
         <v>296</v>
       </c>
-      <c r="B52" s="361"/>
-      <c r="C52" s="361"/>
-      <c r="D52" s="361"/>
-      <c r="E52" s="361"/>
-      <c r="F52" s="361"/>
-      <c r="G52" s="361"/>
-      <c r="H52" s="361"/>
-      <c r="I52" s="361"/>
-      <c r="J52" s="361"/>
-      <c r="K52" s="361"/>
-      <c r="L52" s="361"/>
-      <c r="M52" s="361"/>
-      <c r="N52" s="361"/>
-      <c r="O52" s="361"/>
-      <c r="P52" s="361"/>
-      <c r="Q52" s="361"/>
-      <c r="R52" s="361"/>
-      <c r="S52" s="361"/>
-      <c r="T52" s="361"/>
-      <c r="U52" s="361"/>
-      <c r="V52" s="361"/>
-      <c r="W52" s="362"/>
+      <c r="B52" s="382"/>
+      <c r="C52" s="382"/>
+      <c r="D52" s="382"/>
+      <c r="E52" s="382"/>
+      <c r="F52" s="382"/>
+      <c r="G52" s="382"/>
+      <c r="H52" s="382"/>
+      <c r="I52" s="382"/>
+      <c r="J52" s="382"/>
+      <c r="K52" s="382"/>
+      <c r="L52" s="382"/>
+      <c r="M52" s="382"/>
+      <c r="N52" s="382"/>
+      <c r="O52" s="382"/>
+      <c r="P52" s="382"/>
+      <c r="Q52" s="382"/>
+      <c r="R52" s="382"/>
+      <c r="S52" s="382"/>
+      <c r="T52" s="382"/>
+      <c r="U52" s="382"/>
+      <c r="V52" s="382"/>
+      <c r="W52" s="383"/>
       <c r="X52" s="246"/>
     </row>
     <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="363" t="s">
+      <c r="A53" s="373" t="s">
         <v>297</v>
       </c>
-      <c r="B53" s="364"/>
+      <c r="B53" s="374"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -20173,10 +20176,10 @@
       <c r="X57" s="246"/>
     </row>
     <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="353" t="s">
+      <c r="A58" s="371" t="s">
         <v>299</v>
       </c>
-      <c r="B58" s="354"/>
+      <c r="B58" s="372"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -20358,10 +20361,10 @@
       <c r="X62" s="246"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="353" t="s">
+      <c r="A63" s="371" t="s">
         <v>300</v>
       </c>
-      <c r="B63" s="354"/>
+      <c r="B63" s="372"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -20551,10 +20554,10 @@
       <c r="X67" s="246"/>
     </row>
     <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="353" t="s">
+      <c r="A68" s="371" t="s">
         <v>301</v>
       </c>
-      <c r="B68" s="354"/>
+      <c r="B68" s="372"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -20732,10 +20735,10 @@
       <c r="X72" s="246"/>
     </row>
     <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="353" t="s">
+      <c r="A73" s="371" t="s">
         <v>302</v>
       </c>
-      <c r="B73" s="354"/>
+      <c r="B73" s="372"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -20961,10 +20964,10 @@
       <c r="X77" s="246"/>
     </row>
     <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="353" t="s">
+      <c r="A78" s="371" t="s">
         <v>304</v>
       </c>
-      <c r="B78" s="354"/>
+      <c r="B78" s="372"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -21136,10 +21139,10 @@
       <c r="X82" s="246"/>
     </row>
     <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="353" t="s">
+      <c r="A83" s="371" t="s">
         <v>306</v>
       </c>
-      <c r="B83" s="354"/>
+      <c r="B83" s="372"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -21311,10 +21314,10 @@
       <c r="X87" s="246"/>
     </row>
     <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="353" t="s">
+      <c r="A88" s="371" t="s">
         <v>78</v>
       </c>
-      <c r="B88" s="354"/>
+      <c r="B88" s="372"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -21486,10 +21489,10 @@
       <c r="X92" s="246"/>
     </row>
     <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="353" t="s">
+      <c r="A93" s="371" t="s">
         <v>309</v>
       </c>
-      <c r="B93" s="354"/>
+      <c r="B93" s="372"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -21691,10 +21694,10 @@
       <c r="X97" s="246"/>
     </row>
     <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="353" t="s">
+      <c r="A98" s="371" t="s">
         <v>311</v>
       </c>
-      <c r="B98" s="354"/>
+      <c r="B98" s="372"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -21886,10 +21889,10 @@
       <c r="X102" s="246"/>
     </row>
     <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="353" t="s">
+      <c r="A103" s="371" t="s">
         <v>313</v>
       </c>
-      <c r="B103" s="354"/>
+      <c r="B103" s="372"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -22091,10 +22094,10 @@
       <c r="X107" s="246"/>
     </row>
     <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="353" t="s">
+      <c r="A108" s="371" t="s">
         <v>314</v>
       </c>
-      <c r="B108" s="354"/>
+      <c r="B108" s="372"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -22296,10 +22299,10 @@
       <c r="X112" s="246"/>
     </row>
     <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="353" t="s">
+      <c r="A113" s="371" t="s">
         <v>315</v>
       </c>
-      <c r="B113" s="354"/>
+      <c r="B113" s="372"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -22461,10 +22464,10 @@
       <c r="X117" s="246"/>
     </row>
     <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="353" t="s">
+      <c r="A118" s="371" t="s">
         <v>316</v>
       </c>
-      <c r="B118" s="354"/>
+      <c r="B118" s="372"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -22666,10 +22669,10 @@
       <c r="X122" s="246"/>
     </row>
     <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="353" t="s">
+      <c r="A123" s="371" t="s">
         <v>317</v>
       </c>
-      <c r="B123" s="354"/>
+      <c r="B123" s="372"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -22871,10 +22874,10 @@
       <c r="X127" s="246"/>
     </row>
     <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="353" t="s">
+      <c r="A128" s="371" t="s">
         <v>318</v>
       </c>
-      <c r="B128" s="354"/>
+      <c r="B128" s="372"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -23076,10 +23079,10 @@
       <c r="X132" s="246"/>
     </row>
     <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="353" t="s">
+      <c r="A133" s="371" t="s">
         <v>319</v>
       </c>
-      <c r="B133" s="354"/>
+      <c r="B133" s="372"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -23281,10 +23284,10 @@
       <c r="X137" s="246"/>
     </row>
     <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="353" t="s">
+      <c r="A138" s="371" t="s">
         <v>320</v>
       </c>
-      <c r="B138" s="354"/>
+      <c r="B138" s="372"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -23494,10 +23497,10 @@
       <c r="X142" s="246"/>
     </row>
     <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="353" t="s">
+      <c r="A143" s="371" t="s">
         <v>324</v>
       </c>
-      <c r="B143" s="354"/>
+      <c r="B143" s="372"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -23590,10 +23593,10 @@
       <c r="X144" s="246"/>
     </row>
     <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="363" t="s">
+      <c r="A145" s="373" t="s">
         <v>326</v>
       </c>
-      <c r="B145" s="364"/>
+      <c r="B145" s="374"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -23666,10 +23669,10 @@
       <c r="X146" s="246"/>
     </row>
     <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="363" t="s">
+      <c r="A147" s="373" t="s">
         <v>327</v>
       </c>
-      <c r="B147" s="364"/>
+      <c r="B147" s="374"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -23767,10 +23770,10 @@
       <c r="X148" s="246"/>
     </row>
     <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="363" t="s">
+      <c r="A149" s="373" t="s">
         <v>328</v>
       </c>
-      <c r="B149" s="364"/>
+      <c r="B149" s="374"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -23892,12 +23895,12 @@
       <c r="X151" s="246"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="373" t="s">
+      <c r="A152" s="375" t="s">
         <v>329</v>
       </c>
-      <c r="B152" s="374"/>
-      <c r="C152" s="374"/>
-      <c r="D152" s="375"/>
+      <c r="B152" s="376"/>
+      <c r="C152" s="376"/>
+      <c r="D152" s="377"/>
       <c r="E152" s="317">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -24509,37 +24512,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -24556,6 +24528,37 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -24572,9 +24575,6 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26798,10 +26798,9 @@
   </sheetPr>
   <dimension ref="A1:AG230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147:G230"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26943,7 +26942,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="242" t="s">
         <v>422</v>
       </c>
       <c r="Q10" s="336" t="s">
@@ -26973,6 +26972,9 @@
       </c>
     </row>
     <row r="12" spans="1:33" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="242" t="s">
+        <v>717</v>
+      </c>
       <c r="Q12" s="336"/>
       <c r="R12" s="337"/>
     </row>
@@ -30155,13 +30157,19 @@
       <c r="G146" s="234"/>
     </row>
     <row r="147" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147"/>
-      <c r="B147"/>
-      <c r="C147"/>
-      <c r="D147"/>
-      <c r="E147"/>
-      <c r="F147"/>
-      <c r="G147"/>
+      <c r="A147" s="242" t="s">
+        <v>657</v>
+      </c>
+      <c r="B147" s="242" t="s">
+        <v>693</v>
+      </c>
+      <c r="C147" s="234">
+        <v>1</v>
+      </c>
+      <c r="D147" s="234"/>
+      <c r="E147" s="234"/>
+      <c r="F147" s="234"/>
+      <c r="G147" s="234"/>
       <c r="L147" t="s">
         <v>423</v>
       </c>
@@ -30918,26 +30926,31 @@
     <sortCondition ref="A13:A134"/>
   </sortState>
   <conditionalFormatting sqref="L88:M88 L92:M103 L115:M115 L118:M119 L121:M122 L124:M124 L126:M132 L106:M113 C49:J50 L17:M83 C52:J139 A17:J26 C31:J47 A31:B139 A27:A30 D27:J30 A142:G146">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:C28">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:C28">
+  <conditionalFormatting sqref="B29:C29">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:C29">
+  <conditionalFormatting sqref="B30:C30">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C30">
+  <conditionalFormatting sqref="A147:G147">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
@@ -30949,10 +30962,10 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C17:C19">
       <formula1>$AG$2:$AG$60</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C142:G146">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C142:G147">
       <formula1>"1, 2, 3, 4, 5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B139 B142:B146">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B139 B142:B147">
       <formula1>"not, only"</formula1>
     </dataValidation>
   </dataValidations>
@@ -30972,7 +30985,6 @@
       <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B286" sqref="B286"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -40705,7 +40717,6 @@
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -42853,7 +42864,6 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -43963,7 +43973,6 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45245,7 +45254,6 @@
   <dimension ref="A1:BZ83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45305,69 +45313,69 @@
       <c r="BZ1" s="190"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="376" t="s">
+      <c r="A2" s="353" t="s">
         <v>258</v>
       </c>
-      <c r="B2" s="419"/>
-      <c r="C2" s="420"/>
-      <c r="D2" s="422" t="s">
+      <c r="B2" s="412"/>
+      <c r="C2" s="413"/>
+      <c r="D2" s="415" t="s">
         <v>566</v>
       </c>
-      <c r="E2" s="423"/>
-      <c r="F2" s="423"/>
-      <c r="G2" s="423"/>
-      <c r="H2" s="423"/>
-      <c r="I2" s="423"/>
-      <c r="J2" s="423"/>
-      <c r="K2" s="423"/>
-      <c r="L2" s="423"/>
-      <c r="M2" s="423"/>
-      <c r="N2" s="423"/>
-      <c r="O2" s="423"/>
-      <c r="P2" s="423"/>
-      <c r="Q2" s="423"/>
-      <c r="R2" s="423"/>
-      <c r="S2" s="423"/>
-      <c r="T2" s="423"/>
+      <c r="E2" s="416"/>
+      <c r="F2" s="416"/>
+      <c r="G2" s="416"/>
+      <c r="H2" s="416"/>
+      <c r="I2" s="416"/>
+      <c r="J2" s="416"/>
+      <c r="K2" s="416"/>
+      <c r="L2" s="416"/>
+      <c r="M2" s="416"/>
+      <c r="N2" s="416"/>
+      <c r="O2" s="416"/>
+      <c r="P2" s="416"/>
+      <c r="Q2" s="416"/>
+      <c r="R2" s="416"/>
+      <c r="S2" s="416"/>
+      <c r="T2" s="416"/>
       <c r="AA2" s="132"/>
       <c r="BY2" s="190"/>
       <c r="BZ2" s="190"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="378" t="s">
+      <c r="A3" s="355" t="s">
         <v>259</v>
       </c>
-      <c r="B3" s="419"/>
-      <c r="C3" s="420"/>
+      <c r="B3" s="412"/>
+      <c r="C3" s="413"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="424" t="s">
+      <c r="F3" s="417" t="s">
         <v>567</v>
       </c>
-      <c r="G3" s="425"/>
-      <c r="H3" s="426" t="s">
+      <c r="G3" s="418"/>
+      <c r="H3" s="419" t="s">
         <v>568</v>
       </c>
-      <c r="I3" s="426"/>
-      <c r="J3" s="427"/>
-      <c r="K3" s="428" t="s">
+      <c r="I3" s="419"/>
+      <c r="J3" s="420"/>
+      <c r="K3" s="421" t="s">
         <v>569</v>
       </c>
-      <c r="L3" s="429"/>
-      <c r="M3" s="430"/>
-      <c r="N3" s="427" t="s">
+      <c r="L3" s="422"/>
+      <c r="M3" s="423"/>
+      <c r="N3" s="420" t="s">
         <v>570</v>
       </c>
-      <c r="O3" s="431"/>
-      <c r="P3" s="432"/>
-      <c r="Q3" s="433" t="s">
+      <c r="O3" s="424"/>
+      <c r="P3" s="425"/>
+      <c r="Q3" s="426" t="s">
         <v>571</v>
       </c>
-      <c r="R3" s="434"/>
-      <c r="S3" s="435" t="s">
+      <c r="R3" s="427"/>
+      <c r="S3" s="428" t="s">
         <v>572</v>
       </c>
-      <c r="T3" s="436"/>
+      <c r="T3" s="429"/>
       <c r="AA3" s="133"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -45531,7 +45539,7 @@
       <c r="AC6" s="134"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="413" t="str">
+      <c r="C7" s="434" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -45539,81 +45547,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="414"/>
-      <c r="E7" s="415"/>
-      <c r="F7" s="414" t="s">
+      <c r="D7" s="437"/>
+      <c r="E7" s="435"/>
+      <c r="F7" s="437" t="s">
         <v>595</v>
       </c>
-      <c r="G7" s="414"/>
-      <c r="H7" s="415"/>
-      <c r="I7" s="416" t="str">
+      <c r="G7" s="437"/>
+      <c r="H7" s="435"/>
+      <c r="I7" s="438" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$242.422)</v>
       </c>
-      <c r="J7" s="417"/>
-      <c r="K7" s="417"/>
-      <c r="L7" s="417"/>
-      <c r="M7" s="417"/>
-      <c r="N7" s="417"/>
-      <c r="O7" s="417"/>
-      <c r="P7" s="417"/>
-      <c r="Q7" s="417"/>
-      <c r="R7" s="418"/>
-      <c r="S7" s="413" t="str">
+      <c r="J7" s="439"/>
+      <c r="K7" s="439"/>
+      <c r="L7" s="439"/>
+      <c r="M7" s="439"/>
+      <c r="N7" s="439"/>
+      <c r="O7" s="439"/>
+      <c r="P7" s="439"/>
+      <c r="Q7" s="439"/>
+      <c r="R7" s="440"/>
+      <c r="S7" s="434" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$596.731)</v>
       </c>
-      <c r="T7" s="414"/>
-      <c r="U7" s="414"/>
-      <c r="V7" s="414"/>
-      <c r="W7" s="414"/>
-      <c r="X7" s="415"/>
-      <c r="Y7" s="413" t="s">
+      <c r="T7" s="437"/>
+      <c r="U7" s="437"/>
+      <c r="V7" s="437"/>
+      <c r="W7" s="437"/>
+      <c r="X7" s="435"/>
+      <c r="Y7" s="434" t="s">
         <v>596</v>
       </c>
-      <c r="Z7" s="415"/>
+      <c r="Z7" s="435"/>
       <c r="AA7" s="135"/>
-      <c r="AH7" s="437" t="s">
+      <c r="AH7" s="430" t="s">
         <v>597</v>
       </c>
-      <c r="AI7" s="438"/>
+      <c r="AI7" s="431"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="439" t="s">
+      <c r="AK7" s="432" t="s">
         <v>598</v>
       </c>
       <c r="AL7" s="411"/>
       <c r="AM7" s="411"/>
-      <c r="AN7" s="438"/>
-      <c r="AP7" s="440" t="s">
+      <c r="AN7" s="431"/>
+      <c r="AP7" s="433" t="s">
         <v>599</v>
       </c>
-      <c r="AQ7" s="382"/>
-      <c r="AS7" s="421" t="s">
+      <c r="AQ7" s="359"/>
+      <c r="AS7" s="414" t="s">
         <v>600</v>
       </c>
-      <c r="AT7" s="381"/>
-      <c r="AU7" s="381"/>
-      <c r="AV7" s="381"/>
-      <c r="AW7" s="381"/>
-      <c r="AX7" s="381"/>
-      <c r="AY7" s="381"/>
-      <c r="AZ7" s="381"/>
-      <c r="BA7" s="381"/>
-      <c r="BB7" s="382"/>
-      <c r="BD7" s="440" t="s">
+      <c r="AT7" s="358"/>
+      <c r="AU7" s="358"/>
+      <c r="AV7" s="358"/>
+      <c r="AW7" s="358"/>
+      <c r="AX7" s="358"/>
+      <c r="AY7" s="358"/>
+      <c r="AZ7" s="358"/>
+      <c r="BA7" s="358"/>
+      <c r="BB7" s="359"/>
+      <c r="BD7" s="433" t="s">
         <v>601</v>
       </c>
-      <c r="BE7" s="382"/>
+      <c r="BE7" s="359"/>
       <c r="BF7" s="190"/>
-      <c r="BG7" s="421" t="s">
+      <c r="BG7" s="414" t="s">
         <v>602</v>
       </c>
-      <c r="BH7" s="381"/>
-      <c r="BI7" s="381"/>
+      <c r="BH7" s="358"/>
+      <c r="BI7" s="358"/>
       <c r="BY7" s="190"/>
       <c r="BZ7" s="190"/>
     </row>
@@ -55558,17 +55566,17 @@
       <c r="BZ52" s="190"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="412"/>
-      <c r="D53" s="412"/>
-      <c r="E53" s="412"/>
-      <c r="F53" s="412"/>
-      <c r="G53" s="412"/>
-      <c r="H53" s="412"/>
-      <c r="I53" s="412"/>
-      <c r="J53" s="412"/>
-      <c r="K53" s="412"/>
-      <c r="L53" s="412"/>
-      <c r="M53" s="412"/>
+      <c r="C53" s="436"/>
+      <c r="D53" s="436"/>
+      <c r="E53" s="436"/>
+      <c r="F53" s="436"/>
+      <c r="G53" s="436"/>
+      <c r="H53" s="436"/>
+      <c r="I53" s="436"/>
+      <c r="J53" s="436"/>
+      <c r="K53" s="436"/>
+      <c r="L53" s="436"/>
+      <c r="M53" s="436"/>
       <c r="AC53" s="137" t="s">
         <v>651</v>
       </c>
@@ -55703,6 +55711,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -55719,11 +55732,6 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6">

</xml_diff>

<commit_message>
isolated forced changes and phase step constraints implemented
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11235" tabRatio="725" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11235" tabRatio="725" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3874" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="720">
   <si>
     <t>Scenario</t>
   </si>
@@ -4957,7 +4957,77 @@
     <cellStyle name="Percent 5" xfId="83"/>
     <cellStyle name="Style 1" xfId="84"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7566,7 +7636,7 @@
   </sheetPr>
   <dimension ref="A1:CP243"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
@@ -24681,8 +24751,8 @@
   </sheetPr>
   <dimension ref="A1:P222"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25589,8 +25659,12 @@
       <c r="J48" s="234" t="s">
         <v>83</v>
       </c>
-      <c r="K48" s="343"/>
-      <c r="L48" s="343"/>
+      <c r="K48" s="343" t="s">
+        <v>50</v>
+      </c>
+      <c r="L48" s="343">
+        <v>2</v>
+      </c>
       <c r="N48" s="234" t="s">
         <v>83</v>
       </c>
@@ -26012,12 +26086,8 @@
       <c r="J74" s="234" t="s">
         <v>112</v>
       </c>
-      <c r="K74" s="343" t="s">
-        <v>479</v>
-      </c>
-      <c r="L74" s="343">
-        <v>1</v>
-      </c>
+      <c r="K74" s="343"/>
+      <c r="L74" s="343"/>
       <c r="N74" s="234" t="s">
         <v>112</v>
       </c>
@@ -26032,12 +26102,8 @@
       <c r="J75" s="234" t="s">
         <v>113</v>
       </c>
-      <c r="K75" s="343" t="s">
-        <v>479</v>
-      </c>
-      <c r="L75" s="343">
-        <v>2</v>
-      </c>
+      <c r="K75" s="343"/>
+      <c r="L75" s="343"/>
       <c r="N75" s="234" t="s">
         <v>113</v>
       </c>
@@ -26052,12 +26118,8 @@
       <c r="J76" s="234" t="s">
         <v>114</v>
       </c>
-      <c r="K76" s="343" t="s">
-        <v>479</v>
-      </c>
-      <c r="L76" s="343">
-        <v>3</v>
-      </c>
+      <c r="K76" s="343"/>
+      <c r="L76" s="343"/>
       <c r="N76" s="234" t="s">
         <v>114</v>
       </c>
@@ -26072,12 +26134,8 @@
       <c r="J77" s="234" t="s">
         <v>115</v>
       </c>
-      <c r="K77" s="343" t="s">
-        <v>479</v>
-      </c>
-      <c r="L77" s="343">
-        <v>4</v>
-      </c>
+      <c r="K77" s="343"/>
+      <c r="L77" s="343"/>
       <c r="N77" s="234" t="s">
         <v>115</v>
       </c>
@@ -26092,12 +26150,8 @@
       <c r="J78" s="234" t="s">
         <v>116</v>
       </c>
-      <c r="K78" s="343" t="s">
-        <v>479</v>
-      </c>
-      <c r="L78" s="343">
-        <v>5</v>
-      </c>
+      <c r="K78" s="343"/>
+      <c r="L78" s="343"/>
       <c r="N78" s="234" t="s">
         <v>116</v>
       </c>
@@ -28035,8 +28089,8 @@
   </sheetPr>
   <dimension ref="A1:AG230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31370,7 +31424,7 @@
         <v>693</v>
       </c>
       <c r="C145" s="234">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D145" s="234"/>
       <c r="E145" s="234"/>
@@ -31386,7 +31440,7 @@
         <v>693</v>
       </c>
       <c r="C146" s="234">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D146" s="234"/>
       <c r="E146" s="234"/>
@@ -31401,7 +31455,7 @@
         <v>693</v>
       </c>
       <c r="C147" s="234">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" s="234"/>
       <c r="E147" s="234"/>
@@ -31449,12 +31503,18 @@
       <c r="D150" s="234">
         <v>2</v>
       </c>
-      <c r="E150" s="234"/>
-      <c r="F150" s="234"/>
-      <c r="G150" s="234"/>
+      <c r="E150" s="234">
+        <v>3</v>
+      </c>
+      <c r="F150" s="234">
+        <v>4</v>
+      </c>
+      <c r="G150" s="234">
+        <v>5</v>
+      </c>
     </row>
     <row r="151" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="337">
+      <c r="A151" s="242">
         <v>2</v>
       </c>
       <c r="B151" s="242" t="s">
@@ -31466,12 +31526,18 @@
       <c r="D151" s="234">
         <v>2</v>
       </c>
-      <c r="E151" s="234"/>
-      <c r="F151" s="234"/>
-      <c r="G151" s="234"/>
+      <c r="E151" s="234">
+        <v>3</v>
+      </c>
+      <c r="F151" s="234">
+        <v>4</v>
+      </c>
+      <c r="G151" s="234">
+        <v>5</v>
+      </c>
     </row>
     <row r="152" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="337">
+      <c r="A152" s="242">
         <v>3</v>
       </c>
       <c r="B152" s="242" t="s">
@@ -31483,9 +31549,15 @@
       <c r="D152" s="234">
         <v>2</v>
       </c>
-      <c r="E152" s="234"/>
-      <c r="F152" s="234"/>
-      <c r="G152" s="234"/>
+      <c r="E152" s="234">
+        <v>3</v>
+      </c>
+      <c r="F152" s="234">
+        <v>4</v>
+      </c>
+      <c r="G152" s="234">
+        <v>5</v>
+      </c>
     </row>
     <row r="153" spans="1:12" s="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="242">
@@ -31503,8 +31575,12 @@
       <c r="E153" s="234">
         <v>3</v>
       </c>
-      <c r="F153" s="234"/>
-      <c r="G153" s="234"/>
+      <c r="F153" s="234">
+        <v>4</v>
+      </c>
+      <c r="G153" s="234">
+        <v>5</v>
+      </c>
     </row>
     <row r="154" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="242">
@@ -31514,13 +31590,13 @@
         <v>693</v>
       </c>
       <c r="C154" s="234">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D154" s="234">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E154" s="234">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F154" s="234"/>
       <c r="G154" s="234"/>
@@ -31533,20 +31609,16 @@
         <v>693</v>
       </c>
       <c r="C155" s="234">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D155" s="234">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E155" s="234">
-        <v>3</v>
-      </c>
-      <c r="F155" s="234">
-        <v>4</v>
-      </c>
-      <c r="G155" s="234">
         <v>5</v>
       </c>
+      <c r="F155" s="234"/>
+      <c r="G155" s="234"/>
     </row>
     <row r="156" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="242">
@@ -31556,12 +31628,14 @@
         <v>693</v>
       </c>
       <c r="C156" s="234">
+        <v>3</v>
+      </c>
+      <c r="D156" s="234">
         <v>4</v>
       </c>
-      <c r="D156" s="234">
+      <c r="E156" s="234">
         <v>5</v>
       </c>
-      <c r="E156" s="234"/>
       <c r="F156" s="234"/>
       <c r="G156" s="234"/>
     </row>
@@ -31573,12 +31647,14 @@
         <v>693</v>
       </c>
       <c r="C157" s="234">
+        <v>3</v>
+      </c>
+      <c r="D157" s="234">
         <v>4</v>
       </c>
-      <c r="D157" s="234">
+      <c r="E157" s="234">
         <v>5</v>
       </c>
-      <c r="E157" s="234"/>
       <c r="F157" s="234"/>
       <c r="G157" s="234"/>
     </row>
@@ -31590,12 +31666,14 @@
         <v>693</v>
       </c>
       <c r="C158" s="234">
+        <v>3</v>
+      </c>
+      <c r="D158" s="234">
         <v>4</v>
       </c>
-      <c r="D158" s="234">
+      <c r="E158" s="234">
         <v>5</v>
       </c>
-      <c r="E158" s="234"/>
       <c r="F158" s="234"/>
       <c r="G158" s="234"/>
     </row>
@@ -31607,12 +31685,14 @@
         <v>693</v>
       </c>
       <c r="C159" s="234">
+        <v>3</v>
+      </c>
+      <c r="D159" s="234">
         <v>4</v>
       </c>
-      <c r="D159" s="234">
+      <c r="E159" s="234">
         <v>5</v>
       </c>
-      <c r="E159" s="234"/>
       <c r="F159" s="234"/>
       <c r="G159" s="234"/>
     </row>
@@ -31624,12 +31704,14 @@
         <v>693</v>
       </c>
       <c r="C160" s="234">
+        <v>3</v>
+      </c>
+      <c r="D160" s="234">
         <v>4</v>
       </c>
-      <c r="D160" s="234">
+      <c r="E160" s="234">
         <v>5</v>
       </c>
-      <c r="E160" s="234"/>
       <c r="F160" s="234"/>
       <c r="G160" s="234"/>
     </row>
@@ -32268,47 +32350,47 @@
     <sortCondition ref="A13:A134"/>
   </sortState>
   <conditionalFormatting sqref="L88:M88 L92:M103 L115:M115 L118:M119 L121:M122 L124:M124 L126:M132 L106:M113 C49:J50 L17:M83 C52:J139 A17:J26 C31:J47 A31:B139 A27:A30 D27:J30 A142:G146">
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="27" priority="8">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C28">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="26" priority="7">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="25" priority="6">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:C30">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="24" priority="5">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A147:G147">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150:G154">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155:G160">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B152:B154">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Commit prior to implementing habitat requirements received from J. Nordin.
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41549E7C-0560-BF4A-9907-02223940B4B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29280C98-5492-9146-AF88-6B558D0B355B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="460" windowWidth="31820" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42340" yWindow="1000" windowWidth="31820" windowHeight="21140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3366" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="670">
   <si>
     <t>Scenario</t>
   </si>
@@ -2192,6 +2192,15 @@
   </si>
   <si>
     <t>T30-3_b</t>
+  </si>
+  <si>
+    <t>Channel Areas</t>
+  </si>
+  <si>
+    <t>email from GR to JV, 9/27/18</t>
+  </si>
+  <si>
+    <t>per email from F. Moreno 10/3/18</t>
   </si>
 </sst>
 </file>
@@ -4601,14 +4610,17 @@
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="53" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4737,9 +4749,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="86">
@@ -7559,7 +7568,7 @@
   </sheetPr>
   <dimension ref="A1:CP256"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="95" workbookViewId="0">
+    <sheetView topLeftCell="A150" zoomScale="95" workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
@@ -25043,7 +25052,7 @@
   <dimension ref="A1:P222"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -25115,7 +25124,7 @@
         <v>329</v>
       </c>
       <c r="B4" s="109">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="245" t="s">
         <v>330</v>
@@ -25348,7 +25357,7 @@
         <v>50</v>
       </c>
       <c r="L13" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="234" t="s">
         <v>44</v>
@@ -25371,7 +25380,7 @@
         <v>50</v>
       </c>
       <c r="L14" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="234" t="s">
         <v>45</v>
@@ -25394,7 +25403,7 @@
         <v>50</v>
       </c>
       <c r="L15" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="234" t="s">
         <v>47</v>
@@ -25413,7 +25422,7 @@
         <v>50</v>
       </c>
       <c r="L16" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16" s="234" t="s">
         <v>48</v>
@@ -25436,7 +25445,7 @@
         <v>50</v>
       </c>
       <c r="L17" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N17" s="234" t="s">
         <v>49</v>
@@ -25455,7 +25464,7 @@
         <v>50</v>
       </c>
       <c r="L18" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" s="234" t="s">
         <v>51</v>
@@ -25478,7 +25487,7 @@
         <v>50</v>
       </c>
       <c r="L19" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19" s="234" t="s">
         <v>52</v>
@@ -25503,7 +25512,7 @@
         <v>50</v>
       </c>
       <c r="L20" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N20" s="234" t="s">
         <v>54</v>
@@ -25524,7 +25533,7 @@
         <v>50</v>
       </c>
       <c r="L21" s="342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N21" s="234" t="s">
         <v>637</v>
@@ -25647,14 +25656,14 @@
       <c r="B27" s="234" t="s">
         <v>349</v>
       </c>
-      <c r="C27" s="400" t="s">
+      <c r="C27" s="398" t="s">
         <v>350</v>
       </c>
-      <c r="D27" s="400"/>
-      <c r="E27" s="400"/>
-      <c r="F27" s="400"/>
-      <c r="G27" s="400"/>
-      <c r="H27" s="400"/>
+      <c r="D27" s="398"/>
+      <c r="E27" s="398"/>
+      <c r="F27" s="398"/>
+      <c r="G27" s="398"/>
+      <c r="H27" s="398"/>
       <c r="J27" s="234"/>
       <c r="K27" s="342"/>
       <c r="L27" s="342"/>
@@ -25669,12 +25678,12 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="C28" s="400"/>
-      <c r="D28" s="400"/>
-      <c r="E28" s="400"/>
-      <c r="F28" s="400"/>
-      <c r="G28" s="400"/>
-      <c r="H28" s="400"/>
+      <c r="C28" s="398"/>
+      <c r="D28" s="398"/>
+      <c r="E28" s="398"/>
+      <c r="F28" s="398"/>
+      <c r="G28" s="398"/>
+      <c r="H28" s="398"/>
       <c r="J28" s="234"/>
       <c r="K28" s="342"/>
       <c r="L28" s="342"/>
@@ -25689,12 +25698,12 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="C29" s="445"/>
-      <c r="D29" s="445"/>
-      <c r="E29" s="445"/>
-      <c r="F29" s="445"/>
-      <c r="G29" s="445"/>
-      <c r="H29" s="445"/>
+      <c r="C29" s="399"/>
+      <c r="D29" s="399"/>
+      <c r="E29" s="399"/>
+      <c r="F29" s="399"/>
+      <c r="G29" s="399"/>
+      <c r="H29" s="399"/>
       <c r="J29" s="234"/>
       <c r="K29" s="342"/>
       <c r="L29" s="342"/>
@@ -28055,8 +28064,8 @@
   </sheetPr>
   <dimension ref="A1:AB238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -30851,7 +30860,7 @@
     </row>
     <row r="145" spans="1:8" ht="15.75" customHeight="1">
       <c r="A145" s="234" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B145" s="234" t="s">
         <v>620</v>
@@ -30868,7 +30877,7 @@
     </row>
     <row r="146" spans="1:8" ht="15.75" customHeight="1">
       <c r="A146" s="234" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B146" s="234" t="s">
         <v>620</v>
@@ -32048,10 +32057,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AG384"/>
+  <dimension ref="A1:AG385"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A245" sqref="A245"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="A278" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -32086,14 +32095,14 @@
       <c r="H1" s="238" t="s">
         <v>366</v>
       </c>
-      <c r="J1" s="398" t="s">
+      <c r="J1" s="400" t="s">
         <v>367</v>
       </c>
-      <c r="K1" s="399"/>
-      <c r="L1" s="399"/>
-      <c r="M1" s="399"/>
-      <c r="N1" s="399"/>
-      <c r="O1" s="399"/>
+      <c r="K1" s="401"/>
+      <c r="L1" s="401"/>
+      <c r="M1" s="401"/>
+      <c r="N1" s="401"/>
+      <c r="O1" s="401"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="245" t="s">
@@ -32121,12 +32130,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J2" s="399"/>
-      <c r="K2" s="399"/>
-      <c r="L2" s="399"/>
-      <c r="M2" s="399"/>
-      <c r="N2" s="399"/>
-      <c r="O2" s="399"/>
+      <c r="J2" s="401"/>
+      <c r="K2" s="401"/>
+      <c r="L2" s="401"/>
+      <c r="M2" s="401"/>
+      <c r="N2" s="401"/>
+      <c r="O2" s="401"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="245" t="s">
@@ -32154,12 +32163,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J3" s="399"/>
-      <c r="K3" s="399"/>
-      <c r="L3" s="399"/>
-      <c r="M3" s="399"/>
-      <c r="N3" s="399"/>
-      <c r="O3" s="399"/>
+      <c r="J3" s="401"/>
+      <c r="K3" s="401"/>
+      <c r="L3" s="401"/>
+      <c r="M3" s="401"/>
+      <c r="N3" s="401"/>
+      <c r="O3" s="401"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="245" t="s">
@@ -32187,12 +32196,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J4" s="399"/>
-      <c r="K4" s="399"/>
-      <c r="L4" s="399"/>
-      <c r="M4" s="399"/>
-      <c r="N4" s="399"/>
-      <c r="O4" s="399"/>
+      <c r="J4" s="401"/>
+      <c r="K4" s="401"/>
+      <c r="L4" s="401"/>
+      <c r="M4" s="401"/>
+      <c r="N4" s="401"/>
+      <c r="O4" s="401"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
@@ -32220,12 +32229,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="399"/>
-      <c r="K5" s="399"/>
-      <c r="L5" s="399"/>
-      <c r="M5" s="399"/>
-      <c r="N5" s="399"/>
-      <c r="O5" s="399"/>
+      <c r="J5" s="401"/>
+      <c r="K5" s="401"/>
+      <c r="L5" s="401"/>
+      <c r="M5" s="401"/>
+      <c r="N5" s="401"/>
+      <c r="O5" s="401"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
@@ -32253,12 +32262,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J6" s="399"/>
-      <c r="K6" s="399"/>
-      <c r="L6" s="399"/>
-      <c r="M6" s="399"/>
-      <c r="N6" s="399"/>
-      <c r="O6" s="399"/>
+      <c r="J6" s="401"/>
+      <c r="K6" s="401"/>
+      <c r="L6" s="401"/>
+      <c r="M6" s="401"/>
+      <c r="N6" s="401"/>
+      <c r="O6" s="401"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
@@ -32286,12 +32295,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J7" s="399"/>
-      <c r="K7" s="399"/>
-      <c r="L7" s="399"/>
-      <c r="M7" s="399"/>
-      <c r="N7" s="399"/>
-      <c r="O7" s="399"/>
+      <c r="J7" s="401"/>
+      <c r="K7" s="401"/>
+      <c r="L7" s="401"/>
+      <c r="M7" s="401"/>
+      <c r="N7" s="401"/>
+      <c r="O7" s="401"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
@@ -32318,12 +32327,12 @@
       <c r="H8" s="241">
         <v>1.5475000000000001</v>
       </c>
-      <c r="J8" s="399"/>
-      <c r="K8" s="399"/>
-      <c r="L8" s="399"/>
-      <c r="M8" s="399"/>
-      <c r="N8" s="399"/>
-      <c r="O8" s="399"/>
+      <c r="J8" s="401"/>
+      <c r="K8" s="401"/>
+      <c r="L8" s="401"/>
+      <c r="M8" s="401"/>
+      <c r="N8" s="401"/>
+      <c r="O8" s="401"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
@@ -32351,12 +32360,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J9" s="399"/>
-      <c r="K9" s="399"/>
-      <c r="L9" s="399"/>
-      <c r="M9" s="399"/>
-      <c r="N9" s="399"/>
-      <c r="O9" s="399"/>
+      <c r="J9" s="401"/>
+      <c r="K9" s="401"/>
+      <c r="L9" s="401"/>
+      <c r="M9" s="401"/>
+      <c r="N9" s="401"/>
+      <c r="O9" s="401"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="242" t="s">
@@ -32383,12 +32392,12 @@
       <c r="H10" s="241">
         <v>1.5475000000000001</v>
       </c>
-      <c r="J10" s="399"/>
-      <c r="K10" s="399"/>
-      <c r="L10" s="399"/>
-      <c r="M10" s="399"/>
-      <c r="N10" s="399"/>
-      <c r="O10" s="399"/>
+      <c r="J10" s="401"/>
+      <c r="K10" s="401"/>
+      <c r="L10" s="401"/>
+      <c r="M10" s="401"/>
+      <c r="N10" s="401"/>
+      <c r="O10" s="401"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="242" t="s">
@@ -32416,12 +32425,12 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J11" s="399"/>
-      <c r="K11" s="399"/>
-      <c r="L11" s="399"/>
-      <c r="M11" s="399"/>
-      <c r="N11" s="399"/>
-      <c r="O11" s="399"/>
+      <c r="J11" s="401"/>
+      <c r="K11" s="401"/>
+      <c r="L11" s="401"/>
+      <c r="M11" s="401"/>
+      <c r="N11" s="401"/>
+      <c r="O11" s="401"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="242" t="s">
@@ -32448,12 +32457,12 @@
       <c r="H12" s="241">
         <v>1.5475000000000001</v>
       </c>
-      <c r="J12" s="399"/>
-      <c r="K12" s="399"/>
-      <c r="L12" s="399"/>
-      <c r="M12" s="399"/>
-      <c r="N12" s="399"/>
-      <c r="O12" s="399"/>
+      <c r="J12" s="401"/>
+      <c r="K12" s="401"/>
+      <c r="L12" s="401"/>
+      <c r="M12" s="401"/>
+      <c r="N12" s="401"/>
+      <c r="O12" s="401"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="245" t="s">
@@ -35626,7 +35635,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="16" thickBot="1">
+    <row r="129" spans="1:9" ht="16" thickBot="1">
       <c r="A129" s="241" t="s">
         <v>92</v>
       </c>
@@ -35649,10 +35658,13 @@
         <v>0</v>
       </c>
       <c r="H129" s="344">
-        <v>2.9247662337662339</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="16" thickTop="1">
+        <v>3.13</v>
+      </c>
+      <c r="I129" s="242" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="16" thickTop="1">
       <c r="A130" s="344" t="s">
         <v>94</v>
       </c>
@@ -35679,7 +35691,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:9">
       <c r="A131" s="245" t="s">
         <v>94</v>
       </c>
@@ -35705,7 +35717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:9">
       <c r="A132" s="341" t="s">
         <v>659</v>
       </c>
@@ -35732,7 +35744,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="16" thickBot="1">
+    <row r="133" spans="1:9" ht="16" thickBot="1">
       <c r="A133" s="350" t="s">
         <v>659</v>
       </c>
@@ -35759,7 +35771,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="16" thickTop="1">
+    <row r="134" spans="1:9" ht="16" thickTop="1">
       <c r="A134" s="357" t="s">
         <v>660</v>
       </c>
@@ -35786,7 +35798,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="16" thickBot="1">
+    <row r="135" spans="1:9" ht="16" thickBot="1">
       <c r="A135" s="357" t="s">
         <v>660</v>
       </c>
@@ -35813,7 +35825,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="16" thickTop="1">
+    <row r="136" spans="1:9" ht="16" thickTop="1">
       <c r="A136" s="344" t="s">
         <v>661</v>
       </c>
@@ -35840,7 +35852,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:9">
       <c r="A137" s="357" t="s">
         <v>662</v>
       </c>
@@ -35867,7 +35879,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:9">
       <c r="A138" s="344" t="s">
         <v>98</v>
       </c>
@@ -35894,7 +35906,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:9">
       <c r="A139" s="245" t="s">
         <v>98</v>
       </c>
@@ -35920,7 +35932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:9">
       <c r="A140" s="245" t="s">
         <v>99</v>
       </c>
@@ -35947,7 +35959,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:9">
       <c r="A141" s="241" t="s">
         <v>99</v>
       </c>
@@ -35973,7 +35985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:9">
       <c r="A142" s="341" t="s">
         <v>100</v>
       </c>
@@ -36000,7 +36012,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:9">
       <c r="A143" s="344" t="s">
         <v>100</v>
       </c>
@@ -36026,7 +36038,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:9">
       <c r="A144" s="344" t="s">
         <v>102</v>
       </c>
@@ -38814,10 +38826,10 @@
         <v>0.20204467282352942</v>
       </c>
       <c r="H246" s="242">
-        <v>3.18</v>
+        <v>5.41</v>
       </c>
       <c r="I246" s="244" t="s">
-        <v>101</v>
+        <v>669</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -38870,10 +38882,10 @@
         <v>0.20204467282352942</v>
       </c>
       <c r="H248" s="242">
-        <v>0</v>
+        <v>5.41</v>
       </c>
       <c r="I248" s="244" t="s">
-        <v>34</v>
+        <v>669</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -39527,7 +39539,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:9">
       <c r="A273" s="344" t="s">
         <v>175</v>
       </c>
@@ -39553,7 +39565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:9">
       <c r="A274" s="242" t="s">
         <v>176</v>
       </c>
@@ -39580,7 +39592,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="16" thickBot="1">
+    <row r="275" spans="1:9" ht="16" thickBot="1">
       <c r="A275" t="s">
         <v>176</v>
       </c>
@@ -39602,11 +39614,14 @@
       <c r="G275" s="351">
         <v>5.4073625082268911E-4</v>
       </c>
-      <c r="H275" s="344">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" ht="16" thickTop="1">
+      <c r="H275" s="242">
+        <v>2.46</v>
+      </c>
+      <c r="I275" s="244" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" ht="16" thickTop="1">
       <c r="A276" s="242" t="s">
         <v>177</v>
       </c>
@@ -39633,688 +39648,699 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:9" ht="16" thickBot="1">
       <c r="A277" s="242" t="s">
+        <v>177</v>
+      </c>
+      <c r="B277" s="242" t="s">
+        <v>101</v>
+      </c>
+      <c r="C277" s="351">
+        <v>0</v>
+      </c>
+      <c r="D277" s="351">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E277" s="351">
+        <v>0.1043118553695388</v>
+      </c>
+      <c r="F277" s="351">
+        <v>0.34785054261852177</v>
+      </c>
+      <c r="G277" s="351">
+        <v>5.4073625082268911E-4</v>
+      </c>
+      <c r="H277" s="242">
+        <v>2.46</v>
+      </c>
+      <c r="I277" s="244" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" ht="16" thickTop="1">
+      <c r="A278" s="242" t="s">
         <v>178</v>
       </c>
-      <c r="B277" s="344" t="s">
+      <c r="B278" s="344" t="s">
         <v>34</v>
       </c>
-      <c r="C277" s="344">
-        <v>0</v>
-      </c>
-      <c r="D277" s="344">
+      <c r="C278" s="344">
+        <v>0</v>
+      </c>
+      <c r="D278" s="344">
         <v>2.091053467443091E-3</v>
       </c>
-      <c r="E277" s="344">
-        <v>0</v>
-      </c>
-      <c r="F277" s="344">
+      <c r="E278" s="344">
+        <v>0</v>
+      </c>
+      <c r="F278" s="344">
         <v>3.8935944944415032E-2</v>
       </c>
-      <c r="G277" s="344">
+      <c r="G278" s="344">
         <v>5.2938062466913714E-4</v>
       </c>
-      <c r="H277" s="239" t="e">
+      <c r="H278" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="278" spans="1:8" ht="16" thickBot="1">
-      <c r="A278" s="242" t="s">
+    <row r="279" spans="1:9" ht="16" thickBot="1">
+      <c r="A279" s="242" t="s">
         <v>178</v>
       </c>
-      <c r="B278" s="242" t="s">
+      <c r="B279" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="C278" s="351">
-        <v>0</v>
-      </c>
-      <c r="D278" s="351">
+      <c r="C279" s="351">
+        <v>0</v>
+      </c>
+      <c r="D279" s="351">
         <v>2.4E-2</v>
       </c>
-      <c r="E278" s="351">
+      <c r="E279" s="351">
         <v>0.1043118553695388</v>
       </c>
-      <c r="F278" s="351">
+      <c r="F279" s="351">
         <v>0.34785054261852177</v>
       </c>
-      <c r="G278" s="351">
+      <c r="G279" s="351">
         <v>5.4073625082268911E-4</v>
       </c>
-      <c r="H278" s="344">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="279" spans="1:8" ht="16" thickTop="1">
-      <c r="A279" s="242" t="s">
+      <c r="H279" s="242">
+        <v>2.46</v>
+      </c>
+      <c r="I279" s="244" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" ht="16" thickTop="1">
+      <c r="A280" s="242" t="s">
         <v>592</v>
       </c>
-      <c r="B279" s="345" t="s">
+      <c r="B280" s="345" t="s">
         <v>34</v>
       </c>
-      <c r="C279" s="345">
-        <v>0</v>
-      </c>
-      <c r="D279" s="345">
+      <c r="C280" s="345">
+        <v>0</v>
+      </c>
+      <c r="D280" s="345">
         <v>2.091053467443091E-3</v>
       </c>
-      <c r="E279" s="345">
-        <v>0</v>
-      </c>
-      <c r="F279" s="345">
+      <c r="E280" s="345">
+        <v>0</v>
+      </c>
+      <c r="F280" s="345">
         <v>3.8935944944415032E-2</v>
       </c>
-      <c r="G279" s="345">
+      <c r="G280" s="345">
         <v>5.2938062466913714E-4</v>
       </c>
-      <c r="H279" s="239" t="e">
+      <c r="H280" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="16" thickBot="1">
-      <c r="A280" s="242" t="s">
+    <row r="281" spans="1:9" ht="16" thickBot="1">
+      <c r="A281" s="242" t="s">
         <v>592</v>
       </c>
-      <c r="B280" s="242" t="s">
+      <c r="B281" s="242" t="s">
         <v>40</v>
       </c>
-      <c r="C280" s="351">
-        <v>0</v>
-      </c>
-      <c r="D280" s="351">
+      <c r="C281" s="351">
+        <v>0</v>
+      </c>
+      <c r="D281" s="351">
         <v>2.4E-2</v>
       </c>
-      <c r="E280" s="351">
+      <c r="E281" s="351">
         <v>0.1043118553695388</v>
       </c>
-      <c r="F280" s="351">
+      <c r="F281" s="351">
         <v>0.34785054261852177</v>
       </c>
-      <c r="G280" s="351">
+      <c r="G281" s="351">
         <v>5.4073625082268911E-4</v>
       </c>
-      <c r="H280" s="345">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="281" spans="1:8" ht="16" thickTop="1">
-      <c r="A281" s="242" t="s">
+      <c r="H281" s="242">
+        <v>2.46</v>
+      </c>
+      <c r="I281" s="244" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" ht="16" thickTop="1">
+      <c r="A282" s="242" t="s">
         <v>641</v>
       </c>
-      <c r="B281" s="356" t="s">
+      <c r="B282" s="356" t="s">
         <v>34</v>
       </c>
-      <c r="C281" s="356">
-        <v>0</v>
-      </c>
-      <c r="D281" s="356">
+      <c r="C282" s="356">
+        <v>0</v>
+      </c>
+      <c r="D282" s="356">
         <v>2.091053467443091E-3</v>
       </c>
-      <c r="E281" s="356">
-        <v>0</v>
-      </c>
-      <c r="F281" s="356">
+      <c r="E282" s="356">
+        <v>0</v>
+      </c>
+      <c r="F282" s="356">
         <v>3.8935944944415032E-2</v>
       </c>
-      <c r="G281" s="356">
+      <c r="G282" s="356">
         <v>5.2938062466913714E-4</v>
       </c>
-      <c r="H281" s="239" t="e">
+      <c r="H282" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="16" thickBot="1">
-      <c r="A282" s="242" t="s">
+    <row r="283" spans="1:9" ht="16" thickBot="1">
+      <c r="A283" s="242" t="s">
         <v>641</v>
       </c>
-      <c r="B282" s="242" t="s">
+      <c r="B283" s="242" t="s">
         <v>40</v>
       </c>
-      <c r="C282" s="351">
-        <v>0</v>
-      </c>
-      <c r="D282" s="351">
+      <c r="C283" s="351">
+        <v>0</v>
+      </c>
+      <c r="D283" s="351">
         <v>2.4E-2</v>
       </c>
-      <c r="E282" s="351">
+      <c r="E283" s="351">
         <v>0.1043118553695388</v>
       </c>
-      <c r="F282" s="351">
+      <c r="F283" s="351">
         <v>0.34785054261852177</v>
       </c>
-      <c r="G282" s="351">
+      <c r="G283" s="351">
         <v>5.4073625082268911E-4</v>
       </c>
-      <c r="H282" s="356">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="283" spans="1:8" ht="16" thickTop="1">
-      <c r="A283" s="341" t="s">
+      <c r="H283" s="242">
+        <v>2.46</v>
+      </c>
+      <c r="I283" s="244" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" ht="16" thickTop="1">
+      <c r="A284" s="341" t="s">
         <v>642</v>
       </c>
-      <c r="B283" s="344" t="s">
+      <c r="B284" s="344" t="s">
         <v>34</v>
       </c>
-      <c r="C283" s="344">
+      <c r="C284" s="344">
         <v>2.9418934495912281E-2</v>
       </c>
-      <c r="D283" s="344">
+      <c r="D284" s="344">
         <v>2.3225474602036008E-3</v>
       </c>
-      <c r="E283" s="344">
-        <v>0</v>
-      </c>
-      <c r="F283" s="344">
+      <c r="E284" s="344">
+        <v>0</v>
+      </c>
+      <c r="F284" s="344">
         <v>9.5224445868347635E-2</v>
       </c>
-      <c r="G283" s="344">
+      <c r="G284" s="344">
         <v>1.46234469716523E-2</v>
       </c>
-      <c r="H283" s="239" t="e">
+      <c r="H284" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
-      <c r="A284" s="341" t="s">
+    <row r="285" spans="1:9">
+      <c r="A285" s="341" t="s">
         <v>642</v>
       </c>
-      <c r="B284" s="344" t="s">
+      <c r="B285" s="344" t="s">
         <v>96</v>
       </c>
-      <c r="C284" s="344">
-        <v>0</v>
-      </c>
-      <c r="D284" s="344">
+      <c r="C285" s="344">
+        <v>0</v>
+      </c>
+      <c r="D285" s="344">
         <v>3.6309221840068781E-2</v>
       </c>
-      <c r="E284" s="344">
+      <c r="E285" s="344">
         <v>0.38728245693459468</v>
       </c>
-      <c r="F284" s="344">
+      <c r="F285" s="344">
         <v>0.45553418414651931</v>
       </c>
-      <c r="G284" s="344">
+      <c r="G285" s="344">
         <v>3.76594460237053E-3</v>
       </c>
-      <c r="H284" s="344">
+      <c r="H285" s="344">
         <v>0.98</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
-      <c r="A285" s="341" t="s">
+    <row r="286" spans="1:9">
+      <c r="A286" s="341" t="s">
         <v>179</v>
       </c>
-      <c r="B285" s="344" t="s">
+      <c r="B286" s="344" t="s">
         <v>34</v>
       </c>
-      <c r="C285" s="344">
-        <v>0</v>
-      </c>
-      <c r="D285" s="344">
+      <c r="C286" s="344">
+        <v>0</v>
+      </c>
+      <c r="D286" s="344">
         <v>2.8869327032891401E-3</v>
       </c>
-      <c r="E285" s="344">
+      <c r="E286" s="344">
         <v>6.9767540329487548E-3</v>
       </c>
-      <c r="F285" s="344">
+      <c r="F286" s="344">
         <v>0.14025681383479741</v>
       </c>
-      <c r="G285" s="344">
-        <v>0</v>
-      </c>
-      <c r="H285" s="239" t="e">
+      <c r="G286" s="344">
+        <v>0</v>
+      </c>
+      <c r="H286" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
-      <c r="A286" s="241" t="s">
+    <row r="287" spans="1:9">
+      <c r="A287" s="241" t="s">
         <v>179</v>
       </c>
-      <c r="B286" s="344" t="s">
+      <c r="B287" s="344" t="s">
         <v>40</v>
       </c>
-      <c r="C286" s="344">
-        <v>0</v>
-      </c>
-      <c r="D286" s="344">
-        <v>0</v>
-      </c>
-      <c r="E286" s="344">
+      <c r="C287" s="344">
+        <v>0</v>
+      </c>
+      <c r="D287" s="344">
+        <v>0</v>
+      </c>
+      <c r="E287" s="344">
         <v>6.8719491907401564E-2</v>
       </c>
-      <c r="F286" s="344">
+      <c r="F287" s="344">
         <v>0.13972835910523251</v>
       </c>
-      <c r="G286" s="344">
-        <v>0</v>
-      </c>
-      <c r="H286" s="344">
+      <c r="G287" s="344">
+        <v>0</v>
+      </c>
+      <c r="H287" s="344">
         <v>0.98</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
-      <c r="A287" s="341" t="s">
+    <row r="288" spans="1:9">
+      <c r="A288" s="341" t="s">
         <v>180</v>
       </c>
-      <c r="B287" s="341" t="s">
+      <c r="B288" s="341" t="s">
         <v>34</v>
       </c>
-      <c r="C287" s="341">
-        <v>0</v>
-      </c>
-      <c r="D287" s="341">
+      <c r="C288" s="341">
+        <v>0</v>
+      </c>
+      <c r="D288" s="341">
         <v>2.8783650886296582E-3</v>
       </c>
-      <c r="E287" s="341">
+      <c r="E288" s="341">
         <v>1.471164378632937E-2</v>
       </c>
-      <c r="F287" s="341">
+      <c r="F288" s="341">
         <v>0.17813881715185781</v>
       </c>
-      <c r="G287" s="341">
-        <v>0</v>
-      </c>
-      <c r="H287" s="239" t="e">
+      <c r="G288" s="341">
+        <v>0</v>
+      </c>
+      <c r="H288" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
-      <c r="A288" s="241" t="s">
+    <row r="289" spans="1:8">
+      <c r="A289" s="241" t="s">
         <v>180</v>
       </c>
-      <c r="B288" s="341" t="s">
+      <c r="B289" s="341" t="s">
         <v>40</v>
       </c>
-      <c r="C288" s="341">
-        <v>0</v>
-      </c>
-      <c r="D288" s="341">
-        <v>0</v>
-      </c>
-      <c r="E288" s="341">
+      <c r="C289" s="341">
+        <v>0</v>
+      </c>
+      <c r="D289" s="341">
+        <v>0</v>
+      </c>
+      <c r="E289" s="341">
         <v>7.2062562312362036E-2</v>
       </c>
-      <c r="F288" s="341">
+      <c r="F289" s="341">
         <v>0.14036746238821499</v>
       </c>
-      <c r="G288" s="341">
-        <v>0</v>
-      </c>
-      <c r="H288" s="341">
+      <c r="G289" s="341">
+        <v>0</v>
+      </c>
+      <c r="H289" s="341">
         <v>0.98</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
-      <c r="A289" s="344" t="s">
+    <row r="290" spans="1:8">
+      <c r="A290" s="344" t="s">
         <v>595</v>
       </c>
-      <c r="B289" s="341" t="s">
+      <c r="B290" s="341" t="s">
         <v>34</v>
       </c>
-      <c r="C289" s="341">
-        <v>0</v>
-      </c>
-      <c r="D289" s="341">
+      <c r="C290" s="341">
+        <v>0</v>
+      </c>
+      <c r="D290" s="341">
         <v>3.331904362849717E-3</v>
       </c>
-      <c r="E289" s="341">
+      <c r="E290" s="341">
         <v>2.7571508602581399E-2</v>
       </c>
-      <c r="F289" s="341">
+      <c r="F290" s="341">
         <v>0.18716972758308281</v>
       </c>
-      <c r="G289" s="341">
-        <v>0</v>
-      </c>
-      <c r="H289" s="239" t="e">
+      <c r="G290" s="341">
+        <v>0</v>
+      </c>
+      <c r="H290" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="290" spans="1:8" ht="16" thickBot="1">
-      <c r="A290" s="341" t="s">
+    <row r="291" spans="1:8" ht="16" thickBot="1">
+      <c r="A291" s="341" t="s">
         <v>595</v>
       </c>
-      <c r="B290" s="341" t="s">
+      <c r="B291" s="341" t="s">
         <v>40</v>
       </c>
-      <c r="C290" s="341">
-        <v>0</v>
-      </c>
-      <c r="D290" s="341">
+      <c r="C291" s="341">
+        <v>0</v>
+      </c>
+      <c r="D291" s="341">
         <v>2.2985845129059119E-2</v>
       </c>
-      <c r="E290" s="351">
+      <c r="E291" s="351">
         <v>0.191</v>
       </c>
-      <c r="F290" s="341">
+      <c r="F291" s="341">
         <v>0.28644316422220162</v>
       </c>
-      <c r="G290" s="341">
-        <v>0</v>
-      </c>
-      <c r="H290" s="341">
+      <c r="G291" s="341">
+        <v>0</v>
+      </c>
+      <c r="H291" s="341">
         <v>0.98</v>
       </c>
     </row>
-    <row r="291" spans="1:8" ht="16" thickTop="1">
-      <c r="A291" s="345" t="s">
-        <v>596</v>
-      </c>
-      <c r="B291" s="345" t="s">
-        <v>34</v>
-      </c>
-      <c r="C291" s="345">
-        <v>0</v>
-      </c>
-      <c r="D291" s="345">
-        <v>3.331904362849717E-3</v>
-      </c>
-      <c r="E291" s="345">
-        <v>2.7571508602581399E-2</v>
-      </c>
-      <c r="F291" s="345">
-        <v>0.18716972758308281</v>
-      </c>
-      <c r="G291" s="345">
-        <v>0</v>
-      </c>
-      <c r="H291" s="345"/>
-    </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" ht="16" thickTop="1">
       <c r="A292" s="345" t="s">
         <v>596</v>
       </c>
       <c r="B292" s="345" t="s">
+        <v>34</v>
+      </c>
+      <c r="C292" s="345">
+        <v>0</v>
+      </c>
+      <c r="D292" s="345">
+        <v>3.331904362849717E-3</v>
+      </c>
+      <c r="E292" s="345">
+        <v>2.7571508602581399E-2</v>
+      </c>
+      <c r="F292" s="345">
+        <v>0.18716972758308281</v>
+      </c>
+      <c r="G292" s="345">
+        <v>0</v>
+      </c>
+      <c r="H292" s="345"/>
+    </row>
+    <row r="293" spans="1:8">
+      <c r="A293" s="345" t="s">
+        <v>596</v>
+      </c>
+      <c r="B293" s="345" t="s">
         <v>40</v>
       </c>
-      <c r="C292" s="345">
-        <v>0</v>
-      </c>
-      <c r="D292" s="345">
+      <c r="C293" s="345">
+        <v>0</v>
+      </c>
+      <c r="D293" s="345">
         <v>2.2985845129059119E-2</v>
       </c>
-      <c r="E292" s="345">
+      <c r="E293" s="345">
         <v>0.37025782219610959</v>
       </c>
-      <c r="F292" s="345">
+      <c r="F293" s="345">
         <v>0.28644316422220162</v>
       </c>
-      <c r="G292" s="345">
-        <v>0</v>
-      </c>
-      <c r="H292" s="345"/>
-    </row>
-    <row r="293" spans="1:8">
-      <c r="A293" s="356" t="s">
-        <v>643</v>
-      </c>
-      <c r="B293" s="356" t="s">
-        <v>34</v>
-      </c>
-      <c r="C293" s="356">
-        <v>0</v>
-      </c>
-      <c r="D293" s="356">
-        <v>3.331904362849717E-3</v>
-      </c>
-      <c r="E293" s="356">
-        <v>2.7571508602581399E-2</v>
-      </c>
-      <c r="F293" s="356">
-        <v>0.18716972758308281</v>
-      </c>
-      <c r="G293" s="356">
-        <v>0</v>
-      </c>
-      <c r="H293" s="356"/>
+      <c r="G293" s="345">
+        <v>0</v>
+      </c>
+      <c r="H293" s="345"/>
     </row>
     <row r="294" spans="1:8">
       <c r="A294" s="356" t="s">
         <v>643</v>
       </c>
       <c r="B294" s="356" t="s">
+        <v>34</v>
+      </c>
+      <c r="C294" s="356">
+        <v>0</v>
+      </c>
+      <c r="D294" s="356">
+        <v>3.331904362849717E-3</v>
+      </c>
+      <c r="E294" s="356">
+        <v>2.7571508602581399E-2</v>
+      </c>
+      <c r="F294" s="356">
+        <v>0.18716972758308281</v>
+      </c>
+      <c r="G294" s="356">
+        <v>0</v>
+      </c>
+      <c r="H294" s="356"/>
+    </row>
+    <row r="295" spans="1:8">
+      <c r="A295" s="356" t="s">
+        <v>643</v>
+      </c>
+      <c r="B295" s="356" t="s">
         <v>40</v>
       </c>
-      <c r="C294" s="356">
-        <v>0</v>
-      </c>
-      <c r="D294" s="356">
+      <c r="C295" s="356">
+        <v>0</v>
+      </c>
+      <c r="D295" s="356">
         <v>2.2985845129059119E-2</v>
       </c>
-      <c r="E294" s="356">
+      <c r="E295" s="356">
         <v>0.37025782219610959</v>
       </c>
-      <c r="F294" s="356">
+      <c r="F295" s="356">
         <v>0.28644316422220162</v>
       </c>
-      <c r="G294" s="356">
-        <v>0</v>
-      </c>
-      <c r="H294" s="356"/>
-    </row>
-    <row r="295" spans="1:8">
-      <c r="A295" s="242" t="s">
+      <c r="G295" s="356">
+        <v>0</v>
+      </c>
+      <c r="H295" s="356"/>
+    </row>
+    <row r="296" spans="1:8">
+      <c r="A296" s="242" t="s">
         <v>181</v>
       </c>
-      <c r="B295" s="341" t="s">
+      <c r="B296" s="341" t="s">
         <v>46</v>
       </c>
-      <c r="C295" s="344">
-        <v>0</v>
-      </c>
-      <c r="D295" s="344">
+      <c r="C296" s="344">
+        <v>0</v>
+      </c>
+      <c r="D296" s="344">
         <v>2.6742627345844511E-2</v>
       </c>
-      <c r="E295" s="344">
+      <c r="E296" s="344">
         <v>0.14470509383378019</v>
       </c>
-      <c r="F295" s="344">
+      <c r="F296" s="344">
         <v>0.32587131367292232</v>
       </c>
-      <c r="G295" s="344">
-        <v>0</v>
-      </c>
-      <c r="H295" s="239" t="e">
+      <c r="G296" s="344">
+        <v>0</v>
+      </c>
+      <c r="H296" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="296" spans="1:8" ht="16" thickBot="1">
-      <c r="A296" s="242" t="s">
+    <row r="297" spans="1:8" ht="16" thickBot="1">
+      <c r="A297" s="242" t="s">
         <v>181</v>
       </c>
-      <c r="B296" s="242" t="s">
+      <c r="B297" s="242" t="s">
         <v>55</v>
       </c>
-      <c r="C296" s="351">
-        <v>0</v>
-      </c>
-      <c r="D296" s="351">
-        <v>0</v>
-      </c>
-      <c r="E296" s="351">
+      <c r="C297" s="351">
+        <v>0</v>
+      </c>
+      <c r="D297" s="351">
+        <v>0</v>
+      </c>
+      <c r="E297" s="351">
         <v>5.4270871682504683E-2</v>
       </c>
-      <c r="F296" s="351">
+      <c r="F297" s="351">
         <v>0.16823480336025062</v>
       </c>
-      <c r="G296" s="351">
-        <v>0</v>
-      </c>
-      <c r="H296" s="344">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="1:8" ht="16" thickTop="1">
-      <c r="A297" s="242" t="s">
+      <c r="G297" s="351">
+        <v>0</v>
+      </c>
+      <c r="H297" s="344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" ht="16" thickTop="1">
+      <c r="A298" s="242" t="s">
         <v>182</v>
       </c>
-      <c r="B297" s="341" t="s">
+      <c r="B298" s="341" t="s">
         <v>46</v>
       </c>
-      <c r="C297" s="344">
-        <v>0</v>
-      </c>
-      <c r="D297" s="344">
+      <c r="C298" s="344">
+        <v>0</v>
+      </c>
+      <c r="D298" s="344">
         <v>2.6742627345844511E-2</v>
       </c>
-      <c r="E297" s="344">
+      <c r="E298" s="344">
         <v>0.14470509383378019</v>
       </c>
-      <c r="F297" s="344">
+      <c r="F298" s="344">
         <v>0.32587131367292232</v>
       </c>
-      <c r="G297" s="344">
-        <v>0</v>
-      </c>
-      <c r="H297" s="239" t="e">
+      <c r="G298" s="344">
+        <v>0</v>
+      </c>
+      <c r="H298" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="298" spans="1:8" ht="16" thickBot="1">
-      <c r="A298" s="242" t="s">
+    <row r="299" spans="1:8" ht="16" thickBot="1">
+      <c r="A299" s="242" t="s">
         <v>182</v>
       </c>
-      <c r="B298" s="242" t="s">
+      <c r="B299" s="242" t="s">
         <v>50</v>
       </c>
-      <c r="C298" s="351">
-        <v>0</v>
-      </c>
-      <c r="D298" s="351">
-        <v>0</v>
-      </c>
-      <c r="E298" s="351">
+      <c r="C299" s="351">
+        <v>0</v>
+      </c>
+      <c r="D299" s="351">
+        <v>0</v>
+      </c>
+      <c r="E299" s="351">
         <v>5.4270871682504683E-2</v>
       </c>
-      <c r="F298" s="351">
+      <c r="F299" s="351">
         <v>0.16823480336025062</v>
       </c>
-      <c r="G298" s="351">
-        <v>0</v>
-      </c>
-      <c r="H298" s="344">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="1:8" ht="16" thickTop="1">
-      <c r="A299" s="344" t="s">
+      <c r="G299" s="351">
+        <v>0</v>
+      </c>
+      <c r="H299" s="344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" ht="16" thickTop="1">
+      <c r="A300" s="344" t="s">
         <v>183</v>
       </c>
-      <c r="B299" s="341" t="s">
+      <c r="B300" s="341" t="s">
         <v>46</v>
       </c>
-      <c r="C299" s="344">
-        <v>0</v>
-      </c>
-      <c r="D299" s="344">
+      <c r="C300" s="344">
+        <v>0</v>
+      </c>
+      <c r="D300" s="344">
         <v>6.0244744273611544E-3</v>
       </c>
-      <c r="E299" s="344">
+      <c r="E300" s="344">
         <v>0.1243175400062755</v>
       </c>
-      <c r="F299" s="344">
+      <c r="F300" s="344">
         <v>0.23649199874490121</v>
       </c>
-      <c r="G299" s="344">
-        <v>0</v>
-      </c>
-      <c r="H299" s="239" t="e">
+      <c r="G300" s="344">
+        <v>0</v>
+      </c>
+      <c r="H300" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="300" spans="1:8" ht="16" thickBot="1">
-      <c r="A300" s="344" t="s">
+    <row r="301" spans="1:8" ht="16" thickBot="1">
+      <c r="A301" s="344" t="s">
         <v>183</v>
-      </c>
-      <c r="B300" s="341" t="s">
-        <v>55</v>
-      </c>
-      <c r="C300" s="351">
-        <v>0</v>
-      </c>
-      <c r="D300" s="351">
-        <v>0</v>
-      </c>
-      <c r="E300" s="351">
-        <v>4.0740116165041071E-3</v>
-      </c>
-      <c r="F300" s="351">
-        <v>9.7211110476117912E-2</v>
-      </c>
-      <c r="G300" s="351">
-        <v>0</v>
-      </c>
-      <c r="H300" s="344">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="1:8" ht="16" thickTop="1">
-      <c r="A301" s="344" t="s">
-        <v>372</v>
       </c>
       <c r="B301" s="341" t="s">
         <v>55</v>
       </c>
-      <c r="C301" s="344">
-        <v>0</v>
-      </c>
-      <c r="D301" s="344">
+      <c r="C301" s="351">
+        <v>0</v>
+      </c>
+      <c r="D301" s="351">
+        <v>0</v>
+      </c>
+      <c r="E301" s="351">
+        <v>4.0740116165041071E-3</v>
+      </c>
+      <c r="F301" s="351">
+        <v>9.7211110476117912E-2</v>
+      </c>
+      <c r="G301" s="351">
+        <v>0</v>
+      </c>
+      <c r="H301" s="344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" ht="16" thickTop="1">
+      <c r="A302" s="344" t="s">
+        <v>372</v>
+      </c>
+      <c r="B302" s="341" t="s">
+        <v>55</v>
+      </c>
+      <c r="C302" s="344">
+        <v>0</v>
+      </c>
+      <c r="D302" s="344">
         <v>9.8659793814432989E-2</v>
       </c>
-      <c r="E301" s="344">
+      <c r="E302" s="344">
         <v>0.43114723696141771</v>
       </c>
-      <c r="F301" s="344">
+      <c r="F302" s="344">
         <v>0.53576951114463867</v>
       </c>
-      <c r="G301" s="344">
-        <v>0</v>
-      </c>
-      <c r="H301" s="344">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="1:8">
-      <c r="A302" s="344" t="s">
-        <v>184</v>
-      </c>
-      <c r="B302" s="341" t="s">
-        <v>46</v>
-      </c>
-      <c r="C302" s="344">
-        <v>0</v>
-      </c>
-      <c r="D302" s="344">
-        <v>3.4838709677419361E-3</v>
-      </c>
-      <c r="E302" s="344">
-        <v>0.16425806451612901</v>
-      </c>
-      <c r="F302" s="344">
-        <v>0.22993548387096771</v>
-      </c>
       <c r="G302" s="344">
         <v>0</v>
       </c>
-      <c r="H302" s="239" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="H302" s="344">
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:8">
       <c r="A303" s="344" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B303" s="341" t="s">
         <v>46</v>
@@ -40323,13 +40349,13 @@
         <v>0</v>
       </c>
       <c r="D303" s="344">
-        <v>2.0517464424320831E-2</v>
+        <v>3.4838709677419361E-3</v>
       </c>
       <c r="E303" s="344">
-        <v>0.15777490297542041</v>
+        <v>0.16425806451612901</v>
       </c>
       <c r="F303" s="344">
-        <v>0.27534282018111261</v>
+        <v>0.22993548387096771</v>
       </c>
       <c r="G303" s="344">
         <v>0</v>
@@ -40339,62 +40365,62 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="304" spans="1:8" ht="16" thickBot="1">
+    <row r="304" spans="1:8">
       <c r="A304" s="344" t="s">
         <v>185</v>
       </c>
       <c r="B304" s="341" t="s">
-        <v>55</v>
-      </c>
-      <c r="C304" s="351">
-        <v>0</v>
-      </c>
-      <c r="D304" s="351">
-        <v>0</v>
-      </c>
-      <c r="E304" s="351">
-        <v>0</v>
-      </c>
-      <c r="F304" s="351">
-        <v>4.7434164902525687E-2</v>
-      </c>
-      <c r="G304" s="351">
-        <v>0</v>
-      </c>
-      <c r="H304" s="344">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" spans="1:8" ht="16" thickTop="1">
-      <c r="A305" s="344" t="s">
-        <v>186</v>
-      </c>
-      <c r="B305" s="344" t="s">
         <v>46</v>
       </c>
-      <c r="C305" s="341">
-        <v>0</v>
-      </c>
-      <c r="D305" s="341">
-        <v>1.834002677376171E-2</v>
-      </c>
-      <c r="E305" s="341">
-        <v>0.31981258366800541</v>
-      </c>
-      <c r="F305" s="341">
-        <v>0.38915662650602412</v>
-      </c>
-      <c r="G305" s="341">
-        <v>9.3708165997322633E-4</v>
-      </c>
-      <c r="H305" s="239" t="e">
+      <c r="C304" s="344">
+        <v>0</v>
+      </c>
+      <c r="D304" s="344">
+        <v>2.0517464424320831E-2</v>
+      </c>
+      <c r="E304" s="344">
+        <v>0.15777490297542041</v>
+      </c>
+      <c r="F304" s="344">
+        <v>0.27534282018111261</v>
+      </c>
+      <c r="G304" s="344">
+        <v>0</v>
+      </c>
+      <c r="H304" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="305" spans="1:8" ht="16" thickBot="1">
+      <c r="A305" s="344" t="s">
+        <v>185</v>
+      </c>
+      <c r="B305" s="341" t="s">
+        <v>55</v>
+      </c>
+      <c r="C305" s="351">
+        <v>0</v>
+      </c>
+      <c r="D305" s="351">
+        <v>0</v>
+      </c>
+      <c r="E305" s="351">
+        <v>0</v>
+      </c>
+      <c r="F305" s="351">
+        <v>4.7434164902525687E-2</v>
+      </c>
+      <c r="G305" s="351">
+        <v>0</v>
+      </c>
+      <c r="H305" s="344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" ht="16" thickTop="1">
       <c r="A306" s="344" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B306" s="344" t="s">
         <v>46</v>
@@ -40403,16 +40429,16 @@
         <v>0</v>
       </c>
       <c r="D306" s="341">
-        <v>2.093821510297483E-2</v>
+        <v>1.834002677376171E-2</v>
       </c>
       <c r="E306" s="341">
-        <v>0.37471395881006858</v>
+        <v>0.31981258366800541</v>
       </c>
       <c r="F306" s="341">
-        <v>0.4003432494279176</v>
+        <v>0.38915662650602412</v>
       </c>
       <c r="G306" s="341">
-        <v>1.3729977116704809E-3</v>
+        <v>9.3708165997322633E-4</v>
       </c>
       <c r="H306" s="239" t="e">
         <f>NA()</f>
@@ -40421,25 +40447,25 @@
     </row>
     <row r="307" spans="1:8">
       <c r="A307" s="344" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B307" s="344" t="s">
-        <v>38</v>
-      </c>
-      <c r="C307" s="245">
-        <v>0</v>
-      </c>
-      <c r="D307" s="245">
-        <v>0.13839009287925699</v>
-      </c>
-      <c r="E307" s="245">
-        <v>0.1268730650154799</v>
-      </c>
-      <c r="F307" s="245">
-        <v>0.55999999999999994</v>
-      </c>
-      <c r="G307" s="245">
-        <v>1.5479876160990711E-3</v>
+        <v>46</v>
+      </c>
+      <c r="C307" s="341">
+        <v>0</v>
+      </c>
+      <c r="D307" s="341">
+        <v>2.093821510297483E-2</v>
+      </c>
+      <c r="E307" s="341">
+        <v>0.37471395881006858</v>
+      </c>
+      <c r="F307" s="341">
+        <v>0.4003432494279176</v>
+      </c>
+      <c r="G307" s="341">
+        <v>1.3729977116704809E-3</v>
       </c>
       <c r="H307" s="239" t="e">
         <f>NA()</f>
@@ -40448,7 +40474,7 @@
     </row>
     <row r="308" spans="1:8">
       <c r="A308" s="344" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B308" s="344" t="s">
         <v>38</v>
@@ -40457,16 +40483,16 @@
         <v>0</v>
       </c>
       <c r="D308" s="245">
-        <v>0</v>
+        <v>0.13839009287925699</v>
       </c>
       <c r="E308" s="245">
-        <v>2.6041666666666661E-2</v>
+        <v>0.1268730650154799</v>
       </c>
       <c r="F308" s="245">
-        <v>0.16770833333333329</v>
+        <v>0.55999999999999994</v>
       </c>
       <c r="G308" s="245">
-        <v>0</v>
+        <v>1.5479876160990711E-3</v>
       </c>
       <c r="H308" s="239" t="e">
         <f>NA()</f>
@@ -40475,25 +40501,25 @@
     </row>
     <row r="309" spans="1:8">
       <c r="A309" s="344" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B309" s="344" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C309" s="245">
-        <v>0.33217592592592587</v>
+        <v>0</v>
       </c>
       <c r="D309" s="245">
-        <v>0.16423611111111111</v>
+        <v>0</v>
       </c>
       <c r="E309" s="245">
-        <v>0.1938657407407407</v>
+        <v>2.6041666666666661E-2</v>
       </c>
       <c r="F309" s="245">
-        <v>0.390625</v>
+        <v>0.16770833333333329</v>
       </c>
       <c r="G309" s="245">
-        <v>0.17743055555555551</v>
+        <v>0</v>
       </c>
       <c r="H309" s="239" t="e">
         <f>NA()</f>
@@ -40502,25 +40528,25 @@
     </row>
     <row r="310" spans="1:8">
       <c r="A310" s="344" t="s">
-        <v>191</v>
-      </c>
-      <c r="B310" s="245" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+      <c r="B310" s="344" t="s">
+        <v>46</v>
       </c>
       <c r="C310" s="245">
-        <v>0</v>
+        <v>0.33217592592592587</v>
       </c>
       <c r="D310" s="245">
-        <v>4.3718592964824117E-2</v>
+        <v>0.16423611111111111</v>
       </c>
       <c r="E310" s="245">
-        <v>9.0954773869346736E-2</v>
+        <v>0.1938657407407407</v>
       </c>
       <c r="F310" s="245">
-        <v>0.29798994974874371</v>
+        <v>0.390625</v>
       </c>
       <c r="G310" s="245">
-        <v>0</v>
+        <v>0.17743055555555551</v>
       </c>
       <c r="H310" s="239" t="e">
         <f>NA()</f>
@@ -40529,25 +40555,25 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" s="344" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B311" s="245" t="s">
-        <v>46</v>
-      </c>
-      <c r="C311" s="341">
-        <v>0</v>
-      </c>
-      <c r="D311" s="341">
-        <v>0.19696969696969699</v>
-      </c>
-      <c r="E311" s="341">
-        <v>0.31767676767676772</v>
-      </c>
-      <c r="F311" s="341">
-        <v>0.51464646464646457</v>
-      </c>
-      <c r="G311" s="341">
-        <v>4.0404040404040404E-3</v>
+        <v>192</v>
+      </c>
+      <c r="C311" s="245">
+        <v>0</v>
+      </c>
+      <c r="D311" s="245">
+        <v>4.3718592964824117E-2</v>
+      </c>
+      <c r="E311" s="245">
+        <v>9.0954773869346736E-2</v>
+      </c>
+      <c r="F311" s="245">
+        <v>0.29798994974874371</v>
+      </c>
+      <c r="G311" s="245">
+        <v>0</v>
       </c>
       <c r="H311" s="239" t="e">
         <f>NA()</f>
@@ -40556,25 +40582,25 @@
     </row>
     <row r="312" spans="1:8">
       <c r="A312" s="344" t="s">
-        <v>194</v>
-      </c>
-      <c r="B312" s="338" t="s">
+        <v>193</v>
+      </c>
+      <c r="B312" s="245" t="s">
         <v>46</v>
       </c>
       <c r="C312" s="341">
-        <v>0.36257183908045981</v>
+        <v>0</v>
       </c>
       <c r="D312" s="341">
-        <v>0.25474137931034491</v>
+        <v>0.19696969696969699</v>
       </c>
       <c r="E312" s="341">
-        <v>0.32090517241379313</v>
+        <v>0.31767676767676772</v>
       </c>
       <c r="F312" s="341">
-        <v>0.50093390804597704</v>
+        <v>0.51464646464646457</v>
       </c>
       <c r="G312" s="341">
-        <v>1.6810344827586209E-2</v>
+        <v>4.0404040404040404E-3</v>
       </c>
       <c r="H312" s="239" t="e">
         <f>NA()</f>
@@ -40585,129 +40611,129 @@
       <c r="A313" s="344" t="s">
         <v>194</v>
       </c>
-      <c r="B313" s="344" t="s">
-        <v>618</v>
-      </c>
-      <c r="C313" s="240">
-        <v>0.25623790594558399</v>
-      </c>
-      <c r="D313" s="240">
-        <v>0.12352982042913541</v>
-      </c>
-      <c r="E313" s="240">
-        <v>0.2179322231694599</v>
-      </c>
-      <c r="F313" s="240">
-        <v>0.37231767594101101</v>
-      </c>
-      <c r="G313" s="240">
-        <v>1.661174476170213E-2</v>
-      </c>
-      <c r="H313" s="241">
-        <v>3.9275000000000002</v>
+      <c r="B313" s="338" t="s">
+        <v>46</v>
+      </c>
+      <c r="C313" s="341">
+        <v>0.36257183908045981</v>
+      </c>
+      <c r="D313" s="341">
+        <v>0.25474137931034491</v>
+      </c>
+      <c r="E313" s="341">
+        <v>0.32090517241379313</v>
+      </c>
+      <c r="F313" s="341">
+        <v>0.50093390804597704</v>
+      </c>
+      <c r="G313" s="341">
+        <v>1.6810344827586209E-2</v>
+      </c>
+      <c r="H313" s="239" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="314" spans="1:8">
       <c r="A314" s="344" t="s">
-        <v>195</v>
-      </c>
-      <c r="B314" s="338" t="s">
-        <v>38</v>
-      </c>
-      <c r="C314" s="341">
-        <v>0.3681141439205956</v>
-      </c>
-      <c r="D314" s="341">
-        <v>0.40446650124069478</v>
-      </c>
-      <c r="E314" s="341">
-        <v>0.14416873449131509</v>
-      </c>
-      <c r="F314" s="341">
-        <v>0.40880893300248139</v>
-      </c>
-      <c r="G314" s="341">
-        <v>5.3598014888337479E-2</v>
-      </c>
-      <c r="H314" s="239" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>194</v>
+      </c>
+      <c r="B314" s="344" t="s">
+        <v>618</v>
+      </c>
+      <c r="C314" s="240">
+        <v>0.25623790594558399</v>
+      </c>
+      <c r="D314" s="240">
+        <v>0.12352982042913541</v>
+      </c>
+      <c r="E314" s="240">
+        <v>0.2179322231694599</v>
+      </c>
+      <c r="F314" s="240">
+        <v>0.37231767594101101</v>
+      </c>
+      <c r="G314" s="240">
+        <v>1.661174476170213E-2</v>
+      </c>
+      <c r="H314" s="241">
+        <v>3.9275000000000002</v>
       </c>
     </row>
     <row r="315" spans="1:8">
       <c r="A315" s="344" t="s">
         <v>195</v>
       </c>
-      <c r="B315" s="344" t="s">
-        <v>619</v>
-      </c>
-      <c r="C315" s="240">
-        <v>0.3072719469000792</v>
-      </c>
-      <c r="D315" s="240">
-        <v>0.21172494337484429</v>
-      </c>
-      <c r="E315" s="240">
-        <v>0.27806274130227687</v>
-      </c>
-      <c r="F315" s="240">
-        <v>0.43337399301630702</v>
-      </c>
-      <c r="G315" s="240">
-        <v>3.1523409983521163E-2</v>
-      </c>
-      <c r="H315" s="241">
-        <v>4.8374999999999986</v>
-      </c>
-    </row>
-    <row r="316" spans="1:8">
-      <c r="A316" s="341" t="s">
-        <v>196</v>
-      </c>
-      <c r="B316" s="338" t="s">
-        <v>192</v>
-      </c>
-      <c r="C316" s="341">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="D316" s="341">
-        <v>5.3249999999999999E-2</v>
-      </c>
-      <c r="E316" s="341">
-        <v>2.1749999999999999E-2</v>
-      </c>
-      <c r="F316" s="341">
-        <v>0.23474999999999999</v>
-      </c>
-      <c r="G316" s="341">
-        <v>0.45450000000000002</v>
-      </c>
-      <c r="H316" s="239" t="e">
+      <c r="B315" s="338" t="s">
+        <v>38</v>
+      </c>
+      <c r="C315" s="341">
+        <v>0.3681141439205956</v>
+      </c>
+      <c r="D315" s="341">
+        <v>0.40446650124069478</v>
+      </c>
+      <c r="E315" s="341">
+        <v>0.14416873449131509</v>
+      </c>
+      <c r="F315" s="341">
+        <v>0.40880893300248139</v>
+      </c>
+      <c r="G315" s="341">
+        <v>5.3598014888337479E-2</v>
+      </c>
+      <c r="H315" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
+    <row r="316" spans="1:8">
+      <c r="A316" s="344" t="s">
+        <v>195</v>
+      </c>
+      <c r="B316" s="344" t="s">
+        <v>619</v>
+      </c>
+      <c r="C316" s="240">
+        <v>0.3072719469000792</v>
+      </c>
+      <c r="D316" s="240">
+        <v>0.21172494337484429</v>
+      </c>
+      <c r="E316" s="240">
+        <v>0.27806274130227687</v>
+      </c>
+      <c r="F316" s="240">
+        <v>0.43337399301630702</v>
+      </c>
+      <c r="G316" s="240">
+        <v>3.1523409983521163E-2</v>
+      </c>
+      <c r="H316" s="241">
+        <v>4.8374999999999986</v>
+      </c>
+    </row>
     <row r="317" spans="1:8">
       <c r="A317" s="341" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B317" s="338" t="s">
         <v>192</v>
       </c>
       <c r="C317" s="341">
-        <v>0.20609137055837559</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D317" s="341">
-        <v>5.3299492385786809E-2</v>
+        <v>5.3249999999999999E-2</v>
       </c>
       <c r="E317" s="341">
-        <v>3.654822335025381E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F317" s="341">
-        <v>0.2517766497461929</v>
+        <v>0.23474999999999999</v>
       </c>
       <c r="G317" s="341">
-        <v>0.31827411167512693</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="H317" s="239" t="e">
         <f>NA()</f>
@@ -40715,90 +40741,90 @@
       </c>
     </row>
     <row r="318" spans="1:8">
-      <c r="A318" s="344" t="s">
-        <v>198</v>
+      <c r="A318" s="341" t="s">
+        <v>197</v>
       </c>
       <c r="B318" s="338" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="C318" s="341">
-        <v>0</v>
+        <v>0.20609137055837559</v>
       </c>
       <c r="D318" s="341">
-        <v>0.14838709677419359</v>
+        <v>5.3299492385786809E-2</v>
       </c>
       <c r="E318" s="341">
-        <v>0.34055299539170508</v>
+        <v>3.654822335025381E-2</v>
       </c>
       <c r="F318" s="341">
-        <v>0.59331797235023043</v>
+        <v>0.2517766497461929</v>
       </c>
       <c r="G318" s="341">
-        <v>4.147465437788018E-3</v>
+        <v>0.31827411167512693</v>
       </c>
       <c r="H318" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="319" spans="1:8" ht="16" thickBot="1">
-      <c r="A319" s="341" t="s">
+    <row r="319" spans="1:8">
+      <c r="A319" s="344" t="s">
         <v>198</v>
       </c>
       <c r="B319" s="338" t="s">
-        <v>46</v>
-      </c>
-      <c r="C319" s="351">
-        <v>0</v>
-      </c>
-      <c r="D319" s="351">
-        <v>0</v>
-      </c>
-      <c r="E319" s="351">
-        <v>0</v>
-      </c>
-      <c r="F319" s="351">
-        <v>3.3587572106361013E-2</v>
-      </c>
-      <c r="G319" s="351">
-        <v>0</v>
-      </c>
-      <c r="H319" s="341">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:8" ht="16" thickTop="1">
-      <c r="A320" s="344" t="s">
-        <v>199</v>
-      </c>
-      <c r="B320" s="341" t="s">
-        <v>192</v>
-      </c>
-      <c r="C320" s="341">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="D320" s="341">
-        <v>5.3249999999999999E-2</v>
-      </c>
-      <c r="E320" s="341">
-        <v>2.1749999999999999E-2</v>
-      </c>
-      <c r="F320" s="341">
-        <v>0.23474999999999999</v>
-      </c>
-      <c r="G320" s="341">
-        <v>0.42449999999999999</v>
-      </c>
-      <c r="H320" s="239" t="e">
+        <v>38</v>
+      </c>
+      <c r="C319" s="341">
+        <v>0</v>
+      </c>
+      <c r="D319" s="341">
+        <v>0.14838709677419359</v>
+      </c>
+      <c r="E319" s="341">
+        <v>0.34055299539170508</v>
+      </c>
+      <c r="F319" s="341">
+        <v>0.59331797235023043</v>
+      </c>
+      <c r="G319" s="341">
+        <v>4.147465437788018E-3</v>
+      </c>
+      <c r="H319" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:20">
-      <c r="A321" s="341" t="s">
-        <v>200</v>
-      </c>
-      <c r="B321" s="338" t="s">
+    <row r="320" spans="1:8" ht="16" thickBot="1">
+      <c r="A320" s="341" t="s">
+        <v>198</v>
+      </c>
+      <c r="B320" s="338" t="s">
+        <v>46</v>
+      </c>
+      <c r="C320" s="351">
+        <v>0</v>
+      </c>
+      <c r="D320" s="351">
+        <v>0</v>
+      </c>
+      <c r="E320" s="351">
+        <v>0</v>
+      </c>
+      <c r="F320" s="351">
+        <v>3.3587572106361013E-2</v>
+      </c>
+      <c r="G320" s="351">
+        <v>0</v>
+      </c>
+      <c r="H320" s="341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:20" ht="16" thickTop="1">
+      <c r="A321" s="344" t="s">
+        <v>199</v>
+      </c>
+      <c r="B321" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C321" s="341">
@@ -40808,13 +40834,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E321" s="341">
-        <v>2.75E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F321" s="341">
         <v>0.23474999999999999</v>
       </c>
       <c r="G321" s="341">
-        <v>0.35349999999999998</v>
+        <v>0.42449999999999999</v>
       </c>
       <c r="H321" s="239" t="e">
         <f>NA()</f>
@@ -40823,9 +40849,9 @@
     </row>
     <row r="322" spans="1:20">
       <c r="A322" s="341" t="s">
-        <v>201</v>
-      </c>
-      <c r="B322" s="341" t="s">
+        <v>200</v>
+      </c>
+      <c r="B322" s="338" t="s">
         <v>192</v>
       </c>
       <c r="C322" s="341">
@@ -40835,13 +40861,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E322" s="341">
-        <v>1.4999999999999999E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F322" s="341">
         <v>0.23474999999999999</v>
       </c>
       <c r="G322" s="341">
-        <v>0.51800000000000002</v>
+        <v>0.35349999999999998</v>
       </c>
       <c r="H322" s="239" t="e">
         <f>NA()</f>
@@ -40850,25 +40876,25 @@
     </row>
     <row r="323" spans="1:20">
       <c r="A323" s="341" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B323" s="341" t="s">
         <v>192</v>
       </c>
-      <c r="C323" s="245">
+      <c r="C323" s="341">
         <v>0.16350000000000001</v>
       </c>
-      <c r="D323" s="245">
+      <c r="D323" s="341">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="E323" s="245">
-        <v>2.75E-2</v>
-      </c>
-      <c r="F323" s="245">
+      <c r="E323" s="341">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F323" s="341">
         <v>0.23474999999999999</v>
       </c>
-      <c r="G323" s="245">
-        <v>0.34675</v>
+      <c r="G323" s="341">
+        <v>0.51800000000000002</v>
       </c>
       <c r="H323" s="239" t="e">
         <f>NA()</f>
@@ -40876,26 +40902,26 @@
       </c>
     </row>
     <row r="324" spans="1:20">
-      <c r="A324" s="344" t="s">
-        <v>203</v>
-      </c>
-      <c r="B324" s="344" t="s">
+      <c r="A324" s="341" t="s">
+        <v>202</v>
+      </c>
+      <c r="B324" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C324" s="245">
-        <v>0.22175</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D324" s="245">
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E324" s="245">
-        <v>4.0999999999999988E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F324" s="245">
-        <v>0.2515</v>
+        <v>0.23474999999999999</v>
       </c>
       <c r="G324" s="245">
-        <v>0.20025000000000001</v>
+        <v>0.34675</v>
       </c>
       <c r="H324" s="239" t="e">
         <f>NA()</f>
@@ -40904,25 +40930,25 @@
     </row>
     <row r="325" spans="1:20">
       <c r="A325" s="344" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B325" s="344" t="s">
         <v>192</v>
       </c>
       <c r="C325" s="245">
-        <v>0.16350000000000001</v>
+        <v>0.22175</v>
       </c>
       <c r="D325" s="245">
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E325" s="245">
-        <v>3.2500000000000001E-2</v>
+        <v>4.0999999999999988E-2</v>
       </c>
       <c r="F325" s="245">
-        <v>0.23474999999999999</v>
+        <v>0.2515</v>
       </c>
       <c r="G325" s="245">
-        <v>0.30599999999999999</v>
+        <v>0.20025000000000001</v>
       </c>
       <c r="H325" s="239" t="e">
         <f>NA()</f>
@@ -40931,7 +40957,7 @@
     </row>
     <row r="326" spans="1:20">
       <c r="A326" s="344" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B326" s="344" t="s">
         <v>192</v>
@@ -40943,13 +40969,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E326" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="F326" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G326" s="245">
-        <v>0.44600000000000001</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H326" s="239" t="e">
         <f>NA()</f>
@@ -40958,7 +40984,7 @@
     </row>
     <row r="327" spans="1:20">
       <c r="A327" s="344" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B327" s="344" t="s">
         <v>192</v>
@@ -40976,7 +41002,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G327" s="245">
-        <v>0.44299999999999989</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="H327" s="239" t="e">
         <f>NA()</f>
@@ -40985,7 +41011,7 @@
     </row>
     <row r="328" spans="1:20">
       <c r="A328" s="344" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B328" s="344" t="s">
         <v>192</v>
@@ -40997,13 +41023,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E328" s="245">
-        <v>2.75E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F328" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G328" s="245">
-        <v>0.36049999999999999</v>
+        <v>0.44299999999999989</v>
       </c>
       <c r="H328" s="239" t="e">
         <f>NA()</f>
@@ -41012,7 +41038,7 @@
     </row>
     <row r="329" spans="1:20">
       <c r="A329" s="344" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B329" s="344" t="s">
         <v>192</v>
@@ -41024,13 +41050,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E329" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F329" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G329" s="245">
-        <v>0.35299999999999998</v>
+        <v>0.36049999999999999</v>
       </c>
       <c r="H329" s="239" t="e">
         <f>NA()</f>
@@ -41039,7 +41065,7 @@
     </row>
     <row r="330" spans="1:20">
       <c r="A330" s="344" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B330" s="344" t="s">
         <v>192</v>
@@ -41057,7 +41083,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G330" s="245">
-        <v>0.44524999999999998</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="H330" s="239" t="e">
         <f>NA()</f>
@@ -41066,7 +41092,7 @@
     </row>
     <row r="331" spans="1:20">
       <c r="A331" s="344" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B331" s="344" t="s">
         <v>192</v>
@@ -41084,7 +41110,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G331" s="245">
-        <v>0.35175000000000001</v>
+        <v>0.44524999999999998</v>
       </c>
       <c r="H331" s="239" t="e">
         <f>NA()</f>
@@ -41093,7 +41119,7 @@
     </row>
     <row r="332" spans="1:20">
       <c r="A332" s="344" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B332" s="344" t="s">
         <v>192</v>
@@ -41105,13 +41131,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E332" s="245">
-        <v>2.1749999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F332" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G332" s="245">
-        <v>0.48825000000000002</v>
+        <v>0.35175000000000001</v>
       </c>
       <c r="H332" s="239" t="e">
         <f>NA()</f>
@@ -41120,7 +41146,7 @@
     </row>
     <row r="333" spans="1:20">
       <c r="A333" s="344" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B333" s="344" t="s">
         <v>192</v>
@@ -41132,23 +41158,22 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E333" s="245">
-        <v>2.75E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F333" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G333" s="245">
-        <v>0.36375000000000002</v>
+        <v>0.48825000000000002</v>
       </c>
       <c r="H333" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="T333" s="239"/>
     </row>
     <row r="334" spans="1:20">
       <c r="A334" s="344" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B334" s="344" t="s">
         <v>192</v>
@@ -41160,13 +41185,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E334" s="245">
-        <v>2.1749999999999999E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F334" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G334" s="245">
-        <v>0.38850000000000001</v>
+        <v>0.36375000000000002</v>
       </c>
       <c r="H334" s="239" t="e">
         <f>NA()</f>
@@ -41176,7 +41201,7 @@
     </row>
     <row r="335" spans="1:20">
       <c r="A335" s="344" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B335" s="344" t="s">
         <v>192</v>
@@ -41194,7 +41219,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G335" s="245">
-        <v>0.41325000000000001</v>
+        <v>0.38850000000000001</v>
       </c>
       <c r="H335" s="239" t="e">
         <f>NA()</f>
@@ -41204,7 +41229,7 @@
     </row>
     <row r="336" spans="1:20">
       <c r="A336" s="344" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B336" s="344" t="s">
         <v>192</v>
@@ -41216,13 +41241,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E336" s="245">
-        <v>2.75E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F336" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G336" s="245">
-        <v>0.28549999999999998</v>
+        <v>0.41325000000000001</v>
       </c>
       <c r="H336" s="239" t="e">
         <f>NA()</f>
@@ -41232,7 +41257,7 @@
     </row>
     <row r="337" spans="1:33">
       <c r="A337" s="344" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B337" s="344" t="s">
         <v>192</v>
@@ -41250,16 +41275,17 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G337" s="245">
-        <v>0.26150000000000001</v>
+        <v>0.28549999999999998</v>
       </c>
       <c r="H337" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="T337" s="239"/>
     </row>
     <row r="338" spans="1:33">
       <c r="A338" s="344" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B338" s="344" t="s">
         <v>192</v>
@@ -41271,13 +41297,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E338" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F338" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G338" s="245">
-        <v>0.4405</v>
+        <v>0.26150000000000001</v>
       </c>
       <c r="H338" s="239" t="e">
         <f>NA()</f>
@@ -41286,7 +41312,7 @@
     </row>
     <row r="339" spans="1:33">
       <c r="A339" s="344" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B339" s="344" t="s">
         <v>192</v>
@@ -41304,7 +41330,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G339" s="245">
-        <v>0.4365</v>
+        <v>0.4405</v>
       </c>
       <c r="H339" s="239" t="e">
         <f>NA()</f>
@@ -41313,7 +41339,7 @@
     </row>
     <row r="340" spans="1:33">
       <c r="A340" s="344" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B340" s="344" t="s">
         <v>192</v>
@@ -41325,13 +41351,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E340" s="245">
-        <v>2.75E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F340" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G340" s="245">
-        <v>0.27100000000000002</v>
+        <v>0.4365</v>
       </c>
       <c r="H340" s="239" t="e">
         <f>NA()</f>
@@ -41340,7 +41366,7 @@
     </row>
     <row r="341" spans="1:33">
       <c r="A341" s="344" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B341" s="344" t="s">
         <v>192</v>
@@ -41352,13 +41378,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E341" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F341" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G341" s="245">
-        <v>0.36875000000000002</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="H341" s="239" t="e">
         <f>NA()</f>
@@ -41367,7 +41393,7 @@
     </row>
     <row r="342" spans="1:33">
       <c r="A342" s="344" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B342" s="344" t="s">
         <v>192</v>
@@ -41385,7 +41411,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G342" s="245">
-        <v>0.35799999999999998</v>
+        <v>0.36875000000000002</v>
       </c>
       <c r="H342" s="239" t="e">
         <f>NA()</f>
@@ -41394,25 +41420,25 @@
     </row>
     <row r="343" spans="1:33">
       <c r="A343" s="344" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B343" s="344" t="s">
         <v>192</v>
       </c>
       <c r="C343" s="245">
-        <v>0.22175</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D343" s="245">
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E343" s="245">
-        <v>3.2500000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F343" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G343" s="245">
-        <v>0.23524999999999999</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="H343" s="239" t="e">
         <f>NA()</f>
@@ -41421,25 +41447,25 @@
     </row>
     <row r="344" spans="1:33">
       <c r="A344" s="344" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B344" s="344" t="s">
         <v>192</v>
       </c>
-      <c r="C344" s="344">
+      <c r="C344" s="245">
         <v>0.22175</v>
       </c>
-      <c r="D344" s="344">
+      <c r="D344" s="245">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="E344" s="344">
-        <v>4.0999999999999988E-2</v>
-      </c>
-      <c r="F344" s="344">
-        <v>0.2515</v>
-      </c>
-      <c r="G344" s="344">
-        <v>0.17599999999999999</v>
+      <c r="E344" s="245">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F344" s="245">
+        <v>0.23474999999999999</v>
+      </c>
+      <c r="G344" s="245">
+        <v>0.23524999999999999</v>
       </c>
       <c r="H344" s="239" t="e">
         <f>NA()</f>
@@ -41448,7 +41474,7 @@
     </row>
     <row r="345" spans="1:33">
       <c r="A345" s="344" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B345" s="344" t="s">
         <v>192</v>
@@ -41460,13 +41486,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E345" s="344">
-        <v>3.2500000000000001E-2</v>
+        <v>4.0999999999999988E-2</v>
       </c>
       <c r="F345" s="344">
-        <v>0.23474999999999999</v>
+        <v>0.2515</v>
       </c>
       <c r="G345" s="344">
-        <v>0.188</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="H345" s="239" t="e">
         <f>NA()</f>
@@ -41475,25 +41501,25 @@
     </row>
     <row r="346" spans="1:33">
       <c r="A346" s="344" t="s">
-        <v>225</v>
-      </c>
-      <c r="B346" s="341" t="s">
+        <v>224</v>
+      </c>
+      <c r="B346" s="344" t="s">
         <v>192</v>
       </c>
-      <c r="C346" s="245">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="D346" s="245">
+      <c r="C346" s="344">
+        <v>0.22175</v>
+      </c>
+      <c r="D346" s="344">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="E346" s="245">
-        <v>2.1749999999999999E-2</v>
-      </c>
-      <c r="F346" s="245">
+      <c r="E346" s="344">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F346" s="344">
         <v>0.23474999999999999</v>
       </c>
-      <c r="G346" s="245">
-        <v>0.43824999999999997</v>
+      <c r="G346" s="344">
+        <v>0.188</v>
       </c>
       <c r="H346" s="239" t="e">
         <f>NA()</f>
@@ -41501,8 +41527,8 @@
       </c>
     </row>
     <row r="347" spans="1:33">
-      <c r="A347" s="341" t="s">
-        <v>226</v>
+      <c r="A347" s="344" t="s">
+        <v>225</v>
       </c>
       <c r="B347" s="341" t="s">
         <v>192</v>
@@ -41520,28 +41546,16 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G347" s="245">
-        <v>0.39250000000000002</v>
+        <v>0.43824999999999997</v>
       </c>
       <c r="H347" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="V347" s="400"/>
-      <c r="W347" s="400"/>
-      <c r="X347" s="400"/>
-      <c r="Y347" s="400"/>
-      <c r="Z347" s="400"/>
-      <c r="AA347" s="400"/>
-      <c r="AB347" s="400"/>
-      <c r="AC347" s="400"/>
-      <c r="AD347" s="400"/>
-      <c r="AE347" s="400"/>
-      <c r="AF347" s="400"/>
-      <c r="AG347" s="400"/>
     </row>
     <row r="348" spans="1:33">
       <c r="A348" s="341" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B348" s="341" t="s">
         <v>192</v>
@@ -41553,34 +41567,34 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E348" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F348" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G348" s="245">
-        <v>0.43600000000000011</v>
+        <v>0.39250000000000002</v>
       </c>
       <c r="H348" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="V348" s="400"/>
-      <c r="W348" s="400"/>
-      <c r="X348" s="400"/>
-      <c r="Y348" s="400"/>
-      <c r="Z348" s="400"/>
-      <c r="AA348" s="400"/>
-      <c r="AB348" s="400"/>
-      <c r="AC348" s="400"/>
-      <c r="AD348" s="400"/>
-      <c r="AE348" s="400"/>
-      <c r="AF348" s="400"/>
-      <c r="AG348" s="400"/>
+      <c r="V348" s="398"/>
+      <c r="W348" s="398"/>
+      <c r="X348" s="398"/>
+      <c r="Y348" s="398"/>
+      <c r="Z348" s="398"/>
+      <c r="AA348" s="398"/>
+      <c r="AB348" s="398"/>
+      <c r="AC348" s="398"/>
+      <c r="AD348" s="398"/>
+      <c r="AE348" s="398"/>
+      <c r="AF348" s="398"/>
+      <c r="AG348" s="398"/>
     </row>
     <row r="349" spans="1:33">
-      <c r="A349" s="344" t="s">
-        <v>228</v>
+      <c r="A349" s="341" t="s">
+        <v>227</v>
       </c>
       <c r="B349" s="341" t="s">
         <v>192</v>
@@ -41598,18 +41612,30 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G349" s="245">
-        <v>0.34300000000000003</v>
+        <v>0.43600000000000011</v>
       </c>
       <c r="H349" s="239" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="V349" s="398"/>
+      <c r="W349" s="398"/>
+      <c r="X349" s="398"/>
+      <c r="Y349" s="398"/>
+      <c r="Z349" s="398"/>
+      <c r="AA349" s="398"/>
+      <c r="AB349" s="398"/>
+      <c r="AC349" s="398"/>
+      <c r="AD349" s="398"/>
+      <c r="AE349" s="398"/>
+      <c r="AF349" s="398"/>
+      <c r="AG349" s="398"/>
     </row>
     <row r="350" spans="1:33">
       <c r="A350" s="344" t="s">
-        <v>229</v>
-      </c>
-      <c r="B350" s="344" t="s">
+        <v>228</v>
+      </c>
+      <c r="B350" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C350" s="245">
@@ -41619,13 +41645,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E350" s="245">
-        <v>2.1749999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F350" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G350" s="245">
-        <v>0.31724999999999998</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="H350" s="239" t="e">
         <f>NA()</f>
@@ -41634,7 +41660,7 @@
     </row>
     <row r="351" spans="1:33">
       <c r="A351" s="344" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B351" s="344" t="s">
         <v>192</v>
@@ -41646,13 +41672,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E351" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F351" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G351" s="245">
-        <v>0.45524999999999999</v>
+        <v>0.31724999999999998</v>
       </c>
       <c r="H351" s="239" t="e">
         <f>NA()</f>
@@ -41661,7 +41687,7 @@
     </row>
     <row r="352" spans="1:33">
       <c r="A352" s="344" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B352" s="344" t="s">
         <v>192</v>
@@ -41679,7 +41705,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G352" s="245">
-        <v>0.36525000000000002</v>
+        <v>0.45524999999999999</v>
       </c>
       <c r="H352" s="239" t="e">
         <f>NA()</f>
@@ -41688,7 +41714,7 @@
     </row>
     <row r="353" spans="1:8">
       <c r="A353" s="344" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B353" s="344" t="s">
         <v>192</v>
@@ -41700,13 +41726,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E353" s="245">
-        <v>2.75E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F353" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G353" s="245">
-        <v>0.32900000000000001</v>
+        <v>0.36525000000000002</v>
       </c>
       <c r="H353" s="239" t="e">
         <f>NA()</f>
@@ -41714,10 +41740,10 @@
       </c>
     </row>
     <row r="354" spans="1:8">
-      <c r="A354" s="341" t="s">
-        <v>233</v>
-      </c>
-      <c r="B354" s="341" t="s">
+      <c r="A354" s="344" t="s">
+        <v>232</v>
+      </c>
+      <c r="B354" s="344" t="s">
         <v>192</v>
       </c>
       <c r="C354" s="245">
@@ -41727,13 +41753,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E354" s="245">
-        <v>2.1749999999999999E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F354" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G354" s="245">
-        <v>0.33600000000000002</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="H354" s="239" t="e">
         <f>NA()</f>
@@ -41741,10 +41767,10 @@
       </c>
     </row>
     <row r="355" spans="1:8">
-      <c r="A355" s="344" t="s">
-        <v>234</v>
-      </c>
-      <c r="B355" s="344" t="s">
+      <c r="A355" s="341" t="s">
+        <v>233</v>
+      </c>
+      <c r="B355" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C355" s="245">
@@ -41754,13 +41780,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E355" s="245">
-        <v>1.4999999999999999E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F355" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G355" s="245">
-        <v>0.36299999999999999</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="H355" s="239" t="e">
         <f>NA()</f>
@@ -41769,7 +41795,7 @@
     </row>
     <row r="356" spans="1:8">
       <c r="A356" s="344" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B356" s="344" t="s">
         <v>192</v>
@@ -41787,7 +41813,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G356" s="245">
-        <v>0.35125000000000001</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="H356" s="239" t="e">
         <f>NA()</f>
@@ -41796,7 +41822,7 @@
     </row>
     <row r="357" spans="1:8">
       <c r="A357" s="344" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B357" s="344" t="s">
         <v>192</v>
@@ -41814,7 +41840,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G357" s="245">
-        <v>0.35275000000000001</v>
+        <v>0.35125000000000001</v>
       </c>
       <c r="H357" s="239" t="e">
         <f>NA()</f>
@@ -41822,10 +41848,10 @@
       </c>
     </row>
     <row r="358" spans="1:8">
-      <c r="A358" s="341" t="s">
-        <v>237</v>
-      </c>
-      <c r="B358" s="341" t="s">
+      <c r="A358" s="344" t="s">
+        <v>236</v>
+      </c>
+      <c r="B358" s="344" t="s">
         <v>192</v>
       </c>
       <c r="C358" s="245">
@@ -41841,7 +41867,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G358" s="245">
-        <v>0.36075000000000002</v>
+        <v>0.35275000000000001</v>
       </c>
       <c r="H358" s="239" t="e">
         <f>NA()</f>
@@ -41849,26 +41875,26 @@
       </c>
     </row>
     <row r="359" spans="1:8">
-      <c r="A359" s="344" t="s">
-        <v>238</v>
+      <c r="A359" s="341" t="s">
+        <v>237</v>
       </c>
       <c r="B359" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C359" s="245">
-        <v>0.16340852130325809</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D359" s="245">
-        <v>5.338345864661654E-2</v>
+        <v>5.3249999999999999E-2</v>
       </c>
       <c r="E359" s="245">
-        <v>2.180451127819549E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F359" s="245">
-        <v>0.23483709273182959</v>
+        <v>0.23474999999999999</v>
       </c>
       <c r="G359" s="245">
-        <v>0.31428571428571428</v>
+        <v>0.36075000000000002</v>
       </c>
       <c r="H359" s="239" t="e">
         <f>NA()</f>
@@ -41877,25 +41903,25 @@
     </row>
     <row r="360" spans="1:8">
       <c r="A360" s="344" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B360" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C360" s="245">
-        <v>0.16350000000000001</v>
+        <v>0.16340852130325809</v>
       </c>
       <c r="D360" s="245">
-        <v>5.3249999999999999E-2</v>
+        <v>5.338345864661654E-2</v>
       </c>
       <c r="E360" s="245">
-        <v>2.1749999999999999E-2</v>
+        <v>2.180451127819549E-2</v>
       </c>
       <c r="F360" s="245">
-        <v>0.23474999999999999</v>
+        <v>0.23483709273182959</v>
       </c>
       <c r="G360" s="245">
-        <v>0.32550000000000001</v>
+        <v>0.31428571428571428</v>
       </c>
       <c r="H360" s="239" t="e">
         <f>NA()</f>
@@ -41903,26 +41929,26 @@
       </c>
     </row>
     <row r="361" spans="1:8">
-      <c r="A361" s="341" t="s">
-        <v>240</v>
+      <c r="A361" s="344" t="s">
+        <v>239</v>
       </c>
       <c r="B361" s="341" t="s">
         <v>192</v>
       </c>
-      <c r="C361" s="341">
+      <c r="C361" s="245">
         <v>0.16350000000000001</v>
       </c>
-      <c r="D361" s="341">
+      <c r="D361" s="245">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="E361" s="341">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F361" s="341">
+      <c r="E361" s="245">
+        <v>2.1749999999999999E-2</v>
+      </c>
+      <c r="F361" s="245">
         <v>0.23474999999999999</v>
       </c>
-      <c r="G361" s="341">
-        <v>0.50600000000000001</v>
+      <c r="G361" s="245">
+        <v>0.32550000000000001</v>
       </c>
       <c r="H361" s="239" t="e">
         <f>NA()</f>
@@ -41930,26 +41956,26 @@
       </c>
     </row>
     <row r="362" spans="1:8">
-      <c r="A362" s="344" t="s">
-        <v>241</v>
-      </c>
-      <c r="B362" s="344" t="s">
+      <c r="A362" s="341" t="s">
+        <v>240</v>
+      </c>
+      <c r="B362" s="341" t="s">
         <v>192</v>
       </c>
       <c r="C362" s="341">
-        <v>0.16347607052896729</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D362" s="341">
-        <v>5.3400503778337528E-2</v>
+        <v>5.3249999999999999E-2</v>
       </c>
       <c r="E362" s="341">
-        <v>2.7455919395465999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F362" s="341">
-        <v>0.23476070528967249</v>
+        <v>0.23474999999999999</v>
       </c>
       <c r="G362" s="341">
-        <v>0.37934508816120899</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="H362" s="239" t="e">
         <f>NA()</f>
@@ -41958,25 +41984,25 @@
     </row>
     <row r="363" spans="1:8">
       <c r="A363" s="344" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B363" s="344" t="s">
         <v>192</v>
       </c>
-      <c r="C363" s="245">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="D363" s="245">
-        <v>5.3249999999999999E-2</v>
-      </c>
-      <c r="E363" s="245">
-        <v>2.75E-2</v>
-      </c>
-      <c r="F363" s="245">
-        <v>0.23474999999999999</v>
-      </c>
-      <c r="G363" s="245">
-        <v>0.36049999999999999</v>
+      <c r="C363" s="341">
+        <v>0.16347607052896729</v>
+      </c>
+      <c r="D363" s="341">
+        <v>5.3400503778337528E-2</v>
+      </c>
+      <c r="E363" s="341">
+        <v>2.7455919395465999E-2</v>
+      </c>
+      <c r="F363" s="341">
+        <v>0.23476070528967249</v>
+      </c>
+      <c r="G363" s="341">
+        <v>0.37934508816120899</v>
       </c>
       <c r="H363" s="239" t="e">
         <f>NA()</f>
@@ -41984,10 +42010,10 @@
       </c>
     </row>
     <row r="364" spans="1:8">
-      <c r="A364" s="245" t="s">
-        <v>243</v>
-      </c>
-      <c r="B364" s="245" t="s">
+      <c r="A364" s="344" t="s">
+        <v>242</v>
+      </c>
+      <c r="B364" s="344" t="s">
         <v>192</v>
       </c>
       <c r="C364" s="245">
@@ -41997,13 +42023,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E364" s="245">
-        <v>3.2500000000000001E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F364" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G364" s="245">
-        <v>0.35199999999999998</v>
+        <v>0.36049999999999999</v>
       </c>
       <c r="H364" s="239" t="e">
         <f>NA()</f>
@@ -42012,7 +42038,7 @@
     </row>
     <row r="365" spans="1:8">
       <c r="A365" s="245" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B365" s="245" t="s">
         <v>192</v>
@@ -42024,13 +42050,13 @@
         <v>5.3249999999999999E-2</v>
       </c>
       <c r="E365" s="245">
-        <v>2.1749999999999999E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="F365" s="245">
         <v>0.23474999999999999</v>
       </c>
       <c r="G365" s="245">
-        <v>0.40125</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="H365" s="239" t="e">
         <f>NA()</f>
@@ -42038,26 +42064,26 @@
       </c>
     </row>
     <row r="366" spans="1:8">
-      <c r="A366" s="341" t="s">
-        <v>245</v>
+      <c r="A366" s="245" t="s">
+        <v>244</v>
       </c>
       <c r="B366" s="245" t="s">
         <v>192</v>
       </c>
       <c r="C366" s="245">
-        <v>0.1633663366336634</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D366" s="245">
-        <v>5.3217821782178223E-2</v>
+        <v>5.3249999999999999E-2</v>
       </c>
       <c r="E366" s="245">
-        <v>1.50990099009901E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F366" s="245">
-        <v>0.23490099009900989</v>
+        <v>0.23474999999999999</v>
       </c>
       <c r="G366" s="245">
-        <v>0.35123762376237622</v>
+        <v>0.40125</v>
       </c>
       <c r="H366" s="239" t="e">
         <f>NA()</f>
@@ -42066,25 +42092,25 @@
     </row>
     <row r="367" spans="1:8">
       <c r="A367" s="341" t="s">
-        <v>246</v>
-      </c>
-      <c r="B367" s="341" t="s">
+        <v>245</v>
+      </c>
+      <c r="B367" s="245" t="s">
         <v>192</v>
       </c>
       <c r="C367" s="245">
-        <v>0.16347607052896729</v>
+        <v>0.1633663366336634</v>
       </c>
       <c r="D367" s="245">
-        <v>5.3400503778337528E-2</v>
+        <v>5.3217821782178223E-2</v>
       </c>
       <c r="E367" s="245">
-        <v>1.5113350125944581E-2</v>
+        <v>1.50990099009901E-2</v>
       </c>
       <c r="F367" s="245">
-        <v>0.23476070528967249</v>
+        <v>0.23490099009900989</v>
       </c>
       <c r="G367" s="245">
-        <v>0.36322418136020151</v>
+        <v>0.35123762376237622</v>
       </c>
       <c r="H367" s="239" t="e">
         <f>NA()</f>
@@ -42092,26 +42118,26 @@
       </c>
     </row>
     <row r="368" spans="1:8">
-      <c r="A368" s="344" t="s">
-        <v>247</v>
-      </c>
-      <c r="B368" s="343" t="s">
+      <c r="A368" s="341" t="s">
+        <v>246</v>
+      </c>
+      <c r="B368" s="341" t="s">
         <v>192</v>
       </c>
-      <c r="C368" s="344">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="D368" s="344">
-        <v>5.3249999999999999E-2</v>
-      </c>
-      <c r="E368" s="344">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F368" s="344">
-        <v>0.23474999999999999</v>
-      </c>
-      <c r="G368" s="344">
-        <v>0.35525000000000001</v>
+      <c r="C368" s="245">
+        <v>0.16347607052896729</v>
+      </c>
+      <c r="D368" s="245">
+        <v>5.3400503778337528E-2</v>
+      </c>
+      <c r="E368" s="245">
+        <v>1.5113350125944581E-2</v>
+      </c>
+      <c r="F368" s="245">
+        <v>0.23476070528967249</v>
+      </c>
+      <c r="G368" s="245">
+        <v>0.36322418136020151</v>
       </c>
       <c r="H368" s="239" t="e">
         <f>NA()</f>
@@ -42120,7 +42146,7 @@
     </row>
     <row r="369" spans="1:8">
       <c r="A369" s="344" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B369" s="343" t="s">
         <v>192</v>
@@ -42138,7 +42164,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G369" s="344">
-        <v>0.36125000000000002</v>
+        <v>0.35525000000000001</v>
       </c>
       <c r="H369" s="239" t="e">
         <f>NA()</f>
@@ -42147,7 +42173,7 @@
     </row>
     <row r="370" spans="1:8">
       <c r="A370" s="344" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B370" s="343" t="s">
         <v>192</v>
@@ -42165,7 +42191,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G370" s="344">
-        <v>0.36675000000000002</v>
+        <v>0.36125000000000002</v>
       </c>
       <c r="H370" s="239" t="e">
         <f>NA()</f>
@@ -42174,7 +42200,7 @@
     </row>
     <row r="371" spans="1:8">
       <c r="A371" s="344" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B371" s="343" t="s">
         <v>192</v>
@@ -42192,7 +42218,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G371" s="344">
-        <v>0.36625000000000002</v>
+        <v>0.36675000000000002</v>
       </c>
       <c r="H371" s="239" t="e">
         <f>NA()</f>
@@ -42201,7 +42227,7 @@
     </row>
     <row r="372" spans="1:8">
       <c r="A372" s="344" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B372" s="343" t="s">
         <v>192</v>
@@ -42219,7 +42245,7 @@
         <v>0.23474999999999999</v>
       </c>
       <c r="G372" s="344">
-        <v>0.34899999999999998</v>
+        <v>0.36625000000000002</v>
       </c>
       <c r="H372" s="239" t="e">
         <f>NA()</f>
@@ -42228,25 +42254,25 @@
     </row>
     <row r="373" spans="1:8">
       <c r="A373" s="344" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B373" s="343" t="s">
         <v>192</v>
       </c>
       <c r="C373" s="344">
-        <v>0.16337349397590359</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="D373" s="344">
-        <v>5.3253012048192772E-2</v>
+        <v>5.3249999999999999E-2</v>
       </c>
       <c r="E373" s="344">
-        <v>2.1927710843373499E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F373" s="344">
-        <v>0.2346987951807229</v>
+        <v>0.23474999999999999</v>
       </c>
       <c r="G373" s="344">
-        <v>0.29951807228915661</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="H373" s="239" t="e">
         <f>NA()</f>
@@ -42255,25 +42281,25 @@
     </row>
     <row r="374" spans="1:8">
       <c r="A374" s="344" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B374" s="343" t="s">
         <v>192</v>
       </c>
       <c r="C374" s="344">
-        <v>0.16348837209302319</v>
+        <v>0.16337349397590359</v>
       </c>
       <c r="D374" s="344">
-        <v>5.3255813953488371E-2</v>
+        <v>5.3253012048192772E-2</v>
       </c>
       <c r="E374" s="344">
-        <v>1.511627906976744E-2</v>
+        <v>2.1927710843373499E-2</v>
       </c>
       <c r="F374" s="344">
-        <v>0.23488372093023249</v>
+        <v>0.2346987951807229</v>
       </c>
       <c r="G374" s="344">
-        <v>0.34093023255813948</v>
+        <v>0.29951807228915661</v>
       </c>
       <c r="H374" s="239" t="e">
         <f>NA()</f>
@@ -42282,25 +42308,25 @@
     </row>
     <row r="375" spans="1:8">
       <c r="A375" s="344" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B375" s="343" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="C375" s="344">
-        <v>0</v>
+        <v>0.16348837209302319</v>
       </c>
       <c r="D375" s="344">
-        <v>0</v>
+        <v>5.3255813953488371E-2</v>
       </c>
       <c r="E375" s="344">
-        <v>4.0288924558587479E-2</v>
+        <v>1.511627906976744E-2</v>
       </c>
       <c r="F375" s="344">
-        <v>0.1757624398073836</v>
+        <v>0.23488372093023249</v>
       </c>
       <c r="G375" s="344">
-        <v>0</v>
+        <v>0.34093023255813948</v>
       </c>
       <c r="H375" s="239" t="e">
         <f>NA()</f>
@@ -42309,25 +42335,25 @@
     </row>
     <row r="376" spans="1:8">
       <c r="A376" s="344" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B376" s="343" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C376" s="344">
         <v>0</v>
       </c>
       <c r="D376" s="344">
-        <v>0.1215505464480874</v>
+        <v>0</v>
       </c>
       <c r="E376" s="344">
-        <v>0.25928961748633877</v>
+        <v>4.0288924558587479E-2</v>
       </c>
       <c r="F376" s="344">
-        <v>0.52223360655737705</v>
+        <v>0.1757624398073836</v>
       </c>
       <c r="G376" s="344">
-        <v>1.912568306010929E-3</v>
+        <v>0</v>
       </c>
       <c r="H376" s="239" t="e">
         <f>NA()</f>
@@ -42338,39 +42364,57 @@
       <c r="A377" s="344" t="s">
         <v>255</v>
       </c>
-      <c r="B377" s="240" t="s">
+      <c r="B377" s="343" t="s">
+        <v>38</v>
+      </c>
+      <c r="C377" s="344">
+        <v>0</v>
+      </c>
+      <c r="D377" s="344">
+        <v>0.1215505464480874</v>
+      </c>
+      <c r="E377" s="344">
+        <v>0.25928961748633877</v>
+      </c>
+      <c r="F377" s="344">
+        <v>0.52223360655737705</v>
+      </c>
+      <c r="G377" s="344">
+        <v>1.912568306010929E-3</v>
+      </c>
+      <c r="H377" s="239" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8">
+      <c r="A378" s="344" t="s">
+        <v>255</v>
+      </c>
+      <c r="B378" s="240" t="s">
         <v>39</v>
       </c>
-      <c r="C377" s="240">
-        <v>0</v>
-      </c>
-      <c r="D377" s="240">
+      <c r="C378" s="240">
+        <v>0</v>
+      </c>
+      <c r="D378" s="240">
         <v>9.3123168129999045E-2</v>
       </c>
-      <c r="E377" s="240">
+      <c r="E378" s="240">
         <v>0.25076633684560368</v>
       </c>
-      <c r="F377" s="240">
+      <c r="F378" s="240">
         <v>0.48156651718762372</v>
       </c>
-      <c r="G377" s="240">
+      <c r="G378" s="240">
         <v>1.9060144917171431E-3</v>
       </c>
-      <c r="H377" s="241">
+      <c r="H378" s="241">
         <v>1.07</v>
       </c>
     </row>
-    <row r="378" spans="1:8">
-      <c r="A378" s="245"/>
-      <c r="B378" s="240"/>
-      <c r="C378" s="240"/>
-      <c r="D378" s="240"/>
-      <c r="E378" s="240"/>
-      <c r="F378" s="240"/>
-      <c r="G378" s="240"/>
-    </row>
     <row r="379" spans="1:8">
-      <c r="A379" s="341"/>
+      <c r="A379" s="245"/>
       <c r="B379" s="240"/>
       <c r="C379" s="240"/>
       <c r="D379" s="240"/>
@@ -42379,13 +42423,13 @@
       <c r="G379" s="240"/>
     </row>
     <row r="380" spans="1:8">
+      <c r="A380" s="341"/>
       <c r="B380" s="240"/>
       <c r="C380" s="240"/>
       <c r="D380" s="240"/>
       <c r="E380" s="240"/>
       <c r="F380" s="240"/>
       <c r="G380" s="240"/>
-      <c r="H380" s="241"/>
     </row>
     <row r="381" spans="1:8">
       <c r="B381" s="240"/>
@@ -42406,13 +42450,13 @@
       <c r="H382" s="241"/>
     </row>
     <row r="383" spans="1:8">
-      <c r="A383" s="245"/>
       <c r="B383" s="240"/>
       <c r="C383" s="240"/>
       <c r="D383" s="240"/>
       <c r="E383" s="240"/>
       <c r="F383" s="240"/>
       <c r="G383" s="240"/>
+      <c r="H383" s="241"/>
     </row>
     <row r="384" spans="1:8">
       <c r="A384" s="245"/>
@@ -42423,13 +42467,22 @@
       <c r="F384" s="240"/>
       <c r="G384" s="240"/>
     </row>
+    <row r="385" spans="1:7">
+      <c r="A385" s="245"/>
+      <c r="B385" s="240"/>
+      <c r="C385" s="240"/>
+      <c r="D385" s="240"/>
+      <c r="E385" s="240"/>
+      <c r="F385" s="240"/>
+      <c r="G385" s="240"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:I353">
-    <sortCondition ref="A2:A353"/>
+  <sortState ref="A2:I354">
+    <sortCondition ref="A2:A354"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="J1:O12"/>
-    <mergeCell ref="V347:AG348"/>
+    <mergeCell ref="V348:AG349"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -42444,7 +42497,9 @@
   </sheetPr>
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -42460,27 +42515,27 @@
       </c>
     </row>
     <row r="2" spans="1:27" s="245" customFormat="1" ht="37.5" customHeight="1">
-      <c r="C2" s="401" t="s">
+      <c r="C2" s="402" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="402"/>
-      <c r="E2" s="402"/>
-      <c r="F2" s="402"/>
-      <c r="G2" s="402"/>
+      <c r="D2" s="403"/>
+      <c r="E2" s="403"/>
+      <c r="F2" s="403"/>
+      <c r="G2" s="403"/>
       <c r="H2" s="247" t="s">
         <v>375</v>
       </c>
-      <c r="J2" s="403" t="s">
+      <c r="J2" s="404" t="s">
         <v>376</v>
       </c>
-      <c r="K2" s="404"/>
-      <c r="L2" s="404"/>
-      <c r="M2" s="404"/>
-      <c r="N2" s="404"/>
-      <c r="R2" s="405" t="s">
+      <c r="K2" s="405"/>
+      <c r="L2" s="405"/>
+      <c r="M2" s="405"/>
+      <c r="N2" s="405"/>
+      <c r="R2" s="406" t="s">
         <v>377</v>
       </c>
-      <c r="S2" s="405"/>
+      <c r="S2" s="406"/>
     </row>
     <row r="3" spans="1:27" s="245" customFormat="1" ht="25.5" customHeight="1">
       <c r="A3" s="141" t="s">
@@ -42791,8 +42846,8 @@
 )</f>
         <v>2.0247318804625779E-3</v>
       </c>
-      <c r="H7" s="145">
-        <v>0.72</v>
+      <c r="H7" s="211">
+        <v>0.97</v>
       </c>
       <c r="I7" s="241"/>
       <c r="J7" s="144">
@@ -43105,6 +43160,15 @@
       </c>
       <c r="O11" s="145">
         <v>1.07</v>
+      </c>
+      <c r="R11" s="146" t="s">
+        <v>667</v>
+      </c>
+      <c r="S11" s="212">
+        <v>0.97</v>
+      </c>
+      <c r="T11" s="245" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="12" spans="1:27" s="245" customFormat="1" ht="18" customHeight="1">
@@ -45748,25 +45812,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A3" s="410" t="s">
+      <c r="A3" s="411" t="s">
         <v>435</v>
       </c>
-      <c r="B3" s="408" t="s">
+      <c r="B3" s="409" t="s">
         <v>472</v>
       </c>
-      <c r="C3" s="408" t="s">
+      <c r="C3" s="409" t="s">
         <v>473</v>
       </c>
-      <c r="D3" s="408" t="s">
+      <c r="D3" s="409" t="s">
         <v>474</v>
       </c>
-      <c r="E3" s="408" t="s">
+      <c r="E3" s="409" t="s">
         <v>475</v>
       </c>
-      <c r="F3" s="408" t="s">
+      <c r="F3" s="409" t="s">
         <v>476</v>
       </c>
-      <c r="G3" s="408" t="s">
+      <c r="G3" s="409" t="s">
         <v>477</v>
       </c>
       <c r="J3" s="108" t="s">
@@ -45779,13 +45843,13 @@
       <c r="O3" s="108"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A4" s="411"/>
-      <c r="B4" s="409"/>
-      <c r="C4" s="409"/>
-      <c r="D4" s="409"/>
-      <c r="E4" s="409"/>
-      <c r="F4" s="409"/>
-      <c r="G4" s="409"/>
+      <c r="A4" s="412"/>
+      <c r="B4" s="410"/>
+      <c r="C4" s="410"/>
+      <c r="D4" s="410"/>
+      <c r="E4" s="410"/>
+      <c r="F4" s="410"/>
+      <c r="G4" s="410"/>
       <c r="J4" s="113" t="s">
         <v>15</v>
       </c>
@@ -46057,15 +46121,15 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A16" s="414" t="s">
+      <c r="A16" s="415" t="s">
         <v>479</v>
       </c>
-      <c r="B16" s="415"/>
-      <c r="C16" s="415"/>
-      <c r="D16" s="415"/>
-      <c r="E16" s="415"/>
-      <c r="F16" s="415"/>
-      <c r="G16" s="415"/>
+      <c r="B16" s="416"/>
+      <c r="C16" s="416"/>
+      <c r="D16" s="416"/>
+      <c r="E16" s="416"/>
+      <c r="F16" s="416"/>
+      <c r="G16" s="416"/>
       <c r="K16" s="59"/>
       <c r="L16" s="59"/>
       <c r="M16" s="59"/>
@@ -46409,10 +46473,10 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A28" s="412" t="s">
+      <c r="A28" s="413" t="s">
         <v>487</v>
       </c>
-      <c r="B28" s="413"/>
+      <c r="B28" s="414"/>
       <c r="C28" s="213">
         <f>SUM(C18:C27)</f>
         <v>108.48299999999998</v>
@@ -46435,15 +46499,15 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A29" s="414" t="s">
+      <c r="A29" s="415" t="s">
         <v>488</v>
       </c>
-      <c r="B29" s="415"/>
-      <c r="C29" s="415"/>
-      <c r="D29" s="415"/>
-      <c r="E29" s="415"/>
-      <c r="F29" s="415"/>
-      <c r="G29" s="415"/>
+      <c r="B29" s="416"/>
+      <c r="C29" s="416"/>
+      <c r="D29" s="416"/>
+      <c r="E29" s="416"/>
+      <c r="F29" s="416"/>
+      <c r="G29" s="416"/>
     </row>
     <row r="30" spans="1:16" ht="32.25" customHeight="1">
       <c r="A30" s="98"/>
@@ -46815,15 +46879,15 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A43" s="406" t="s">
+      <c r="A43" s="407" t="s">
         <v>497</v>
       </c>
-      <c r="B43" s="407"/>
-      <c r="C43" s="407"/>
-      <c r="D43" s="407"/>
-      <c r="E43" s="407"/>
-      <c r="F43" s="407"/>
-      <c r="G43" s="407"/>
+      <c r="B43" s="408"/>
+      <c r="C43" s="408"/>
+      <c r="D43" s="408"/>
+      <c r="E43" s="408"/>
+      <c r="F43" s="408"/>
+      <c r="G43" s="408"/>
     </row>
     <row r="44" spans="1:7" ht="36.75" customHeight="1">
       <c r="A44" s="98"/>
@@ -47055,27 +47119,27 @@
       <c r="A2" s="382" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="423"/>
-      <c r="C2" s="424"/>
-      <c r="D2" s="426" t="s">
+      <c r="B2" s="424"/>
+      <c r="C2" s="425"/>
+      <c r="D2" s="427" t="s">
         <v>502</v>
       </c>
-      <c r="E2" s="427"/>
-      <c r="F2" s="427"/>
-      <c r="G2" s="427"/>
-      <c r="H2" s="427"/>
-      <c r="I2" s="427"/>
-      <c r="J2" s="427"/>
-      <c r="K2" s="427"/>
-      <c r="L2" s="427"/>
-      <c r="M2" s="427"/>
-      <c r="N2" s="427"/>
-      <c r="O2" s="427"/>
-      <c r="P2" s="427"/>
-      <c r="Q2" s="427"/>
-      <c r="R2" s="427"/>
-      <c r="S2" s="427"/>
-      <c r="T2" s="427"/>
+      <c r="E2" s="428"/>
+      <c r="F2" s="428"/>
+      <c r="G2" s="428"/>
+      <c r="H2" s="428"/>
+      <c r="I2" s="428"/>
+      <c r="J2" s="428"/>
+      <c r="K2" s="428"/>
+      <c r="L2" s="428"/>
+      <c r="M2" s="428"/>
+      <c r="N2" s="428"/>
+      <c r="O2" s="428"/>
+      <c r="P2" s="428"/>
+      <c r="Q2" s="428"/>
+      <c r="R2" s="428"/>
+      <c r="S2" s="428"/>
+      <c r="T2" s="428"/>
       <c r="AA2" s="132"/>
       <c r="BY2" s="190"/>
       <c r="BZ2" s="190"/>
@@ -47084,37 +47148,37 @@
       <c r="A3" s="384" t="s">
         <v>257</v>
       </c>
-      <c r="B3" s="423"/>
-      <c r="C3" s="424"/>
+      <c r="B3" s="424"/>
+      <c r="C3" s="425"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="428" t="s">
+      <c r="F3" s="429" t="s">
         <v>503</v>
       </c>
-      <c r="G3" s="429"/>
-      <c r="H3" s="430" t="s">
+      <c r="G3" s="430"/>
+      <c r="H3" s="431" t="s">
         <v>504</v>
       </c>
-      <c r="I3" s="430"/>
-      <c r="J3" s="431"/>
-      <c r="K3" s="432" t="s">
+      <c r="I3" s="431"/>
+      <c r="J3" s="432"/>
+      <c r="K3" s="433" t="s">
         <v>505</v>
       </c>
-      <c r="L3" s="433"/>
-      <c r="M3" s="434"/>
-      <c r="N3" s="431" t="s">
+      <c r="L3" s="434"/>
+      <c r="M3" s="435"/>
+      <c r="N3" s="432" t="s">
         <v>506</v>
       </c>
-      <c r="O3" s="435"/>
-      <c r="P3" s="436"/>
-      <c r="Q3" s="437" t="s">
+      <c r="O3" s="436"/>
+      <c r="P3" s="437"/>
+      <c r="Q3" s="438" t="s">
         <v>507</v>
       </c>
-      <c r="R3" s="438"/>
-      <c r="S3" s="439" t="s">
+      <c r="R3" s="439"/>
+      <c r="S3" s="440" t="s">
         <v>508</v>
       </c>
-      <c r="T3" s="440"/>
+      <c r="T3" s="441"/>
       <c r="AA3" s="133"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1">
@@ -47278,7 +47342,7 @@
       <c r="AC6" s="134"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1">
-      <c r="C7" s="417" t="str">
+      <c r="C7" s="418" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -47286,60 +47350,60 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="418"/>
-      <c r="E7" s="419"/>
-      <c r="F7" s="418" t="s">
+      <c r="D7" s="419"/>
+      <c r="E7" s="420"/>
+      <c r="F7" s="419" t="s">
         <v>531</v>
       </c>
-      <c r="G7" s="418"/>
-      <c r="H7" s="419"/>
-      <c r="I7" s="420" t="str">
+      <c r="G7" s="419"/>
+      <c r="H7" s="420"/>
+      <c r="I7" s="421" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$242.422)</v>
       </c>
-      <c r="J7" s="421"/>
-      <c r="K7" s="421"/>
-      <c r="L7" s="421"/>
-      <c r="M7" s="421"/>
-      <c r="N7" s="421"/>
-      <c r="O7" s="421"/>
-      <c r="P7" s="421"/>
-      <c r="Q7" s="421"/>
-      <c r="R7" s="422"/>
-      <c r="S7" s="417" t="str">
+      <c r="J7" s="422"/>
+      <c r="K7" s="422"/>
+      <c r="L7" s="422"/>
+      <c r="M7" s="422"/>
+      <c r="N7" s="422"/>
+      <c r="O7" s="422"/>
+      <c r="P7" s="422"/>
+      <c r="Q7" s="422"/>
+      <c r="R7" s="423"/>
+      <c r="S7" s="418" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$596.731)</v>
       </c>
-      <c r="T7" s="418"/>
-      <c r="U7" s="418"/>
-      <c r="V7" s="418"/>
-      <c r="W7" s="418"/>
-      <c r="X7" s="419"/>
-      <c r="Y7" s="417" t="s">
+      <c r="T7" s="419"/>
+      <c r="U7" s="419"/>
+      <c r="V7" s="419"/>
+      <c r="W7" s="419"/>
+      <c r="X7" s="420"/>
+      <c r="Y7" s="418" t="s">
         <v>532</v>
       </c>
-      <c r="Z7" s="419"/>
+      <c r="Z7" s="420"/>
       <c r="AA7" s="135"/>
-      <c r="AH7" s="441" t="s">
+      <c r="AH7" s="442" t="s">
         <v>533</v>
       </c>
-      <c r="AI7" s="442"/>
+      <c r="AI7" s="443"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="443" t="s">
+      <c r="AK7" s="444" t="s">
         <v>534</v>
       </c>
-      <c r="AL7" s="415"/>
-      <c r="AM7" s="415"/>
-      <c r="AN7" s="442"/>
-      <c r="AP7" s="444" t="s">
+      <c r="AL7" s="416"/>
+      <c r="AM7" s="416"/>
+      <c r="AN7" s="443"/>
+      <c r="AP7" s="445" t="s">
         <v>535</v>
       </c>
       <c r="AQ7" s="388"/>
-      <c r="AS7" s="425" t="s">
+      <c r="AS7" s="426" t="s">
         <v>536</v>
       </c>
       <c r="AT7" s="387"/>
@@ -47351,12 +47415,12 @@
       <c r="AZ7" s="387"/>
       <c r="BA7" s="387"/>
       <c r="BB7" s="388"/>
-      <c r="BD7" s="444" t="s">
+      <c r="BD7" s="445" t="s">
         <v>537</v>
       </c>
       <c r="BE7" s="388"/>
       <c r="BF7" s="190"/>
-      <c r="BG7" s="425" t="s">
+      <c r="BG7" s="426" t="s">
         <v>538</v>
       </c>
       <c r="BH7" s="387"/>
@@ -57305,17 +57369,17 @@
       <c r="BZ52" s="190"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1">
-      <c r="C53" s="416"/>
-      <c r="D53" s="416"/>
-      <c r="E53" s="416"/>
-      <c r="F53" s="416"/>
-      <c r="G53" s="416"/>
-      <c r="H53" s="416"/>
-      <c r="I53" s="416"/>
-      <c r="J53" s="416"/>
-      <c r="K53" s="416"/>
-      <c r="L53" s="416"/>
-      <c r="M53" s="416"/>
+      <c r="C53" s="417"/>
+      <c r="D53" s="417"/>
+      <c r="E53" s="417"/>
+      <c r="F53" s="417"/>
+      <c r="G53" s="417"/>
+      <c r="H53" s="417"/>
+      <c r="I53" s="417"/>
+      <c r="J53" s="417"/>
+      <c r="K53" s="417"/>
+      <c r="L53" s="417"/>
+      <c r="M53" s="417"/>
       <c r="AC53" s="137" t="s">
         <v>587</v>
       </c>

</xml_diff>

<commit_message>
fixed issue with guild prioritization
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3F13D8-7008-4848-846A-D1999F44607F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3701B8D0-75E8-D644-91B4-9F86757009A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -3498,7 +3498,7 @@
     <xf numFmtId="0" fontId="24" fillId="12" borderId="78"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="454">
+  <cellXfs count="455">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4666,6 +4666,9 @@
     </xf>
     <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="86">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -7633,7 +7636,7 @@
   </sheetPr>
   <dimension ref="A1:CP199"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="95" workbookViewId="0">
+    <sheetView zoomScale="95" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
@@ -14232,7 +14235,9 @@
   </sheetPr>
   <dimension ref="A1:BZ83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
@@ -14429,7 +14434,7 @@
     <row r="5" spans="1:78" s="20" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="333">
         <f>MAX(AA9:AA51)</f>
-        <v>2021</v>
+        <v>2034</v>
       </c>
       <c r="B5" s="327">
         <f>Y52-Q52</f>
@@ -14490,6 +14495,7 @@
       <c r="T5" s="200">
         <v>73</v>
       </c>
+      <c r="Z5" s="454"/>
       <c r="AA5" s="133"/>
     </row>
     <row r="6" spans="1:78" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -15094,28 +15100,28 @@
         <v>3.4508939020000007</v>
       </c>
       <c r="Z10" s="223">
-        <f t="shared" ref="Z10:Z51" si="25">X10-R10</f>
+        <f>X10-R10</f>
         <v>5.4258939020000003</v>
       </c>
       <c r="AA10" s="223">
-        <f>IF(SUM(AA$9:AA9)&gt;0,0,IF(SUM(X10-R10)&gt;0,B10,0))</f>
-        <v>2021</v>
+        <f>IF(SUM(AA$9:AA9)&gt;0,0,IF(AND(Z10&gt;0, MIN(Z11:Z$51)&gt;0),B10,0))</f>
+        <v>0</v>
       </c>
       <c r="AB10" s="223">
         <f>ABS(Z10)*1000000/SUM(U$9:U10)</f>
         <v>361.72626013333337</v>
       </c>
       <c r="AH10" s="19">
-        <f t="shared" ref="AH10:AH51" si="26">AH9+1</f>
+        <f t="shared" ref="AH10:AH51" si="25">AH9+1</f>
         <v>2019</v>
       </c>
       <c r="AI10" s="181">
-        <f t="shared" ref="AI10:AI51" si="27">IF($J$13= "A",AM10, IF($J$13 = "B",AN10,0))</f>
+        <f t="shared" ref="AI10:AI51" si="26">IF($J$13= "A",AM10, IF($J$13 = "B",AN10,0))</f>
         <v>0</v>
       </c>
       <c r="AJ10" s="13"/>
       <c r="AK10" s="19">
-        <f t="shared" ref="AK10:AK51" si="28">AK9+1</f>
+        <f t="shared" ref="AK10:AK51" si="27">AK9+1</f>
         <v>2019</v>
       </c>
       <c r="AL10" s="227"/>
@@ -15140,39 +15146,39 @@
         <v>2021</v>
       </c>
       <c r="AT10" s="29">
-        <f t="shared" ref="AT10:BB10" si="29">$M$9</f>
+        <f t="shared" ref="AT10:BB10" si="28">$M$9</f>
         <v>0</v>
       </c>
       <c r="AU10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AV10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AW10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AX10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AY10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AZ10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="BA10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="BB10" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="BC10" s="14"/>
@@ -15322,11 +15328,11 @@
         <v>-16.096964172945988</v>
       </c>
       <c r="Z11" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="Z10:Z51" si="29">X11-R11</f>
         <v>-10.671070270945989</v>
       </c>
-      <c r="AA11" s="216">
-        <f>IF(SUM(AA$9:AA10)&gt;0,0,IF(SUM(X11-R11)&gt;0,B11,0))</f>
+      <c r="AA11" s="223">
+        <f>IF(SUM(AA$9:AA10)&gt;0,0,IF(AND(Z11&gt;0, MIN(Z12:Z$51)&gt;0),B11,0))</f>
         <v>0</v>
       </c>
       <c r="AB11" s="216">
@@ -15334,16 +15340,16 @@
         <v>426.84281083783952</v>
       </c>
       <c r="AH11" s="17">
+        <f t="shared" si="25"/>
+        <v>2020</v>
+      </c>
+      <c r="AI11" s="182">
         <f t="shared" si="26"/>
-        <v>2020</v>
-      </c>
-      <c r="AI11" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="180"/>
       <c r="AK11" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2020</v>
       </c>
       <c r="AL11" s="222"/>
@@ -15545,11 +15551,11 @@
         <v>-102.57602609564437</v>
       </c>
       <c r="Z12" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-113.24709636659037</v>
       </c>
       <c r="AA12" s="223">
-        <f>IF(SUM(AA$9:AA11)&gt;0,0,IF(SUM(X12-R12)&gt;0,B12,0))</f>
+        <f>IF(SUM(AA$9:AA11)&gt;0,0,IF(AND(Z12&gt;0, MIN(Z13:Z$51)&gt;0),B12,0))</f>
         <v>0</v>
       </c>
       <c r="AB12" s="223">
@@ -15557,16 +15563,16 @@
         <v>2903.7717017074451</v>
       </c>
       <c r="AH12" s="19">
+        <f t="shared" si="25"/>
+        <v>2021</v>
+      </c>
+      <c r="AI12" s="181">
         <f t="shared" si="26"/>
-        <v>2021</v>
-      </c>
-      <c r="AI12" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="13"/>
       <c r="AK12" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2021</v>
       </c>
       <c r="AL12" s="228"/>
@@ -15773,11 +15779,11 @@
         <v>-36.225349969338453</v>
       </c>
       <c r="Z13" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-149.47244633592882</v>
       </c>
-      <c r="AA13" s="216">
-        <f>IF(SUM(AA$9:AA12)&gt;0,0,IF(SUM(X13-R13)&gt;0,B13,0))</f>
+      <c r="AA13" s="223">
+        <f>IF(SUM(AA$9:AA12)&gt;0,0,IF(AND(Z13&gt;0, MIN(Z14:Z$51)&gt;0),B13,0))</f>
         <v>0</v>
       </c>
       <c r="AB13" s="216">
@@ -15785,16 +15791,16 @@
         <v>2820.234836526959</v>
       </c>
       <c r="AH13" s="17">
+        <f t="shared" si="25"/>
+        <v>2022</v>
+      </c>
+      <c r="AI13" s="182">
         <f t="shared" si="26"/>
-        <v>2022</v>
-      </c>
-      <c r="AI13" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="180"/>
       <c r="AK13" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2022</v>
       </c>
       <c r="AL13" s="228"/>
@@ -15996,11 +16002,11 @@
         <v>11.949311395264216</v>
       </c>
       <c r="Z14" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-137.52313494066462</v>
       </c>
       <c r="AA14" s="223">
-        <f>IF(SUM(AA$9:AA13)&gt;0,0,IF(SUM(X14-R14)&gt;0,B14,0))</f>
+        <f>IF(SUM(AA$9:AA13)&gt;0,0,IF(AND(Z14&gt;0, MIN(Z15:Z$51)&gt;0),B14,0))</f>
         <v>0</v>
       </c>
       <c r="AB14" s="223">
@@ -16008,16 +16014,16 @@
         <v>2054.8345854105228</v>
       </c>
       <c r="AH14" s="19">
+        <f t="shared" si="25"/>
+        <v>2023</v>
+      </c>
+      <c r="AI14" s="181">
         <f t="shared" si="26"/>
-        <v>2023</v>
-      </c>
-      <c r="AI14" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="20"/>
       <c r="AK14" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2023</v>
       </c>
       <c r="AL14" s="228"/>
@@ -16224,11 +16230,11 @@
         <v>13.170628921191897</v>
       </c>
       <c r="Z15" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-124.3525060194727</v>
       </c>
-      <c r="AA15" s="216">
-        <f>IF(SUM(AA$9:AA14)&gt;0,0,IF(SUM(X15-R15)&gt;0,B15,0))</f>
+      <c r="AA15" s="223">
+        <f>IF(SUM(AA$9:AA14)&gt;0,0,IF(AND(Z15&gt;0, MIN(Z16:Z$51)&gt;0),B15,0))</f>
         <v>0</v>
       </c>
       <c r="AB15" s="216">
@@ -16236,16 +16242,16 @@
         <v>1538.0027294381312</v>
       </c>
       <c r="AH15" s="17">
+        <f t="shared" si="25"/>
+        <v>2024</v>
+      </c>
+      <c r="AI15" s="182">
         <f t="shared" si="26"/>
-        <v>2024</v>
-      </c>
-      <c r="AI15" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="184"/>
       <c r="AK15" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2024</v>
       </c>
       <c r="AL15" s="228"/>
@@ -16447,11 +16453,11 @@
         <v>14.180093855279438</v>
       </c>
       <c r="Z16" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-110.17241216419325</v>
       </c>
       <c r="AA16" s="223">
-        <f>IF(SUM(AA$9:AA15)&gt;0,0,IF(SUM(X16-R16)&gt;0,B16,0))</f>
+        <f>IF(SUM(AA$9:AA15)&gt;0,0,IF(AND(Z16&gt;0, MIN(Z17:Z$51)&gt;0),B16,0))</f>
         <v>0</v>
       </c>
       <c r="AB16" s="223">
@@ -16459,16 +16465,16 @@
         <v>1162.4031693279417</v>
       </c>
       <c r="AH16" s="19">
+        <f t="shared" si="25"/>
+        <v>2025</v>
+      </c>
+      <c r="AI16" s="181">
         <f t="shared" si="26"/>
-        <v>2025</v>
-      </c>
-      <c r="AI16" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="13"/>
       <c r="AK16" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2025</v>
       </c>
       <c r="AL16" s="228"/>
@@ -16675,11 +16681,11 @@
         <v>14.685145774514755</v>
       </c>
       <c r="Z17" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-95.487266389678496</v>
       </c>
-      <c r="AA17" s="216">
-        <f>IF(SUM(AA$9:AA16)&gt;0,0,IF(SUM(X17-R17)&gt;0,B17,0))</f>
+      <c r="AA17" s="223">
+        <f>IF(SUM(AA$9:AA16)&gt;0,0,IF(AND(Z17&gt;0, MIN(Z18:Z$51)&gt;0),B17,0))</f>
         <v>0</v>
       </c>
       <c r="AB17" s="216">
@@ -16687,16 +16693,16 @@
         <v>878.39532527360859</v>
       </c>
       <c r="AH17" s="17">
+        <f t="shared" si="25"/>
+        <v>2026</v>
+      </c>
+      <c r="AI17" s="182">
         <f t="shared" si="26"/>
-        <v>2026</v>
-      </c>
-      <c r="AI17" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="180"/>
       <c r="AK17" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2026</v>
       </c>
       <c r="AL17" s="228"/>
@@ -16898,11 +16904,11 @@
         <v>16.217608017026429</v>
       </c>
       <c r="Z18" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-79.26965837265206</v>
       </c>
       <c r="AA18" s="223">
-        <f>IF(SUM(AA$9:AA17)&gt;0,0,IF(SUM(X18-R18)&gt;0,B18,0))</f>
+        <f>IF(SUM(AA$9:AA17)&gt;0,0,IF(AND(Z18&gt;0, MIN(Z19:Z$51)&gt;0),B18,0))</f>
         <v>0</v>
       </c>
       <c r="AB18" s="223">
@@ -16910,16 +16916,16 @@
         <v>646.39690299559004</v>
       </c>
       <c r="AH18" s="19">
+        <f t="shared" si="25"/>
+        <v>2027</v>
+      </c>
+      <c r="AI18" s="181">
         <f t="shared" si="26"/>
-        <v>2027</v>
-      </c>
-      <c r="AI18" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ18" s="13"/>
       <c r="AK18" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2027</v>
       </c>
       <c r="AL18" s="228"/>
@@ -17126,11 +17132,11 @@
         <v>17.259370302929383</v>
       </c>
       <c r="Z19" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-62.010288069722662</v>
       </c>
-      <c r="AA19" s="216">
-        <f>IF(SUM(AA$9:AA18)&gt;0,0,IF(SUM(X19-R19)&gt;0,B19,0))</f>
+      <c r="AA19" s="223">
+        <f>IF(SUM(AA$9:AA18)&gt;0,0,IF(AND(Z19&gt;0, MIN(Z20:Z$51)&gt;0),B19,0))</f>
         <v>0</v>
       </c>
       <c r="AB19" s="216">
@@ -17138,16 +17144,16 @@
         <v>454.08914215202105</v>
       </c>
       <c r="AH19" s="17">
+        <f t="shared" si="25"/>
+        <v>2028</v>
+      </c>
+      <c r="AI19" s="182">
         <f t="shared" si="26"/>
-        <v>2028</v>
-      </c>
-      <c r="AI19" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="180"/>
       <c r="AK19" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2028</v>
       </c>
       <c r="AL19" s="228"/>
@@ -17352,11 +17358,11 @@
         <v>17.90780654392568</v>
       </c>
       <c r="Z20" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-44.102481525796975</v>
       </c>
       <c r="AA20" s="223">
-        <f>IF(SUM(AA$9:AA19)&gt;0,0,IF(SUM(X20-R20)&gt;0,B20,0))</f>
+        <f>IF(SUM(AA$9:AA19)&gt;0,0,IF(AND(Z20&gt;0, MIN(Z21:Z$51)&gt;0),B20,0))</f>
         <v>0</v>
       </c>
       <c r="AB20" s="223">
@@ -17364,16 +17370,16 @@
         <v>293.06633444728226</v>
       </c>
       <c r="AH20" s="19">
+        <f t="shared" si="25"/>
+        <v>2029</v>
+      </c>
+      <c r="AI20" s="181">
         <f t="shared" si="26"/>
-        <v>2029</v>
-      </c>
-      <c r="AI20" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ20" s="13"/>
       <c r="AK20" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2029</v>
       </c>
       <c r="AL20" s="228"/>
@@ -17578,11 +17584,11 @@
         <v>19.973261051854557</v>
       </c>
       <c r="Z21" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-24.129220473942439</v>
       </c>
-      <c r="AA21" s="216">
-        <f>IF(SUM(AA$9:AA20)&gt;0,0,IF(SUM(X21-R21)&gt;0,B21,0))</f>
+      <c r="AA21" s="223">
+        <f>IF(SUM(AA$9:AA20)&gt;0,0,IF(AND(Z21&gt;0, MIN(Z22:Z$51)&gt;0),B21,0))</f>
         <v>0</v>
       </c>
       <c r="AB21" s="216">
@@ -17590,16 +17596,16 @@
         <v>146.75983954238163</v>
       </c>
       <c r="AH21" s="17">
+        <f t="shared" si="25"/>
+        <v>2030</v>
+      </c>
+      <c r="AI21" s="182">
         <f t="shared" si="26"/>
-        <v>2030</v>
-      </c>
-      <c r="AI21" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="180"/>
       <c r="AK21" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2030</v>
       </c>
       <c r="AL21" s="228"/>
@@ -17801,11 +17807,11 @@
         <v>21.394473488391981</v>
       </c>
       <c r="Z22" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-2.7347469855504585</v>
       </c>
       <c r="AA22" s="223">
-        <f>IF(SUM(AA$9:AA21)&gt;0,0,IF(SUM(X22-R22)&gt;0,B22,0))</f>
+        <f>IF(SUM(AA$9:AA21)&gt;0,0,IF(AND(Z22&gt;0, MIN(Z23:Z$51)&gt;0),B22,0))</f>
         <v>0</v>
       </c>
       <c r="AB22" s="223">
@@ -17813,16 +17819,16 @@
         <v>15.334492130942543</v>
       </c>
       <c r="AH22" s="19">
+        <f t="shared" si="25"/>
+        <v>2031</v>
+      </c>
+      <c r="AI22" s="181">
         <f t="shared" si="26"/>
-        <v>2031</v>
-      </c>
-      <c r="AI22" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ22" s="13"/>
       <c r="AK22" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2031</v>
       </c>
       <c r="AL22" s="228"/>
@@ -18029,28 +18035,28 @@
         <v>21.976346455165356</v>
       </c>
       <c r="Z23" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>19.241599469614897</v>
       </c>
-      <c r="AA23" s="216">
-        <f>IF(SUM(AA$9:AA22)&gt;0,0,IF(SUM(X23-R23)&gt;0,B23,0))</f>
-        <v>0</v>
+      <c r="AA23" s="223">
+        <f>IF(SUM(AA$9:AA22)&gt;0,0,IF(AND(Z23&gt;0, MIN(Z24:Z$51)&gt;0),B23,0))</f>
+        <v>2034</v>
       </c>
       <c r="AB23" s="216">
         <f>ABS(Z23)*1000000/SUM(U$9:U23)</f>
         <v>100.0779063027361</v>
       </c>
       <c r="AH23" s="17">
+        <f t="shared" si="25"/>
+        <v>2032</v>
+      </c>
+      <c r="AI23" s="182">
         <f t="shared" si="26"/>
-        <v>2032</v>
-      </c>
-      <c r="AI23" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ23" s="180"/>
       <c r="AK23" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2032</v>
       </c>
       <c r="AL23" s="228"/>
@@ -18252,11 +18258,11 @@
         <v>24.880093758829005</v>
       </c>
       <c r="Z24" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>44.121693228443917</v>
       </c>
       <c r="AA24" s="223">
-        <f>IF(SUM(AA$9:AA23)&gt;0,0,IF(SUM(X24-R24)&gt;0,B24,0))</f>
+        <f>IF(SUM(AA$9:AA23)&gt;0,0,IF(AND(Z24&gt;0, MIN(Z25:Z$51)&gt;0),B24,0))</f>
         <v>0</v>
       </c>
       <c r="AB24" s="223">
@@ -18264,16 +18270,16 @@
         <v>213.98267666674366</v>
       </c>
       <c r="AH24" s="19">
+        <f t="shared" si="25"/>
+        <v>2033</v>
+      </c>
+      <c r="AI24" s="181">
         <f t="shared" si="26"/>
-        <v>2033</v>
-      </c>
-      <c r="AI24" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ24" s="13"/>
       <c r="AK24" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2033</v>
       </c>
       <c r="AL24" s="228"/>
@@ -18480,11 +18486,11 @@
         <v>25.565503401620141</v>
       </c>
       <c r="Z25" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>69.687196630064079</v>
       </c>
-      <c r="AA25" s="216">
-        <f>IF(SUM(AA$9:AA24)&gt;0,0,IF(SUM(X25-R25)&gt;0,B25,0))</f>
+      <c r="AA25" s="223">
+        <f>IF(SUM(AA$9:AA24)&gt;0,0,IF(AND(Z25&gt;0, MIN(Z26:Z$51)&gt;0),B25,0))</f>
         <v>0</v>
       </c>
       <c r="AB25" s="216">
@@ -18492,16 +18498,16 @@
         <v>316.58809369002017</v>
       </c>
       <c r="AH25" s="17">
+        <f t="shared" si="25"/>
+        <v>2034</v>
+      </c>
+      <c r="AI25" s="182">
         <f t="shared" si="26"/>
-        <v>2034</v>
-      </c>
-      <c r="AI25" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ25" s="180"/>
       <c r="AK25" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2034</v>
       </c>
       <c r="AL25" s="228"/>
@@ -18703,11 +18709,11 @@
         <v>25.313686137430359</v>
       </c>
       <c r="Z26" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>95.00088276749446</v>
       </c>
       <c r="AA26" s="223">
-        <f>IF(SUM(AA$9:AA25)&gt;0,0,IF(SUM(X26-R26)&gt;0,B26,0))</f>
+        <f>IF(SUM(AA$9:AA25)&gt;0,0,IF(AND(Z26&gt;0, MIN(Z27:Z$51)&gt;0),B26,0))</f>
         <v>0</v>
       </c>
       <c r="AB26" s="223">
@@ -18715,16 +18721,16 @@
         <v>405.90676453506211</v>
       </c>
       <c r="AH26" s="19">
+        <f t="shared" si="25"/>
+        <v>2035</v>
+      </c>
+      <c r="AI26" s="181">
         <f t="shared" si="26"/>
-        <v>2035</v>
-      </c>
-      <c r="AI26" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ26" s="13"/>
       <c r="AK26" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2035</v>
       </c>
       <c r="AL26" s="228"/>
@@ -18931,11 +18937,11 @@
         <v>27.076942327877223</v>
       </c>
       <c r="Z27" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>122.07782509537168</v>
       </c>
-      <c r="AA27" s="216">
-        <f>IF(SUM(AA$9:AA26)&gt;0,0,IF(SUM(X27-R27)&gt;0,B27,0))</f>
+      <c r="AA27" s="223">
+        <f>IF(SUM(AA$9:AA26)&gt;0,0,IF(AND(Z27&gt;0, MIN(Z28:Z$51)&gt;0),B27,0))</f>
         <v>0</v>
       </c>
       <c r="AB27" s="216">
@@ -18943,16 +18949,16 @@
         <v>492.30350751174279</v>
       </c>
       <c r="AH27" s="17">
+        <f t="shared" si="25"/>
+        <v>2036</v>
+      </c>
+      <c r="AI27" s="182">
         <f t="shared" si="26"/>
-        <v>2036</v>
-      </c>
-      <c r="AI27" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ27" s="180"/>
       <c r="AK27" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2036</v>
       </c>
       <c r="AL27" s="228"/>
@@ -19154,11 +19160,11 @@
         <v>27.902680094990416</v>
       </c>
       <c r="Z28" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>149.98050519036212</v>
       </c>
       <c r="AA28" s="223">
-        <f>IF(SUM(AA$9:AA27)&gt;0,0,IF(SUM(X28-R28)&gt;0,B28,0))</f>
+        <f>IF(SUM(AA$9:AA27)&gt;0,0,IF(AND(Z28&gt;0, MIN(Z29:Z$51)&gt;0),B28,0))</f>
         <v>0</v>
       </c>
       <c r="AB28" s="223">
@@ -19166,16 +19172,16 @@
         <v>572.66475703928165</v>
       </c>
       <c r="AH28" s="19">
+        <f t="shared" si="25"/>
+        <v>2037</v>
+      </c>
+      <c r="AI28" s="181">
         <f t="shared" si="26"/>
-        <v>2037</v>
-      </c>
-      <c r="AI28" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ28" s="13"/>
       <c r="AK28" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2037</v>
       </c>
       <c r="AL28" s="228"/>
@@ -19382,11 +19388,11 @@
         <v>27.804672538107951</v>
       </c>
       <c r="Z29" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>177.7851777284701</v>
       </c>
-      <c r="AA29" s="216">
-        <f>IF(SUM(AA$9:AA28)&gt;0,0,IF(SUM(X29-R29)&gt;0,B29,0))</f>
+      <c r="AA29" s="223">
+        <f>IF(SUM(AA$9:AA28)&gt;0,0,IF(AND(Z29&gt;0, MIN(Z30:Z$51)&gt;0),B29,0))</f>
         <v>0</v>
       </c>
       <c r="AB29" s="216">
@@ -19394,16 +19400,16 @@
         <v>644.55570491851267</v>
       </c>
       <c r="AH29" s="17">
+        <f t="shared" si="25"/>
+        <v>2038</v>
+      </c>
+      <c r="AI29" s="182">
         <f t="shared" si="26"/>
-        <v>2038</v>
-      </c>
-      <c r="AI29" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ29" s="180"/>
       <c r="AK29" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2038</v>
       </c>
       <c r="AL29" s="228"/>
@@ -19605,11 +19611,11 @@
         <v>29.267269847649153</v>
       </c>
       <c r="Z30" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>207.05244757611925</v>
       </c>
       <c r="AA30" s="223">
-        <f>IF(SUM(AA$9:AA29)&gt;0,0,IF(SUM(X30-R30)&gt;0,B30,0))</f>
+        <f>IF(SUM(AA$9:AA29)&gt;0,0,IF(AND(Z30&gt;0, MIN(Z31:Z$51)&gt;0),B30,0))</f>
         <v>0</v>
       </c>
       <c r="AB30" s="223">
@@ -19617,16 +19623,16 @@
         <v>714.58368864109752</v>
       </c>
       <c r="AH30" s="19">
+        <f t="shared" si="25"/>
+        <v>2039</v>
+      </c>
+      <c r="AI30" s="181">
         <f t="shared" si="26"/>
-        <v>2039</v>
-      </c>
-      <c r="AI30" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ30" s="13"/>
       <c r="AK30" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2039</v>
       </c>
       <c r="AL30" s="228">
@@ -19838,11 +19844,11 @@
         <v>30.805311889936988</v>
       </c>
       <c r="Z31" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>237.85775946605628</v>
       </c>
-      <c r="AA31" s="216">
-        <f>IF(SUM(AA$9:AA30)&gt;0,0,IF(SUM(X31-R31)&gt;0,B31,0))</f>
+      <c r="AA31" s="223">
+        <f>IF(SUM(AA$9:AA30)&gt;0,0,IF(AND(Z31&gt;0, MIN(Z32:Z$51)&gt;0),B31,0))</f>
         <v>0</v>
       </c>
       <c r="AB31" s="216">
@@ -19850,16 +19856,16 @@
         <v>783.25344851215993</v>
       </c>
       <c r="AH31" s="17">
+        <f t="shared" si="25"/>
+        <v>2040</v>
+      </c>
+      <c r="AI31" s="182">
         <f t="shared" si="26"/>
-        <v>2040</v>
-      </c>
-      <c r="AI31" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="180"/>
       <c r="AK31" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2040</v>
       </c>
       <c r="AL31" s="228">
@@ -20066,11 +20072,11 @@
         <v>32.422646105898487</v>
       </c>
       <c r="Z32" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>270.28040557195476</v>
       </c>
       <c r="AA32" s="223">
-        <f>IF(SUM(AA$9:AA31)&gt;0,0,IF(SUM(X32-R32)&gt;0,B32,0))</f>
+        <f>IF(SUM(AA$9:AA31)&gt;0,0,IF(AND(Z32&gt;0, MIN(Z33:Z$51)&gt;0),B32,0))</f>
         <v>0</v>
       </c>
       <c r="AB32" s="223">
@@ -20078,16 +20084,16 @@
         <v>850.9933097753775</v>
       </c>
       <c r="AH32" s="19">
+        <f t="shared" si="25"/>
+        <v>2041</v>
+      </c>
+      <c r="AI32" s="181">
         <f t="shared" si="26"/>
-        <v>2041</v>
-      </c>
-      <c r="AI32" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ32" s="189"/>
       <c r="AK32" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2041</v>
       </c>
       <c r="AL32" s="228">
@@ -20299,11 +20305,11 @@
         <v>34.123314794966618</v>
       </c>
       <c r="Z33" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>304.40372036692133</v>
       </c>
-      <c r="AA33" s="216">
-        <f>IF(SUM(AA$9:AA32)&gt;0,0,IF(SUM(X33-R33)&gt;0,B33,0))</f>
+      <c r="AA33" s="223">
+        <f>IF(SUM(AA$9:AA32)&gt;0,0,IF(AND(Z33&gt;0, MIN(Z34:Z$51)&gt;0),B33,0))</f>
         <v>0</v>
       </c>
       <c r="AB33" s="216">
@@ -20311,15 +20317,15 @@
         <v>918.17182013063359</v>
       </c>
       <c r="AH33" s="17">
+        <f t="shared" si="25"/>
+        <v>2042</v>
+      </c>
+      <c r="AI33" s="182">
         <f t="shared" si="26"/>
-        <v>2042</v>
-      </c>
-      <c r="AI33" s="182">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="17">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="AK33" s="17">
-        <f t="shared" si="28"/>
         <v>2042</v>
       </c>
       <c r="AL33" s="228">
@@ -20526,11 +20532,11 @@
         <v>35.911564941812529</v>
       </c>
       <c r="Z34" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>340.31528530873391</v>
       </c>
       <c r="AA34" s="223">
-        <f>IF(SUM(AA$9:AA33)&gt;0,0,IF(SUM(X34-R34)&gt;0,B34,0))</f>
+        <f>IF(SUM(AA$9:AA33)&gt;0,0,IF(AND(Z34&gt;0, MIN(Z35:Z$51)&gt;0),B34,0))</f>
         <v>0</v>
       </c>
       <c r="AB34" s="223">
@@ -20538,16 +20544,16 @@
         <v>985.11039140985815</v>
       </c>
       <c r="AH34" s="19">
+        <f t="shared" si="25"/>
+        <v>2043</v>
+      </c>
+      <c r="AI34" s="181">
         <f t="shared" si="26"/>
-        <v>2043</v>
-      </c>
-      <c r="AI34" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ34" s="13"/>
       <c r="AK34" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2043</v>
       </c>
       <c r="AL34" s="228">
@@ -20759,11 +20765,11 @@
         <v>37.791858537297287</v>
       </c>
       <c r="Z35" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>378.10714384603119</v>
       </c>
-      <c r="AA35" s="216">
-        <f>IF(SUM(AA$9:AA34)&gt;0,0,IF(SUM(X35-R35)&gt;0,B35,0))</f>
+      <c r="AA35" s="223">
+        <f>IF(SUM(AA$9:AA34)&gt;0,0,IF(AND(Z35&gt;0, MIN(Z36:Z$51)&gt;0),B35,0))</f>
         <v>0</v>
       </c>
       <c r="AB35" s="216">
@@ -20771,16 +20777,16 @@
         <v>1052.0930306915252</v>
       </c>
       <c r="AH35" s="17">
+        <f t="shared" si="25"/>
+        <v>2044</v>
+      </c>
+      <c r="AI35" s="182">
         <f t="shared" si="26"/>
-        <v>2044</v>
-      </c>
-      <c r="AI35" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ35" s="180"/>
       <c r="AK35" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2044</v>
       </c>
       <c r="AL35" s="228">
@@ -20987,11 +20993,11 @@
         <v>39.768883418455097</v>
       </c>
       <c r="Z36" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>417.87602726448631</v>
       </c>
       <c r="AA36" s="223">
-        <f>IF(SUM(AA$9:AA35)&gt;0,0,IF(SUM(X36-R36)&gt;0,B36,0))</f>
+        <f>IF(SUM(AA$9:AA35)&gt;0,0,IF(AND(Z36&gt;0, MIN(Z37:Z$51)&gt;0),B36,0))</f>
         <v>0</v>
       </c>
       <c r="AB36" s="223">
@@ -20999,16 +21005,16 @@
         <v>1119.3739223048462</v>
       </c>
       <c r="AH36" s="19">
+        <f t="shared" si="25"/>
+        <v>2045</v>
+      </c>
+      <c r="AI36" s="181">
         <f t="shared" si="26"/>
-        <v>2045</v>
-      </c>
-      <c r="AI36" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="13"/>
       <c r="AK36" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2045</v>
       </c>
       <c r="AL36" s="228">
@@ -21220,11 +21226,11 @@
         <v>41.847564653564447</v>
       </c>
       <c r="Z37" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>459.72359191805077</v>
       </c>
-      <c r="AA37" s="216">
-        <f>IF(SUM(AA$9:AA36)&gt;0,0,IF(SUM(X37-R37)&gt;0,B37,0))</f>
+      <c r="AA37" s="223">
+        <f>IF(SUM(AA$9:AA36)&gt;0,0,IF(AND(Z37&gt;0, MIN(Z38:Z$51)&gt;0),B37,0))</f>
         <v>0</v>
       </c>
       <c r="AB37" s="216">
@@ -21232,16 +21238,16 @@
         <v>1187.1834031639864</v>
       </c>
       <c r="AH37" s="17">
+        <f t="shared" si="25"/>
+        <v>2046</v>
+      </c>
+      <c r="AI37" s="182">
         <f t="shared" si="26"/>
-        <v>2046</v>
-      </c>
-      <c r="AI37" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ37" s="180"/>
       <c r="AK37" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2046</v>
       </c>
       <c r="AL37" s="228">
@@ -21451,11 +21457,11 @@
         <v>44.033076499670308</v>
       </c>
       <c r="Z38" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>503.75666841772107</v>
       </c>
       <c r="AA38" s="223">
-        <f>IF(SUM(AA$9:AA37)&gt;0,0,IF(SUM(X38-R38)&gt;0,B38,0))</f>
+        <f>IF(SUM(AA$9:AA37)&gt;0,0,IF(AND(Z38&gt;0, MIN(Z39:Z$51)&gt;0),B38,0))</f>
         <v>0</v>
       </c>
       <c r="AB38" s="223">
@@ -21468,16 +21474,16 @@
       <c r="AF38" s="189"/>
       <c r="AG38" s="189"/>
       <c r="AH38" s="19">
+        <f t="shared" si="25"/>
+        <v>2047</v>
+      </c>
+      <c r="AI38" s="181">
         <f t="shared" si="26"/>
-        <v>2047</v>
-      </c>
-      <c r="AI38" s="181">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ38" s="189"/>
       <c r="AK38" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2047</v>
       </c>
       <c r="AL38" s="228">
@@ -21704,11 +21710,11 @@
         <v>46.330854961292353</v>
       </c>
       <c r="Z39" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>550.08752337901342</v>
       </c>
-      <c r="AA39" s="216">
-        <f>IF(SUM(AA$9:AA38)&gt;0,0,IF(SUM(X39-R39)&gt;0,B39,0))</f>
+      <c r="AA39" s="223">
+        <f>IF(SUM(AA$9:AA38)&gt;0,0,IF(AND(Z39&gt;0, MIN(Z40:Z$51)&gt;0),B39,0))</f>
         <v>0</v>
       </c>
       <c r="AB39" s="216">
@@ -21716,16 +21722,16 @@
         <v>1325.2178782907513</v>
       </c>
       <c r="AH39" s="17">
+        <f t="shared" si="25"/>
+        <v>2048</v>
+      </c>
+      <c r="AI39" s="182">
         <f t="shared" si="26"/>
-        <v>2048</v>
-      </c>
-      <c r="AI39" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ39" s="180"/>
       <c r="AK39" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2048</v>
       </c>
       <c r="AL39" s="228">
@@ -21932,11 +21938,11 @@
         <v>48.746610980495056</v>
       </c>
       <c r="Z40" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>598.83413435950843</v>
       </c>
       <c r="AA40" s="223">
-        <f>IF(SUM(AA$9:AA39)&gt;0,0,IF(SUM(X40-R40)&gt;0,B40,0))</f>
+        <f>IF(SUM(AA$9:AA39)&gt;0,0,IF(AND(Z40&gt;0, MIN(Z41:Z$51)&gt;0),B40,0))</f>
         <v>0</v>
       </c>
       <c r="AB40" s="223">
@@ -21944,16 +21950,16 @@
         <v>1395.8227260993663</v>
       </c>
       <c r="AH40" s="17">
+        <f t="shared" si="25"/>
+        <v>2049</v>
+      </c>
+      <c r="AI40" s="182">
         <f t="shared" si="26"/>
-        <v>2049</v>
-      </c>
-      <c r="AI40" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ40" s="180"/>
       <c r="AK40" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2049</v>
       </c>
       <c r="AL40" s="228">
@@ -22165,11 +22171,11 @@
         <v>51.286344290008465</v>
       </c>
       <c r="Z41" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>650.12047864951683</v>
       </c>
-      <c r="AA41" s="216">
-        <f>IF(SUM(AA$9:AA40)&gt;0,0,IF(SUM(X41-R41)&gt;0,B41,0))</f>
+      <c r="AA41" s="223">
+        <f>IF(SUM(AA$9:AA40)&gt;0,0,IF(AND(Z41&gt;0, MIN(Z42:Z$51)&gt;0),B41,0))</f>
         <v>0</v>
       </c>
       <c r="AB41" s="216">
@@ -22177,16 +22183,16 @@
         <v>1467.7215470755323</v>
       </c>
       <c r="AH41" s="17">
+        <f t="shared" si="25"/>
+        <v>2050</v>
+      </c>
+      <c r="AI41" s="182">
         <f t="shared" si="26"/>
-        <v>2050</v>
-      </c>
-      <c r="AI41" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ41" s="180"/>
       <c r="AK41" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2050</v>
       </c>
       <c r="AL41" s="228">
@@ -22393,11 +22399,11 @@
         <v>53.956357962677245</v>
       </c>
       <c r="Z42" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>704.07683661219426</v>
       </c>
       <c r="AA42" s="223">
-        <f>IF(SUM(AA$9:AA41)&gt;0,0,IF(SUM(X42-R42)&gt;0,B42,0))</f>
+        <f>IF(SUM(AA$9:AA41)&gt;0,0,IF(AND(Z42&gt;0, MIN(Z43:Z$51)&gt;0),B42,0))</f>
         <v>0</v>
       </c>
       <c r="AB42" s="223">
@@ -22405,16 +22411,16 @@
         <v>1541.0811676879914</v>
       </c>
       <c r="AH42" s="17">
+        <f t="shared" si="25"/>
+        <v>2051</v>
+      </c>
+      <c r="AI42" s="182">
         <f t="shared" si="26"/>
-        <v>2051</v>
-      </c>
-      <c r="AI42" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ42" s="180"/>
       <c r="AK42" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2051</v>
       </c>
       <c r="AL42" s="228">
@@ -22626,11 +22632,11 @@
         <v>56.763273692184185</v>
       </c>
       <c r="Z43" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>760.84011030437841</v>
       </c>
-      <c r="AA43" s="216">
-        <f>IF(SUM(AA$9:AA42)&gt;0,0,IF(SUM(X43-R43)&gt;0,B43,0))</f>
+      <c r="AA43" s="223">
+        <f>IF(SUM(AA$9:AA42)&gt;0,0,IF(AND(Z43&gt;0, MIN(Z44:Z$51)&gt;0),B43,0))</f>
         <v>0</v>
       </c>
       <c r="AB43" s="216">
@@ -22638,16 +22644,16 @@
         <v>1616.0627397454084</v>
       </c>
       <c r="AH43" s="17">
+        <f t="shared" si="25"/>
+        <v>2052</v>
+      </c>
+      <c r="AI43" s="182">
         <f t="shared" si="26"/>
-        <v>2052</v>
-      </c>
-      <c r="AI43" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ43" s="180"/>
       <c r="AK43" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2052</v>
       </c>
       <c r="AL43" s="228">
@@ -22854,11 +22860,11 @@
         <v>59.714047841745725</v>
       </c>
       <c r="Z44" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>820.55415814612411</v>
       </c>
       <c r="AA44" s="223">
-        <f>IF(SUM(AA$9:AA43)&gt;0,0,IF(SUM(X44-R44)&gt;0,B44,0))</f>
+        <f>IF(SUM(AA$9:AA43)&gt;0,0,IF(AND(Z44&gt;0, MIN(Z45:Z$51)&gt;0),B44,0))</f>
         <v>0</v>
       </c>
       <c r="AB44" s="223">
@@ -22866,16 +22872,16 @@
         <v>1692.8232460198942</v>
       </c>
       <c r="AH44" s="17">
+        <f t="shared" si="25"/>
+        <v>2053</v>
+      </c>
+      <c r="AI44" s="182">
         <f t="shared" si="26"/>
-        <v>2053</v>
-      </c>
-      <c r="AI44" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ44" s="180"/>
       <c r="AK44" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2053</v>
       </c>
       <c r="AL44" s="228">
@@ -23087,11 +23093,11 @@
         <v>62.815988299317503</v>
       </c>
       <c r="Z45" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>883.37014644544172</v>
       </c>
-      <c r="AA45" s="216">
-        <f>IF(SUM(AA$9:AA44)&gt;0,0,IF(SUM(X45-R45)&gt;0,B45,0))</f>
+      <c r="AA45" s="223">
+        <f>IF(SUM(AA$9:AA44)&gt;0,0,IF(AND(Z45&gt;0, MIN(Z46:Z$51)&gt;0),B45,0))</f>
         <v>0</v>
       </c>
       <c r="AB45" s="216">
@@ -23099,16 +23105,16 @@
         <v>1771.516787372836</v>
       </c>
       <c r="AH45" s="17">
+        <f t="shared" si="25"/>
+        <v>2054</v>
+      </c>
+      <c r="AI45" s="182">
         <f t="shared" si="26"/>
-        <v>2054</v>
-      </c>
-      <c r="AI45" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ45" s="180"/>
       <c r="AK45" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2054</v>
       </c>
       <c r="AL45" s="228">
@@ -23315,11 +23321,11 @@
         <v>66.076772179779297</v>
       </c>
       <c r="Z46" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>949.44691862522086</v>
       </c>
       <c r="AA46" s="223">
-        <f>IF(SUM(AA$9:AA45)&gt;0,0,IF(SUM(X46-R46)&gt;0,B46,0))</f>
+        <f>IF(SUM(AA$9:AA45)&gt;0,0,IF(AND(Z46&gt;0, MIN(Z47:Z$51)&gt;0),B46,0))</f>
         <v>0</v>
       </c>
       <c r="AB46" s="223">
@@ -23327,16 +23333,16 @@
         <v>1852.2956945910933</v>
       </c>
       <c r="AH46" s="17">
+        <f t="shared" si="25"/>
+        <v>2055</v>
+      </c>
+      <c r="AI46" s="182">
         <f t="shared" si="26"/>
-        <v>2055</v>
-      </c>
-      <c r="AI46" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ46" s="180"/>
       <c r="AK46" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2055</v>
       </c>
       <c r="AL46" s="228">
@@ -23548,11 +23554,11 @@
         <v>69.50446441659787</v>
       </c>
       <c r="Z47" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1018.9513830418189</v>
       </c>
-      <c r="AA47" s="216">
-        <f>IF(SUM(AA$9:AA46)&gt;0,0,IF(SUM(X47-R47)&gt;0,B47,0))</f>
+      <c r="AA47" s="223">
+        <f>IF(SUM(AA$9:AA46)&gt;0,0,IF(AND(Z47&gt;0, MIN(Z48:Z$51)&gt;0),B47,0))</f>
         <v>0</v>
       </c>
       <c r="AB47" s="216">
@@ -23560,16 +23566,16 @@
         <v>1935.3114990791464</v>
       </c>
       <c r="AH47" s="17">
+        <f t="shared" si="25"/>
+        <v>2056</v>
+      </c>
+      <c r="AI47" s="182">
         <f t="shared" si="26"/>
-        <v>2056</v>
-      </c>
-      <c r="AI47" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ47" s="180"/>
       <c r="AK47" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2056</v>
       </c>
       <c r="AL47" s="228">
@@ -23776,11 +23782,11 @@
         <v>73.107537287595804</v>
       </c>
       <c r="Z48" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1092.0589203294146</v>
       </c>
       <c r="AA48" s="223">
-        <f>IF(SUM(AA$9:AA47)&gt;0,0,IF(SUM(X48-R48)&gt;0,B48,0))</f>
+        <f>IF(SUM(AA$9:AA47)&gt;0,0,IF(AND(Z48&gt;0, MIN(Z49:Z$51)&gt;0),B48,0))</f>
         <v>0</v>
       </c>
       <c r="AB48" s="223">
@@ -23788,16 +23794,16 @@
         <v>2020.7157895960515</v>
       </c>
       <c r="AH48" s="17">
+        <f t="shared" si="25"/>
+        <v>2057</v>
+      </c>
+      <c r="AI48" s="182">
         <f t="shared" si="26"/>
-        <v>2057</v>
-      </c>
-      <c r="AI48" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ48" s="180"/>
       <c r="AK48" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2057</v>
       </c>
       <c r="AL48" s="228">
@@ -24009,11 +24015,11 @@
         <v>76.894890921692365</v>
       </c>
       <c r="Z49" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1168.9538112511068</v>
       </c>
-      <c r="AA49" s="216">
-        <f>IF(SUM(AA$9:AA48)&gt;0,0,IF(SUM(X49-R49)&gt;0,B49,0))</f>
+      <c r="AA49" s="223">
+        <f>IF(SUM(AA$9:AA48)&gt;0,0,IF(AND(Z49&gt;0, MIN(Z50:Z$51)&gt;0),B49,0))</f>
         <v>0</v>
       </c>
       <c r="AB49" s="216">
@@ -24021,16 +24027,16 @@
         <v>2108.6609768462936</v>
       </c>
       <c r="AH49" s="17">
+        <f t="shared" si="25"/>
+        <v>2058</v>
+      </c>
+      <c r="AI49" s="182">
         <f t="shared" si="26"/>
-        <v>2058</v>
-      </c>
-      <c r="AI49" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ49" s="180"/>
       <c r="AK49" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2058</v>
       </c>
       <c r="AL49" s="228">
@@ -24237,11 +24243,11 @@
         <v>80.8758748358307</v>
       </c>
       <c r="Z50" s="223">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1249.8296860869375</v>
       </c>
       <c r="AA50" s="223">
-        <f>IF(SUM(AA$9:AA49)&gt;0,0,IF(SUM(X50-R50)&gt;0,B50,0))</f>
+        <f>IF(SUM(AA$9:AA49)&gt;0,0,IF(AND(Z50&gt;0, MIN(Z51:Z$51)&gt;0),B50,0))</f>
         <v>0</v>
       </c>
       <c r="AB50" s="223">
@@ -24249,16 +24255,16 @@
         <v>2199.3009835445168</v>
       </c>
       <c r="AH50" s="17">
+        <f t="shared" si="25"/>
+        <v>2059</v>
+      </c>
+      <c r="AI50" s="182">
         <f t="shared" si="26"/>
-        <v>2059</v>
-      </c>
-      <c r="AI50" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ50" s="180"/>
       <c r="AK50" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2059</v>
       </c>
       <c r="AL50" s="228">
@@ -24470,11 +24476,11 @@
         <v>85.060310553772808</v>
       </c>
       <c r="Z51" s="216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1334.8899966407103</v>
       </c>
-      <c r="AA51" s="216">
-        <f>IF(SUM(AA$9:AA50)&gt;0,0,IF(SUM(X51-R51)&gt;0,B51,0))</f>
+      <c r="AA51" s="223">
+        <f>IF(SUM(AA$9:AA50)&gt;0,0,IF(AND(Z51&gt;0, MIN(Z$51:Z52)&gt;0),B51,0))</f>
         <v>0</v>
       </c>
       <c r="AB51" s="216">
@@ -24482,16 +24488,16 @@
         <v>2292.7918742911006</v>
       </c>
       <c r="AH51" s="17">
+        <f t="shared" si="25"/>
+        <v>2060</v>
+      </c>
+      <c r="AI51" s="182">
         <f t="shared" si="26"/>
-        <v>2060</v>
-      </c>
-      <c r="AI51" s="182">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ51" s="180"/>
       <c r="AK51" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2060</v>
       </c>
       <c r="AL51" s="228">
@@ -24750,7 +24756,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24799,7 +24805,7 @@
         <v>272</v>
       </c>
       <c r="B4" s="109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="243" t="s">
         <v>273</v>
@@ -24813,7 +24819,7 @@
         <v>274</v>
       </c>
       <c r="B5" s="109">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="C5" s="243" t="s">
         <v>273</v>
@@ -26156,7 +26162,7 @@
   </sheetPr>
   <dimension ref="A1:AB186"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -39195,7 +39201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC2A0AA-4720-724C-873E-D9D973DEB249}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
updated constraints in LAUNCHPAD after audit with A. Agahi
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047384AE-F775-3849-91D9-F6F0C23D4CF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB67FE7-7038-4A4D-AD33-B48AF79E7288}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
+    <workbookView xWindow="43580" yWindow="1320" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="616">
   <si>
     <t>Scenario</t>
   </si>
@@ -2087,6 +2087,9 @@
   </si>
   <si>
     <t>habitat values for DWM are not used, since each DWM area has as-built habitat values assigned.</t>
+  </si>
+  <si>
+    <t>* current configuration from "DCA Prescriptions"</t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="82">
+  <borders count="83">
     <border>
       <left/>
       <right/>
@@ -3445,6 +3448,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3534,7 +3552,7 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="78"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="493">
+  <cellXfs count="494">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4522,15 +4540,25 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="82" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4772,13 +4800,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="86">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -8163,8 +8184,8 @@
   </sheetPr>
   <dimension ref="A1:CP191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21:K189"/>
+    <sheetView topLeftCell="A34" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9017,10 +9038,10 @@
       <c r="I21" s="128" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="490" t="s">
+      <c r="J21" s="405" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="491"/>
+      <c r="K21" s="406"/>
       <c r="L21" s="253"/>
       <c r="M21" s="124"/>
       <c r="N21" s="124"/>
@@ -9555,7 +9576,7 @@
         <f>IF(EXACT(G37, H37), "none", IF(ISNUMBER(MATCH(H37, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K37" s="492"/>
+      <c r="K37" s="407"/>
       <c r="L37" s="238"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -9899,7 +9920,7 @@
         <v>35</v>
       </c>
       <c r="G48" s="230" t="s">
-        <v>35</v>
+        <v>561</v>
       </c>
       <c r="H48" s="129"/>
       <c r="I48" s="137"/>
@@ -10739,7 +10760,7 @@
         <f>IF(EXACT(G68, H68), "none", IF(ISNUMBER(MATCH(H68, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K68" s="492"/>
+      <c r="K68" s="407"/>
       <c r="L68" s="238"/>
     </row>
     <row r="69" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11283,7 +11304,7 @@
         <f>IF(EXACT(G81, H81), "none", IF(ISNUMBER(MATCH(H81, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K81" s="492"/>
+      <c r="K81" s="407"/>
       <c r="L81" s="238"/>
     </row>
     <row r="82" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11315,7 +11336,7 @@
         <f>IF(EXACT(G82, H82), "none", IF(ISNUMBER(MATCH(H82, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K82" s="492"/>
+      <c r="K82" s="407"/>
       <c r="L82" s="238"/>
     </row>
     <row r="83" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11507,7 +11528,7 @@
         <f>IF(EXACT(G88, H88), "none", IF(ISNUMBER(MATCH(H88, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K88" s="492"/>
+      <c r="K88" s="407"/>
       <c r="L88" s="238"/>
     </row>
     <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11539,7 +11560,7 @@
         <f>IF(EXACT(G89, H89), "none", IF(ISNUMBER(MATCH(H89, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K89" s="492"/>
+      <c r="K89" s="407"/>
       <c r="L89" s="238"/>
     </row>
     <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11667,7 +11688,7 @@
         <f>IF(EXACT(G93, H93), "none", IF(ISNUMBER(MATCH(H93, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K93" s="492"/>
+      <c r="K93" s="407"/>
       <c r="L93" s="238"/>
     </row>
     <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11987,7 +12008,7 @@
         <f>IF(EXACT(G103, H103), "none", IF(ISNUMBER(MATCH(H103, 'MP Analysis Input'!$A$15:$A$21, 0)), "soft", "hard"))</f>
         <v>hard</v>
       </c>
-      <c r="K103" s="492"/>
+      <c r="K103" s="407"/>
       <c r="L103" s="238"/>
     </row>
     <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14774,25 +14795,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="419" t="s">
+      <c r="A3" s="423" t="s">
         <v>308</v>
       </c>
-      <c r="B3" s="417" t="s">
+      <c r="B3" s="421" t="s">
         <v>322</v>
       </c>
-      <c r="C3" s="417" t="s">
+      <c r="C3" s="421" t="s">
         <v>323</v>
       </c>
-      <c r="D3" s="417" t="s">
+      <c r="D3" s="421" t="s">
         <v>324</v>
       </c>
-      <c r="E3" s="417" t="s">
+      <c r="E3" s="421" t="s">
         <v>325</v>
       </c>
-      <c r="F3" s="417" t="s">
+      <c r="F3" s="421" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="417" t="s">
+      <c r="G3" s="421" t="s">
         <v>327</v>
       </c>
       <c r="J3" s="108" t="s">
@@ -14805,13 +14826,13 @@
       <c r="O3" s="108"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="420"/>
-      <c r="B4" s="418"/>
-      <c r="C4" s="418"/>
-      <c r="D4" s="418"/>
-      <c r="E4" s="418"/>
-      <c r="F4" s="418"/>
-      <c r="G4" s="418"/>
+      <c r="A4" s="424"/>
+      <c r="B4" s="422"/>
+      <c r="C4" s="422"/>
+      <c r="D4" s="422"/>
+      <c r="E4" s="422"/>
+      <c r="F4" s="422"/>
+      <c r="G4" s="422"/>
       <c r="J4" s="113" t="s">
         <v>15</v>
       </c>
@@ -15083,15 +15104,15 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="423" t="s">
+      <c r="A16" s="427" t="s">
         <v>329</v>
       </c>
-      <c r="B16" s="424"/>
-      <c r="C16" s="424"/>
-      <c r="D16" s="424"/>
-      <c r="E16" s="424"/>
-      <c r="F16" s="424"/>
-      <c r="G16" s="424"/>
+      <c r="B16" s="428"/>
+      <c r="C16" s="428"/>
+      <c r="D16" s="428"/>
+      <c r="E16" s="428"/>
+      <c r="F16" s="428"/>
+      <c r="G16" s="428"/>
       <c r="K16" s="59"/>
       <c r="L16" s="59"/>
       <c r="M16" s="59"/>
@@ -15435,10 +15456,10 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="421" t="s">
+      <c r="A28" s="425" t="s">
         <v>337</v>
       </c>
-      <c r="B28" s="422"/>
+      <c r="B28" s="426"/>
       <c r="C28" s="209">
         <f>SUM(C18:C27)</f>
         <v>1421.9080000000004</v>
@@ -15461,15 +15482,15 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="423" t="s">
+      <c r="A29" s="427" t="s">
         <v>338</v>
       </c>
-      <c r="B29" s="424"/>
-      <c r="C29" s="424"/>
-      <c r="D29" s="424"/>
-      <c r="E29" s="424"/>
-      <c r="F29" s="424"/>
-      <c r="G29" s="424"/>
+      <c r="B29" s="428"/>
+      <c r="C29" s="428"/>
+      <c r="D29" s="428"/>
+      <c r="E29" s="428"/>
+      <c r="F29" s="428"/>
+      <c r="G29" s="428"/>
     </row>
     <row r="30" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="98"/>
@@ -15841,15 +15862,15 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="415" t="s">
+      <c r="A43" s="419" t="s">
         <v>347</v>
       </c>
-      <c r="B43" s="416"/>
-      <c r="C43" s="416"/>
-      <c r="D43" s="416"/>
-      <c r="E43" s="416"/>
-      <c r="F43" s="416"/>
-      <c r="G43" s="416"/>
+      <c r="B43" s="420"/>
+      <c r="C43" s="420"/>
+      <c r="D43" s="420"/>
+      <c r="E43" s="420"/>
+      <c r="F43" s="420"/>
+      <c r="G43" s="420"/>
     </row>
     <row r="44" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="98"/>
@@ -16035,16 +16056,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="448" t="s">
+      <c r="A1" s="452" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="449"/>
+      <c r="B1" s="453"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="450" t="s">
+      <c r="A2" s="454" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="451"/>
+      <c r="B2" s="455"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="X3" s="239" t="s">
@@ -16052,33 +16073,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="455" t="s">
+      <c r="A4" s="459" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="456"/>
+      <c r="B4" s="460"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="459" t="s">
+      <c r="D4" s="463" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="452" t="s">
+      <c r="E4" s="456" t="s">
         <v>177</v>
       </c>
-      <c r="F4" s="453"/>
-      <c r="G4" s="453"/>
-      <c r="H4" s="453"/>
-      <c r="I4" s="453"/>
-      <c r="J4" s="453"/>
-      <c r="K4" s="453"/>
-      <c r="L4" s="453"/>
-      <c r="M4" s="453"/>
-      <c r="N4" s="453"/>
-      <c r="O4" s="453"/>
-      <c r="P4" s="453"/>
-      <c r="Q4" s="453"/>
-      <c r="R4" s="453"/>
-      <c r="S4" s="453"/>
-      <c r="T4" s="453"/>
-      <c r="U4" s="454"/>
+      <c r="F4" s="457"/>
+      <c r="G4" s="457"/>
+      <c r="H4" s="457"/>
+      <c r="I4" s="457"/>
+      <c r="J4" s="457"/>
+      <c r="K4" s="457"/>
+      <c r="L4" s="457"/>
+      <c r="M4" s="457"/>
+      <c r="N4" s="457"/>
+      <c r="O4" s="457"/>
+      <c r="P4" s="457"/>
+      <c r="Q4" s="457"/>
+      <c r="R4" s="457"/>
+      <c r="S4" s="457"/>
+      <c r="T4" s="457"/>
+      <c r="U4" s="458"/>
       <c r="Y4" s="239">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -16145,12 +16166,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="457"/>
-      <c r="B5" s="458"/>
+      <c r="A5" s="461"/>
+      <c r="B5" s="462"/>
       <c r="C5" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="460"/>
+      <c r="D5" s="464"/>
       <c r="E5" s="69">
         <f>'Step Cost Analysis'!E5</f>
         <v>2020</v>
@@ -16288,10 +16309,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="427" t="s">
+      <c r="A6" s="431" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="428"/>
+      <c r="B6" s="432"/>
       <c r="C6" s="160">
         <v>10</v>
       </c>
@@ -16809,12 +16830,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="442" t="s">
+      <c r="A12" s="446" t="s">
         <v>191</v>
       </c>
-      <c r="B12" s="443"/>
-      <c r="C12" s="443"/>
-      <c r="D12" s="444"/>
+      <c r="B12" s="447"/>
+      <c r="C12" s="447"/>
+      <c r="D12" s="448"/>
       <c r="E12" s="279">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -16949,12 +16970,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="442" t="s">
+      <c r="A13" s="446" t="s">
         <v>192</v>
       </c>
-      <c r="B13" s="443"/>
-      <c r="C13" s="443"/>
-      <c r="D13" s="444"/>
+      <c r="B13" s="447"/>
+      <c r="C13" s="447"/>
+      <c r="D13" s="448"/>
       <c r="E13" s="279"/>
       <c r="F13" s="279"/>
       <c r="G13" s="279"/>
@@ -17047,10 +17068,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="427" t="s">
+      <c r="A14" s="431" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="428"/>
+      <c r="B14" s="432"/>
       <c r="C14" s="162">
         <v>10</v>
       </c>
@@ -17565,12 +17586,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="442" t="s">
+      <c r="A20" s="446" t="s">
         <v>196</v>
       </c>
-      <c r="B20" s="443"/>
-      <c r="C20" s="443"/>
-      <c r="D20" s="444"/>
+      <c r="B20" s="447"/>
+      <c r="C20" s="447"/>
+      <c r="D20" s="448"/>
       <c r="E20" s="279">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -17641,12 +17662,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="442" t="s">
+      <c r="A21" s="446" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="443"/>
-      <c r="C21" s="443"/>
-      <c r="D21" s="444"/>
+      <c r="B21" s="447"/>
+      <c r="C21" s="447"/>
+      <c r="D21" s="448"/>
       <c r="E21" s="279"/>
       <c r="F21" s="279"/>
       <c r="G21" s="279"/>
@@ -17672,10 +17693,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="427" t="s">
+      <c r="A22" s="431" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="428"/>
+      <c r="B22" s="432"/>
       <c r="C22" s="160">
         <v>10</v>
       </c>
@@ -17922,12 +17943,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="442" t="s">
+      <c r="A28" s="446" t="s">
         <v>199</v>
       </c>
-      <c r="B28" s="443"/>
-      <c r="C28" s="443"/>
-      <c r="D28" s="444"/>
+      <c r="B28" s="447"/>
+      <c r="C28" s="447"/>
+      <c r="D28" s="448"/>
       <c r="E28" s="279">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -17998,12 +18019,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="442" t="s">
+      <c r="A29" s="446" t="s">
         <v>200</v>
       </c>
-      <c r="B29" s="443"/>
-      <c r="C29" s="443"/>
-      <c r="D29" s="444"/>
+      <c r="B29" s="447"/>
+      <c r="C29" s="447"/>
+      <c r="D29" s="448"/>
       <c r="E29" s="279"/>
       <c r="F29" s="279"/>
       <c r="G29" s="279"/>
@@ -18029,10 +18050,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="427" t="s">
+      <c r="A30" s="431" t="s">
         <v>201</v>
       </c>
-      <c r="B30" s="428"/>
+      <c r="B30" s="432"/>
       <c r="C30" s="160">
         <v>10</v>
       </c>
@@ -18279,12 +18300,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="442" t="s">
+      <c r="A36" s="446" t="s">
         <v>202</v>
       </c>
-      <c r="B36" s="443"/>
-      <c r="C36" s="443"/>
-      <c r="D36" s="444"/>
+      <c r="B36" s="447"/>
+      <c r="C36" s="447"/>
+      <c r="D36" s="448"/>
       <c r="E36" s="279">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -18355,12 +18376,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="442" t="s">
+      <c r="A37" s="446" t="s">
         <v>203</v>
       </c>
-      <c r="B37" s="443"/>
-      <c r="C37" s="443"/>
-      <c r="D37" s="444"/>
+      <c r="B37" s="447"/>
+      <c r="C37" s="447"/>
+      <c r="D37" s="448"/>
       <c r="E37" s="279"/>
       <c r="F37" s="279"/>
       <c r="G37" s="279"/>
@@ -18386,10 +18407,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="427" t="s">
+      <c r="A38" s="431" t="s">
         <v>204</v>
       </c>
-      <c r="B38" s="428"/>
+      <c r="B38" s="432"/>
       <c r="C38" s="160">
         <v>10</v>
       </c>
@@ -18636,12 +18657,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="442" t="s">
+      <c r="A44" s="446" t="s">
         <v>205</v>
       </c>
-      <c r="B44" s="443"/>
-      <c r="C44" s="443"/>
-      <c r="D44" s="444"/>
+      <c r="B44" s="447"/>
+      <c r="C44" s="447"/>
+      <c r="D44" s="448"/>
       <c r="E44" s="279">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -18712,12 +18733,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="442" t="s">
+      <c r="A45" s="446" t="s">
         <v>206</v>
       </c>
-      <c r="B45" s="443"/>
-      <c r="C45" s="443"/>
-      <c r="D45" s="444"/>
+      <c r="B45" s="447"/>
+      <c r="C45" s="447"/>
+      <c r="D45" s="448"/>
       <c r="E45" s="279"/>
       <c r="F45" s="279"/>
       <c r="G45" s="279"/>
@@ -18743,11 +18764,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="429" t="s">
+      <c r="A46" s="433" t="s">
         <v>207</v>
       </c>
-      <c r="B46" s="430"/>
-      <c r="C46" s="431"/>
+      <c r="B46" s="434"/>
+      <c r="C46" s="435"/>
       <c r="D46" s="170"/>
       <c r="E46" s="287">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -18820,12 +18841,12 @@
       <c r="V46" s="240"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="437" t="s">
+      <c r="A47" s="441" t="s">
         <v>208</v>
       </c>
-      <c r="B47" s="438"/>
-      <c r="C47" s="438"/>
-      <c r="D47" s="439"/>
+      <c r="B47" s="442"/>
+      <c r="C47" s="442"/>
+      <c r="D47" s="443"/>
       <c r="E47" s="288">
         <f>E46</f>
         <v>1500000</v>
@@ -18896,7 +18917,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A48" s="171"/>
       <c r="B48" s="171"/>
-      <c r="C48" s="440" t="s">
+      <c r="C48" s="444" t="s">
         <v>209</v>
       </c>
       <c r="D48" s="172">
@@ -18971,7 +18992,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A49" s="171"/>
-      <c r="C49" s="441"/>
+      <c r="C49" s="445"/>
       <c r="D49" s="242">
         <v>37</v>
       </c>
@@ -19042,7 +19063,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A50" s="171"/>
-      <c r="C50" s="441"/>
+      <c r="C50" s="445"/>
       <c r="D50" s="242">
         <v>30</v>
       </c>
@@ -19113,7 +19134,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A51" s="171"/>
-      <c r="C51" s="441"/>
+      <c r="C51" s="445"/>
       <c r="D51" s="242">
         <v>41</v>
       </c>
@@ -19183,38 +19204,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="432" t="s">
+      <c r="A52" s="436" t="s">
         <v>210</v>
       </c>
-      <c r="B52" s="433"/>
-      <c r="C52" s="433"/>
-      <c r="D52" s="433"/>
-      <c r="E52" s="433"/>
-      <c r="F52" s="433"/>
-      <c r="G52" s="433"/>
-      <c r="H52" s="433"/>
-      <c r="I52" s="433"/>
-      <c r="J52" s="433"/>
-      <c r="K52" s="433"/>
-      <c r="L52" s="433"/>
-      <c r="M52" s="433"/>
-      <c r="N52" s="433"/>
-      <c r="O52" s="433"/>
-      <c r="P52" s="433"/>
-      <c r="Q52" s="433"/>
-      <c r="R52" s="433"/>
-      <c r="S52" s="433"/>
-      <c r="T52" s="433"/>
-      <c r="U52" s="433"/>
-      <c r="V52" s="433"/>
-      <c r="W52" s="434"/>
+      <c r="B52" s="437"/>
+      <c r="C52" s="437"/>
+      <c r="D52" s="437"/>
+      <c r="E52" s="437"/>
+      <c r="F52" s="437"/>
+      <c r="G52" s="437"/>
+      <c r="H52" s="437"/>
+      <c r="I52" s="437"/>
+      <c r="J52" s="437"/>
+      <c r="K52" s="437"/>
+      <c r="L52" s="437"/>
+      <c r="M52" s="437"/>
+      <c r="N52" s="437"/>
+      <c r="O52" s="437"/>
+      <c r="P52" s="437"/>
+      <c r="Q52" s="437"/>
+      <c r="R52" s="437"/>
+      <c r="S52" s="437"/>
+      <c r="T52" s="437"/>
+      <c r="U52" s="437"/>
+      <c r="V52" s="437"/>
+      <c r="W52" s="438"/>
       <c r="X52" s="240"/>
     </row>
     <row r="53" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="435" t="s">
+      <c r="A53" s="439" t="s">
         <v>211</v>
       </c>
-      <c r="B53" s="436"/>
+      <c r="B53" s="440"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -19391,10 +19412,10 @@
       <c r="X57" s="240"/>
     </row>
     <row r="58" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="425" t="s">
+      <c r="A58" s="429" t="s">
         <v>213</v>
       </c>
-      <c r="B58" s="426"/>
+      <c r="B58" s="430"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -19576,10 +19597,10 @@
       <c r="X62" s="240"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="425" t="s">
+      <c r="A63" s="429" t="s">
         <v>214</v>
       </c>
-      <c r="B63" s="426"/>
+      <c r="B63" s="430"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -19769,10 +19790,10 @@
       <c r="X67" s="240"/>
     </row>
     <row r="68" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="425" t="s">
+      <c r="A68" s="429" t="s">
         <v>215</v>
       </c>
-      <c r="B68" s="426"/>
+      <c r="B68" s="430"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -19950,10 +19971,10 @@
       <c r="X72" s="240"/>
     </row>
     <row r="73" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="425" t="s">
+      <c r="A73" s="429" t="s">
         <v>216</v>
       </c>
-      <c r="B73" s="426"/>
+      <c r="B73" s="430"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -20179,10 +20200,10 @@
       <c r="X77" s="240"/>
     </row>
     <row r="78" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="425" t="s">
+      <c r="A78" s="429" t="s">
         <v>218</v>
       </c>
-      <c r="B78" s="426"/>
+      <c r="B78" s="430"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -20354,10 +20375,10 @@
       <c r="X82" s="240"/>
     </row>
     <row r="83" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="425" t="s">
+      <c r="A83" s="429" t="s">
         <v>220</v>
       </c>
-      <c r="B83" s="426"/>
+      <c r="B83" s="430"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -20529,10 +20550,10 @@
       <c r="X87" s="240"/>
     </row>
     <row r="88" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="425" t="s">
+      <c r="A88" s="429" t="s">
         <v>51</v>
       </c>
-      <c r="B88" s="426"/>
+      <c r="B88" s="430"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -20704,10 +20725,10 @@
       <c r="X92" s="240"/>
     </row>
     <row r="93" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="425" t="s">
+      <c r="A93" s="429" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="426"/>
+      <c r="B93" s="430"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -20909,10 +20930,10 @@
       <c r="X97" s="240"/>
     </row>
     <row r="98" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="425" t="s">
+      <c r="A98" s="429" t="s">
         <v>225</v>
       </c>
-      <c r="B98" s="426"/>
+      <c r="B98" s="430"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -21104,10 +21125,10 @@
       <c r="X102" s="240"/>
     </row>
     <row r="103" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="425" t="s">
+      <c r="A103" s="429" t="s">
         <v>227</v>
       </c>
-      <c r="B103" s="426"/>
+      <c r="B103" s="430"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -21309,10 +21330,10 @@
       <c r="X107" s="240"/>
     </row>
     <row r="108" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="425" t="s">
+      <c r="A108" s="429" t="s">
         <v>228</v>
       </c>
-      <c r="B108" s="426"/>
+      <c r="B108" s="430"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -21514,10 +21535,10 @@
       <c r="X112" s="240"/>
     </row>
     <row r="113" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="425" t="s">
+      <c r="A113" s="429" t="s">
         <v>229</v>
       </c>
-      <c r="B113" s="426"/>
+      <c r="B113" s="430"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -21679,10 +21700,10 @@
       <c r="X117" s="240"/>
     </row>
     <row r="118" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="425" t="s">
+      <c r="A118" s="429" t="s">
         <v>230</v>
       </c>
-      <c r="B118" s="426"/>
+      <c r="B118" s="430"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -21884,10 +21905,10 @@
       <c r="X122" s="240"/>
     </row>
     <row r="123" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="425" t="s">
+      <c r="A123" s="429" t="s">
         <v>231</v>
       </c>
-      <c r="B123" s="426"/>
+      <c r="B123" s="430"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -22089,10 +22110,10 @@
       <c r="X127" s="240"/>
     </row>
     <row r="128" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="425" t="s">
+      <c r="A128" s="429" t="s">
         <v>232</v>
       </c>
-      <c r="B128" s="426"/>
+      <c r="B128" s="430"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -22294,10 +22315,10 @@
       <c r="X132" s="240"/>
     </row>
     <row r="133" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="425" t="s">
+      <c r="A133" s="429" t="s">
         <v>233</v>
       </c>
-      <c r="B133" s="426"/>
+      <c r="B133" s="430"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -22499,10 +22520,10 @@
       <c r="X137" s="240"/>
     </row>
     <row r="138" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="425" t="s">
+      <c r="A138" s="429" t="s">
         <v>234</v>
       </c>
-      <c r="B138" s="426"/>
+      <c r="B138" s="430"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -22712,10 +22733,10 @@
       <c r="X142" s="240"/>
     </row>
     <row r="143" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="425" t="s">
+      <c r="A143" s="429" t="s">
         <v>238</v>
       </c>
-      <c r="B143" s="426"/>
+      <c r="B143" s="430"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -22808,10 +22829,10 @@
       <c r="X144" s="240"/>
     </row>
     <row r="145" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="435" t="s">
+      <c r="A145" s="439" t="s">
         <v>240</v>
       </c>
-      <c r="B145" s="436"/>
+      <c r="B145" s="440"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -22884,10 +22905,10 @@
       <c r="X146" s="240"/>
     </row>
     <row r="147" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="435" t="s">
+      <c r="A147" s="439" t="s">
         <v>241</v>
       </c>
-      <c r="B147" s="436"/>
+      <c r="B147" s="440"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -22985,10 +23006,10 @@
       <c r="X148" s="240"/>
     </row>
     <row r="149" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="435" t="s">
+      <c r="A149" s="439" t="s">
         <v>242</v>
       </c>
-      <c r="B149" s="436"/>
+      <c r="B149" s="440"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -23110,12 +23131,12 @@
       <c r="X151" s="240"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="445" t="s">
+      <c r="A152" s="449" t="s">
         <v>243</v>
       </c>
-      <c r="B152" s="446"/>
-      <c r="C152" s="446"/>
-      <c r="D152" s="447"/>
+      <c r="B152" s="450"/>
+      <c r="C152" s="450"/>
+      <c r="D152" s="451"/>
       <c r="E152" s="311">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -23852,69 +23873,69 @@
       <c r="BZ1" s="186"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="448" t="s">
+      <c r="A2" s="452" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="468"/>
-      <c r="C2" s="469"/>
-      <c r="D2" s="471" t="s">
+      <c r="B2" s="472"/>
+      <c r="C2" s="473"/>
+      <c r="D2" s="475" t="s">
         <v>352</v>
       </c>
-      <c r="E2" s="472"/>
-      <c r="F2" s="472"/>
-      <c r="G2" s="472"/>
-      <c r="H2" s="472"/>
-      <c r="I2" s="472"/>
-      <c r="J2" s="472"/>
-      <c r="K2" s="472"/>
-      <c r="L2" s="472"/>
-      <c r="M2" s="472"/>
-      <c r="N2" s="472"/>
-      <c r="O2" s="472"/>
-      <c r="P2" s="472"/>
-      <c r="Q2" s="472"/>
-      <c r="R2" s="472"/>
-      <c r="S2" s="472"/>
-      <c r="T2" s="472"/>
+      <c r="E2" s="476"/>
+      <c r="F2" s="476"/>
+      <c r="G2" s="476"/>
+      <c r="H2" s="476"/>
+      <c r="I2" s="476"/>
+      <c r="J2" s="476"/>
+      <c r="K2" s="476"/>
+      <c r="L2" s="476"/>
+      <c r="M2" s="476"/>
+      <c r="N2" s="476"/>
+      <c r="O2" s="476"/>
+      <c r="P2" s="476"/>
+      <c r="Q2" s="476"/>
+      <c r="R2" s="476"/>
+      <c r="S2" s="476"/>
+      <c r="T2" s="476"/>
       <c r="AA2" s="131"/>
       <c r="BY2" s="186"/>
       <c r="BZ2" s="186"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="450" t="s">
+      <c r="A3" s="454" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="468"/>
-      <c r="C3" s="469"/>
+      <c r="B3" s="472"/>
+      <c r="C3" s="473"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="473" t="s">
+      <c r="F3" s="477" t="s">
         <v>353</v>
       </c>
-      <c r="G3" s="474"/>
-      <c r="H3" s="475" t="s">
+      <c r="G3" s="478"/>
+      <c r="H3" s="479" t="s">
         <v>354</v>
       </c>
-      <c r="I3" s="475"/>
-      <c r="J3" s="476"/>
-      <c r="K3" s="477" t="s">
+      <c r="I3" s="479"/>
+      <c r="J3" s="480"/>
+      <c r="K3" s="481" t="s">
         <v>355</v>
       </c>
-      <c r="L3" s="478"/>
-      <c r="M3" s="479"/>
-      <c r="N3" s="476" t="s">
+      <c r="L3" s="482"/>
+      <c r="M3" s="483"/>
+      <c r="N3" s="480" t="s">
         <v>356</v>
       </c>
-      <c r="O3" s="480"/>
-      <c r="P3" s="481"/>
-      <c r="Q3" s="482" t="s">
+      <c r="O3" s="484"/>
+      <c r="P3" s="485"/>
+      <c r="Q3" s="486" t="s">
         <v>357</v>
       </c>
-      <c r="R3" s="483"/>
-      <c r="S3" s="484" t="s">
+      <c r="R3" s="487"/>
+      <c r="S3" s="488" t="s">
         <v>358</v>
       </c>
-      <c r="T3" s="485"/>
+      <c r="T3" s="489"/>
       <c r="AA3" s="132"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -24079,7 +24100,7 @@
       <c r="AC6" s="133"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="462" t="str">
+      <c r="C7" s="466" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -24087,81 +24108,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="463"/>
-      <c r="E7" s="464"/>
-      <c r="F7" s="463" t="s">
+      <c r="D7" s="467"/>
+      <c r="E7" s="468"/>
+      <c r="F7" s="467" t="s">
         <v>381</v>
       </c>
-      <c r="G7" s="463"/>
-      <c r="H7" s="464"/>
-      <c r="I7" s="465" t="str">
+      <c r="G7" s="467"/>
+      <c r="H7" s="468"/>
+      <c r="I7" s="469" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$2620.741)</v>
       </c>
-      <c r="J7" s="466"/>
-      <c r="K7" s="466"/>
-      <c r="L7" s="466"/>
-      <c r="M7" s="466"/>
-      <c r="N7" s="466"/>
-      <c r="O7" s="466"/>
-      <c r="P7" s="466"/>
-      <c r="Q7" s="466"/>
-      <c r="R7" s="467"/>
-      <c r="S7" s="462" t="str">
+      <c r="J7" s="470"/>
+      <c r="K7" s="470"/>
+      <c r="L7" s="470"/>
+      <c r="M7" s="470"/>
+      <c r="N7" s="470"/>
+      <c r="O7" s="470"/>
+      <c r="P7" s="470"/>
+      <c r="Q7" s="470"/>
+      <c r="R7" s="471"/>
+      <c r="S7" s="466" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$319.295)</v>
       </c>
-      <c r="T7" s="463"/>
-      <c r="U7" s="463"/>
-      <c r="V7" s="463"/>
-      <c r="W7" s="463"/>
-      <c r="X7" s="464"/>
-      <c r="Y7" s="462" t="s">
+      <c r="T7" s="467"/>
+      <c r="U7" s="467"/>
+      <c r="V7" s="467"/>
+      <c r="W7" s="467"/>
+      <c r="X7" s="468"/>
+      <c r="Y7" s="466" t="s">
         <v>382</v>
       </c>
-      <c r="Z7" s="464"/>
+      <c r="Z7" s="468"/>
       <c r="AA7" s="134"/>
-      <c r="AH7" s="486" t="s">
+      <c r="AH7" s="490" t="s">
         <v>383</v>
       </c>
-      <c r="AI7" s="487"/>
+      <c r="AI7" s="491"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="488" t="s">
+      <c r="AK7" s="492" t="s">
         <v>384</v>
       </c>
-      <c r="AL7" s="424"/>
-      <c r="AM7" s="424"/>
-      <c r="AN7" s="487"/>
-      <c r="AP7" s="489" t="s">
+      <c r="AL7" s="428"/>
+      <c r="AM7" s="428"/>
+      <c r="AN7" s="491"/>
+      <c r="AP7" s="493" t="s">
         <v>385</v>
       </c>
-      <c r="AQ7" s="454"/>
-      <c r="AS7" s="470" t="s">
+      <c r="AQ7" s="458"/>
+      <c r="AS7" s="474" t="s">
         <v>386</v>
       </c>
-      <c r="AT7" s="453"/>
-      <c r="AU7" s="453"/>
-      <c r="AV7" s="453"/>
-      <c r="AW7" s="453"/>
-      <c r="AX7" s="453"/>
-      <c r="AY7" s="453"/>
-      <c r="AZ7" s="453"/>
-      <c r="BA7" s="453"/>
-      <c r="BB7" s="454"/>
-      <c r="BD7" s="489" t="s">
+      <c r="AT7" s="457"/>
+      <c r="AU7" s="457"/>
+      <c r="AV7" s="457"/>
+      <c r="AW7" s="457"/>
+      <c r="AX7" s="457"/>
+      <c r="AY7" s="457"/>
+      <c r="AZ7" s="457"/>
+      <c r="BA7" s="457"/>
+      <c r="BB7" s="458"/>
+      <c r="BD7" s="493" t="s">
         <v>387</v>
       </c>
-      <c r="BE7" s="454"/>
+      <c r="BE7" s="458"/>
       <c r="BF7" s="186"/>
-      <c r="BG7" s="470" t="s">
+      <c r="BG7" s="474" t="s">
         <v>388</v>
       </c>
-      <c r="BH7" s="453"/>
-      <c r="BI7" s="453"/>
+      <c r="BH7" s="457"/>
+      <c r="BI7" s="457"/>
       <c r="BY7" s="186"/>
       <c r="BZ7" s="186"/>
     </row>
@@ -34106,17 +34127,17 @@
       <c r="BZ52" s="186"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="461"/>
-      <c r="D53" s="461"/>
-      <c r="E53" s="461"/>
-      <c r="F53" s="461"/>
-      <c r="G53" s="461"/>
-      <c r="H53" s="461"/>
-      <c r="I53" s="461"/>
-      <c r="J53" s="461"/>
-      <c r="K53" s="461"/>
-      <c r="L53" s="461"/>
-      <c r="M53" s="461"/>
+      <c r="C53" s="465"/>
+      <c r="D53" s="465"/>
+      <c r="E53" s="465"/>
+      <c r="F53" s="465"/>
+      <c r="G53" s="465"/>
+      <c r="H53" s="465"/>
+      <c r="I53" s="465"/>
+      <c r="J53" s="465"/>
+      <c r="K53" s="465"/>
+      <c r="L53" s="465"/>
+      <c r="M53" s="465"/>
       <c r="AC53" s="136" t="s">
         <v>437</v>
       </c>
@@ -34311,8 +34332,8 @@
   </sheetPr>
   <dimension ref="A1:Q221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A14" zoomScale="225" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34368,10 +34389,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="404" t="s">
+      <c r="A3" s="409" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="405"/>
+      <c r="B3" s="410"/>
       <c r="J3" s="230" t="s">
         <v>521</v>
       </c>
@@ -34402,7 +34423,7 @@
         <v>245</v>
       </c>
       <c r="B4" s="109">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="239" t="s">
         <v>246</v>
@@ -34437,7 +34458,7 @@
         <v>247</v>
       </c>
       <c r="B5" s="109">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="239" t="s">
         <v>246</v>
@@ -34494,10 +34515,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="404" t="s">
+      <c r="A7" s="409" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="405"/>
+      <c r="B7" s="410"/>
       <c r="C7" s="115" t="s">
         <v>249</v>
       </c>
@@ -34825,10 +34846,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="406" t="s">
+      <c r="A23" s="411" t="s">
         <v>256</v>
       </c>
-      <c r="B23" s="405"/>
+      <c r="B23" s="410"/>
       <c r="C23" t="s">
         <v>257</v>
       </c>
@@ -36029,10 +36050,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AB166"/>
+  <dimension ref="A1:AB177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36169,9 +36190,7 @@
       <c r="C11" s="230" t="s">
         <v>533</v>
       </c>
-      <c r="D11" s="230" t="s">
-        <v>469</v>
-      </c>
+      <c r="D11" s="230"/>
       <c r="E11" s="230"/>
       <c r="F11" s="230"/>
       <c r="G11" s="230"/>
@@ -36180,27 +36199,6 @@
       <c r="J11" s="230"/>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="230" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C12" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="230" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="230" t="s">
-        <v>43</v>
-      </c>
       <c r="H12" s="331"/>
       <c r="I12" s="230"/>
       <c r="J12" s="230"/>
@@ -36235,12 +36233,7 @@
       <c r="C14" s="230" t="s">
         <v>534</v>
       </c>
-      <c r="D14" s="230" t="s">
-        <v>458</v>
-      </c>
-      <c r="E14" s="230" t="s">
-        <v>47</v>
-      </c>
+      <c r="D14" s="230"/>
       <c r="F14" s="230"/>
       <c r="G14" s="230"/>
       <c r="H14" s="230"/>
@@ -36248,15 +36241,9 @@
       <c r="J14" s="230"/>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="230" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="230" t="s">
-        <v>445</v>
-      </c>
-      <c r="C15" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="A15" s="230"/>
+      <c r="B15" s="230"/>
+      <c r="C15" s="230"/>
       <c r="D15" s="230"/>
       <c r="E15" s="230"/>
       <c r="F15" s="230"/>
@@ -36333,15 +36320,9 @@
       <c r="C19" s="230" t="s">
         <v>536</v>
       </c>
-      <c r="D19" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="D19" s="230"/>
+      <c r="E19" s="230"/>
+      <c r="F19" s="230"/>
       <c r="G19" s="230"/>
       <c r="H19" s="230"/>
       <c r="I19" s="230"/>
@@ -36514,8 +36495,12 @@
       <c r="D28" s="230" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="230"/>
-      <c r="F28" s="230"/>
+      <c r="E28" s="230" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="230" t="s">
+        <v>47</v>
+      </c>
       <c r="G28" s="230"/>
       <c r="H28" s="230"/>
       <c r="I28" s="230"/>
@@ -36606,18 +36591,10 @@
       <c r="J32" s="230"/>
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="340" t="s">
-        <v>520</v>
-      </c>
-      <c r="B33" s="340" t="s">
-        <v>442</v>
-      </c>
-      <c r="C33" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="230" t="s">
-        <v>63</v>
-      </c>
+      <c r="A33" s="340"/>
+      <c r="B33" s="340"/>
+      <c r="C33" s="230"/>
+      <c r="D33" s="230"/>
       <c r="E33" s="331"/>
       <c r="F33" s="230"/>
       <c r="G33" s="230"/>
@@ -36626,18 +36603,10 @@
       <c r="J33" s="230"/>
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="230" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C34" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="230" t="s">
-        <v>63</v>
-      </c>
+      <c r="A34" s="230"/>
+      <c r="B34" s="230"/>
+      <c r="C34" s="230"/>
+      <c r="D34" s="230"/>
       <c r="E34" s="230"/>
       <c r="F34" s="230"/>
       <c r="G34" s="230"/>
@@ -36673,7 +36642,9 @@
       <c r="C36" s="230" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="230"/>
+      <c r="D36" s="230" t="s">
+        <v>32</v>
+      </c>
       <c r="E36" s="230"/>
       <c r="F36" s="230"/>
       <c r="G36" s="230"/>
@@ -36891,9 +36862,7 @@
       <c r="C47" s="230" t="s">
         <v>544</v>
       </c>
-      <c r="D47" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="D47" s="230"/>
       <c r="E47" s="230"/>
       <c r="F47" s="230"/>
       <c r="G47" s="230"/>
@@ -36920,30 +36889,7 @@
       <c r="J48" s="230"/>
     </row>
     <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="230" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C49" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="E49" s="230" t="s">
-        <v>39</v>
-      </c>
-      <c r="F49" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="G49" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="H49" s="230" t="s">
-        <v>58</v>
-      </c>
+      <c r="H49" s="230"/>
       <c r="I49" s="230"/>
       <c r="J49" s="230"/>
     </row>
@@ -37036,24 +36982,12 @@
       <c r="J53" s="230"/>
     </row>
     <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="230" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="230" t="s">
-        <v>445</v>
-      </c>
-      <c r="C54" s="230" t="s">
-        <v>547</v>
-      </c>
-      <c r="D54" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="349" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="A54" s="230"/>
+      <c r="B54" s="230"/>
+      <c r="C54" s="230"/>
+      <c r="D54" s="230"/>
+      <c r="E54" s="349"/>
+      <c r="F54" s="230"/>
       <c r="G54" s="230"/>
       <c r="H54" s="230"/>
       <c r="I54" s="230"/>
@@ -37064,15 +36998,14 @@
         <v>522</v>
       </c>
       <c r="B55" s="230" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C55" s="230" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="D55" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="E55" s="230"/>
+        <v>47</v>
+      </c>
       <c r="F55" s="230"/>
       <c r="G55" s="230"/>
       <c r="H55" s="230"/>
@@ -37196,39 +37129,21 @@
       <c r="J61" s="230"/>
     </row>
     <row r="62" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="230" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C62" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="E62" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="F62" s="230" t="s">
-        <v>32</v>
-      </c>
+      <c r="A62" s="230"/>
+      <c r="B62" s="230"/>
+      <c r="C62" s="230"/>
+      <c r="D62" s="230"/>
+      <c r="E62" s="230"/>
+      <c r="F62" s="230"/>
       <c r="G62" s="230"/>
       <c r="H62" s="230"/>
       <c r="I62" s="230"/>
       <c r="J62" s="230"/>
     </row>
     <row r="63" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="230" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63" s="230" t="s">
-        <v>445</v>
-      </c>
-      <c r="C63" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="A63" s="230"/>
+      <c r="B63" s="230"/>
+      <c r="C63" s="230"/>
       <c r="D63" s="230"/>
       <c r="E63" s="230"/>
       <c r="F63" s="230"/>
@@ -37240,15 +37155,9 @@
       <c r="M63" s="331"/>
     </row>
     <row r="64" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="230" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="230" t="s">
-        <v>445</v>
-      </c>
-      <c r="C64" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="A64" s="230"/>
+      <c r="B64" s="230"/>
+      <c r="C64" s="230"/>
       <c r="D64" s="230"/>
       <c r="E64" s="230"/>
       <c r="F64" s="230"/>
@@ -37364,27 +37273,10 @@
       <c r="J69" s="230"/>
     </row>
     <row r="70" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="230" t="s">
-        <v>100</v>
-      </c>
-      <c r="B70" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C70" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="D70" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E70" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="F70" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="G70" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="D70" s="230"/>
+      <c r="E70" s="230"/>
+      <c r="F70" s="230"/>
+      <c r="G70" s="230"/>
       <c r="H70" s="230"/>
       <c r="I70" s="230"/>
       <c r="J70" s="230"/>
@@ -37394,93 +37286,37 @@
       </c>
     </row>
     <row r="71" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="230" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C71" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="D71" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E71" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="F71" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="G71" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="E71" s="230"/>
+      <c r="F71" s="230"/>
+      <c r="G71" s="230"/>
       <c r="H71" s="230"/>
       <c r="I71" s="230"/>
       <c r="J71" s="230"/>
     </row>
     <row r="72" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="230" t="s">
-        <v>103</v>
-      </c>
-      <c r="B72" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C72" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="D72" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E72" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="F72" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="G72" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="C72" s="230"/>
+      <c r="D72" s="230"/>
+      <c r="E72" s="230"/>
+      <c r="F72" s="230"/>
+      <c r="G72" s="230"/>
       <c r="H72" s="230"/>
       <c r="I72" s="230"/>
       <c r="J72" s="230"/>
     </row>
     <row r="73" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="230" t="s">
-        <v>104</v>
-      </c>
-      <c r="B73" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C73" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="D73" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E73" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="F73" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="G73" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="C73" s="230"/>
+      <c r="D73" s="230"/>
+      <c r="E73" s="230"/>
+      <c r="F73" s="230"/>
+      <c r="G73" s="230"/>
       <c r="H73" s="230"/>
       <c r="I73" s="230"/>
       <c r="J73" s="230"/>
     </row>
     <row r="74" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="230" t="s">
-        <v>105</v>
-      </c>
-      <c r="B74" s="230" t="s">
-        <v>445</v>
-      </c>
-      <c r="C74" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="C74" s="230"/>
       <c r="D74" s="230"/>
       <c r="E74" s="230"/>
       <c r="F74" s="230"/>
@@ -37496,17 +37332,13 @@
         <v>106</v>
       </c>
       <c r="B75" s="230" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C75" s="230" t="s">
         <v>32</v>
       </c>
-      <c r="D75" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E75" s="230" t="s">
-        <v>43</v>
-      </c>
+      <c r="D75" s="230"/>
+      <c r="E75" s="230"/>
       <c r="F75" s="230"/>
       <c r="G75" s="230"/>
       <c r="H75" s="230"/>
@@ -37518,14 +37350,12 @@
         <v>109</v>
       </c>
       <c r="B76" s="230" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C76" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="D76" s="230" t="s">
-        <v>63</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D76" s="230"/>
       <c r="E76" s="230"/>
       <c r="F76" s="230"/>
       <c r="G76" s="230"/>
@@ -37534,21 +37364,8 @@
       <c r="J76" s="230"/>
     </row>
     <row r="77" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="230" t="s">
-        <v>110</v>
-      </c>
-      <c r="B77" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C77" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="D77" s="230" t="s">
-        <v>63</v>
-      </c>
-      <c r="E77" s="230" t="s">
-        <v>47</v>
-      </c>
+      <c r="D77" s="230"/>
+      <c r="E77" s="230"/>
       <c r="F77" s="230"/>
       <c r="G77" s="230"/>
       <c r="H77" s="230"/>
@@ -37576,48 +37393,24 @@
       <c r="J78" s="230"/>
     </row>
     <row r="79" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="230" t="s">
-        <v>112</v>
-      </c>
-      <c r="B79" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C79" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="D79" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E79" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="F79" s="230" t="s">
-        <v>63</v>
-      </c>
+      <c r="A79" s="230"/>
+      <c r="B79" s="230"/>
+      <c r="C79" s="230"/>
+      <c r="D79" s="230"/>
+      <c r="E79" s="230"/>
+      <c r="F79" s="230"/>
       <c r="G79" s="230"/>
       <c r="H79" s="230"/>
       <c r="I79" s="230"/>
       <c r="J79" s="230"/>
     </row>
     <row r="80" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="230" t="s">
-        <v>113</v>
-      </c>
-      <c r="B80" s="230" t="s">
-        <v>442</v>
-      </c>
-      <c r="C80" s="230" t="s">
-        <v>32</v>
-      </c>
-      <c r="D80" s="230" t="s">
-        <v>47</v>
-      </c>
-      <c r="E80" s="230" t="s">
-        <v>108</v>
-      </c>
-      <c r="F80" s="230" t="s">
-        <v>63</v>
-      </c>
+      <c r="A80" s="230"/>
+      <c r="B80" s="230"/>
+      <c r="C80" s="230"/>
+      <c r="D80" s="230"/>
+      <c r="E80" s="230"/>
+      <c r="F80" s="230"/>
       <c r="G80" s="230"/>
       <c r="H80" s="230"/>
       <c r="I80" s="230"/>
@@ -37646,18 +37439,10 @@
       </c>
     </row>
     <row r="82" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="342" t="s">
-        <v>170</v>
-      </c>
-      <c r="B82" s="342" t="s">
-        <v>442</v>
-      </c>
-      <c r="C82" s="342" t="s">
-        <v>108</v>
-      </c>
-      <c r="D82" s="331" t="s">
-        <v>63</v>
-      </c>
+      <c r="A82" s="342"/>
+      <c r="B82" s="342"/>
+      <c r="C82" s="342"/>
+      <c r="D82" s="331"/>
       <c r="E82" s="331"/>
       <c r="F82" s="331"/>
       <c r="G82" s="230"/>
@@ -37690,9 +37475,6 @@
       <c r="J83" s="230"/>
     </row>
     <row r="84" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="230"/>
-      <c r="B84" s="230"/>
-      <c r="C84" s="230"/>
       <c r="D84" s="230"/>
       <c r="E84" s="230"/>
       <c r="F84" s="230"/>
@@ -37702,9 +37484,6 @@
       <c r="J84" s="230"/>
     </row>
     <row r="85" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="230"/>
-      <c r="B85" s="230"/>
-      <c r="C85" s="230"/>
       <c r="D85" s="230"/>
       <c r="E85" s="230"/>
       <c r="F85" s="230"/>
@@ -37714,9 +37493,15 @@
       <c r="J85" s="230"/>
     </row>
     <row r="86" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="230"/>
-      <c r="B86" s="230"/>
-      <c r="C86" s="230"/>
+      <c r="A86" s="230" t="s">
+        <v>577</v>
+      </c>
+      <c r="B86" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C86" s="230" t="s">
+        <v>47</v>
+      </c>
       <c r="D86" s="230"/>
       <c r="E86" s="230"/>
       <c r="F86" s="230"/>
@@ -37854,7 +37639,7 @@
       <c r="F96" s="230"/>
       <c r="G96" s="230"/>
     </row>
-    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="238" t="s">
         <v>512</v>
       </c>
@@ -37869,7 +37654,7 @@
       <c r="F97" s="230"/>
       <c r="G97" s="230"/>
     </row>
-    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="238" t="s">
         <v>507</v>
       </c>
@@ -37884,7 +37669,7 @@
       <c r="F98" s="230"/>
       <c r="G98" s="230"/>
     </row>
-    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="361" t="s">
         <v>57</v>
       </c>
@@ -37899,7 +37684,7 @@
       <c r="F99" s="230"/>
       <c r="G99" s="230"/>
     </row>
-    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="361" t="s">
         <v>36</v>
       </c>
@@ -37914,7 +37699,7 @@
       <c r="F100" s="230"/>
       <c r="G100" s="230"/>
     </row>
-    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="361" t="s">
         <v>454</v>
       </c>
@@ -37931,7 +37716,7 @@
       <c r="F101" s="230"/>
       <c r="G101" s="230"/>
     </row>
-    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="361" t="s">
         <v>95</v>
       </c>
@@ -37948,7 +37733,7 @@
       <c r="F102" s="230"/>
       <c r="G102" s="230"/>
     </row>
-    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="361" t="s">
         <v>96</v>
       </c>
@@ -37965,7 +37750,7 @@
       <c r="F103" s="230"/>
       <c r="G103" s="230"/>
     </row>
-    <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="361" t="s">
         <v>524</v>
       </c>
@@ -37982,7 +37767,7 @@
       <c r="F104" s="230"/>
       <c r="G104" s="230"/>
     </row>
-    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="361" t="s">
         <v>523</v>
       </c>
@@ -37997,43 +37782,104 @@
       <c r="F105" s="230"/>
       <c r="G105" s="230"/>
     </row>
-    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="230"/>
-      <c r="B106" s="230"/>
-      <c r="C106" s="340"/>
-      <c r="D106" s="230"/>
-      <c r="E106" s="230"/>
-      <c r="F106" s="230"/>
-      <c r="G106" s="230"/>
-    </row>
-    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="230"/>
-      <c r="B107" s="230"/>
-      <c r="C107" s="340"/>
-      <c r="D107" s="230"/>
-      <c r="E107" s="230"/>
-      <c r="F107" s="230"/>
-      <c r="G107" s="230"/>
-    </row>
-    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="155" t="s">
-        <v>451</v>
-      </c>
-      <c r="B109" s="155"/>
-      <c r="C109" s="155" t="s">
-        <v>446</v>
-      </c>
-      <c r="H109" s="238" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="230">
+    <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="230" t="s">
+        <v>100</v>
+      </c>
+      <c r="B106" s="230" t="s">
+        <v>442</v>
+      </c>
+      <c r="C106" s="230">
         <v>1</v>
       </c>
+      <c r="D106" s="230">
+        <v>2</v>
+      </c>
+      <c r="E106" s="230">
+        <v>3</v>
+      </c>
+      <c r="F106" s="230">
+        <v>4</v>
+      </c>
+      <c r="G106" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="230" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="230" t="s">
+        <v>442</v>
+      </c>
+      <c r="C107" s="230">
+        <v>1</v>
+      </c>
+      <c r="D107" s="230">
+        <v>2</v>
+      </c>
+      <c r="E107" s="230">
+        <v>3</v>
+      </c>
+      <c r="F107" s="230">
+        <v>4</v>
+      </c>
+      <c r="G107" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="230" t="s">
+        <v>103</v>
+      </c>
+      <c r="B108" s="230" t="s">
+        <v>442</v>
+      </c>
+      <c r="C108" s="230">
+        <v>1</v>
+      </c>
+      <c r="D108" s="230">
+        <v>2</v>
+      </c>
+      <c r="E108" s="230">
+        <v>3</v>
+      </c>
+      <c r="F108" s="230">
+        <v>4</v>
+      </c>
+      <c r="G108" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="230" t="s">
+        <v>104</v>
+      </c>
+      <c r="B109" s="230" t="s">
+        <v>442</v>
+      </c>
+      <c r="C109" s="230">
+        <v>1</v>
+      </c>
+      <c r="D109" s="230">
+        <v>2</v>
+      </c>
+      <c r="E109" s="230">
+        <v>3</v>
+      </c>
+      <c r="F109" s="230">
+        <v>4</v>
+      </c>
+      <c r="G109" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="230" t="s">
+        <v>105</v>
+      </c>
       <c r="B110" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C110" s="230">
         <v>1</v>
@@ -38051,12 +37897,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="230">
-        <v>2</v>
+    <row r="111" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="230" t="s">
+        <v>107</v>
       </c>
       <c r="B111" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C111" s="230">
         <v>1</v>
@@ -38074,12 +37920,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="230">
-        <v>3</v>
+    <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="230" t="s">
+        <v>36</v>
       </c>
       <c r="B112" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C112" s="230">
         <v>1</v>
@@ -38098,11 +37944,11 @@
       </c>
     </row>
     <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="230">
-        <v>4</v>
+      <c r="A113" s="230" t="s">
+        <v>76</v>
       </c>
       <c r="B113" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C113" s="230">
         <v>1</v>
@@ -38121,11 +37967,11 @@
       </c>
     </row>
     <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="230">
-        <v>5</v>
+      <c r="A114" s="230" t="s">
+        <v>110</v>
       </c>
       <c r="B114" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C114" s="230">
         <v>1</v>
@@ -38144,45 +37990,54 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="230">
-        <v>7</v>
+      <c r="A115" s="230" t="s">
+        <v>62</v>
       </c>
       <c r="B115" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C115" s="230">
+        <v>1</v>
+      </c>
+      <c r="D115" s="230">
         <v>2</v>
       </c>
-      <c r="D115" s="230">
+      <c r="E115" s="230">
         <v>3</v>
       </c>
-      <c r="E115" s="230">
+      <c r="F115" s="230">
         <v>4</v>
       </c>
-      <c r="F115" s="230">
+      <c r="G115" s="230">
         <v>5</v>
       </c>
-      <c r="G115" s="230"/>
     </row>
     <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="230">
-        <v>7.1</v>
+      <c r="A116" s="230" t="s">
+        <v>64</v>
       </c>
       <c r="B116" s="230" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C116" s="230">
+        <v>1</v>
+      </c>
+      <c r="D116" s="230">
+        <v>2</v>
+      </c>
+      <c r="E116" s="230">
+        <v>3</v>
+      </c>
+      <c r="F116" s="230">
         <v>4</v>
       </c>
-      <c r="D116" s="230">
+      <c r="G116" s="230">
         <v>5</v>
       </c>
-      <c r="F116" s="230"/>
-      <c r="G116" s="230"/>
     </row>
     <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="230">
-        <v>7.2</v>
+      <c r="A117" s="230" t="s">
+        <v>565</v>
       </c>
       <c r="B117" s="230" t="s">
         <v>442</v>
@@ -38202,89 +38057,277 @@
       <c r="G117" s="230">
         <v>5</v>
       </c>
-      <c r="H117" s="238" t="s">
+    </row>
+    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="230"/>
+      <c r="B118" s="230"/>
+      <c r="C118" s="340"/>
+      <c r="D118" s="230"/>
+      <c r="E118" s="230"/>
+      <c r="F118" s="230"/>
+      <c r="G118" s="230"/>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="155" t="s">
+        <v>451</v>
+      </c>
+      <c r="B120" s="155"/>
+      <c r="C120" s="155" t="s">
+        <v>446</v>
+      </c>
+      <c r="H120" s="238" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="230">
+        <v>1</v>
+      </c>
+      <c r="B121" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C121" s="230">
+        <v>1</v>
+      </c>
+      <c r="D121" s="230">
+        <v>2</v>
+      </c>
+      <c r="E121" s="230">
+        <v>3</v>
+      </c>
+      <c r="F121" s="230">
+        <v>4</v>
+      </c>
+      <c r="G121" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="230">
+        <v>2</v>
+      </c>
+      <c r="B122" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C122" s="230">
+        <v>1</v>
+      </c>
+      <c r="D122" s="230">
+        <v>2</v>
+      </c>
+      <c r="E122" s="230">
+        <v>3</v>
+      </c>
+      <c r="F122" s="230">
+        <v>4</v>
+      </c>
+      <c r="G122" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="230">
+        <v>3</v>
+      </c>
+      <c r="B123" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C123" s="230">
+        <v>1</v>
+      </c>
+      <c r="D123" s="230">
+        <v>2</v>
+      </c>
+      <c r="E123" s="230">
+        <v>3</v>
+      </c>
+      <c r="F123" s="230">
+        <v>4</v>
+      </c>
+      <c r="G123" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="230">
+        <v>4</v>
+      </c>
+      <c r="B124" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C124" s="230">
+        <v>1</v>
+      </c>
+      <c r="D124" s="230">
+        <v>2</v>
+      </c>
+      <c r="E124" s="230">
+        <v>3</v>
+      </c>
+      <c r="F124" s="230">
+        <v>4</v>
+      </c>
+      <c r="G124" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="230">
+        <v>5</v>
+      </c>
+      <c r="B125" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C125" s="230">
+        <v>1</v>
+      </c>
+      <c r="D125" s="230">
+        <v>2</v>
+      </c>
+      <c r="E125" s="230">
+        <v>3</v>
+      </c>
+      <c r="F125" s="230">
+        <v>4</v>
+      </c>
+      <c r="G125" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="230">
+        <v>7</v>
+      </c>
+      <c r="B126" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C126" s="230">
+        <v>1</v>
+      </c>
+      <c r="D126" s="230">
+        <v>2</v>
+      </c>
+      <c r="E126" s="230">
+        <v>3</v>
+      </c>
+      <c r="F126" s="230">
+        <v>4</v>
+      </c>
+      <c r="G126" s="230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="230">
+        <v>7.1</v>
+      </c>
+      <c r="B127" s="230" t="s">
+        <v>445</v>
+      </c>
+      <c r="C127" s="230">
+        <v>4</v>
+      </c>
+      <c r="D127" s="230">
+        <v>5</v>
+      </c>
+      <c r="F127" s="230"/>
+      <c r="G127" s="230"/>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="230">
+        <v>7.2</v>
+      </c>
+      <c r="B128" s="230" t="s">
+        <v>442</v>
+      </c>
+      <c r="C128" s="230">
+        <v>1</v>
+      </c>
+      <c r="D128" s="230">
+        <v>2</v>
+      </c>
+      <c r="E128" s="230">
+        <v>3</v>
+      </c>
+      <c r="F128" s="230">
+        <v>4</v>
+      </c>
+      <c r="G128" s="230">
+        <v>5</v>
+      </c>
+      <c r="H128" s="238" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="230">
+    <row r="129" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="230">
         <v>8</v>
       </c>
-      <c r="B118" s="230" t="s">
+      <c r="B129" s="230" t="s">
         <v>442</v>
       </c>
-      <c r="C118" s="230">
+      <c r="C129" s="230">
         <v>1</v>
       </c>
-      <c r="D118" s="230">
+      <c r="D129" s="230">
         <v>2</v>
       </c>
-      <c r="E118" s="230">
+      <c r="E129" s="230">
         <v>3</v>
       </c>
-      <c r="F118" s="230">
+      <c r="F129" s="230">
         <v>4</v>
       </c>
-      <c r="G118" s="230">
+      <c r="G129" s="230">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="230">
+    <row r="130" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="230">
         <v>9</v>
       </c>
-      <c r="B119" s="230" t="s">
+      <c r="B130" s="230" t="s">
         <v>445</v>
       </c>
-      <c r="C119" s="230">
+      <c r="C130" s="230">
         <v>4</v>
       </c>
-      <c r="D119" s="230">
+      <c r="D130" s="230">
         <v>5</v>
       </c>
-      <c r="F119" s="230"/>
-      <c r="G119" s="230"/>
-    </row>
-    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="230">
+      <c r="F130" s="230"/>
+      <c r="G130" s="230"/>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="230">
         <v>10</v>
       </c>
-      <c r="B120" s="230" t="s">
+      <c r="B131" s="230" t="s">
         <v>445</v>
       </c>
-      <c r="C120" s="230">
+      <c r="C131" s="230">
         <v>4</v>
       </c>
-      <c r="D120" s="230">
+      <c r="D131" s="230">
         <v>5</v>
       </c>
-      <c r="F120" s="230"/>
-      <c r="G120" s="230"/>
-    </row>
-    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F131" s="230"/>
+      <c r="G131" s="230"/>
+    </row>
+    <row r="132" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -38307,216 +38350,206 @@
     <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sortState ref="A10:J83">
     <sortCondition ref="A10:A83"/>
   </sortState>
-  <conditionalFormatting sqref="A107:G107">
-    <cfRule type="expression" dxfId="64" priority="129">
+  <conditionalFormatting sqref="A118:G118 C69:J69 D70:J70 A68:B69 A75:J75 C71:J74 A13:J13 A15:J17 F14:J14 A14:D14 A34:J48 H49:J49 A113:G113 A51:J54 A56:J60 F55:J55 A55:D55 A76 D84:J85 A106:C117">
+    <cfRule type="expression" dxfId="64" priority="132">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D98:G98 A97:C97 A98:B98 A99:G106 A90:B96">
-    <cfRule type="expression" dxfId="63" priority="82">
+  <conditionalFormatting sqref="D98:G98 A97:C97 A98:B98 A90:B96 A99:G117">
+    <cfRule type="expression" dxfId="63" priority="85">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96:G97">
-    <cfRule type="expression" dxfId="62" priority="81">
+    <cfRule type="expression" dxfId="62" priority="84">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:G95">
-    <cfRule type="expression" dxfId="61" priority="80">
+    <cfRule type="expression" dxfId="61" priority="83">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:G94">
-    <cfRule type="expression" dxfId="60" priority="79">
+    <cfRule type="expression" dxfId="60" priority="82">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93:G93">
-    <cfRule type="expression" dxfId="59" priority="78">
+    <cfRule type="expression" dxfId="59" priority="81">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:G92">
-    <cfRule type="expression" dxfId="58" priority="77">
+    <cfRule type="expression" dxfId="58" priority="80">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:G91">
-    <cfRule type="expression" dxfId="57" priority="76">
+    <cfRule type="expression" dxfId="57" priority="79">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:G90">
-    <cfRule type="expression" dxfId="56" priority="75">
+    <cfRule type="expression" dxfId="56" priority="78">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A116:B120">
-    <cfRule type="expression" dxfId="55" priority="74">
+  <conditionalFormatting sqref="A127:B131">
+    <cfRule type="expression" dxfId="55" priority="77">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A110:B114">
-    <cfRule type="expression" dxfId="54" priority="73">
+  <conditionalFormatting sqref="A121:B125">
+    <cfRule type="expression" dxfId="54" priority="76">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A115:B115">
-    <cfRule type="expression" dxfId="53" priority="72">
+  <conditionalFormatting sqref="A126:B126">
+    <cfRule type="expression" dxfId="53" priority="75">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B112:B114">
-    <cfRule type="expression" dxfId="52" priority="71">
+  <conditionalFormatting sqref="B123:B125">
+    <cfRule type="expression" dxfId="52" priority="74">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F116:G116 C116:D116 C117:G118 F119:G120 C119:D120">
-    <cfRule type="expression" dxfId="51" priority="70">
+  <conditionalFormatting sqref="F127:G127 C127:D127 C128:G129 F130:G131 C130:D131">
+    <cfRule type="expression" dxfId="51" priority="73">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C110:G112">
-    <cfRule type="expression" dxfId="50" priority="69">
+  <conditionalFormatting sqref="C121:G123">
+    <cfRule type="expression" dxfId="50" priority="72">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G115">
-    <cfRule type="expression" dxfId="49" priority="68">
-      <formula>MOD(ROW(), 2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C115:F115">
-    <cfRule type="expression" dxfId="48" priority="67">
-      <formula>MOD(ROW(), 2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C113:G114">
-    <cfRule type="expression" dxfId="47" priority="66">
+  <conditionalFormatting sqref="C124:G125">
+    <cfRule type="expression" dxfId="49" priority="69">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:J87">
-    <cfRule type="expression" dxfId="46" priority="33">
+    <cfRule type="expression" dxfId="48" priority="36">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A84:J85">
-    <cfRule type="expression" dxfId="45" priority="32">
+  <conditionalFormatting sqref="A29 J83 I29:J29 C82 A18 D18:J18 A31:A33 I12:J12 A112:G112 H68:J68 C68:F68 A19:J20 A21:B28 C21:J27 A81:B82 A80 F65:J67 A65:A67 A64:J64 F61:J63 A61:A63 A30:J30 A50 E50:J50 A10:J11 D31:J31 F32:J33 C32:D33 A83:F83 C81:F81 F80 F76 G76:J82 A78:F79 D77:F77">
+    <cfRule type="expression" dxfId="47" priority="18">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29 J83 I29:J29 C82 A18 D18:J18 A31:A33 I12:J12 A12:G12 H68:J68 C68:F68 A13:J17 A19:J20 A21:B28 C21:J27 A81:B82 A80 F65:J67 A65:A67 A64:J64 F61:J63 A61:A63 A30:J30 A34:J49 A50 E50:J50 C69:J75 A68:B75 A51:J60 A10:J11 D31:J31 F32:J33 C32:D33 A83:F83 C81:F81 F80 F76 G76:J82 A77:F79 A76">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="46" priority="17">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29 D29:H29">
+    <cfRule type="expression" dxfId="45" priority="16">
+      <formula>MOD(ROW(), 2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
     <cfRule type="expression" dxfId="44" priority="15">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
+  <conditionalFormatting sqref="B31:C31">
     <cfRule type="expression" dxfId="43" priority="14">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29 D29:H29">
+  <conditionalFormatting sqref="B32:B33">
     <cfRule type="expression" dxfId="42" priority="13">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="B80:E80">
     <cfRule type="expression" dxfId="41" priority="12">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:C31">
+  <conditionalFormatting sqref="D76:E76">
     <cfRule type="expression" dxfId="40" priority="11">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B33">
+  <conditionalFormatting sqref="B67:E67">
     <cfRule type="expression" dxfId="39" priority="10">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80:E80">
+  <conditionalFormatting sqref="B66:E66">
     <cfRule type="expression" dxfId="38" priority="9">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B76:E76">
+  <conditionalFormatting sqref="B65:E65">
     <cfRule type="expression" dxfId="37" priority="8">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E67">
+  <conditionalFormatting sqref="B62:E62">
     <cfRule type="expression" dxfId="36" priority="7">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B66:E66">
+  <conditionalFormatting sqref="B63:E63">
     <cfRule type="expression" dxfId="35" priority="6">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B65:E65">
+  <conditionalFormatting sqref="B61:E61">
     <cfRule type="expression" dxfId="34" priority="5">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:E62">
+  <conditionalFormatting sqref="B50:D50">
     <cfRule type="expression" dxfId="33" priority="4">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B63:E63">
+  <conditionalFormatting sqref="B76:C76">
     <cfRule type="expression" dxfId="32" priority="3">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61:E61">
+  <conditionalFormatting sqref="B114:C116">
     <cfRule type="expression" dxfId="31" priority="2">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:D50">
+  <conditionalFormatting sqref="C126:G126">
     <cfRule type="expression" dxfId="30" priority="1">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D97:G98 C90:G96 C99:G107 C97 F119:G120 C119:D120 C117:G118 F116:G116 C116:D116 C110:G115" xr:uid="{C65133BC-AAC4-8F45-A472-8E04B60B630B}">
-      <formula1>"1, 2, 3, 4, 5"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B106:B107 B110:B120 B83 B10:B81" xr:uid="{8D1D524A-C617-AC40-8D5B-96059B1CB9AC}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B121:B131 B83 B10:B11 B13:B48 B50:B69 B78:B81 B75:B76 B106:B118" xr:uid="{8D1D524A-C617-AC40-8D5B-96059B1CB9AC}">
       <formula1>"not, only"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B90:B97 B84:B87" xr:uid="{4EEC21E0-40C6-EA41-881A-9C235CF911B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B90:B97 B86:B87" xr:uid="{4EEC21E0-40C6-EA41-881A-9C235CF911B0}">
       <formula1>"not, only"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32:D33 F32:J33 C34:J83" xr:uid="{04B15702-78C0-CE47-9D5B-CC1E5EED853C}">
-      <formula1>$A$4:$A$48</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C84:J87" xr:uid="{3A72C915-DDF9-FD48-A6C7-BA397E2973E1}">
-      <formula1>$A$4:$A$48</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2BD65379-2279-0A40-9372-2CEFB7D997D1}">
-          <x14:formula1>
-            <xm:f>'Design HV &amp; WD'!$A$4:$A$53</xm:f>
-          </x14:formula1>
-          <xm:sqref>C10:J31</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -40984,10 +41017,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AG250"/>
+  <dimension ref="A1:Z250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41057,14 +41090,14 @@
         <v>11</v>
       </c>
       <c r="I2" s="365"/>
-      <c r="J2" s="408" t="s">
+      <c r="J2" s="412" t="s">
         <v>504</v>
       </c>
-      <c r="K2" s="409"/>
-      <c r="L2" s="409"/>
-      <c r="M2" s="409"/>
-      <c r="N2" s="409"/>
-      <c r="O2" s="409"/>
+      <c r="K2" s="413"/>
+      <c r="L2" s="413"/>
+      <c r="M2" s="413"/>
+      <c r="N2" s="413"/>
+      <c r="O2" s="413"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="239" t="s">
@@ -41092,12 +41125,12 @@
         <v>11</v>
       </c>
       <c r="I3" s="365"/>
-      <c r="J3" s="409"/>
-      <c r="K3" s="409"/>
-      <c r="L3" s="409"/>
-      <c r="M3" s="409"/>
-      <c r="N3" s="409"/>
-      <c r="O3" s="409"/>
+      <c r="J3" s="413"/>
+      <c r="K3" s="413"/>
+      <c r="L3" s="413"/>
+      <c r="M3" s="413"/>
+      <c r="N3" s="413"/>
+      <c r="O3" s="413"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="239" t="s">
@@ -41125,12 +41158,12 @@
         <v>11</v>
       </c>
       <c r="I4" s="365"/>
-      <c r="J4" s="409"/>
-      <c r="K4" s="409"/>
-      <c r="L4" s="409"/>
-      <c r="M4" s="409"/>
-      <c r="N4" s="409"/>
-      <c r="O4" s="409"/>
+      <c r="J4" s="413"/>
+      <c r="K4" s="413"/>
+      <c r="L4" s="413"/>
+      <c r="M4" s="413"/>
+      <c r="N4" s="413"/>
+      <c r="O4" s="413"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -41803,7 +41836,7 @@
       </c>
       <c r="I27" s="365"/>
     </row>
-    <row r="28" spans="1:9" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="238" t="s">
         <v>505</v>
       </c>
@@ -42213,7 +42246,7 @@
       </c>
       <c r="I42" s="365"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="334" t="s">
         <v>54</v>
       </c>
@@ -42240,59 +42273,61 @@
       </c>
       <c r="I43" s="365"/>
     </row>
-    <row r="44" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>506</v>
       </c>
       <c r="B44" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="352">
-        <v>0</v>
-      </c>
-      <c r="D44" s="352">
-        <v>0.378</v>
-      </c>
-      <c r="E44" s="352">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="F44" s="352">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="G44" s="352">
-        <v>0</v>
+      <c r="C44" s="408">
+        <v>0</v>
+      </c>
+      <c r="D44" s="408">
+        <v>0.3912800206593785</v>
+      </c>
+      <c r="E44" s="408">
+        <v>0.1636136696221055</v>
+      </c>
+      <c r="F44" s="408">
+        <v>0.54432297495050352</v>
+      </c>
+      <c r="G44" s="408">
+        <v>8.6080743737625887E-6</v>
       </c>
       <c r="H44" s="392">
         <v>1.28</v>
       </c>
       <c r="I44" s="365"/>
     </row>
-    <row r="45" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="238" t="s">
         <v>506</v>
       </c>
       <c r="B45" s="92" t="s">
         <v>561</v>
       </c>
-      <c r="C45" s="238">
-        <v>0</v>
-      </c>
-      <c r="D45" s="238">
-        <v>5.6744061613737996E-2</v>
-      </c>
-      <c r="E45" s="238">
-        <v>4.1355841515097191E-2</v>
-      </c>
-      <c r="F45" s="238">
-        <v>0.12570252293077214</v>
-      </c>
-      <c r="G45" s="238">
+      <c r="C45" s="348">
+        <v>0</v>
+      </c>
+      <c r="D45" s="348">
+        <v>0.23</v>
+      </c>
+      <c r="E45" s="348">
+        <v>0.12</v>
+      </c>
+      <c r="F45" s="348">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G45" s="348">
         <v>0</v>
       </c>
       <c r="H45" s="392">
         <v>1.28</v>
       </c>
-      <c r="I45" s="365"/>
+      <c r="I45" s="365" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="336" t="s">
@@ -45827,7 +45862,7 @@
         <v>1.661174476170213E-2</v>
       </c>
       <c r="H176" s="392">
-        <v>3.94</v>
+        <v>5.36</v>
       </c>
       <c r="I176" s="365"/>
     </row>
@@ -45881,7 +45916,7 @@
         <v>3.1523409983521163E-2</v>
       </c>
       <c r="H178" s="392">
-        <v>5.36</v>
+        <v>3.94</v>
       </c>
       <c r="I178" s="365"/>
     </row>
@@ -45908,7 +45943,7 @@
         <v>3.1523409983521163E-2</v>
       </c>
       <c r="H179" s="392">
-        <v>5.36</v>
+        <v>3.94</v>
       </c>
       <c r="I179" s="365"/>
     </row>
@@ -47127,7 +47162,7 @@
       </c>
       <c r="I224" s="365"/>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" s="334" t="s">
         <v>156</v>
       </c>
@@ -47154,7 +47189,7 @@
       </c>
       <c r="I225" s="365"/>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" s="336" t="s">
         <v>157</v>
       </c>
@@ -47181,7 +47216,7 @@
       </c>
       <c r="I226" s="365"/>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" s="336" t="s">
         <v>158</v>
       </c>
@@ -47208,7 +47243,7 @@
       </c>
       <c r="I227" s="365"/>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" s="239" t="s">
         <v>159</v>
       </c>
@@ -47235,7 +47270,7 @@
       </c>
       <c r="I228" s="365"/>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" s="239" t="s">
         <v>160</v>
       </c>
@@ -47262,7 +47297,7 @@
       </c>
       <c r="I229" s="365"/>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" s="334" t="s">
         <v>161</v>
       </c>
@@ -47289,7 +47324,7 @@
       </c>
       <c r="I230" s="365"/>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" s="334" t="s">
         <v>162</v>
       </c>
@@ -47316,7 +47351,7 @@
       </c>
       <c r="I231" s="365"/>
     </row>
-    <row r="232" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" s="336" t="s">
         <v>163</v>
       </c>
@@ -47343,7 +47378,7 @@
       </c>
       <c r="I232" s="365"/>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" s="336" t="s">
         <v>164</v>
       </c>
@@ -47370,7 +47405,7 @@
       </c>
       <c r="I233" s="365"/>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" s="336" t="s">
         <v>165</v>
       </c>
@@ -47397,7 +47432,7 @@
       </c>
       <c r="I234" s="365"/>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" s="336" t="s">
         <v>166</v>
       </c>
@@ -47423,9 +47458,8 @@
         <v>0.93</v>
       </c>
       <c r="I235" s="365"/>
-      <c r="T235" s="235"/>
-    </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" s="336" t="s">
         <v>167</v>
       </c>
@@ -47451,9 +47485,8 @@
         <v>0.93</v>
       </c>
       <c r="I236" s="365"/>
-      <c r="T236" s="235"/>
-    </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" s="336" t="s">
         <v>168</v>
       </c>
@@ -47479,9 +47512,8 @@
         <v>0.93</v>
       </c>
       <c r="I237" s="365"/>
-      <c r="T237" s="235"/>
-    </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" s="336" t="s">
         <v>169</v>
       </c>
@@ -47507,9 +47539,8 @@
         <v>0.93</v>
       </c>
       <c r="I238" s="365"/>
-      <c r="T238" s="235"/>
-    </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" s="336" t="s">
         <v>170</v>
       </c>
@@ -47536,7 +47567,7 @@
       </c>
       <c r="I239" s="365"/>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" s="336" t="s">
         <v>171</v>
       </c>
@@ -47563,7 +47594,7 @@
       </c>
       <c r="I240" s="365"/>
     </row>
-    <row r="241" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A241" s="336" t="s">
         <v>171</v>
       </c>
@@ -47590,7 +47621,7 @@
       </c>
       <c r="I241" s="365"/>
     </row>
-    <row r="242" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A242" s="239"/>
       <c r="B242" s="373"/>
       <c r="C242" s="236"/>
@@ -47599,7 +47630,7 @@
       <c r="F242" s="236"/>
       <c r="G242" s="236"/>
     </row>
-    <row r="243" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A243" s="334"/>
       <c r="B243" s="373"/>
       <c r="C243" s="236"/>
@@ -47608,7 +47639,7 @@
       <c r="F243" s="236"/>
       <c r="G243" s="236"/>
     </row>
-    <row r="244" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B244" s="373"/>
       <c r="C244" s="236"/>
       <c r="D244" s="236"/>
@@ -47617,7 +47648,7 @@
       <c r="G244" s="236"/>
       <c r="H244" s="366"/>
     </row>
-    <row r="245" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B245" s="373"/>
       <c r="C245" s="236"/>
       <c r="D245" s="236"/>
@@ -47626,7 +47657,7 @@
       <c r="G245" s="236"/>
       <c r="H245" s="366"/>
     </row>
-    <row r="246" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B246" s="373"/>
       <c r="C246" s="236"/>
       <c r="D246" s="236"/>
@@ -47635,7 +47666,7 @@
       <c r="G246" s="236"/>
       <c r="H246" s="366"/>
     </row>
-    <row r="247" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A247" s="239"/>
       <c r="B247" s="373"/>
       <c r="C247" s="236"/>
@@ -47644,7 +47675,7 @@
       <c r="F247" s="236"/>
       <c r="G247" s="236"/>
     </row>
-    <row r="248" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A248" s="239"/>
       <c r="B248" s="373"/>
       <c r="C248" s="236"/>
@@ -47653,40 +47684,31 @@
       <c r="F248" s="236"/>
       <c r="G248" s="236"/>
     </row>
-    <row r="249" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="V249" s="407"/>
-      <c r="W249" s="407"/>
-      <c r="X249" s="407"/>
-      <c r="Y249" s="407"/>
-      <c r="Z249" s="407"/>
-      <c r="AA249" s="407"/>
-      <c r="AB249" s="407"/>
-      <c r="AC249" s="407"/>
-      <c r="AD249" s="407"/>
-      <c r="AE249" s="407"/>
-      <c r="AF249" s="407"/>
-      <c r="AG249" s="407"/>
-    </row>
-    <row r="250" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="V250" s="407"/>
-      <c r="W250" s="407"/>
-      <c r="X250" s="407"/>
-      <c r="Y250" s="407"/>
-      <c r="Z250" s="407"/>
-      <c r="AA250" s="407"/>
-      <c r="AB250" s="407"/>
-      <c r="AC250" s="407"/>
-      <c r="AD250" s="407"/>
-      <c r="AE250" s="407"/>
-      <c r="AF250" s="407"/>
-      <c r="AG250" s="407"/>
+    <row r="249" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="S249" s="404"/>
+      <c r="T249" s="404"/>
+      <c r="U249" s="404"/>
+      <c r="V249" s="404"/>
+      <c r="W249" s="404"/>
+      <c r="X249" s="404"/>
+      <c r="Y249" s="404"/>
+      <c r="Z249" s="404"/>
+    </row>
+    <row r="250" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="S250" s="404"/>
+      <c r="T250" s="404"/>
+      <c r="U250" s="404"/>
+      <c r="V250" s="404"/>
+      <c r="W250" s="404"/>
+      <c r="X250" s="404"/>
+      <c r="Y250" s="404"/>
+      <c r="Z250" s="404"/>
     </row>
   </sheetData>
-  <sortState ref="A2:I217">
-    <sortCondition ref="A2:A217"/>
+  <sortState ref="A2:I215">
+    <sortCondition ref="A2:A215"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="V249:AG250"/>
+  <mergeCells count="1">
     <mergeCell ref="J2:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -47703,8 +47725,8 @@
   </sheetPr>
   <dimension ref="A1:AB74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X54" sqref="X54"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47723,18 +47745,18 @@
     </row>
     <row r="2" spans="1:28" s="239" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="343"/>
-      <c r="D2" s="410" t="s">
+      <c r="D2" s="414" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="411"/>
-      <c r="F2" s="411"/>
-      <c r="G2" s="411"/>
-      <c r="H2" s="411"/>
+      <c r="E2" s="415"/>
+      <c r="F2" s="415"/>
+      <c r="G2" s="415"/>
+      <c r="H2" s="415"/>
       <c r="I2" s="241"/>
-      <c r="S2" s="414" t="s">
+      <c r="S2" s="418" t="s">
         <v>279</v>
       </c>
-      <c r="T2" s="414"/>
+      <c r="T2" s="418"/>
     </row>
     <row r="3" spans="1:28" s="239" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="140" t="s">
@@ -47791,28 +47813,28 @@
     SUMIFS('As-Built HV &amp; WD'!D:D, 'As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4)/COUNTIFS('As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4),
     V28
 )</f>
-        <v>0.30640866955624207</v>
+        <v>0.30675814378412047</v>
       </c>
       <c r="F4" s="143">
         <f>IFERROR(
     SUMIFS('As-Built HV &amp; WD'!E:E, 'As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4)/COUNTIFS('As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4),
     W28
 )</f>
-        <v>0.14165648650312915</v>
+        <v>0.14004105675634246</v>
       </c>
       <c r="G4" s="143">
         <f>IFERROR(
     SUMIFS('As-Built HV &amp; WD'!F:F, 'As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4)/COUNTIFS('As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4),
     X28
 )</f>
-        <v>0.48086693680729431</v>
+        <v>0.47819122562178124</v>
       </c>
       <c r="H4" s="143">
         <f>IFERROR(
     SUMIFS('As-Built HV &amp; WD'!G:G, 'As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4)/COUNTIFS('As-Built HV &amp; WD'!$B:$B, 'Design HV &amp; WD'!$A4),
     Y28
 )</f>
-        <v>3.4631986020090405E-3</v>
+        <v>3.4634251302820339E-3</v>
       </c>
       <c r="I4" s="207">
         <v>3.13</v>
@@ -48320,19 +48342,19 @@
       </c>
       <c r="E14" s="143">
         <f t="shared" si="0"/>
-        <v>0.1986286024112309</v>
+        <v>0.19876839210238226</v>
       </c>
       <c r="F14" s="143">
         <f t="shared" si="0"/>
-        <v>0.14887314652130029</v>
+        <v>0.14822697462258561</v>
       </c>
       <c r="G14" s="143">
         <f t="shared" si="0"/>
-        <v>0.3594920387351046</v>
+        <v>0.35842175426089934</v>
       </c>
       <c r="H14" s="143">
         <f t="shared" si="0"/>
-        <v>9.6255279958561632E-3</v>
+        <v>9.6256186071653621E-3</v>
       </c>
       <c r="I14" s="396">
         <v>2.6598581560283683</v>
@@ -48355,19 +48377,19 @@
       </c>
       <c r="E15" s="143">
         <f t="shared" si="0"/>
-        <v>0.1986286024112309</v>
+        <v>0.19876839210238226</v>
       </c>
       <c r="F15" s="143">
         <f t="shared" si="0"/>
-        <v>0.14887314652130029</v>
+        <v>0.14822697462258561</v>
       </c>
       <c r="G15" s="143">
         <f t="shared" si="0"/>
-        <v>0.3594920387351046</v>
+        <v>0.35842175426089934</v>
       </c>
       <c r="H15" s="143">
         <f t="shared" si="0"/>
-        <v>9.6255279958561632E-3</v>
+        <v>9.6256186071653621E-3</v>
       </c>
       <c r="I15" s="396">
         <v>2.3273758865248224</v>
@@ -48390,19 +48412,19 @@
       </c>
       <c r="E16" s="143">
         <f t="shared" si="0"/>
-        <v>0.1986286024112309</v>
+        <v>0.19876839210238226</v>
       </c>
       <c r="F16" s="143">
         <f t="shared" si="0"/>
-        <v>0.14887314652130029</v>
+        <v>0.14822697462258561</v>
       </c>
       <c r="G16" s="143">
         <f t="shared" si="0"/>
-        <v>0.3594920387351046</v>
+        <v>0.35842175426089934</v>
       </c>
       <c r="H16" s="143">
         <f t="shared" si="0"/>
-        <v>9.6255279958561632E-3</v>
+        <v>9.6256186071653621E-3</v>
       </c>
       <c r="I16" s="396">
         <v>2.3273758865248224</v>
@@ -48425,19 +48447,19 @@
       </c>
       <c r="E17" s="143">
         <f t="shared" si="0"/>
-        <v>0.1986286024112309</v>
+        <v>0.19876839210238226</v>
       </c>
       <c r="F17" s="143">
         <f t="shared" si="0"/>
-        <v>0.14887314652130029</v>
+        <v>0.14822697462258561</v>
       </c>
       <c r="G17" s="143">
         <f t="shared" si="0"/>
-        <v>0.3594920387351046</v>
+        <v>0.35842175426089934</v>
       </c>
       <c r="H17" s="143">
         <f t="shared" si="0"/>
-        <v>9.6255279958561632E-3</v>
+        <v>9.6256186071653621E-3</v>
       </c>
       <c r="I17" s="396">
         <v>1.6624113475177305</v>
@@ -48463,19 +48485,19 @@
       </c>
       <c r="E18" s="143">
         <f t="shared" si="0"/>
-        <v>0.1986286024112309</v>
+        <v>0.19876839210238226</v>
       </c>
       <c r="F18" s="143">
         <f t="shared" si="0"/>
-        <v>0.14887314652130029</v>
+        <v>0.14822697462258561</v>
       </c>
       <c r="G18" s="143">
         <f t="shared" si="0"/>
-        <v>0.3594920387351046</v>
+        <v>0.35842175426089934</v>
       </c>
       <c r="H18" s="143">
         <f t="shared" si="0"/>
-        <v>9.6255279958561632E-3</v>
+        <v>9.6256186071653621E-3</v>
       </c>
       <c r="I18" s="396">
         <v>1.33</v>
@@ -48498,19 +48520,19 @@
       </c>
       <c r="E19" s="143">
         <f t="shared" si="0"/>
-        <v>0.1986286024112309</v>
+        <v>0.19876839210238226</v>
       </c>
       <c r="F19" s="143">
         <f t="shared" si="0"/>
-        <v>0.14887314652130029</v>
+        <v>0.14822697462258561</v>
       </c>
       <c r="G19" s="143">
         <f t="shared" si="0"/>
-        <v>0.3594920387351046</v>
+        <v>0.35842175426089934</v>
       </c>
       <c r="H19" s="143">
         <f t="shared" si="0"/>
-        <v>9.6255279958561632E-3</v>
+        <v>9.6256186071653621E-3</v>
       </c>
       <c r="I19" s="396">
         <v>1.6624113475177305</v>
@@ -48752,11 +48774,11 @@
       <c r="J26" s="237"/>
       <c r="K26"/>
       <c r="L26"/>
-      <c r="U26" s="412"/>
-      <c r="V26" s="413"/>
-      <c r="W26" s="413"/>
-      <c r="X26" s="413"/>
-      <c r="Y26" s="413"/>
+      <c r="U26" s="416"/>
+      <c r="V26" s="417"/>
+      <c r="W26" s="417"/>
+      <c r="X26" s="417"/>
+      <c r="Y26" s="417"/>
       <c r="Z26" s="397"/>
     </row>
     <row r="27" spans="1:26" s="239" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
commit prior to deleting DWM column in MP_new sheet
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18E94A1-FF35-694B-BBBF-393DE718C224}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D011A696-B003-DA49-A0EB-211CE6836100}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="3" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{C75C2548-8912-304F-B1DD-477CFCE62736}"/>
+    <workbookView xWindow="5800" yWindow="680" windowWidth="27720" windowHeight="17620" activeTab="2" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -4557,6 +4556,40 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="175" fontId="3" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="80" xfId="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="3" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="80" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="80" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="82" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4803,40 +4836,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="175" fontId="3" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="80" xfId="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="80" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="80" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="82" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="86">
@@ -8082,11 +8081,8 @@
   </sheetPr>
   <dimension ref="A1:CP191"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="1">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9468,7 +9464,7 @@
       <c r="F37" s="340" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="501" t="s">
+      <c r="G37" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H37" s="129"/>
@@ -9692,7 +9688,7 @@
       <c r="F44" s="255" t="s">
         <v>582</v>
       </c>
-      <c r="G44" s="490" t="s">
+      <c r="G44" s="405" t="s">
         <v>617</v>
       </c>
       <c r="H44" s="129"/>
@@ -10012,7 +10008,7 @@
       <c r="F54" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G54" s="490" t="s">
+      <c r="G54" s="405" t="s">
         <v>617</v>
       </c>
       <c r="H54" s="129"/>
@@ -10036,7 +10032,7 @@
         <v>0.38421875000000005</v>
       </c>
       <c r="D55" s="238">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E55" s="255" t="s">
         <v>39</v>
@@ -10396,7 +10392,7 @@
       <c r="F62" s="255" t="s">
         <v>35</v>
       </c>
-      <c r="G62" s="490" t="s">
+      <c r="G62" s="405" t="s">
         <v>617</v>
       </c>
       <c r="H62" s="129"/>
@@ -10716,7 +10712,7 @@
       <c r="F70" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G70" s="501" t="s">
+      <c r="G70" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H70" s="129"/>
@@ -10748,7 +10744,7 @@
       <c r="F71" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G71" s="501" t="s">
+      <c r="G71" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H71" s="129"/>
@@ -10780,7 +10776,7 @@
       <c r="F72" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G72" s="501" t="s">
+      <c r="G72" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H72" s="129"/>
@@ -10876,7 +10872,7 @@
       <c r="F73" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G73" s="501" t="s">
+      <c r="G73" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H73" s="129"/>
@@ -10908,7 +10904,7 @@
       <c r="F74" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G74" s="501" t="s">
+      <c r="G74" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H74" s="129"/>
@@ -10940,7 +10936,7 @@
       <c r="F75" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G75" s="501" t="s">
+      <c r="G75" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H75" s="129"/>
@@ -11164,7 +11160,7 @@
       <c r="F80" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G80" s="501" t="s">
+      <c r="G80" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H80" s="129"/>
@@ -11196,7 +11192,7 @@
       <c r="F81" s="340" t="s">
         <v>39</v>
       </c>
-      <c r="G81" s="501" t="s">
+      <c r="G81" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H81" s="129"/>
@@ -12668,7 +12664,7 @@
       <c r="F127" s="255" t="s">
         <v>39</v>
       </c>
-      <c r="G127" s="501" t="s">
+      <c r="G127" s="416" t="s">
         <v>612</v>
       </c>
       <c r="H127" s="129"/>
@@ -14661,7 +14657,6 @@
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17119,9 +17114,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:B1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -17140,16 +17132,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="446" t="s">
+      <c r="A1" s="460" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="447"/>
+      <c r="B1" s="461"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="448" t="s">
+      <c r="A2" s="462" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="449"/>
+      <c r="B2" s="463"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="X3" s="239" t="s">
@@ -17157,33 +17149,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="453" t="s">
+      <c r="A4" s="467" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="454"/>
+      <c r="B4" s="468"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="457" t="s">
+      <c r="D4" s="471" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="450" t="s">
+      <c r="E4" s="464" t="s">
         <v>177</v>
       </c>
-      <c r="F4" s="451"/>
-      <c r="G4" s="451"/>
-      <c r="H4" s="451"/>
-      <c r="I4" s="451"/>
-      <c r="J4" s="451"/>
-      <c r="K4" s="451"/>
-      <c r="L4" s="451"/>
-      <c r="M4" s="451"/>
-      <c r="N4" s="451"/>
-      <c r="O4" s="451"/>
-      <c r="P4" s="451"/>
-      <c r="Q4" s="451"/>
-      <c r="R4" s="451"/>
-      <c r="S4" s="451"/>
-      <c r="T4" s="451"/>
-      <c r="U4" s="452"/>
+      <c r="F4" s="465"/>
+      <c r="G4" s="465"/>
+      <c r="H4" s="465"/>
+      <c r="I4" s="465"/>
+      <c r="J4" s="465"/>
+      <c r="K4" s="465"/>
+      <c r="L4" s="465"/>
+      <c r="M4" s="465"/>
+      <c r="N4" s="465"/>
+      <c r="O4" s="465"/>
+      <c r="P4" s="465"/>
+      <c r="Q4" s="465"/>
+      <c r="R4" s="465"/>
+      <c r="S4" s="465"/>
+      <c r="T4" s="465"/>
+      <c r="U4" s="466"/>
       <c r="Y4" s="239">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -17250,12 +17242,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="455"/>
-      <c r="B5" s="456"/>
+      <c r="A5" s="469"/>
+      <c r="B5" s="470"/>
       <c r="C5" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="458"/>
+      <c r="D5" s="472"/>
       <c r="E5" s="69">
         <f>'Step Cost Analysis'!E5</f>
         <v>2020</v>
@@ -17393,10 +17385,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="425" t="s">
+      <c r="A6" s="439" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="426"/>
+      <c r="B6" s="440"/>
       <c r="C6" s="160">
         <v>10</v>
       </c>
@@ -17914,12 +17906,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="440" t="s">
+      <c r="A12" s="454" t="s">
         <v>191</v>
       </c>
-      <c r="B12" s="441"/>
-      <c r="C12" s="441"/>
-      <c r="D12" s="442"/>
+      <c r="B12" s="455"/>
+      <c r="C12" s="455"/>
+      <c r="D12" s="456"/>
       <c r="E12" s="279">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -18054,12 +18046,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="440" t="s">
+      <c r="A13" s="454" t="s">
         <v>192</v>
       </c>
-      <c r="B13" s="441"/>
-      <c r="C13" s="441"/>
-      <c r="D13" s="442"/>
+      <c r="B13" s="455"/>
+      <c r="C13" s="455"/>
+      <c r="D13" s="456"/>
       <c r="E13" s="279"/>
       <c r="F13" s="279"/>
       <c r="G13" s="279"/>
@@ -18152,10 +18144,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="425" t="s">
+      <c r="A14" s="439" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="426"/>
+      <c r="B14" s="440"/>
       <c r="C14" s="162">
         <v>10</v>
       </c>
@@ -18670,12 +18662,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="440" t="s">
+      <c r="A20" s="454" t="s">
         <v>196</v>
       </c>
-      <c r="B20" s="441"/>
-      <c r="C20" s="441"/>
-      <c r="D20" s="442"/>
+      <c r="B20" s="455"/>
+      <c r="C20" s="455"/>
+      <c r="D20" s="456"/>
       <c r="E20" s="279">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -18746,12 +18738,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="440" t="s">
+      <c r="A21" s="454" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="441"/>
-      <c r="C21" s="441"/>
-      <c r="D21" s="442"/>
+      <c r="B21" s="455"/>
+      <c r="C21" s="455"/>
+      <c r="D21" s="456"/>
       <c r="E21" s="279"/>
       <c r="F21" s="279"/>
       <c r="G21" s="279"/>
@@ -18777,10 +18769,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="425" t="s">
+      <c r="A22" s="439" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="426"/>
+      <c r="B22" s="440"/>
       <c r="C22" s="160">
         <v>10</v>
       </c>
@@ -19027,12 +19019,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="440" t="s">
+      <c r="A28" s="454" t="s">
         <v>199</v>
       </c>
-      <c r="B28" s="441"/>
-      <c r="C28" s="441"/>
-      <c r="D28" s="442"/>
+      <c r="B28" s="455"/>
+      <c r="C28" s="455"/>
+      <c r="D28" s="456"/>
       <c r="E28" s="279">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -19103,12 +19095,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="440" t="s">
+      <c r="A29" s="454" t="s">
         <v>200</v>
       </c>
-      <c r="B29" s="441"/>
-      <c r="C29" s="441"/>
-      <c r="D29" s="442"/>
+      <c r="B29" s="455"/>
+      <c r="C29" s="455"/>
+      <c r="D29" s="456"/>
       <c r="E29" s="279"/>
       <c r="F29" s="279"/>
       <c r="G29" s="279"/>
@@ -19134,10 +19126,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="425" t="s">
+      <c r="A30" s="439" t="s">
         <v>201</v>
       </c>
-      <c r="B30" s="426"/>
+      <c r="B30" s="440"/>
       <c r="C30" s="160">
         <v>10</v>
       </c>
@@ -19384,12 +19376,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="440" t="s">
+      <c r="A36" s="454" t="s">
         <v>202</v>
       </c>
-      <c r="B36" s="441"/>
-      <c r="C36" s="441"/>
-      <c r="D36" s="442"/>
+      <c r="B36" s="455"/>
+      <c r="C36" s="455"/>
+      <c r="D36" s="456"/>
       <c r="E36" s="279">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -19460,12 +19452,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="440" t="s">
+      <c r="A37" s="454" t="s">
         <v>203</v>
       </c>
-      <c r="B37" s="441"/>
-      <c r="C37" s="441"/>
-      <c r="D37" s="442"/>
+      <c r="B37" s="455"/>
+      <c r="C37" s="455"/>
+      <c r="D37" s="456"/>
       <c r="E37" s="279"/>
       <c r="F37" s="279"/>
       <c r="G37" s="279"/>
@@ -19491,10 +19483,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="425" t="s">
+      <c r="A38" s="439" t="s">
         <v>204</v>
       </c>
-      <c r="B38" s="426"/>
+      <c r="B38" s="440"/>
       <c r="C38" s="160">
         <v>10</v>
       </c>
@@ -19741,12 +19733,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="440" t="s">
+      <c r="A44" s="454" t="s">
         <v>205</v>
       </c>
-      <c r="B44" s="441"/>
-      <c r="C44" s="441"/>
-      <c r="D44" s="442"/>
+      <c r="B44" s="455"/>
+      <c r="C44" s="455"/>
+      <c r="D44" s="456"/>
       <c r="E44" s="279">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -19817,12 +19809,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="440" t="s">
+      <c r="A45" s="454" t="s">
         <v>206</v>
       </c>
-      <c r="B45" s="441"/>
-      <c r="C45" s="441"/>
-      <c r="D45" s="442"/>
+      <c r="B45" s="455"/>
+      <c r="C45" s="455"/>
+      <c r="D45" s="456"/>
       <c r="E45" s="279"/>
       <c r="F45" s="279"/>
       <c r="G45" s="279"/>
@@ -19848,11 +19840,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="427" t="s">
+      <c r="A46" s="441" t="s">
         <v>207</v>
       </c>
-      <c r="B46" s="428"/>
-      <c r="C46" s="429"/>
+      <c r="B46" s="442"/>
+      <c r="C46" s="443"/>
       <c r="D46" s="170"/>
       <c r="E46" s="287">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -19925,12 +19917,12 @@
       <c r="V46" s="240"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="435" t="s">
+      <c r="A47" s="449" t="s">
         <v>208</v>
       </c>
-      <c r="B47" s="436"/>
-      <c r="C47" s="436"/>
-      <c r="D47" s="437"/>
+      <c r="B47" s="450"/>
+      <c r="C47" s="450"/>
+      <c r="D47" s="451"/>
       <c r="E47" s="288">
         <f>E46</f>
         <v>1500000</v>
@@ -20001,7 +19993,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A48" s="171"/>
       <c r="B48" s="171"/>
-      <c r="C48" s="438" t="s">
+      <c r="C48" s="452" t="s">
         <v>209</v>
       </c>
       <c r="D48" s="172">
@@ -20076,7 +20068,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A49" s="171"/>
-      <c r="C49" s="439"/>
+      <c r="C49" s="453"/>
       <c r="D49" s="242">
         <v>37</v>
       </c>
@@ -20147,7 +20139,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A50" s="171"/>
-      <c r="C50" s="439"/>
+      <c r="C50" s="453"/>
       <c r="D50" s="242">
         <v>30</v>
       </c>
@@ -20218,7 +20210,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A51" s="171"/>
-      <c r="C51" s="439"/>
+      <c r="C51" s="453"/>
       <c r="D51" s="242">
         <v>41</v>
       </c>
@@ -20288,38 +20280,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="430" t="s">
+      <c r="A52" s="444" t="s">
         <v>210</v>
       </c>
-      <c r="B52" s="431"/>
-      <c r="C52" s="431"/>
-      <c r="D52" s="431"/>
-      <c r="E52" s="431"/>
-      <c r="F52" s="431"/>
-      <c r="G52" s="431"/>
-      <c r="H52" s="431"/>
-      <c r="I52" s="431"/>
-      <c r="J52" s="431"/>
-      <c r="K52" s="431"/>
-      <c r="L52" s="431"/>
-      <c r="M52" s="431"/>
-      <c r="N52" s="431"/>
-      <c r="O52" s="431"/>
-      <c r="P52" s="431"/>
-      <c r="Q52" s="431"/>
-      <c r="R52" s="431"/>
-      <c r="S52" s="431"/>
-      <c r="T52" s="431"/>
-      <c r="U52" s="431"/>
-      <c r="V52" s="431"/>
-      <c r="W52" s="432"/>
+      <c r="B52" s="445"/>
+      <c r="C52" s="445"/>
+      <c r="D52" s="445"/>
+      <c r="E52" s="445"/>
+      <c r="F52" s="445"/>
+      <c r="G52" s="445"/>
+      <c r="H52" s="445"/>
+      <c r="I52" s="445"/>
+      <c r="J52" s="445"/>
+      <c r="K52" s="445"/>
+      <c r="L52" s="445"/>
+      <c r="M52" s="445"/>
+      <c r="N52" s="445"/>
+      <c r="O52" s="445"/>
+      <c r="P52" s="445"/>
+      <c r="Q52" s="445"/>
+      <c r="R52" s="445"/>
+      <c r="S52" s="445"/>
+      <c r="T52" s="445"/>
+      <c r="U52" s="445"/>
+      <c r="V52" s="445"/>
+      <c r="W52" s="446"/>
       <c r="X52" s="240"/>
     </row>
     <row r="53" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="433" t="s">
+      <c r="A53" s="447" t="s">
         <v>211</v>
       </c>
-      <c r="B53" s="434"/>
+      <c r="B53" s="448"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -20496,10 +20488,10 @@
       <c r="X57" s="240"/>
     </row>
     <row r="58" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="423" t="s">
+      <c r="A58" s="437" t="s">
         <v>213</v>
       </c>
-      <c r="B58" s="424"/>
+      <c r="B58" s="438"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -20681,10 +20673,10 @@
       <c r="X62" s="240"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="423" t="s">
+      <c r="A63" s="437" t="s">
         <v>214</v>
       </c>
-      <c r="B63" s="424"/>
+      <c r="B63" s="438"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -20874,10 +20866,10 @@
       <c r="X67" s="240"/>
     </row>
     <row r="68" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="423" t="s">
+      <c r="A68" s="437" t="s">
         <v>215</v>
       </c>
-      <c r="B68" s="424"/>
+      <c r="B68" s="438"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -21055,10 +21047,10 @@
       <c r="X72" s="240"/>
     </row>
     <row r="73" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="423" t="s">
+      <c r="A73" s="437" t="s">
         <v>216</v>
       </c>
-      <c r="B73" s="424"/>
+      <c r="B73" s="438"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -21284,10 +21276,10 @@
       <c r="X77" s="240"/>
     </row>
     <row r="78" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="423" t="s">
+      <c r="A78" s="437" t="s">
         <v>218</v>
       </c>
-      <c r="B78" s="424"/>
+      <c r="B78" s="438"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -21459,10 +21451,10 @@
       <c r="X82" s="240"/>
     </row>
     <row r="83" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="423" t="s">
+      <c r="A83" s="437" t="s">
         <v>220</v>
       </c>
-      <c r="B83" s="424"/>
+      <c r="B83" s="438"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -21634,10 +21626,10 @@
       <c r="X87" s="240"/>
     </row>
     <row r="88" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="423" t="s">
+      <c r="A88" s="437" t="s">
         <v>51</v>
       </c>
-      <c r="B88" s="424"/>
+      <c r="B88" s="438"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -21809,10 +21801,10 @@
       <c r="X92" s="240"/>
     </row>
     <row r="93" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="423" t="s">
+      <c r="A93" s="437" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="424"/>
+      <c r="B93" s="438"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -22014,10 +22006,10 @@
       <c r="X97" s="240"/>
     </row>
     <row r="98" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="423" t="s">
+      <c r="A98" s="437" t="s">
         <v>225</v>
       </c>
-      <c r="B98" s="424"/>
+      <c r="B98" s="438"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -22209,10 +22201,10 @@
       <c r="X102" s="240"/>
     </row>
     <row r="103" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="423" t="s">
+      <c r="A103" s="437" t="s">
         <v>227</v>
       </c>
-      <c r="B103" s="424"/>
+      <c r="B103" s="438"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -22414,10 +22406,10 @@
       <c r="X107" s="240"/>
     </row>
     <row r="108" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="423" t="s">
+      <c r="A108" s="437" t="s">
         <v>228</v>
       </c>
-      <c r="B108" s="424"/>
+      <c r="B108" s="438"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -22619,10 +22611,10 @@
       <c r="X112" s="240"/>
     </row>
     <row r="113" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="423" t="s">
+      <c r="A113" s="437" t="s">
         <v>229</v>
       </c>
-      <c r="B113" s="424"/>
+      <c r="B113" s="438"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -22784,10 +22776,10 @@
       <c r="X117" s="240"/>
     </row>
     <row r="118" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="423" t="s">
+      <c r="A118" s="437" t="s">
         <v>230</v>
       </c>
-      <c r="B118" s="424"/>
+      <c r="B118" s="438"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -22989,10 +22981,10 @@
       <c r="X122" s="240"/>
     </row>
     <row r="123" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="423" t="s">
+      <c r="A123" s="437" t="s">
         <v>231</v>
       </c>
-      <c r="B123" s="424"/>
+      <c r="B123" s="438"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -23194,10 +23186,10 @@
       <c r="X127" s="240"/>
     </row>
     <row r="128" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="423" t="s">
+      <c r="A128" s="437" t="s">
         <v>232</v>
       </c>
-      <c r="B128" s="424"/>
+      <c r="B128" s="438"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -23399,10 +23391,10 @@
       <c r="X132" s="240"/>
     </row>
     <row r="133" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="423" t="s">
+      <c r="A133" s="437" t="s">
         <v>233</v>
       </c>
-      <c r="B133" s="424"/>
+      <c r="B133" s="438"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -23604,10 +23596,10 @@
       <c r="X137" s="240"/>
     </row>
     <row r="138" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="423" t="s">
+      <c r="A138" s="437" t="s">
         <v>234</v>
       </c>
-      <c r="B138" s="424"/>
+      <c r="B138" s="438"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -23817,10 +23809,10 @@
       <c r="X142" s="240"/>
     </row>
     <row r="143" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="423" t="s">
+      <c r="A143" s="437" t="s">
         <v>238</v>
       </c>
-      <c r="B143" s="424"/>
+      <c r="B143" s="438"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -23913,10 +23905,10 @@
       <c r="X144" s="240"/>
     </row>
     <row r="145" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="433" t="s">
+      <c r="A145" s="447" t="s">
         <v>240</v>
       </c>
-      <c r="B145" s="434"/>
+      <c r="B145" s="448"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -23989,10 +23981,10 @@
       <c r="X146" s="240"/>
     </row>
     <row r="147" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="433" t="s">
+      <c r="A147" s="447" t="s">
         <v>241</v>
       </c>
-      <c r="B147" s="434"/>
+      <c r="B147" s="448"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -24090,10 +24082,10 @@
       <c r="X148" s="240"/>
     </row>
     <row r="149" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="433" t="s">
+      <c r="A149" s="447" t="s">
         <v>242</v>
       </c>
-      <c r="B149" s="434"/>
+      <c r="B149" s="448"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -24215,12 +24207,12 @@
       <c r="X151" s="240"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="443" t="s">
+      <c r="A152" s="457" t="s">
         <v>243</v>
       </c>
-      <c r="B152" s="444"/>
-      <c r="C152" s="444"/>
-      <c r="D152" s="445"/>
+      <c r="B152" s="458"/>
+      <c r="C152" s="458"/>
+      <c r="D152" s="459"/>
       <c r="E152" s="311">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -24895,7 +24887,6 @@
   <dimension ref="A1:BZ83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24958,69 +24949,69 @@
       <c r="BZ1" s="186"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="446" t="s">
+      <c r="A2" s="460" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="466"/>
-      <c r="C2" s="467"/>
-      <c r="D2" s="469" t="s">
+      <c r="B2" s="480"/>
+      <c r="C2" s="481"/>
+      <c r="D2" s="483" t="s">
         <v>352</v>
       </c>
-      <c r="E2" s="470"/>
-      <c r="F2" s="470"/>
-      <c r="G2" s="470"/>
-      <c r="H2" s="470"/>
-      <c r="I2" s="470"/>
-      <c r="J2" s="470"/>
-      <c r="K2" s="470"/>
-      <c r="L2" s="470"/>
-      <c r="M2" s="470"/>
-      <c r="N2" s="470"/>
-      <c r="O2" s="470"/>
-      <c r="P2" s="470"/>
-      <c r="Q2" s="470"/>
-      <c r="R2" s="470"/>
-      <c r="S2" s="470"/>
-      <c r="T2" s="470"/>
+      <c r="E2" s="484"/>
+      <c r="F2" s="484"/>
+      <c r="G2" s="484"/>
+      <c r="H2" s="484"/>
+      <c r="I2" s="484"/>
+      <c r="J2" s="484"/>
+      <c r="K2" s="484"/>
+      <c r="L2" s="484"/>
+      <c r="M2" s="484"/>
+      <c r="N2" s="484"/>
+      <c r="O2" s="484"/>
+      <c r="P2" s="484"/>
+      <c r="Q2" s="484"/>
+      <c r="R2" s="484"/>
+      <c r="S2" s="484"/>
+      <c r="T2" s="484"/>
       <c r="AA2" s="131"/>
       <c r="BY2" s="186"/>
       <c r="BZ2" s="186"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="448" t="s">
+      <c r="A3" s="462" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="466"/>
-      <c r="C3" s="467"/>
+      <c r="B3" s="480"/>
+      <c r="C3" s="481"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="471" t="s">
+      <c r="F3" s="485" t="s">
         <v>353</v>
       </c>
-      <c r="G3" s="472"/>
-      <c r="H3" s="473" t="s">
+      <c r="G3" s="486"/>
+      <c r="H3" s="487" t="s">
         <v>354</v>
       </c>
-      <c r="I3" s="473"/>
-      <c r="J3" s="474"/>
-      <c r="K3" s="475" t="s">
+      <c r="I3" s="487"/>
+      <c r="J3" s="488"/>
+      <c r="K3" s="489" t="s">
         <v>355</v>
       </c>
-      <c r="L3" s="476"/>
-      <c r="M3" s="477"/>
-      <c r="N3" s="474" t="s">
+      <c r="L3" s="490"/>
+      <c r="M3" s="491"/>
+      <c r="N3" s="488" t="s">
         <v>356</v>
       </c>
-      <c r="O3" s="478"/>
-      <c r="P3" s="479"/>
-      <c r="Q3" s="480" t="s">
+      <c r="O3" s="492"/>
+      <c r="P3" s="493"/>
+      <c r="Q3" s="494" t="s">
         <v>357</v>
       </c>
-      <c r="R3" s="481"/>
-      <c r="S3" s="482" t="s">
+      <c r="R3" s="495"/>
+      <c r="S3" s="496" t="s">
         <v>358</v>
       </c>
-      <c r="T3" s="483"/>
+      <c r="T3" s="497"/>
       <c r="AA3" s="132"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -25185,7 +25176,7 @@
       <c r="AC6" s="133"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="460" t="str">
+      <c r="C7" s="474" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -25193,81 +25184,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="461"/>
-      <c r="E7" s="462"/>
-      <c r="F7" s="461" t="s">
+      <c r="D7" s="475"/>
+      <c r="E7" s="476"/>
+      <c r="F7" s="475" t="s">
         <v>381</v>
       </c>
-      <c r="G7" s="461"/>
-      <c r="H7" s="462"/>
-      <c r="I7" s="463" t="str">
+      <c r="G7" s="475"/>
+      <c r="H7" s="476"/>
+      <c r="I7" s="477" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$2620.741)</v>
       </c>
-      <c r="J7" s="464"/>
-      <c r="K7" s="464"/>
-      <c r="L7" s="464"/>
-      <c r="M7" s="464"/>
-      <c r="N7" s="464"/>
-      <c r="O7" s="464"/>
-      <c r="P7" s="464"/>
-      <c r="Q7" s="464"/>
-      <c r="R7" s="465"/>
-      <c r="S7" s="460" t="str">
+      <c r="J7" s="478"/>
+      <c r="K7" s="478"/>
+      <c r="L7" s="478"/>
+      <c r="M7" s="478"/>
+      <c r="N7" s="478"/>
+      <c r="O7" s="478"/>
+      <c r="P7" s="478"/>
+      <c r="Q7" s="478"/>
+      <c r="R7" s="479"/>
+      <c r="S7" s="474" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$319.295)</v>
       </c>
-      <c r="T7" s="461"/>
-      <c r="U7" s="461"/>
-      <c r="V7" s="461"/>
-      <c r="W7" s="461"/>
-      <c r="X7" s="462"/>
-      <c r="Y7" s="460" t="s">
+      <c r="T7" s="475"/>
+      <c r="U7" s="475"/>
+      <c r="V7" s="475"/>
+      <c r="W7" s="475"/>
+      <c r="X7" s="476"/>
+      <c r="Y7" s="474" t="s">
         <v>382</v>
       </c>
-      <c r="Z7" s="462"/>
+      <c r="Z7" s="476"/>
       <c r="AA7" s="134"/>
-      <c r="AH7" s="484" t="s">
+      <c r="AH7" s="498" t="s">
         <v>383</v>
       </c>
-      <c r="AI7" s="485"/>
+      <c r="AI7" s="499"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="486" t="s">
+      <c r="AK7" s="500" t="s">
         <v>384</v>
       </c>
-      <c r="AL7" s="422"/>
-      <c r="AM7" s="422"/>
-      <c r="AN7" s="485"/>
-      <c r="AP7" s="487" t="s">
+      <c r="AL7" s="436"/>
+      <c r="AM7" s="436"/>
+      <c r="AN7" s="499"/>
+      <c r="AP7" s="501" t="s">
         <v>385</v>
       </c>
-      <c r="AQ7" s="452"/>
-      <c r="AS7" s="468" t="s">
+      <c r="AQ7" s="466"/>
+      <c r="AS7" s="482" t="s">
         <v>386</v>
       </c>
-      <c r="AT7" s="451"/>
-      <c r="AU7" s="451"/>
-      <c r="AV7" s="451"/>
-      <c r="AW7" s="451"/>
-      <c r="AX7" s="451"/>
-      <c r="AY7" s="451"/>
-      <c r="AZ7" s="451"/>
-      <c r="BA7" s="451"/>
-      <c r="BB7" s="452"/>
-      <c r="BD7" s="487" t="s">
+      <c r="AT7" s="465"/>
+      <c r="AU7" s="465"/>
+      <c r="AV7" s="465"/>
+      <c r="AW7" s="465"/>
+      <c r="AX7" s="465"/>
+      <c r="AY7" s="465"/>
+      <c r="AZ7" s="465"/>
+      <c r="BA7" s="465"/>
+      <c r="BB7" s="466"/>
+      <c r="BD7" s="501" t="s">
         <v>387</v>
       </c>
-      <c r="BE7" s="452"/>
+      <c r="BE7" s="466"/>
       <c r="BF7" s="186"/>
-      <c r="BG7" s="468" t="s">
+      <c r="BG7" s="482" t="s">
         <v>388</v>
       </c>
-      <c r="BH7" s="451"/>
-      <c r="BI7" s="451"/>
+      <c r="BH7" s="465"/>
+      <c r="BI7" s="465"/>
       <c r="BY7" s="186"/>
       <c r="BZ7" s="186"/>
     </row>
@@ -35212,17 +35203,17 @@
       <c r="BZ52" s="186"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="459"/>
-      <c r="D53" s="459"/>
-      <c r="E53" s="459"/>
-      <c r="F53" s="459"/>
-      <c r="G53" s="459"/>
-      <c r="H53" s="459"/>
-      <c r="I53" s="459"/>
-      <c r="J53" s="459"/>
-      <c r="K53" s="459"/>
-      <c r="L53" s="459"/>
-      <c r="M53" s="459"/>
+      <c r="C53" s="473"/>
+      <c r="D53" s="473"/>
+      <c r="E53" s="473"/>
+      <c r="F53" s="473"/>
+      <c r="G53" s="473"/>
+      <c r="H53" s="473"/>
+      <c r="I53" s="473"/>
+      <c r="J53" s="473"/>
+      <c r="K53" s="473"/>
+      <c r="L53" s="473"/>
+      <c r="M53" s="473"/>
       <c r="AC53" s="136" t="s">
         <v>437</v>
       </c>
@@ -35420,7 +35411,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -35475,10 +35465,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="403" t="s">
+      <c r="A3" s="417" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="404"/>
+      <c r="B3" s="418"/>
       <c r="J3" s="230" t="s">
         <v>521</v>
       </c>
@@ -35601,10 +35591,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="403" t="s">
+      <c r="A7" s="417" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="404"/>
+      <c r="B7" s="418"/>
       <c r="C7" s="115" t="s">
         <v>249</v>
       </c>
@@ -35932,10 +35922,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="405" t="s">
+      <c r="A23" s="419" t="s">
         <v>256</v>
       </c>
-      <c r="B23" s="404"/>
+      <c r="B23" s="418"/>
       <c r="C23" t="s">
         <v>257</v>
       </c>
@@ -37138,11 +37128,8 @@
   </sheetPr>
   <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38770,12 +38757,14 @@
         <v>557</v>
       </c>
       <c r="B96" s="341" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C96" s="230">
-        <v>5</v>
-      </c>
-      <c r="D96" s="230"/>
+        <v>1</v>
+      </c>
+      <c r="D96" s="230">
+        <v>2</v>
+      </c>
       <c r="E96" s="230">
         <v>3</v>
       </c>
@@ -38791,15 +38780,23 @@
         <v>560</v>
       </c>
       <c r="B97" s="341" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C97" s="230">
+        <v>1</v>
+      </c>
+      <c r="D97" s="230">
+        <v>2</v>
+      </c>
+      <c r="E97" s="230">
+        <v>3</v>
+      </c>
+      <c r="F97" s="230">
+        <v>4</v>
+      </c>
+      <c r="G97" s="230">
         <v>5</v>
       </c>
-      <c r="D97" s="230"/>
-      <c r="E97" s="230"/>
-      <c r="F97" s="230"/>
-      <c r="G97" s="230"/>
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="331" t="s">
@@ -38823,12 +38820,14 @@
         <v>83</v>
       </c>
       <c r="B99" s="341" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C99" s="230">
-        <v>5</v>
-      </c>
-      <c r="D99" s="230"/>
+        <v>1</v>
+      </c>
+      <c r="D99" s="230">
+        <v>2</v>
+      </c>
       <c r="E99" s="230">
         <v>3</v>
       </c>
@@ -38844,15 +38843,23 @@
         <v>84</v>
       </c>
       <c r="B100" s="341" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C100" s="230">
+        <v>1</v>
+      </c>
+      <c r="D100" s="230">
+        <v>2</v>
+      </c>
+      <c r="E100" s="230">
+        <v>3</v>
+      </c>
+      <c r="F100" s="230">
+        <v>4</v>
+      </c>
+      <c r="G100" s="230">
         <v>5</v>
       </c>
-      <c r="D100" s="230"/>
-      <c r="E100" s="230"/>
-      <c r="F100" s="230"/>
-      <c r="G100" s="230"/>
     </row>
     <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="238" t="s">
@@ -39539,10 +39546,9 @@
   </sheetPr>
   <dimension ref="A1:Z248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -39611,14 +39617,14 @@
         <v>11</v>
       </c>
       <c r="I2" s="361"/>
-      <c r="J2" s="406" t="s">
+      <c r="J2" s="420" t="s">
         <v>504</v>
       </c>
-      <c r="K2" s="407"/>
-      <c r="L2" s="407"/>
-      <c r="M2" s="407"/>
-      <c r="N2" s="407"/>
-      <c r="O2" s="407"/>
+      <c r="K2" s="421"/>
+      <c r="L2" s="421"/>
+      <c r="M2" s="421"/>
+      <c r="N2" s="421"/>
+      <c r="O2" s="421"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="238" t="s">
@@ -39627,31 +39633,31 @@
       <c r="B3" s="370" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="492">
-        <v>0</v>
-      </c>
-      <c r="D3" s="492">
-        <v>0</v>
-      </c>
-      <c r="E3" s="492">
+      <c r="C3" s="407">
+        <v>0</v>
+      </c>
+      <c r="D3" s="407">
+        <v>0</v>
+      </c>
+      <c r="E3" s="407">
         <v>1.2725677550423923E-2</v>
       </c>
-      <c r="F3" s="492">
+      <c r="F3" s="407">
         <v>0.10503743093220913</v>
       </c>
-      <c r="G3" s="492">
+      <c r="G3" s="407">
         <v>0</v>
       </c>
       <c r="H3" s="361" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="361"/>
-      <c r="J3" s="407"/>
-      <c r="K3" s="407"/>
-      <c r="L3" s="407"/>
-      <c r="M3" s="407"/>
-      <c r="N3" s="407"/>
-      <c r="O3" s="407"/>
+      <c r="J3" s="421"/>
+      <c r="K3" s="421"/>
+      <c r="L3" s="421"/>
+      <c r="M3" s="421"/>
+      <c r="N3" s="421"/>
+      <c r="O3" s="421"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="239" t="s">
@@ -39679,12 +39685,12 @@
         <v>11</v>
       </c>
       <c r="I4" s="361"/>
-      <c r="J4" s="407"/>
-      <c r="K4" s="407"/>
-      <c r="L4" s="407"/>
-      <c r="M4" s="407"/>
-      <c r="N4" s="407"/>
-      <c r="O4" s="407"/>
+      <c r="J4" s="421"/>
+      <c r="K4" s="421"/>
+      <c r="L4" s="421"/>
+      <c r="M4" s="421"/>
+      <c r="N4" s="421"/>
+      <c r="O4" s="421"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="402" t="s">
@@ -39798,19 +39804,19 @@
       <c r="B8" s="370" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="492">
-        <v>0</v>
-      </c>
-      <c r="D8" s="492">
-        <v>0</v>
-      </c>
-      <c r="E8" s="492">
+      <c r="C8" s="407">
+        <v>0</v>
+      </c>
+      <c r="D8" s="407">
+        <v>0</v>
+      </c>
+      <c r="E8" s="407">
         <v>5.4270871682504683E-2</v>
       </c>
-      <c r="F8" s="492">
+      <c r="F8" s="407">
         <v>0.16823480336025062</v>
       </c>
-      <c r="G8" s="492">
+      <c r="G8" s="407">
         <v>0</v>
       </c>
       <c r="H8" s="361" t="s">
@@ -39837,7 +39843,7 @@
       <c r="D9" s="239">
         <v>0</v>
       </c>
-      <c r="E9" s="494">
+      <c r="E9" s="409">
         <v>4.0288924558587479E-2</v>
       </c>
       <c r="F9" s="239">
@@ -40067,19 +40073,19 @@
       <c r="B17" s="369" t="s">
         <v>620</v>
       </c>
-      <c r="C17" s="492">
-        <v>0</v>
-      </c>
-      <c r="D17" s="492">
+      <c r="C17" s="407">
+        <v>0</v>
+      </c>
+      <c r="D17" s="407">
         <v>3.6480243166666666E-3</v>
       </c>
-      <c r="E17" s="492">
+      <c r="E17" s="407">
         <v>4.4604244955585862E-2</v>
       </c>
-      <c r="F17" s="492">
+      <c r="F17" s="407">
         <v>0.20342634008944738</v>
       </c>
-      <c r="G17" s="492">
+      <c r="G17" s="407">
         <v>3.9634540783578566E-3</v>
       </c>
       <c r="H17" s="386">
@@ -40094,19 +40100,19 @@
       <c r="B18" s="369" t="s">
         <v>620</v>
       </c>
-      <c r="C18" s="497">
-        <v>0</v>
-      </c>
-      <c r="D18" s="497">
+      <c r="C18" s="412">
+        <v>0</v>
+      </c>
+      <c r="D18" s="412">
         <v>0.52499029068965686</v>
       </c>
-      <c r="E18" s="497">
+      <c r="E18" s="412">
         <v>0.24903484866613099</v>
       </c>
-      <c r="F18" s="497">
+      <c r="F18" s="412">
         <v>0.54357983562975276</v>
       </c>
-      <c r="G18" s="497">
+      <c r="G18" s="412">
         <v>1.409108259904528E-4</v>
       </c>
       <c r="H18" s="386">
@@ -40202,19 +40208,19 @@
       <c r="B22" s="369" t="s">
         <v>620</v>
       </c>
-      <c r="C22" s="494">
-        <v>0</v>
-      </c>
-      <c r="D22" s="494">
-        <v>0</v>
-      </c>
-      <c r="E22" s="494">
+      <c r="C22" s="409">
+        <v>0</v>
+      </c>
+      <c r="D22" s="409">
+        <v>0</v>
+      </c>
+      <c r="E22" s="409">
         <v>6.8719491907401564E-2</v>
       </c>
-      <c r="F22" s="494">
+      <c r="F22" s="409">
         <v>0.13972835910523251</v>
       </c>
-      <c r="G22" s="494">
+      <c r="G22" s="409">
         <v>0</v>
       </c>
       <c r="H22" s="386">
@@ -40256,19 +40262,19 @@
       <c r="B24" s="369" t="s">
         <v>620</v>
       </c>
-      <c r="C24" s="494">
-        <v>0</v>
-      </c>
-      <c r="D24" s="494">
+      <c r="C24" s="409">
+        <v>0</v>
+      </c>
+      <c r="D24" s="409">
         <v>1.8076642335766419E-2</v>
       </c>
       <c r="E24" s="337">
         <v>0.191</v>
       </c>
-      <c r="F24" s="494">
+      <c r="F24" s="409">
         <v>0.29215017674351029</v>
       </c>
-      <c r="G24" s="494">
+      <c r="G24" s="409">
         <v>0</v>
       </c>
       <c r="H24" s="386">
@@ -40310,19 +40316,19 @@
       <c r="B26" s="92" t="s">
         <v>621</v>
       </c>
-      <c r="C26" s="494">
-        <v>0</v>
-      </c>
-      <c r="D26" s="494">
+      <c r="C26" s="409">
+        <v>0</v>
+      </c>
+      <c r="D26" s="409">
         <v>2.2985845129059119E-2</v>
       </c>
       <c r="E26" s="337">
         <v>0.191</v>
       </c>
-      <c r="F26" s="494">
+      <c r="F26" s="409">
         <v>0.28644316422220162</v>
       </c>
-      <c r="G26" s="494">
+      <c r="G26" s="409">
         <v>0</v>
       </c>
       <c r="H26" s="386">
@@ -40337,19 +40343,19 @@
       <c r="B27" s="92" t="s">
         <v>621</v>
       </c>
-      <c r="C27" s="492">
-        <v>0</v>
-      </c>
-      <c r="D27" s="492">
+      <c r="C27" s="407">
+        <v>0</v>
+      </c>
+      <c r="D27" s="407">
         <v>2.4E-2</v>
       </c>
-      <c r="E27" s="492">
+      <c r="E27" s="407">
         <v>0.1043118553695388</v>
       </c>
-      <c r="F27" s="492">
+      <c r="F27" s="407">
         <v>0.34785054261852177</v>
       </c>
-      <c r="G27" s="492">
+      <c r="G27" s="407">
         <v>5.4073625082268911E-4</v>
       </c>
       <c r="H27" s="386">
@@ -40388,22 +40394,22 @@
       <c r="A29" s="333" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="490" t="s">
+      <c r="B29" s="405" t="s">
         <v>617</v>
       </c>
-      <c r="C29" s="495">
-        <v>0</v>
-      </c>
-      <c r="D29" s="495">
+      <c r="C29" s="410">
+        <v>0</v>
+      </c>
+      <c r="D29" s="410">
         <v>0.47</v>
       </c>
-      <c r="E29" s="495">
+      <c r="E29" s="410">
         <v>0.25</v>
       </c>
-      <c r="F29" s="495">
+      <c r="F29" s="410">
         <v>0.42</v>
       </c>
-      <c r="G29" s="495">
+      <c r="G29" s="410">
         <v>0</v>
       </c>
       <c r="H29" s="386">
@@ -40415,22 +40421,22 @@
       <c r="A30" s="335" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="490" t="s">
+      <c r="B30" s="405" t="s">
         <v>617</v>
       </c>
-      <c r="C30" s="492">
-        <v>0</v>
-      </c>
-      <c r="D30" s="492">
+      <c r="C30" s="407">
+        <v>0</v>
+      </c>
+      <c r="D30" s="407">
         <v>0.64200844190326456</v>
       </c>
-      <c r="E30" s="492">
+      <c r="E30" s="407">
         <v>7.61897584552889E-2</v>
       </c>
-      <c r="F30" s="492">
+      <c r="F30" s="407">
         <v>0.51786417518545891</v>
       </c>
-      <c r="G30" s="492">
+      <c r="G30" s="407">
         <v>1.1484357992070844E-3</v>
       </c>
       <c r="H30" s="389">
@@ -40442,22 +40448,22 @@
       <c r="A31" s="402" t="s">
         <v>564</v>
       </c>
-      <c r="B31" s="490" t="s">
+      <c r="B31" s="405" t="s">
         <v>617</v>
       </c>
-      <c r="C31" s="492">
-        <v>0</v>
-      </c>
-      <c r="D31" s="492">
+      <c r="C31" s="407">
+        <v>0</v>
+      </c>
+      <c r="D31" s="407">
         <v>0.41525828268882248</v>
       </c>
-      <c r="E31" s="492">
+      <c r="E31" s="407">
         <v>0.17229585664434177</v>
       </c>
-      <c r="F31" s="492">
+      <c r="F31" s="407">
         <v>0.55288996427807113</v>
       </c>
-      <c r="G31" s="492">
+      <c r="G31" s="407">
         <v>2.8832038140427256E-3</v>
       </c>
       <c r="H31" s="389">
@@ -40472,19 +40478,19 @@
       <c r="B32" s="92" t="s">
         <v>582</v>
       </c>
-      <c r="C32" s="492">
-        <v>0</v>
-      </c>
-      <c r="D32" s="492">
+      <c r="C32" s="407">
+        <v>0</v>
+      </c>
+      <c r="D32" s="407">
         <v>0.41525828268882248</v>
       </c>
-      <c r="E32" s="492">
+      <c r="E32" s="407">
         <v>0.17229585664434177</v>
       </c>
-      <c r="F32" s="492">
+      <c r="F32" s="407">
         <v>0.55288996427807113</v>
       </c>
-      <c r="G32" s="492">
+      <c r="G32" s="407">
         <v>2.8832038140427256E-3</v>
       </c>
       <c r="H32" s="389">
@@ -40500,19 +40506,19 @@
       <c r="B33" s="92" t="s">
         <v>582</v>
       </c>
-      <c r="C33" s="494">
-        <v>0</v>
-      </c>
-      <c r="D33" s="494">
+      <c r="C33" s="409">
+        <v>0</v>
+      </c>
+      <c r="D33" s="409">
         <v>0.43735933983495873</v>
       </c>
-      <c r="E33" s="494">
+      <c r="E33" s="409">
         <v>0.20997749437359339</v>
       </c>
-      <c r="F33" s="494">
+      <c r="F33" s="409">
         <v>0.63968492123030751</v>
       </c>
-      <c r="G33" s="494">
+      <c r="G33" s="409">
         <v>0</v>
       </c>
       <c r="H33" s="389">
@@ -40553,22 +40559,22 @@
       <c r="A35" s="333" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="491" t="s">
+      <c r="B35" s="406" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="494">
+      <c r="C35" s="409">
         <v>0.1619548872180451</v>
       </c>
-      <c r="D35" s="494">
+      <c r="D35" s="409">
         <v>6.4285714285714293E-2</v>
       </c>
-      <c r="E35" s="494">
-        <v>0</v>
-      </c>
-      <c r="F35" s="494">
+      <c r="E35" s="409">
+        <v>0</v>
+      </c>
+      <c r="F35" s="409">
         <v>6.7593984962406012E-2</v>
       </c>
-      <c r="G35" s="494">
+      <c r="G35" s="409">
         <v>9.0225563909774437E-4</v>
       </c>
       <c r="H35" s="361" t="s">
@@ -40609,22 +40615,22 @@
       <c r="A37" s="335" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="491" t="s">
+      <c r="B37" s="406" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="494">
-        <v>0</v>
-      </c>
-      <c r="D37" s="494">
+      <c r="C37" s="409">
+        <v>0</v>
+      </c>
+      <c r="D37" s="409">
         <v>2.0819112627986351E-2</v>
       </c>
-      <c r="E37" s="494">
-        <v>0</v>
-      </c>
-      <c r="F37" s="494">
+      <c r="E37" s="409">
+        <v>0</v>
+      </c>
+      <c r="F37" s="409">
         <v>5.3014789533560862E-2</v>
       </c>
-      <c r="G37" s="494">
+      <c r="G37" s="409">
         <v>0</v>
       </c>
       <c r="H37" s="361" t="s">
@@ -40747,19 +40753,19 @@
       <c r="B42" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="500">
-        <v>0</v>
-      </c>
-      <c r="D42" s="500">
+      <c r="C42" s="415">
+        <v>0</v>
+      </c>
+      <c r="D42" s="415">
         <v>2.0833333333333342E-3</v>
       </c>
-      <c r="E42" s="500">
-        <v>0</v>
-      </c>
-      <c r="F42" s="500">
+      <c r="E42" s="415">
+        <v>0</v>
+      </c>
+      <c r="F42" s="415">
         <v>3.8890872965260122E-2</v>
       </c>
-      <c r="G42" s="500">
+      <c r="G42" s="415">
         <v>0</v>
       </c>
       <c r="H42" s="361" t="s">
@@ -40855,19 +40861,19 @@
       <c r="B46" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C46" s="494">
+      <c r="C46" s="409">
         <v>2.939815783088038E-2</v>
       </c>
-      <c r="D46" s="494">
+      <c r="D46" s="409">
         <v>2.0833333333333342E-3</v>
       </c>
-      <c r="E46" s="494">
-        <v>0</v>
-      </c>
-      <c r="F46" s="494">
+      <c r="E46" s="409">
+        <v>0</v>
+      </c>
+      <c r="F46" s="409">
         <v>3.0052038200428271E-2</v>
       </c>
-      <c r="G46" s="494">
+      <c r="G46" s="409">
         <v>4.490836985388337E-2</v>
       </c>
       <c r="H46" s="361" t="s">
@@ -40882,19 +40888,19 @@
       <c r="B47" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="492">
-        <v>0</v>
-      </c>
-      <c r="D47" s="492">
-        <v>0</v>
-      </c>
-      <c r="E47" s="492">
-        <v>0</v>
-      </c>
-      <c r="F47" s="492">
+      <c r="C47" s="407">
+        <v>0</v>
+      </c>
+      <c r="D47" s="407">
+        <v>0</v>
+      </c>
+      <c r="E47" s="407">
+        <v>0</v>
+      </c>
+      <c r="F47" s="407">
         <v>2.121320343559643E-2</v>
       </c>
-      <c r="G47" s="492">
+      <c r="G47" s="407">
         <v>0</v>
       </c>
       <c r="H47" s="361" t="s">
@@ -40909,19 +40915,19 @@
       <c r="B48" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="492">
-        <v>0</v>
-      </c>
-      <c r="D48" s="492">
-        <v>0</v>
-      </c>
-      <c r="E48" s="492">
-        <v>0</v>
-      </c>
-      <c r="F48" s="492">
+      <c r="C48" s="407">
+        <v>0</v>
+      </c>
+      <c r="D48" s="407">
+        <v>0</v>
+      </c>
+      <c r="E48" s="407">
+        <v>0</v>
+      </c>
+      <c r="F48" s="407">
         <v>2.121320343559643E-2</v>
       </c>
-      <c r="G48" s="492">
+      <c r="G48" s="407">
         <v>0</v>
       </c>
       <c r="H48" s="361" t="s">
@@ -40963,19 +40969,19 @@
       <c r="B50" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="494">
+      <c r="C50" s="409">
         <v>6.7304979947679047E-2</v>
       </c>
-      <c r="D50" s="494">
+      <c r="D50" s="409">
         <v>2.0833333333333339E-2</v>
       </c>
-      <c r="E50" s="494">
-        <v>0</v>
-      </c>
-      <c r="F50" s="494">
+      <c r="E50" s="409">
+        <v>0</v>
+      </c>
+      <c r="F50" s="409">
         <v>3.7123106012293752E-2</v>
       </c>
-      <c r="G50" s="494">
+      <c r="G50" s="409">
         <v>9.8457156410669558E-2</v>
       </c>
       <c r="H50" s="363" t="s">
@@ -41071,19 +41077,19 @@
       <c r="B54" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="494">
-        <v>0</v>
-      </c>
-      <c r="D54" s="494">
+      <c r="C54" s="409">
+        <v>0</v>
+      </c>
+      <c r="D54" s="409">
         <v>2.102078453719498E-3</v>
       </c>
-      <c r="E54" s="494">
-        <v>0</v>
-      </c>
-      <c r="F54" s="494">
+      <c r="E54" s="409">
+        <v>0</v>
+      </c>
+      <c r="F54" s="409">
         <v>3.8888451393810697E-2</v>
       </c>
-      <c r="G54" s="494">
+      <c r="G54" s="409">
         <v>0</v>
       </c>
       <c r="H54" s="361" t="s">
@@ -41125,19 +41131,19 @@
       <c r="B56" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="494">
-        <v>0</v>
-      </c>
-      <c r="D56" s="494">
+      <c r="C56" s="409">
+        <v>0</v>
+      </c>
+      <c r="D56" s="409">
         <v>2.0972199642334578E-3</v>
       </c>
-      <c r="E56" s="494">
-        <v>0</v>
-      </c>
-      <c r="F56" s="494">
+      <c r="E56" s="409">
+        <v>0</v>
+      </c>
+      <c r="F56" s="409">
         <v>3.8936758250690942E-2</v>
       </c>
-      <c r="G56" s="494">
+      <c r="G56" s="409">
         <v>0</v>
       </c>
       <c r="H56" s="364" t="s">
@@ -41449,19 +41455,19 @@
       <c r="B68" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C68" s="494">
-        <v>0</v>
-      </c>
-      <c r="D68" s="494">
+      <c r="C68" s="409">
+        <v>0</v>
+      </c>
+      <c r="D68" s="409">
         <v>2.091053467443091E-3</v>
       </c>
-      <c r="E68" s="494">
-        <v>0</v>
-      </c>
-      <c r="F68" s="494">
+      <c r="E68" s="409">
+        <v>0</v>
+      </c>
+      <c r="F68" s="409">
         <v>3.8935944944415032E-2</v>
       </c>
-      <c r="G68" s="494">
+      <c r="G68" s="409">
         <v>5.2938062466913714E-4</v>
       </c>
       <c r="H68" s="364" t="s">
@@ -41611,19 +41617,19 @@
       <c r="B74" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C74" s="494">
-        <v>0</v>
-      </c>
-      <c r="D74" s="494">
+      <c r="C74" s="409">
+        <v>0</v>
+      </c>
+      <c r="D74" s="409">
         <v>4.3914680050188204E-3</v>
       </c>
-      <c r="E74" s="494">
+      <c r="E74" s="409">
         <v>4.6800501882057713E-2</v>
       </c>
-      <c r="F74" s="494">
+      <c r="F74" s="409">
         <v>0.16461731493099119</v>
       </c>
-      <c r="G74" s="494">
+      <c r="G74" s="409">
         <v>4.0150564617314928E-3</v>
       </c>
       <c r="H74" s="361" t="s">
@@ -41719,19 +41725,19 @@
       <c r="B78" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="494">
-        <v>0</v>
-      </c>
-      <c r="D78" s="494">
+      <c r="C78" s="409">
+        <v>0</v>
+      </c>
+      <c r="D78" s="409">
         <v>0.4315694527961515</v>
       </c>
-      <c r="E78" s="494">
+      <c r="E78" s="409">
         <v>0.28854479855682502</v>
       </c>
-      <c r="F78" s="494">
+      <c r="F78" s="409">
         <v>0.5662056524353577</v>
       </c>
-      <c r="G78" s="494">
+      <c r="G78" s="409">
         <v>2.886349969933854E-3</v>
       </c>
       <c r="H78" s="364" t="s">
@@ -42097,19 +42103,19 @@
       <c r="B92" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C92" s="494">
-        <v>0</v>
-      </c>
-      <c r="D92" s="494">
+      <c r="C92" s="409">
+        <v>0</v>
+      </c>
+      <c r="D92" s="409">
         <v>2.6742627345844511E-2</v>
       </c>
-      <c r="E92" s="494">
+      <c r="E92" s="409">
         <v>0.14470509383378019</v>
       </c>
-      <c r="F92" s="494">
+      <c r="F92" s="409">
         <v>0.32587131367292232</v>
       </c>
-      <c r="G92" s="494">
+      <c r="G92" s="409">
         <v>0</v>
       </c>
       <c r="H92" s="364" t="s">
@@ -42283,7 +42289,7 @@
       <c r="A99" s="402" t="s">
         <v>110</v>
       </c>
-      <c r="B99" s="501" t="s">
+      <c r="B99" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C99" s="236">
@@ -42310,22 +42316,22 @@
       <c r="A100" s="238" t="s">
         <v>505</v>
       </c>
-      <c r="B100" s="501" t="s">
+      <c r="B100" s="416" t="s">
         <v>612</v>
       </c>
-      <c r="C100" s="492">
-        <v>0</v>
-      </c>
-      <c r="D100" s="492">
+      <c r="C100" s="407">
+        <v>0</v>
+      </c>
+      <c r="D100" s="407">
         <v>0.48728965659847873</v>
       </c>
-      <c r="E100" s="492">
+      <c r="E100" s="407">
         <v>0.33366159871042783</v>
       </c>
-      <c r="F100" s="492">
+      <c r="F100" s="407">
         <v>0.49256453984889137</v>
       </c>
-      <c r="G100" s="492">
+      <c r="G100" s="407">
         <v>7.4933146926309587E-3</v>
       </c>
       <c r="H100" s="386">
@@ -42337,7 +42343,7 @@
       <c r="A101" s="238" t="s">
         <v>570</v>
       </c>
-      <c r="B101" s="501" t="s">
+      <c r="B101" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C101" s="239">
@@ -42364,7 +42370,7 @@
       <c r="A102" s="238" t="s">
         <v>571</v>
       </c>
-      <c r="B102" s="501" t="s">
+      <c r="B102" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C102" s="239">
@@ -42391,7 +42397,7 @@
       <c r="A103" s="333" t="s">
         <v>70</v>
       </c>
-      <c r="B103" s="501" t="s">
+      <c r="B103" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C103" s="239">
@@ -42418,7 +42424,7 @@
       <c r="A104" s="402" t="s">
         <v>568</v>
       </c>
-      <c r="B104" s="501" t="s">
+      <c r="B104" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C104" s="239">
@@ -42445,22 +42451,22 @@
       <c r="A105" s="402" t="s">
         <v>569</v>
       </c>
-      <c r="B105" s="501" t="s">
+      <c r="B105" s="416" t="s">
         <v>612</v>
       </c>
-      <c r="C105" s="494">
-        <v>0</v>
-      </c>
-      <c r="D105" s="494">
+      <c r="C105" s="409">
+        <v>0</v>
+      </c>
+      <c r="D105" s="409">
         <v>0.32497781721384211</v>
       </c>
-      <c r="E105" s="494">
+      <c r="E105" s="409">
         <v>0.26228926353149962</v>
       </c>
-      <c r="F105" s="494">
+      <c r="F105" s="409">
         <v>0.53402839396628221</v>
       </c>
-      <c r="G105" s="494">
+      <c r="G105" s="409">
         <v>0</v>
       </c>
       <c r="H105" s="389">
@@ -42472,7 +42478,7 @@
       <c r="A106" s="238" t="s">
         <v>521</v>
       </c>
-      <c r="B106" s="501" t="s">
+      <c r="B106" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C106" s="239">
@@ -42499,22 +42505,22 @@
       <c r="A107" s="402" t="s">
         <v>74</v>
       </c>
-      <c r="B107" s="501" t="s">
+      <c r="B107" s="416" t="s">
         <v>612</v>
       </c>
-      <c r="C107" s="494">
-        <v>0</v>
-      </c>
-      <c r="D107" s="494">
+      <c r="C107" s="409">
+        <v>0</v>
+      </c>
+      <c r="D107" s="409">
         <v>0.30314807617567041</v>
       </c>
-      <c r="E107" s="494">
+      <c r="E107" s="409">
         <v>0.2201321414691022</v>
       </c>
-      <c r="F107" s="494">
+      <c r="F107" s="409">
         <v>0.56424407306645941</v>
       </c>
-      <c r="G107" s="494">
+      <c r="G107" s="409">
         <v>1.5934706568208311E-3</v>
       </c>
       <c r="H107" s="389">
@@ -42526,7 +42532,7 @@
       <c r="A108" s="333" t="s">
         <v>75</v>
       </c>
-      <c r="B108" s="501" t="s">
+      <c r="B108" s="416" t="s">
         <v>612</v>
       </c>
       <c r="C108" s="236">
@@ -42610,19 +42616,19 @@
       <c r="B111" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C111" s="498">
-        <v>0</v>
-      </c>
-      <c r="D111" s="498">
+      <c r="C111" s="413">
+        <v>0</v>
+      </c>
+      <c r="D111" s="413">
         <v>0.30608533229200491</v>
       </c>
-      <c r="E111" s="498">
+      <c r="E111" s="413">
         <v>0.41117301236614612</v>
       </c>
-      <c r="F111" s="498">
+      <c r="F111" s="413">
         <v>0.54295054684716015</v>
       </c>
-      <c r="G111" s="498">
+      <c r="G111" s="413">
         <v>2.7297156609814698E-3</v>
       </c>
       <c r="H111" s="386">
@@ -42718,19 +42724,19 @@
       <c r="B115" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C115" s="492">
-        <v>0</v>
-      </c>
-      <c r="D115" s="492">
-        <v>0</v>
-      </c>
-      <c r="E115" s="492">
-        <v>0</v>
-      </c>
-      <c r="F115" s="492">
+      <c r="C115" s="407">
+        <v>0</v>
+      </c>
+      <c r="D115" s="407">
+        <v>0</v>
+      </c>
+      <c r="E115" s="407">
+        <v>0</v>
+      </c>
+      <c r="F115" s="407">
         <v>3.3587572106361013E-2</v>
       </c>
-      <c r="G115" s="492">
+      <c r="G115" s="407">
         <v>0</v>
       </c>
       <c r="H115" s="386">
@@ -42742,22 +42748,22 @@
       <c r="A116" s="402" t="s">
         <v>107</v>
       </c>
-      <c r="B116" s="489" t="s">
+      <c r="B116" s="404" t="s">
         <v>39</v>
       </c>
-      <c r="C116" s="494">
-        <v>0</v>
-      </c>
-      <c r="D116" s="494">
+      <c r="C116" s="409">
+        <v>0</v>
+      </c>
+      <c r="D116" s="409">
         <v>4.3718592964824117E-2</v>
       </c>
-      <c r="E116" s="494">
+      <c r="E116" s="409">
         <v>9.0954773869346736E-2</v>
       </c>
-      <c r="F116" s="494">
+      <c r="F116" s="409">
         <v>0.29798994974874371</v>
       </c>
-      <c r="G116" s="494">
+      <c r="G116" s="409">
         <v>0</v>
       </c>
       <c r="H116" s="389">
@@ -42853,19 +42859,19 @@
       <c r="B120" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="C120" s="492">
-        <v>0</v>
-      </c>
-      <c r="D120" s="492">
-        <v>0</v>
-      </c>
-      <c r="E120" s="492">
+      <c r="C120" s="407">
+        <v>0</v>
+      </c>
+      <c r="D120" s="407">
+        <v>0</v>
+      </c>
+      <c r="E120" s="407">
         <v>9.7573944890787745E-2</v>
       </c>
-      <c r="F120" s="492">
+      <c r="F120" s="407">
         <v>0.28224832976536918</v>
       </c>
-      <c r="G120" s="492">
+      <c r="G120" s="407">
         <v>0</v>
       </c>
       <c r="H120" s="386">
@@ -43042,19 +43048,19 @@
       <c r="B127" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C127" s="494">
-        <v>0</v>
-      </c>
-      <c r="D127" s="494">
+      <c r="C127" s="409">
+        <v>0</v>
+      </c>
+      <c r="D127" s="409">
         <v>0.41572819240313041</v>
       </c>
-      <c r="E127" s="494">
+      <c r="E127" s="409">
         <v>0.1913914869249857</v>
       </c>
-      <c r="F127" s="494">
+      <c r="F127" s="409">
         <v>0.53254437869822491</v>
       </c>
-      <c r="G127" s="494">
+      <c r="G127" s="409">
         <v>1.3361328497804931E-4</v>
       </c>
       <c r="H127" s="361" t="s">
@@ -43096,19 +43102,19 @@
       <c r="B129" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C129" s="494">
-        <v>0</v>
-      </c>
-      <c r="D129" s="494">
+      <c r="C129" s="409">
+        <v>0</v>
+      </c>
+      <c r="D129" s="409">
         <v>0.6426647144948755</v>
       </c>
-      <c r="E129" s="494">
+      <c r="E129" s="409">
         <v>0.10120058565153731</v>
       </c>
-      <c r="F129" s="494">
+      <c r="F129" s="409">
         <v>0.72368960468521226</v>
       </c>
-      <c r="G129" s="494">
+      <c r="G129" s="409">
         <v>0</v>
       </c>
       <c r="H129" s="361" t="s">
@@ -43204,19 +43210,19 @@
       <c r="B133" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C133" s="494">
-        <v>0</v>
-      </c>
-      <c r="D133" s="494">
+      <c r="C133" s="409">
+        <v>0</v>
+      </c>
+      <c r="D133" s="409">
         <v>6.1546184738955817E-2</v>
       </c>
-      <c r="E133" s="494">
+      <c r="E133" s="409">
         <v>9.9497991967871499E-2</v>
       </c>
-      <c r="F133" s="494">
+      <c r="F133" s="409">
         <v>0.32545180722891559</v>
       </c>
-      <c r="G133" s="494">
+      <c r="G133" s="409">
         <v>0</v>
       </c>
       <c r="H133" s="364" t="s">
@@ -43258,19 +43264,19 @@
       <c r="B135" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C135" s="494">
-        <v>0</v>
-      </c>
-      <c r="D135" s="494">
+      <c r="C135" s="409">
+        <v>0</v>
+      </c>
+      <c r="D135" s="409">
         <v>0.5521383075523203</v>
       </c>
-      <c r="E135" s="494">
+      <c r="E135" s="409">
         <v>2.1337579617834401E-2</v>
       </c>
-      <c r="F135" s="494">
+      <c r="F135" s="409">
         <v>0.28480436760691541</v>
       </c>
-      <c r="G135" s="494">
+      <c r="G135" s="409">
         <v>0</v>
       </c>
       <c r="H135" s="364" t="s">
@@ -43555,19 +43561,19 @@
       <c r="B146" s="92" t="s">
         <v>613</v>
       </c>
-      <c r="C146" s="498">
-        <v>0</v>
-      </c>
-      <c r="D146" s="498">
+      <c r="C146" s="413">
+        <v>0</v>
+      </c>
+      <c r="D146" s="413">
         <v>0.58798747718506816</v>
       </c>
-      <c r="E146" s="498">
+      <c r="E146" s="413">
         <v>7.3501832031808434E-2</v>
       </c>
-      <c r="F146" s="498">
+      <c r="F146" s="413">
         <v>0.30122057297965832</v>
       </c>
-      <c r="G146" s="498">
+      <c r="G146" s="413">
         <v>0</v>
       </c>
       <c r="H146" s="386">
@@ -43609,19 +43615,19 @@
       <c r="B148" s="92" t="s">
         <v>613</v>
       </c>
-      <c r="C148" s="492">
-        <v>0</v>
-      </c>
-      <c r="D148" s="492">
+      <c r="C148" s="407">
+        <v>0</v>
+      </c>
+      <c r="D148" s="407">
         <v>0.60011947188187509</v>
       </c>
-      <c r="E148" s="492">
+      <c r="E148" s="407">
         <v>0.2199624227256384</v>
       </c>
-      <c r="F148" s="492">
+      <c r="F148" s="407">
         <v>0.5291255036964656</v>
       </c>
-      <c r="G148" s="492">
+      <c r="G148" s="407">
         <v>1.5985626027693395E-2</v>
       </c>
       <c r="H148" s="386">
@@ -43777,7 +43783,7 @@
       <c r="D154" s="236">
         <v>0.21697225607815959</v>
       </c>
-      <c r="E154" s="498">
+      <c r="E154" s="413">
         <v>0.13520166179601231</v>
       </c>
       <c r="F154" s="236">
@@ -43825,19 +43831,19 @@
       <c r="B156" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C156" s="499">
-        <v>0</v>
-      </c>
-      <c r="D156" s="499">
+      <c r="C156" s="414">
+        <v>0</v>
+      </c>
+      <c r="D156" s="414">
         <v>0.3912800206593785</v>
       </c>
-      <c r="E156" s="499">
+      <c r="E156" s="414">
         <v>0.1636136696221055</v>
       </c>
-      <c r="F156" s="499">
+      <c r="F156" s="414">
         <v>0.54432297495050352</v>
       </c>
-      <c r="G156" s="499">
+      <c r="G156" s="414">
         <v>8.6080743737625887E-6</v>
       </c>
       <c r="H156" s="386">
@@ -43879,19 +43885,19 @@
       <c r="B158" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C158" s="494">
-        <v>0</v>
-      </c>
-      <c r="D158" s="494">
-        <v>0</v>
-      </c>
-      <c r="E158" s="494">
+      <c r="C158" s="409">
+        <v>0</v>
+      </c>
+      <c r="D158" s="409">
+        <v>0</v>
+      </c>
+      <c r="E158" s="409">
         <v>2.6041666666666661E-2</v>
       </c>
-      <c r="F158" s="494">
+      <c r="F158" s="409">
         <v>0.16770833333333329</v>
       </c>
-      <c r="G158" s="494">
+      <c r="G158" s="409">
         <v>0</v>
       </c>
       <c r="H158" s="389">
@@ -43906,19 +43912,19 @@
       <c r="B159" s="92" t="s">
         <v>525</v>
       </c>
-      <c r="C159" s="496">
-        <v>0</v>
-      </c>
-      <c r="D159" s="496">
+      <c r="C159" s="411">
+        <v>0</v>
+      </c>
+      <c r="D159" s="411">
         <v>0.3</v>
       </c>
-      <c r="E159" s="496">
+      <c r="E159" s="411">
         <v>0.15</v>
       </c>
-      <c r="F159" s="496">
+      <c r="F159" s="411">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G159" s="496">
+      <c r="G159" s="411">
         <v>0</v>
       </c>
       <c r="H159" s="387">
@@ -43933,19 +43939,19 @@
       <c r="B160" s="92" t="s">
         <v>558</v>
       </c>
-      <c r="C160" s="493">
-        <v>0</v>
-      </c>
-      <c r="D160" s="493">
+      <c r="C160" s="408">
+        <v>0</v>
+      </c>
+      <c r="D160" s="408">
         <v>0.23</v>
       </c>
-      <c r="E160" s="493">
+      <c r="E160" s="408">
         <v>0.12</v>
       </c>
-      <c r="F160" s="493">
+      <c r="F160" s="408">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G160" s="493">
+      <c r="G160" s="408">
         <v>0</v>
       </c>
       <c r="H160" s="386">
@@ -43962,19 +43968,19 @@
       <c r="B161" s="370" t="s">
         <v>526</v>
       </c>
-      <c r="C161" s="495">
-        <v>0</v>
-      </c>
-      <c r="D161" s="495">
+      <c r="C161" s="410">
+        <v>0</v>
+      </c>
+      <c r="D161" s="410">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E161" s="495">
+      <c r="E161" s="410">
         <v>0.18</v>
       </c>
-      <c r="F161" s="495">
+      <c r="F161" s="410">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G161" s="495">
+      <c r="G161" s="410">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H161" s="388">
@@ -44016,19 +44022,19 @@
       <c r="B163" s="370" t="s">
         <v>527</v>
       </c>
-      <c r="C163" s="492">
+      <c r="C163" s="407">
         <v>0.34803254277541351</v>
       </c>
-      <c r="D163" s="492">
+      <c r="D163" s="407">
         <v>0.32266961000735833</v>
       </c>
-      <c r="E163" s="492">
+      <c r="E163" s="407">
         <v>0.14476172684383654</v>
       </c>
-      <c r="F163" s="492">
+      <c r="F163" s="407">
         <v>0.46229302241777243</v>
       </c>
-      <c r="G163" s="492">
+      <c r="G163" s="407">
         <v>0.21279071553663778</v>
       </c>
       <c r="H163" s="388">
@@ -44094,22 +44100,22 @@
       <c r="A166" s="238" t="s">
         <v>562</v>
       </c>
-      <c r="B166" s="488" t="s">
+      <c r="B166" s="403" t="s">
         <v>529</v>
       </c>
-      <c r="C166" s="492">
+      <c r="C166" s="407">
         <v>0.5414832609436544</v>
       </c>
-      <c r="D166" s="492">
+      <c r="D166" s="407">
         <v>0.29768460757290005</v>
       </c>
-      <c r="E166" s="492">
+      <c r="E166" s="407">
         <v>0.20116835482122966</v>
       </c>
-      <c r="F166" s="492">
+      <c r="F166" s="407">
         <v>0.52641603374234747</v>
       </c>
-      <c r="G166" s="492">
+      <c r="G166" s="407">
         <v>0.41477160525693013</v>
       </c>
       <c r="H166" s="388">
@@ -44178,19 +44184,19 @@
       <c r="B169" s="370" t="s">
         <v>531</v>
       </c>
-      <c r="C169" s="492">
+      <c r="C169" s="407">
         <v>0.4142065629142177</v>
       </c>
-      <c r="D169" s="492">
+      <c r="D169" s="407">
         <v>0.47306056403143798</v>
       </c>
-      <c r="E169" s="492">
+      <c r="E169" s="407">
         <v>0.13678842689369236</v>
       </c>
-      <c r="F169" s="492">
+      <c r="F169" s="407">
         <v>0.54310201597607943</v>
       </c>
-      <c r="G169" s="492">
+      <c r="G169" s="407">
         <v>0.24358090387648199</v>
       </c>
       <c r="H169" s="388">
@@ -44205,19 +44211,19 @@
       <c r="B170" s="370" t="s">
         <v>532</v>
       </c>
-      <c r="C170" s="492">
+      <c r="C170" s="407">
         <v>0.3692127724785545</v>
       </c>
-      <c r="D170" s="492">
+      <c r="D170" s="407">
         <v>0.35513111235535644</v>
       </c>
-      <c r="E170" s="492">
+      <c r="E170" s="407">
         <v>0.1405804778980789</v>
       </c>
-      <c r="F170" s="492">
+      <c r="F170" s="407">
         <v>0.29070914370896944</v>
       </c>
-      <c r="G170" s="492">
+      <c r="G170" s="407">
         <v>0.23732078140008395</v>
       </c>
       <c r="H170" s="388">
@@ -44259,19 +44265,19 @@
       <c r="B172" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C172" s="492">
-        <v>0</v>
-      </c>
-      <c r="D172" s="492">
-        <v>0</v>
-      </c>
-      <c r="E172" s="492">
+      <c r="C172" s="407">
+        <v>0</v>
+      </c>
+      <c r="D172" s="407">
+        <v>0</v>
+      </c>
+      <c r="E172" s="407">
         <v>2E-3</v>
       </c>
-      <c r="F172" s="492">
+      <c r="F172" s="407">
         <v>4.7E-2</v>
       </c>
-      <c r="G172" s="492">
+      <c r="G172" s="407">
         <v>0</v>
       </c>
       <c r="H172" s="361" t="s">
@@ -44286,19 +44292,19 @@
       <c r="B173" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C173" s="496">
-        <v>0</v>
-      </c>
-      <c r="D173" s="496">
-        <v>0</v>
-      </c>
-      <c r="E173" s="496">
-        <v>0</v>
-      </c>
-      <c r="F173" s="496">
+      <c r="C173" s="411">
+        <v>0</v>
+      </c>
+      <c r="D173" s="411">
+        <v>0</v>
+      </c>
+      <c r="E173" s="411">
+        <v>0</v>
+      </c>
+      <c r="F173" s="411">
         <v>0.1</v>
       </c>
-      <c r="G173" s="496">
+      <c r="G173" s="411">
         <v>0</v>
       </c>
       <c r="H173" s="361" t="s">
@@ -44313,19 +44319,19 @@
       <c r="B174" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C174" s="492">
-        <v>0</v>
-      </c>
-      <c r="D174" s="492">
-        <v>0</v>
-      </c>
-      <c r="E174" s="492">
-        <v>0</v>
-      </c>
-      <c r="F174" s="492">
+      <c r="C174" s="407">
+        <v>0</v>
+      </c>
+      <c r="D174" s="407">
+        <v>0</v>
+      </c>
+      <c r="E174" s="407">
+        <v>0</v>
+      </c>
+      <c r="F174" s="407">
         <v>2.121320343559643E-2</v>
       </c>
-      <c r="G174" s="492">
+      <c r="G174" s="407">
         <v>0</v>
       </c>
       <c r="H174" s="361" t="s">
@@ -44367,19 +44373,19 @@
       <c r="B176" s="370" t="s">
         <v>47</v>
       </c>
-      <c r="C176" s="492">
-        <v>0</v>
-      </c>
-      <c r="D176" s="492">
-        <v>0</v>
-      </c>
-      <c r="E176" s="492">
+      <c r="C176" s="407">
+        <v>0</v>
+      </c>
+      <c r="D176" s="407">
+        <v>0</v>
+      </c>
+      <c r="E176" s="407">
         <v>5.4270871682504683E-2</v>
       </c>
-      <c r="F176" s="492">
+      <c r="F176" s="407">
         <v>0.16823480336025062</v>
       </c>
-      <c r="G176" s="492">
+      <c r="G176" s="407">
         <v>0</v>
       </c>
       <c r="H176" s="361" t="s">
@@ -44394,19 +44400,19 @@
       <c r="B177" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C177" s="492">
-        <v>0</v>
-      </c>
-      <c r="D177" s="492">
-        <v>0</v>
-      </c>
-      <c r="E177" s="492">
+      <c r="C177" s="407">
+        <v>0</v>
+      </c>
+      <c r="D177" s="407">
+        <v>0</v>
+      </c>
+      <c r="E177" s="407">
         <v>4.0740116165041071E-3</v>
       </c>
-      <c r="F177" s="492">
+      <c r="F177" s="407">
         <v>9.7211110476117912E-2</v>
       </c>
-      <c r="G177" s="492">
+      <c r="G177" s="407">
         <v>0</v>
       </c>
       <c r="H177" s="361" t="s">
@@ -44448,19 +44454,19 @@
       <c r="B179" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C179" s="492">
-        <v>0</v>
-      </c>
-      <c r="D179" s="492">
-        <v>0</v>
-      </c>
-      <c r="E179" s="492">
-        <v>0</v>
-      </c>
-      <c r="F179" s="492">
+      <c r="C179" s="407">
+        <v>0</v>
+      </c>
+      <c r="D179" s="407">
+        <v>0</v>
+      </c>
+      <c r="E179" s="407">
+        <v>0</v>
+      </c>
+      <c r="F179" s="407">
         <v>4.7434164902525687E-2</v>
       </c>
-      <c r="G179" s="492">
+      <c r="G179" s="407">
         <v>0</v>
       </c>
       <c r="H179" s="361" t="s">
@@ -44502,19 +44508,19 @@
       <c r="B181" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="C181" s="494">
+      <c r="C181" s="409">
         <v>0.16350000000000001</v>
       </c>
-      <c r="D181" s="494">
+      <c r="D181" s="409">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="E181" s="494">
+      <c r="E181" s="409">
         <v>2.1749999999999999E-2</v>
       </c>
-      <c r="F181" s="494">
+      <c r="F181" s="409">
         <v>0.23474999999999999</v>
       </c>
-      <c r="G181" s="494">
+      <c r="G181" s="409">
         <v>0.45450000000000002</v>
       </c>
       <c r="H181" s="389">
@@ -46196,7 +46202,6 @@
     <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -46214,18 +46219,18 @@
     </row>
     <row r="2" spans="1:28" s="239" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="342"/>
-      <c r="D2" s="408" t="s">
+      <c r="D2" s="422" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="409"/>
-      <c r="F2" s="409"/>
-      <c r="G2" s="409"/>
-      <c r="H2" s="409"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
       <c r="I2" s="241"/>
-      <c r="S2" s="412" t="s">
+      <c r="S2" s="426" t="s">
         <v>279</v>
       </c>
-      <c r="T2" s="412"/>
+      <c r="T2" s="426"/>
     </row>
     <row r="3" spans="1:28" s="239" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="140" t="s">
@@ -47243,11 +47248,11 @@
       <c r="J26" s="237"/>
       <c r="K26"/>
       <c r="L26"/>
-      <c r="U26" s="410"/>
-      <c r="V26" s="411"/>
-      <c r="W26" s="411"/>
-      <c r="X26" s="411"/>
-      <c r="Y26" s="411"/>
+      <c r="U26" s="424"/>
+      <c r="V26" s="425"/>
+      <c r="W26" s="425"/>
+      <c r="X26" s="425"/>
+      <c r="Y26" s="425"/>
       <c r="Z26" s="391"/>
     </row>
     <row r="27" spans="1:26" s="239" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -48869,7 +48874,6 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -49403,7 +49407,6 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -49608,7 +49611,6 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -49624,7 +49626,6 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -49662,25 +49663,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="417" t="s">
+      <c r="A3" s="431" t="s">
         <v>308</v>
       </c>
-      <c r="B3" s="415" t="s">
+      <c r="B3" s="429" t="s">
         <v>322</v>
       </c>
-      <c r="C3" s="415" t="s">
+      <c r="C3" s="429" t="s">
         <v>323</v>
       </c>
-      <c r="D3" s="415" t="s">
+      <c r="D3" s="429" t="s">
         <v>324</v>
       </c>
-      <c r="E3" s="415" t="s">
+      <c r="E3" s="429" t="s">
         <v>325</v>
       </c>
-      <c r="F3" s="415" t="s">
+      <c r="F3" s="429" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="415" t="s">
+      <c r="G3" s="429" t="s">
         <v>327</v>
       </c>
       <c r="J3" s="108" t="s">
@@ -49693,13 +49694,13 @@
       <c r="O3" s="108"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="418"/>
-      <c r="B4" s="416"/>
-      <c r="C4" s="416"/>
-      <c r="D4" s="416"/>
-      <c r="E4" s="416"/>
-      <c r="F4" s="416"/>
-      <c r="G4" s="416"/>
+      <c r="A4" s="432"/>
+      <c r="B4" s="430"/>
+      <c r="C4" s="430"/>
+      <c r="D4" s="430"/>
+      <c r="E4" s="430"/>
+      <c r="F4" s="430"/>
+      <c r="G4" s="430"/>
       <c r="J4" s="113" t="s">
         <v>15</v>
       </c>
@@ -49971,15 +49972,15 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="421" t="s">
+      <c r="A16" s="435" t="s">
         <v>329</v>
       </c>
-      <c r="B16" s="422"/>
-      <c r="C16" s="422"/>
-      <c r="D16" s="422"/>
-      <c r="E16" s="422"/>
-      <c r="F16" s="422"/>
-      <c r="G16" s="422"/>
+      <c r="B16" s="436"/>
+      <c r="C16" s="436"/>
+      <c r="D16" s="436"/>
+      <c r="E16" s="436"/>
+      <c r="F16" s="436"/>
+      <c r="G16" s="436"/>
       <c r="K16" s="59"/>
       <c r="L16" s="59"/>
       <c r="M16" s="59"/>
@@ -50323,10 +50324,10 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="419" t="s">
+      <c r="A28" s="433" t="s">
         <v>337</v>
       </c>
-      <c r="B28" s="420"/>
+      <c r="B28" s="434"/>
       <c r="C28" s="209">
         <f>SUM(C18:C27)</f>
         <v>1421.9080000000004</v>
@@ -50349,15 +50350,15 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="421" t="s">
+      <c r="A29" s="435" t="s">
         <v>338</v>
       </c>
-      <c r="B29" s="422"/>
-      <c r="C29" s="422"/>
-      <c r="D29" s="422"/>
-      <c r="E29" s="422"/>
-      <c r="F29" s="422"/>
-      <c r="G29" s="422"/>
+      <c r="B29" s="436"/>
+      <c r="C29" s="436"/>
+      <c r="D29" s="436"/>
+      <c r="E29" s="436"/>
+      <c r="F29" s="436"/>
+      <c r="G29" s="436"/>
     </row>
     <row r="30" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="98"/>
@@ -50729,15 +50730,15 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="413" t="s">
+      <c r="A43" s="427" t="s">
         <v>347</v>
       </c>
-      <c r="B43" s="414"/>
-      <c r="C43" s="414"/>
-      <c r="D43" s="414"/>
-      <c r="E43" s="414"/>
-      <c r="F43" s="414"/>
-      <c r="G43" s="414"/>
+      <c r="B43" s="428"/>
+      <c r="C43" s="428"/>
+      <c r="D43" s="428"/>
+      <c r="E43" s="428"/>
+      <c r="F43" s="428"/>
+      <c r="G43" s="428"/>
     </row>
     <row r="44" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="98"/>

</xml_diff>

<commit_message>
step 0 change to T13-1 Addition
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A990EC-0499-FB41-89A0-75FE89852D3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D82B05-82B9-B643-A239-BB3CD93DB8C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42880" yWindow="1740" windowWidth="23640" windowHeight="17540" activeTab="4" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
+    <workbookView xWindow="42880" yWindow="1740" windowWidth="23640" windowHeight="17540" activeTab="3" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="625">
   <si>
     <t>Scenario</t>
   </si>
@@ -2114,6 +2114,9 @@
   </si>
   <si>
     <t>SNPL with Brine and Summer Water DWM</t>
+  </si>
+  <si>
+    <t>Updated for new project, per A. Agahi email 01/04/19</t>
   </si>
 </sst>
 </file>
@@ -3595,7 +3598,7 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="78"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="517">
+  <cellXfs count="519">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4646,7 +4649,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4705,16 +4707,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4735,12 +4798,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4755,82 +4812,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -4893,6 +4874,34 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="3" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="86">
@@ -8152,7 +8161,7 @@
   </sheetPr>
   <dimension ref="A1:CP191"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
@@ -17670,16 +17679,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="475" t="s">
+      <c r="A1" s="451" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="476"/>
+      <c r="B1" s="452"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="477" t="s">
+      <c r="A2" s="453" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="478"/>
+      <c r="B2" s="454"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="X3" s="239" t="s">
@@ -17687,33 +17696,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="482" t="s">
+      <c r="A4" s="461" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="483"/>
+      <c r="B4" s="462"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="486" t="s">
+      <c r="D4" s="465" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="479" t="s">
+      <c r="E4" s="455" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="480"/>
-      <c r="G4" s="480"/>
-      <c r="H4" s="480"/>
-      <c r="I4" s="480"/>
-      <c r="J4" s="480"/>
-      <c r="K4" s="480"/>
-      <c r="L4" s="480"/>
-      <c r="M4" s="480"/>
-      <c r="N4" s="480"/>
-      <c r="O4" s="480"/>
-      <c r="P4" s="480"/>
-      <c r="Q4" s="480"/>
-      <c r="R4" s="480"/>
-      <c r="S4" s="480"/>
-      <c r="T4" s="480"/>
-      <c r="U4" s="481"/>
+      <c r="F4" s="456"/>
+      <c r="G4" s="456"/>
+      <c r="H4" s="456"/>
+      <c r="I4" s="456"/>
+      <c r="J4" s="456"/>
+      <c r="K4" s="456"/>
+      <c r="L4" s="456"/>
+      <c r="M4" s="456"/>
+      <c r="N4" s="456"/>
+      <c r="O4" s="456"/>
+      <c r="P4" s="456"/>
+      <c r="Q4" s="456"/>
+      <c r="R4" s="456"/>
+      <c r="S4" s="456"/>
+      <c r="T4" s="456"/>
+      <c r="U4" s="457"/>
       <c r="Y4" s="239">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -17780,12 +17789,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="484"/>
-      <c r="B5" s="485"/>
+      <c r="A5" s="463"/>
+      <c r="B5" s="464"/>
       <c r="C5" s="68" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="487"/>
+      <c r="D5" s="466"/>
       <c r="E5" s="69">
         <f>'Step Cost Analysis'!E5</f>
         <v>2020</v>
@@ -17923,10 +17932,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="454" t="s">
+      <c r="A6" s="467" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="455"/>
+      <c r="B6" s="468"/>
       <c r="C6" s="160">
         <v>10</v>
       </c>
@@ -18444,12 +18453,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="469" t="s">
+      <c r="A12" s="458" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="470"/>
-      <c r="C12" s="470"/>
-      <c r="D12" s="471"/>
+      <c r="B12" s="459"/>
+      <c r="C12" s="459"/>
+      <c r="D12" s="460"/>
       <c r="E12" s="279">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -18584,12 +18593,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="469" t="s">
+      <c r="A13" s="458" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="470"/>
-      <c r="C13" s="470"/>
-      <c r="D13" s="471"/>
+      <c r="B13" s="459"/>
+      <c r="C13" s="459"/>
+      <c r="D13" s="460"/>
       <c r="E13" s="279"/>
       <c r="F13" s="279"/>
       <c r="G13" s="279"/>
@@ -18682,10 +18691,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="454" t="s">
+      <c r="A14" s="467" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="455"/>
+      <c r="B14" s="468"/>
       <c r="C14" s="162">
         <v>10</v>
       </c>
@@ -19200,12 +19209,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="469" t="s">
+      <c r="A20" s="458" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="470"/>
-      <c r="C20" s="470"/>
-      <c r="D20" s="471"/>
+      <c r="B20" s="459"/>
+      <c r="C20" s="459"/>
+      <c r="D20" s="460"/>
       <c r="E20" s="279">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -19276,12 +19285,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="469" t="s">
+      <c r="A21" s="458" t="s">
         <v>196</v>
       </c>
-      <c r="B21" s="470"/>
-      <c r="C21" s="470"/>
-      <c r="D21" s="471"/>
+      <c r="B21" s="459"/>
+      <c r="C21" s="459"/>
+      <c r="D21" s="460"/>
       <c r="E21" s="279"/>
       <c r="F21" s="279"/>
       <c r="G21" s="279"/>
@@ -19307,10 +19316,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="454" t="s">
+      <c r="A22" s="467" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="455"/>
+      <c r="B22" s="468"/>
       <c r="C22" s="160">
         <v>10</v>
       </c>
@@ -19557,12 +19566,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="469" t="s">
+      <c r="A28" s="458" t="s">
         <v>198</v>
       </c>
-      <c r="B28" s="470"/>
-      <c r="C28" s="470"/>
-      <c r="D28" s="471"/>
+      <c r="B28" s="459"/>
+      <c r="C28" s="459"/>
+      <c r="D28" s="460"/>
       <c r="E28" s="279">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -19633,12 +19642,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="469" t="s">
+      <c r="A29" s="458" t="s">
         <v>199</v>
       </c>
-      <c r="B29" s="470"/>
-      <c r="C29" s="470"/>
-      <c r="D29" s="471"/>
+      <c r="B29" s="459"/>
+      <c r="C29" s="459"/>
+      <c r="D29" s="460"/>
       <c r="E29" s="279"/>
       <c r="F29" s="279"/>
       <c r="G29" s="279"/>
@@ -19664,10 +19673,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="454" t="s">
+      <c r="A30" s="467" t="s">
         <v>200</v>
       </c>
-      <c r="B30" s="455"/>
+      <c r="B30" s="468"/>
       <c r="C30" s="160">
         <v>10</v>
       </c>
@@ -19914,12 +19923,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="469" t="s">
+      <c r="A36" s="458" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="470"/>
-      <c r="C36" s="470"/>
-      <c r="D36" s="471"/>
+      <c r="B36" s="459"/>
+      <c r="C36" s="459"/>
+      <c r="D36" s="460"/>
       <c r="E36" s="279">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -19990,12 +19999,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="469" t="s">
+      <c r="A37" s="458" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="470"/>
-      <c r="C37" s="470"/>
-      <c r="D37" s="471"/>
+      <c r="B37" s="459"/>
+      <c r="C37" s="459"/>
+      <c r="D37" s="460"/>
       <c r="E37" s="279"/>
       <c r="F37" s="279"/>
       <c r="G37" s="279"/>
@@ -20021,10 +20030,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="454" t="s">
+      <c r="A38" s="467" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="455"/>
+      <c r="B38" s="468"/>
       <c r="C38" s="160">
         <v>10</v>
       </c>
@@ -20271,12 +20280,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="469" t="s">
+      <c r="A44" s="458" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="470"/>
-      <c r="C44" s="470"/>
-      <c r="D44" s="471"/>
+      <c r="B44" s="459"/>
+      <c r="C44" s="459"/>
+      <c r="D44" s="460"/>
       <c r="E44" s="279">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -20347,12 +20356,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="469" t="s">
+      <c r="A45" s="458" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="470"/>
-      <c r="C45" s="470"/>
-      <c r="D45" s="471"/>
+      <c r="B45" s="459"/>
+      <c r="C45" s="459"/>
+      <c r="D45" s="460"/>
       <c r="E45" s="279"/>
       <c r="F45" s="279"/>
       <c r="G45" s="279"/>
@@ -20378,11 +20387,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="456" t="s">
+      <c r="A46" s="476" t="s">
         <v>206</v>
       </c>
-      <c r="B46" s="457"/>
-      <c r="C46" s="458"/>
+      <c r="B46" s="477"/>
+      <c r="C46" s="478"/>
       <c r="D46" s="170"/>
       <c r="E46" s="287">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -20455,12 +20464,12 @@
       <c r="V46" s="240"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="464" t="s">
+      <c r="A47" s="482" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="465"/>
-      <c r="C47" s="465"/>
-      <c r="D47" s="466"/>
+      <c r="B47" s="483"/>
+      <c r="C47" s="483"/>
+      <c r="D47" s="484"/>
       <c r="E47" s="288">
         <f>E46</f>
         <v>1500000</v>
@@ -20531,7 +20540,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A48" s="171"/>
       <c r="B48" s="171"/>
-      <c r="C48" s="467" t="s">
+      <c r="C48" s="485" t="s">
         <v>208</v>
       </c>
       <c r="D48" s="172">
@@ -20606,7 +20615,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A49" s="171"/>
-      <c r="C49" s="468"/>
+      <c r="C49" s="486"/>
       <c r="D49" s="242">
         <v>37</v>
       </c>
@@ -20677,7 +20686,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A50" s="171"/>
-      <c r="C50" s="468"/>
+      <c r="C50" s="486"/>
       <c r="D50" s="242">
         <v>30</v>
       </c>
@@ -20748,7 +20757,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A51" s="171"/>
-      <c r="C51" s="468"/>
+      <c r="C51" s="486"/>
       <c r="D51" s="242">
         <v>41</v>
       </c>
@@ -20818,38 +20827,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="459" t="s">
+      <c r="A52" s="479" t="s">
         <v>209</v>
       </c>
-      <c r="B52" s="460"/>
-      <c r="C52" s="460"/>
-      <c r="D52" s="460"/>
-      <c r="E52" s="460"/>
-      <c r="F52" s="460"/>
-      <c r="G52" s="460"/>
-      <c r="H52" s="460"/>
-      <c r="I52" s="460"/>
-      <c r="J52" s="460"/>
-      <c r="K52" s="460"/>
-      <c r="L52" s="460"/>
-      <c r="M52" s="460"/>
-      <c r="N52" s="460"/>
-      <c r="O52" s="460"/>
-      <c r="P52" s="460"/>
-      <c r="Q52" s="460"/>
-      <c r="R52" s="460"/>
-      <c r="S52" s="460"/>
-      <c r="T52" s="460"/>
-      <c r="U52" s="460"/>
-      <c r="V52" s="460"/>
-      <c r="W52" s="461"/>
+      <c r="B52" s="480"/>
+      <c r="C52" s="480"/>
+      <c r="D52" s="480"/>
+      <c r="E52" s="480"/>
+      <c r="F52" s="480"/>
+      <c r="G52" s="480"/>
+      <c r="H52" s="480"/>
+      <c r="I52" s="480"/>
+      <c r="J52" s="480"/>
+      <c r="K52" s="480"/>
+      <c r="L52" s="480"/>
+      <c r="M52" s="480"/>
+      <c r="N52" s="480"/>
+      <c r="O52" s="480"/>
+      <c r="P52" s="480"/>
+      <c r="Q52" s="480"/>
+      <c r="R52" s="480"/>
+      <c r="S52" s="480"/>
+      <c r="T52" s="480"/>
+      <c r="U52" s="480"/>
+      <c r="V52" s="480"/>
+      <c r="W52" s="481"/>
       <c r="X52" s="240"/>
     </row>
     <row r="53" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="462" t="s">
+      <c r="A53" s="471" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="463"/>
+      <c r="B53" s="472"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -21026,10 +21035,10 @@
       <c r="X57" s="240"/>
     </row>
     <row r="58" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="452" t="s">
+      <c r="A58" s="469" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="453"/>
+      <c r="B58" s="470"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -21211,10 +21220,10 @@
       <c r="X62" s="240"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="452" t="s">
+      <c r="A63" s="469" t="s">
         <v>213</v>
       </c>
-      <c r="B63" s="453"/>
+      <c r="B63" s="470"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -21404,10 +21413,10 @@
       <c r="X67" s="240"/>
     </row>
     <row r="68" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="452" t="s">
+      <c r="A68" s="469" t="s">
         <v>214</v>
       </c>
-      <c r="B68" s="453"/>
+      <c r="B68" s="470"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -21585,10 +21594,10 @@
       <c r="X72" s="240"/>
     </row>
     <row r="73" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="452" t="s">
+      <c r="A73" s="469" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="453"/>
+      <c r="B73" s="470"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -21814,10 +21823,10 @@
       <c r="X77" s="240"/>
     </row>
     <row r="78" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="452" t="s">
+      <c r="A78" s="469" t="s">
         <v>217</v>
       </c>
-      <c r="B78" s="453"/>
+      <c r="B78" s="470"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -21989,10 +21998,10 @@
       <c r="X82" s="240"/>
     </row>
     <row r="83" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="452" t="s">
+      <c r="A83" s="469" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="453"/>
+      <c r="B83" s="470"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -22164,10 +22173,10 @@
       <c r="X87" s="240"/>
     </row>
     <row r="88" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="452" t="s">
+      <c r="A88" s="469" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="453"/>
+      <c r="B88" s="470"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -22339,10 +22348,10 @@
       <c r="X92" s="240"/>
     </row>
     <row r="93" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="452" t="s">
+      <c r="A93" s="469" t="s">
         <v>222</v>
       </c>
-      <c r="B93" s="453"/>
+      <c r="B93" s="470"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -22544,10 +22553,10 @@
       <c r="X97" s="240"/>
     </row>
     <row r="98" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="452" t="s">
+      <c r="A98" s="469" t="s">
         <v>224</v>
       </c>
-      <c r="B98" s="453"/>
+      <c r="B98" s="470"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -22739,10 +22748,10 @@
       <c r="X102" s="240"/>
     </row>
     <row r="103" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="452" t="s">
+      <c r="A103" s="469" t="s">
         <v>226</v>
       </c>
-      <c r="B103" s="453"/>
+      <c r="B103" s="470"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -22944,10 +22953,10 @@
       <c r="X107" s="240"/>
     </row>
     <row r="108" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="452" t="s">
+      <c r="A108" s="469" t="s">
         <v>227</v>
       </c>
-      <c r="B108" s="453"/>
+      <c r="B108" s="470"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -23149,10 +23158,10 @@
       <c r="X112" s="240"/>
     </row>
     <row r="113" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="452" t="s">
+      <c r="A113" s="469" t="s">
         <v>228</v>
       </c>
-      <c r="B113" s="453"/>
+      <c r="B113" s="470"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -23314,10 +23323,10 @@
       <c r="X117" s="240"/>
     </row>
     <row r="118" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="452" t="s">
+      <c r="A118" s="469" t="s">
         <v>229</v>
       </c>
-      <c r="B118" s="453"/>
+      <c r="B118" s="470"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -23519,10 +23528,10 @@
       <c r="X122" s="240"/>
     </row>
     <row r="123" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="452" t="s">
+      <c r="A123" s="469" t="s">
         <v>230</v>
       </c>
-      <c r="B123" s="453"/>
+      <c r="B123" s="470"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -23724,10 +23733,10 @@
       <c r="X127" s="240"/>
     </row>
     <row r="128" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="452" t="s">
+      <c r="A128" s="469" t="s">
         <v>231</v>
       </c>
-      <c r="B128" s="453"/>
+      <c r="B128" s="470"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -23929,10 +23938,10 @@
       <c r="X132" s="240"/>
     </row>
     <row r="133" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="452" t="s">
+      <c r="A133" s="469" t="s">
         <v>232</v>
       </c>
-      <c r="B133" s="453"/>
+      <c r="B133" s="470"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -24134,10 +24143,10 @@
       <c r="X137" s="240"/>
     </row>
     <row r="138" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="452" t="s">
+      <c r="A138" s="469" t="s">
         <v>233</v>
       </c>
-      <c r="B138" s="453"/>
+      <c r="B138" s="470"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -24347,10 +24356,10 @@
       <c r="X142" s="240"/>
     </row>
     <row r="143" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="452" t="s">
+      <c r="A143" s="469" t="s">
         <v>237</v>
       </c>
-      <c r="B143" s="453"/>
+      <c r="B143" s="470"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -24443,10 +24452,10 @@
       <c r="X144" s="240"/>
     </row>
     <row r="145" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="462" t="s">
+      <c r="A145" s="471" t="s">
         <v>239</v>
       </c>
-      <c r="B145" s="463"/>
+      <c r="B145" s="472"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -24519,10 +24528,10 @@
       <c r="X146" s="240"/>
     </row>
     <row r="147" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="462" t="s">
+      <c r="A147" s="471" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="463"/>
+      <c r="B147" s="472"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -24620,10 +24629,10 @@
       <c r="X148" s="240"/>
     </row>
     <row r="149" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="462" t="s">
+      <c r="A149" s="471" t="s">
         <v>241</v>
       </c>
-      <c r="B149" s="463"/>
+      <c r="B149" s="472"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -24745,12 +24754,12 @@
       <c r="X151" s="240"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="472" t="s">
+      <c r="A152" s="473" t="s">
         <v>242</v>
       </c>
-      <c r="B152" s="473"/>
-      <c r="C152" s="473"/>
-      <c r="D152" s="474"/>
+      <c r="B152" s="474"/>
+      <c r="C152" s="474"/>
+      <c r="D152" s="475"/>
       <c r="E152" s="311">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -25362,37 +25371,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -25409,6 +25387,37 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -25487,69 +25496,69 @@
       <c r="BZ1" s="186"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="475" t="s">
+      <c r="A2" s="451" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="495"/>
-      <c r="C2" s="496"/>
-      <c r="D2" s="498" t="s">
+      <c r="B2" s="487"/>
+      <c r="C2" s="488"/>
+      <c r="D2" s="490" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="499"/>
-      <c r="F2" s="499"/>
-      <c r="G2" s="499"/>
-      <c r="H2" s="499"/>
-      <c r="I2" s="499"/>
-      <c r="J2" s="499"/>
-      <c r="K2" s="499"/>
-      <c r="L2" s="499"/>
-      <c r="M2" s="499"/>
-      <c r="N2" s="499"/>
-      <c r="O2" s="499"/>
-      <c r="P2" s="499"/>
-      <c r="Q2" s="499"/>
-      <c r="R2" s="499"/>
-      <c r="S2" s="499"/>
-      <c r="T2" s="499"/>
+      <c r="E2" s="491"/>
+      <c r="F2" s="491"/>
+      <c r="G2" s="491"/>
+      <c r="H2" s="491"/>
+      <c r="I2" s="491"/>
+      <c r="J2" s="491"/>
+      <c r="K2" s="491"/>
+      <c r="L2" s="491"/>
+      <c r="M2" s="491"/>
+      <c r="N2" s="491"/>
+      <c r="O2" s="491"/>
+      <c r="P2" s="491"/>
+      <c r="Q2" s="491"/>
+      <c r="R2" s="491"/>
+      <c r="S2" s="491"/>
+      <c r="T2" s="491"/>
       <c r="AA2" s="131"/>
       <c r="BY2" s="186"/>
       <c r="BZ2" s="186"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477" t="s">
+      <c r="A3" s="453" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="495"/>
-      <c r="C3" s="496"/>
+      <c r="B3" s="487"/>
+      <c r="C3" s="488"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="500" t="s">
+      <c r="F3" s="492" t="s">
         <v>352</v>
       </c>
-      <c r="G3" s="501"/>
-      <c r="H3" s="502" t="s">
+      <c r="G3" s="493"/>
+      <c r="H3" s="494" t="s">
         <v>353</v>
       </c>
-      <c r="I3" s="502"/>
-      <c r="J3" s="503"/>
-      <c r="K3" s="504" t="s">
+      <c r="I3" s="494"/>
+      <c r="J3" s="495"/>
+      <c r="K3" s="496" t="s">
         <v>354</v>
       </c>
-      <c r="L3" s="505"/>
-      <c r="M3" s="506"/>
-      <c r="N3" s="503" t="s">
+      <c r="L3" s="497"/>
+      <c r="M3" s="498"/>
+      <c r="N3" s="495" t="s">
         <v>355</v>
       </c>
-      <c r="O3" s="507"/>
-      <c r="P3" s="508"/>
-      <c r="Q3" s="509" t="s">
+      <c r="O3" s="499"/>
+      <c r="P3" s="500"/>
+      <c r="Q3" s="501" t="s">
         <v>356</v>
       </c>
-      <c r="R3" s="510"/>
-      <c r="S3" s="511" t="s">
+      <c r="R3" s="502"/>
+      <c r="S3" s="503" t="s">
         <v>357</v>
       </c>
-      <c r="T3" s="512"/>
+      <c r="T3" s="504"/>
       <c r="AA3" s="132"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -25714,7 +25723,7 @@
       <c r="AC6" s="133"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="489" t="str">
+      <c r="C7" s="509" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -25722,81 +25731,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="490"/>
-      <c r="E7" s="491"/>
-      <c r="F7" s="490" t="s">
+      <c r="D7" s="512"/>
+      <c r="E7" s="510"/>
+      <c r="F7" s="512" t="s">
         <v>380</v>
       </c>
-      <c r="G7" s="490"/>
-      <c r="H7" s="491"/>
-      <c r="I7" s="492" t="str">
+      <c r="G7" s="512"/>
+      <c r="H7" s="510"/>
+      <c r="I7" s="513" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$2620.741)</v>
       </c>
-      <c r="J7" s="493"/>
-      <c r="K7" s="493"/>
-      <c r="L7" s="493"/>
-      <c r="M7" s="493"/>
-      <c r="N7" s="493"/>
-      <c r="O7" s="493"/>
-      <c r="P7" s="493"/>
-      <c r="Q7" s="493"/>
-      <c r="R7" s="494"/>
-      <c r="S7" s="489" t="str">
+      <c r="J7" s="514"/>
+      <c r="K7" s="514"/>
+      <c r="L7" s="514"/>
+      <c r="M7" s="514"/>
+      <c r="N7" s="514"/>
+      <c r="O7" s="514"/>
+      <c r="P7" s="514"/>
+      <c r="Q7" s="514"/>
+      <c r="R7" s="515"/>
+      <c r="S7" s="509" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$319.295)</v>
       </c>
-      <c r="T7" s="490"/>
-      <c r="U7" s="490"/>
-      <c r="V7" s="490"/>
-      <c r="W7" s="490"/>
-      <c r="X7" s="491"/>
-      <c r="Y7" s="489" t="s">
+      <c r="T7" s="512"/>
+      <c r="U7" s="512"/>
+      <c r="V7" s="512"/>
+      <c r="W7" s="512"/>
+      <c r="X7" s="510"/>
+      <c r="Y7" s="509" t="s">
         <v>381</v>
       </c>
-      <c r="Z7" s="491"/>
+      <c r="Z7" s="510"/>
       <c r="AA7" s="134"/>
-      <c r="AH7" s="513" t="s">
+      <c r="AH7" s="505" t="s">
         <v>382</v>
       </c>
-      <c r="AI7" s="514"/>
+      <c r="AI7" s="506"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="515" t="s">
+      <c r="AK7" s="507" t="s">
         <v>383</v>
       </c>
-      <c r="AL7" s="451"/>
-      <c r="AM7" s="451"/>
-      <c r="AN7" s="514"/>
-      <c r="AP7" s="516" t="s">
+      <c r="AL7" s="450"/>
+      <c r="AM7" s="450"/>
+      <c r="AN7" s="506"/>
+      <c r="AP7" s="508" t="s">
         <v>384</v>
       </c>
-      <c r="AQ7" s="481"/>
-      <c r="AS7" s="497" t="s">
+      <c r="AQ7" s="457"/>
+      <c r="AS7" s="489" t="s">
         <v>385</v>
       </c>
-      <c r="AT7" s="480"/>
-      <c r="AU7" s="480"/>
-      <c r="AV7" s="480"/>
-      <c r="AW7" s="480"/>
-      <c r="AX7" s="480"/>
-      <c r="AY7" s="480"/>
-      <c r="AZ7" s="480"/>
-      <c r="BA7" s="480"/>
-      <c r="BB7" s="481"/>
-      <c r="BD7" s="516" t="s">
+      <c r="AT7" s="456"/>
+      <c r="AU7" s="456"/>
+      <c r="AV7" s="456"/>
+      <c r="AW7" s="456"/>
+      <c r="AX7" s="456"/>
+      <c r="AY7" s="456"/>
+      <c r="AZ7" s="456"/>
+      <c r="BA7" s="456"/>
+      <c r="BB7" s="457"/>
+      <c r="BD7" s="508" t="s">
         <v>386</v>
       </c>
-      <c r="BE7" s="481"/>
+      <c r="BE7" s="457"/>
       <c r="BF7" s="186"/>
-      <c r="BG7" s="497" t="s">
+      <c r="BG7" s="489" t="s">
         <v>387</v>
       </c>
-      <c r="BH7" s="480"/>
-      <c r="BI7" s="480"/>
+      <c r="BH7" s="456"/>
+      <c r="BI7" s="456"/>
       <c r="BY7" s="186"/>
       <c r="BZ7" s="186"/>
     </row>
@@ -35741,17 +35750,17 @@
       <c r="BZ52" s="186"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="488"/>
-      <c r="D53" s="488"/>
-      <c r="E53" s="488"/>
-      <c r="F53" s="488"/>
-      <c r="G53" s="488"/>
-      <c r="H53" s="488"/>
-      <c r="I53" s="488"/>
-      <c r="J53" s="488"/>
-      <c r="K53" s="488"/>
-      <c r="L53" s="488"/>
-      <c r="M53" s="488"/>
+      <c r="C53" s="511"/>
+      <c r="D53" s="511"/>
+      <c r="E53" s="511"/>
+      <c r="F53" s="511"/>
+      <c r="G53" s="511"/>
+      <c r="H53" s="511"/>
+      <c r="I53" s="511"/>
+      <c r="J53" s="511"/>
+      <c r="K53" s="511"/>
+      <c r="L53" s="511"/>
+      <c r="M53" s="511"/>
       <c r="AC53" s="136" t="s">
         <v>436</v>
       </c>
@@ -35890,6 +35899,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -35906,11 +35920,6 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -36003,10 +36012,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="432" t="s">
+      <c r="A3" s="431" t="s">
         <v>243</v>
       </c>
-      <c r="B3" s="433"/>
+      <c r="B3" s="432"/>
       <c r="J3" s="230" t="s">
         <v>520</v>
       </c>
@@ -36129,10 +36138,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="432" t="s">
+      <c r="A7" s="431" t="s">
         <v>247</v>
       </c>
-      <c r="B7" s="433"/>
+      <c r="B7" s="432"/>
       <c r="C7" s="115" t="s">
         <v>248</v>
       </c>
@@ -36460,10 +36469,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="434" t="s">
+      <c r="A23" s="433" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="433"/>
+      <c r="B23" s="432"/>
       <c r="C23" t="s">
         <v>256</v>
       </c>
@@ -37666,8 +37675,8 @@
   </sheetPr>
   <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37893,33 +37902,31 @@
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="230" t="s">
-        <v>516</v>
+        <v>47</v>
       </c>
       <c r="B16" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C16" s="230" t="s">
-        <v>470</v>
-      </c>
-      <c r="D16" s="431"/>
+        <v>535</v>
+      </c>
+      <c r="D16" s="230"/>
       <c r="E16" s="230"/>
       <c r="F16" s="230"/>
       <c r="G16" s="230"/>
       <c r="H16" s="230"/>
       <c r="I16" s="230"/>
       <c r="J16" s="230"/>
-      <c r="L16" s="330"/>
-      <c r="M16" s="331"/>
     </row>
     <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="230" t="s">
-        <v>47</v>
+        <v>517</v>
       </c>
       <c r="B17" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C17" s="230" t="s">
-        <v>535</v>
+        <v>42</v>
       </c>
       <c r="D17" s="230"/>
       <c r="E17" s="230"/>
@@ -37931,15 +37938,15 @@
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="230" t="s">
-        <v>517</v>
+        <v>49</v>
       </c>
       <c r="B18" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C18" s="230" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="230"/>
+        <v>536</v>
+      </c>
+      <c r="D18" s="430"/>
       <c r="E18" s="230"/>
       <c r="F18" s="230"/>
       <c r="G18" s="230"/>
@@ -37949,13 +37956,13 @@
     </row>
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="230" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C19" s="230" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D19" s="430"/>
       <c r="E19" s="230"/>
@@ -37964,40 +37971,40 @@
       <c r="H19" s="230"/>
       <c r="I19" s="230"/>
       <c r="J19" s="230"/>
+      <c r="L19" s="330"/>
+      <c r="M19" s="331"/>
+      <c r="AB19" s="238" t="e">
+        <f>'Design HV &amp; WD'!#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="230" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C20" s="230" t="s">
-        <v>537</v>
-      </c>
-      <c r="D20" s="430"/>
+        <v>458</v>
+      </c>
+      <c r="D20" s="230"/>
       <c r="E20" s="230"/>
       <c r="F20" s="230"/>
       <c r="G20" s="230"/>
       <c r="H20" s="230"/>
       <c r="I20" s="230"/>
       <c r="J20" s="230"/>
-      <c r="L20" s="330"/>
-      <c r="M20" s="331"/>
-      <c r="AB20" s="238" t="e">
-        <f>'Design HV &amp; WD'!#REF!</f>
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="230" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C21" s="230" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D21" s="230"/>
       <c r="E21" s="230"/>
@@ -38009,13 +38016,13 @@
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="230" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C22" s="230" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D22" s="230"/>
       <c r="E22" s="230"/>
@@ -38026,14 +38033,14 @@
       <c r="J22" s="230"/>
     </row>
     <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="230" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="230" t="s">
+      <c r="A23" s="339" t="s">
+        <v>505</v>
+      </c>
+      <c r="B23" s="339" t="s">
         <v>444</v>
       </c>
       <c r="C23" s="230" t="s">
-        <v>462</v>
+        <v>538</v>
       </c>
       <c r="D23" s="230"/>
       <c r="E23" s="230"/>
@@ -38045,13 +38052,13 @@
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="339" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B24" s="339" t="s">
         <v>444</v>
       </c>
       <c r="C24" s="230" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D24" s="230"/>
       <c r="E24" s="230"/>
@@ -38060,48 +38067,48 @@
       <c r="H24" s="230"/>
       <c r="I24" s="230"/>
       <c r="J24" s="230"/>
+      <c r="AB24" s="238" t="str">
+        <f>'Design HV &amp; WD'!A12</f>
+        <v>Sand Fences</v>
+      </c>
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="339" t="s">
-        <v>506</v>
-      </c>
-      <c r="B25" s="339" t="s">
+      <c r="A25" s="230" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C25" s="230" t="s">
-        <v>539</v>
-      </c>
-      <c r="D25" s="230"/>
-      <c r="E25" s="230"/>
-      <c r="F25" s="230"/>
+        <v>468</v>
+      </c>
+      <c r="D25" s="230" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="230" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="230" t="s">
+        <v>46</v>
+      </c>
       <c r="G25" s="230"/>
       <c r="H25" s="230"/>
       <c r="I25" s="230"/>
       <c r="J25" s="230"/>
-      <c r="AB25" s="238" t="str">
-        <f>'Design HV &amp; WD'!A12</f>
-        <v>Sand Fences</v>
-      </c>
     </row>
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="230" t="s">
-        <v>56</v>
+        <v>565</v>
       </c>
       <c r="B26" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C26" s="230" t="s">
-        <v>468</v>
-      </c>
-      <c r="D26" s="230" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="230" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="230" t="s">
-        <v>46</v>
-      </c>
+      <c r="D26" s="230"/>
+      <c r="E26" s="230"/>
+      <c r="F26" s="230"/>
       <c r="G26" s="230"/>
       <c r="H26" s="230"/>
       <c r="I26" s="230"/>
@@ -38109,13 +38116,13 @@
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="230" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B27" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C27" s="230" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D27" s="230"/>
       <c r="E27" s="230"/>
@@ -38127,13 +38134,13 @@
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="230" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B28" s="230" t="s">
         <v>444</v>
       </c>
-      <c r="C28" s="230" t="s">
-        <v>46</v>
+      <c r="C28" s="142" t="s">
+        <v>42</v>
       </c>
       <c r="D28" s="230"/>
       <c r="E28" s="230"/>
@@ -38142,16 +38149,22 @@
       <c r="H28" s="230"/>
       <c r="I28" s="230"/>
       <c r="J28" s="230"/>
+      <c r="L28" s="330"/>
+      <c r="M28" s="331"/>
+      <c r="AB28" s="238" t="str">
+        <f>'Design HV &amp; WD'!A22</f>
+        <v>WF and SB</v>
+      </c>
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="230" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B29" s="230" t="s">
         <v>444</v>
       </c>
-      <c r="C29" s="142" t="s">
-        <v>42</v>
+      <c r="C29" s="230" t="s">
+        <v>46</v>
       </c>
       <c r="D29" s="230"/>
       <c r="E29" s="230"/>
@@ -38160,16 +38173,10 @@
       <c r="H29" s="230"/>
       <c r="I29" s="230"/>
       <c r="J29" s="230"/>
-      <c r="L29" s="330"/>
-      <c r="M29" s="331"/>
-      <c r="AB29" s="238" t="str">
-        <f>'Design HV &amp; WD'!A22</f>
-        <v>WF and SB</v>
-      </c>
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="230" t="s">
-        <v>564</v>
+        <v>573</v>
       </c>
       <c r="B30" s="230" t="s">
         <v>444</v>
@@ -38183,43 +38190,45 @@
       <c r="G30" s="230"/>
       <c r="H30" s="230"/>
       <c r="I30" s="230"/>
-      <c r="J30" s="230"/>
+      <c r="J30" s="142"/>
+      <c r="L30" s="330"/>
+      <c r="M30" s="331"/>
+      <c r="AB30" s="238" t="str">
+        <f>'Design HV &amp; WD'!A21</f>
+        <v>WF</v>
+      </c>
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="230" t="s">
-        <v>573</v>
+        <v>64</v>
       </c>
       <c r="B31" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C31" s="230" t="s">
-        <v>46</v>
+        <v>458</v>
       </c>
       <c r="D31" s="230"/>
-      <c r="E31" s="230"/>
+      <c r="E31" s="331"/>
       <c r="F31" s="230"/>
       <c r="G31" s="230"/>
       <c r="H31" s="230"/>
       <c r="I31" s="230"/>
-      <c r="J31" s="142"/>
-      <c r="L31" s="330"/>
-      <c r="M31" s="331"/>
-      <c r="AB31" s="238" t="str">
-        <f>'Design HV &amp; WD'!A21</f>
-        <v>WF</v>
-      </c>
+      <c r="J31" s="230"/>
     </row>
     <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="230" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C32" s="230" t="s">
-        <v>458</v>
-      </c>
-      <c r="D32" s="230"/>
+        <v>46</v>
+      </c>
+      <c r="D32" s="230" t="s">
+        <v>31</v>
+      </c>
       <c r="E32" s="331"/>
       <c r="F32" s="230"/>
       <c r="G32" s="230"/>
@@ -38229,18 +38238,16 @@
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="230" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B33" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C33" s="230" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="230" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="331"/>
+        <v>540</v>
+      </c>
+      <c r="D33" s="230"/>
+      <c r="E33" s="230"/>
       <c r="F33" s="230"/>
       <c r="G33" s="230"/>
       <c r="H33" s="230"/>
@@ -38249,13 +38256,13 @@
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="230" t="s">
-        <v>68</v>
+        <v>507</v>
       </c>
       <c r="B34" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C34" s="230" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D34" s="230"/>
       <c r="E34" s="230"/>
@@ -38267,51 +38274,53 @@
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="230" t="s">
-        <v>507</v>
+        <v>569</v>
       </c>
       <c r="B35" s="230" t="s">
         <v>444</v>
       </c>
-      <c r="C35" s="230" t="s">
-        <v>541</v>
-      </c>
-      <c r="D35" s="230"/>
-      <c r="E35" s="230"/>
-      <c r="F35" s="230"/>
-      <c r="G35" s="230"/>
-      <c r="H35" s="230"/>
-      <c r="I35" s="230"/>
+      <c r="C35" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="142"/>
+      <c r="G35" s="142"/>
+      <c r="H35" s="142"/>
+      <c r="I35" s="142"/>
       <c r="J35" s="230"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="230" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B36" s="230" t="s">
         <v>444</v>
       </c>
-      <c r="C36" s="142" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="142"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="142"/>
-      <c r="H36" s="142"/>
-      <c r="I36" s="142"/>
+      <c r="C36" s="230" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="230"/>
+      <c r="E36" s="230"/>
+      <c r="F36" s="230"/>
+      <c r="G36" s="230"/>
+      <c r="H36" s="230"/>
+      <c r="I36" s="230"/>
       <c r="J36" s="230"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="230" t="s">
-        <v>570</v>
+        <v>69</v>
       </c>
       <c r="B37" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C37" s="230" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="230"/>
+        <v>464</v>
+      </c>
+      <c r="D37" s="230" t="s">
+        <v>542</v>
+      </c>
       <c r="E37" s="230"/>
       <c r="F37" s="230"/>
       <c r="G37" s="230"/>
@@ -38321,33 +38330,37 @@
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="230" t="s">
-        <v>69</v>
+        <v>567</v>
       </c>
       <c r="B38" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C38" s="230" t="s">
-        <v>464</v>
-      </c>
-      <c r="D38" s="230" t="s">
-        <v>542</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D38" s="230"/>
       <c r="E38" s="230"/>
       <c r="F38" s="230"/>
       <c r="G38" s="230"/>
       <c r="H38" s="230"/>
       <c r="I38" s="230"/>
-      <c r="J38" s="230"/>
+      <c r="J38" s="142"/>
+      <c r="L38" s="330"/>
+      <c r="M38" s="331"/>
+      <c r="AB38" s="238" t="str">
+        <f>'Design HV &amp; WD'!A23</f>
+        <v>WF and SB_SW</v>
+      </c>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="230" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B39" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C39" s="230" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D39" s="230"/>
       <c r="E39" s="230"/>
@@ -38355,25 +38368,21 @@
       <c r="G39" s="230"/>
       <c r="H39" s="230"/>
       <c r="I39" s="230"/>
-      <c r="J39" s="142"/>
-      <c r="L39" s="330"/>
-      <c r="M39" s="331"/>
-      <c r="AB39" s="238" t="str">
-        <f>'Design HV &amp; WD'!A23</f>
-        <v>WF and SB_SW</v>
-      </c>
+      <c r="J39" s="230"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="230" t="s">
-        <v>568</v>
+        <v>520</v>
       </c>
       <c r="B40" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C40" s="230" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="230"/>
+        <v>465</v>
+      </c>
+      <c r="D40" s="230" t="s">
+        <v>464</v>
+      </c>
       <c r="E40" s="230"/>
       <c r="F40" s="230"/>
       <c r="G40" s="230"/>
@@ -38383,33 +38392,37 @@
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="230" t="s">
-        <v>520</v>
+        <v>72</v>
       </c>
       <c r="B41" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C41" s="230" t="s">
-        <v>465</v>
-      </c>
-      <c r="D41" s="230" t="s">
-        <v>464</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D41" s="230"/>
       <c r="E41" s="230"/>
       <c r="F41" s="230"/>
       <c r="G41" s="230"/>
       <c r="H41" s="230"/>
       <c r="I41" s="230"/>
       <c r="J41" s="230"/>
+      <c r="L41" s="330"/>
+      <c r="M41" s="331"/>
+      <c r="AB41" s="238" t="str">
+        <f>'Design HV &amp; WD'!A24</f>
+        <v>WF and SB_Br</v>
+      </c>
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="230" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B42" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C42" s="230" t="s">
-        <v>42</v>
+        <v>464</v>
       </c>
       <c r="D42" s="230"/>
       <c r="E42" s="230"/>
@@ -38418,22 +38431,16 @@
       <c r="H42" s="230"/>
       <c r="I42" s="230"/>
       <c r="J42" s="230"/>
-      <c r="L42" s="330"/>
-      <c r="M42" s="331"/>
-      <c r="AB42" s="238" t="str">
-        <f>'Design HV &amp; WD'!A24</f>
-        <v>WF and SB_Br</v>
-      </c>
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="230" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B43" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C43" s="230" t="s">
-        <v>464</v>
+        <v>543</v>
       </c>
       <c r="D43" s="230"/>
       <c r="E43" s="230"/>
@@ -38445,13 +38452,13 @@
     </row>
     <row r="44" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="230" t="s">
-        <v>74</v>
+        <v>508</v>
       </c>
       <c r="B44" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C44" s="230" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D44" s="230"/>
       <c r="E44" s="230"/>
@@ -38460,30 +38467,32 @@
       <c r="H44" s="230"/>
       <c r="I44" s="230"/>
       <c r="J44" s="230"/>
+      <c r="L44" s="330"/>
+      <c r="M44" s="331"/>
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="230" t="s">
-        <v>508</v>
+        <v>76</v>
       </c>
       <c r="B45" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C45" s="230" t="s">
-        <v>544</v>
-      </c>
-      <c r="D45" s="230"/>
+        <v>463</v>
+      </c>
+      <c r="D45" s="230" t="s">
+        <v>462</v>
+      </c>
       <c r="E45" s="230"/>
       <c r="F45" s="230"/>
       <c r="G45" s="230"/>
       <c r="H45" s="230"/>
       <c r="I45" s="230"/>
       <c r="J45" s="230"/>
-      <c r="L45" s="330"/>
-      <c r="M45" s="331"/>
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="230" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B46" s="230" t="s">
         <v>444</v>
@@ -38503,16 +38512,16 @@
     </row>
     <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="230" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B47" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C47" s="230" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D47" s="230" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E47" s="230"/>
       <c r="F47" s="230"/>
@@ -38522,57 +38531,61 @@
       <c r="J47" s="230"/>
     </row>
     <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="230" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="230" t="s">
+      <c r="A48" s="331" t="s">
+        <v>509</v>
+      </c>
+      <c r="B48" s="331" t="s">
         <v>444</v>
       </c>
-      <c r="C48" s="230" t="s">
+      <c r="C48" s="331" t="s">
+        <v>545</v>
+      </c>
+      <c r="D48" s="331" t="s">
         <v>458</v>
       </c>
-      <c r="D48" s="230" t="s">
-        <v>457</v>
-      </c>
-      <c r="E48" s="230"/>
-      <c r="F48" s="230"/>
-      <c r="G48" s="230"/>
+      <c r="E48" s="430"/>
+      <c r="F48" s="331"/>
+      <c r="G48" s="331"/>
       <c r="H48" s="230"/>
       <c r="I48" s="230"/>
       <c r="J48" s="230"/>
     </row>
     <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="331" t="s">
-        <v>509</v>
-      </c>
-      <c r="B49" s="331" t="s">
+      <c r="A49" s="230" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="230" t="s">
         <v>444</v>
       </c>
-      <c r="C49" s="331" t="s">
-        <v>545</v>
-      </c>
-      <c r="D49" s="331" t="s">
+      <c r="C49" s="230" t="s">
         <v>458</v>
       </c>
-      <c r="E49" s="430"/>
-      <c r="F49" s="331"/>
-      <c r="G49" s="331"/>
+      <c r="D49" s="230" t="s">
+        <v>457</v>
+      </c>
+      <c r="E49" s="230"/>
+      <c r="F49" s="230"/>
+      <c r="G49" s="230"/>
       <c r="H49" s="230"/>
       <c r="I49" s="230"/>
       <c r="J49" s="230"/>
+      <c r="AB49" s="238" t="str">
+        <f>'Design HV &amp; WD'!A13</f>
+        <v>Brine</v>
+      </c>
     </row>
     <row r="50" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="230" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C50" s="230" t="s">
+        <v>457</v>
+      </c>
+      <c r="D50" s="230" t="s">
         <v>458</v>
-      </c>
-      <c r="D50" s="230" t="s">
-        <v>457</v>
       </c>
       <c r="E50" s="230"/>
       <c r="F50" s="230"/>
@@ -38581,45 +38594,39 @@
       <c r="I50" s="230"/>
       <c r="J50" s="230"/>
       <c r="AB50" s="238" t="str">
-        <f>'Design HV &amp; WD'!A13</f>
-        <v>Brine</v>
+        <f>'Design HV &amp; WD'!A35</f>
+        <v>SNPL_SW_DWM</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="230" t="s">
-        <v>81</v>
+        <v>510</v>
       </c>
       <c r="B51" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C51" s="230" t="s">
-        <v>457</v>
-      </c>
-      <c r="D51" s="230" t="s">
-        <v>458</v>
-      </c>
-      <c r="E51" s="230"/>
+        <v>547</v>
+      </c>
+      <c r="D51" s="230"/>
+      <c r="E51" s="341"/>
       <c r="F51" s="230"/>
       <c r="G51" s="230"/>
       <c r="H51" s="230"/>
       <c r="I51" s="230"/>
       <c r="J51" s="230"/>
-      <c r="AB51" s="238" t="str">
-        <f>'Design HV &amp; WD'!A35</f>
-        <v>SNPL_SW_DWM</v>
-      </c>
     </row>
     <row r="52" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="230" t="s">
-        <v>510</v>
-      </c>
-      <c r="B52" s="230" t="s">
+      <c r="A52" s="339" t="s">
+        <v>511</v>
+      </c>
+      <c r="B52" s="339" t="s">
         <v>444</v>
       </c>
-      <c r="C52" s="230" t="s">
-        <v>547</v>
-      </c>
-      <c r="D52" s="230"/>
+      <c r="C52" s="339" t="s">
+        <v>548</v>
+      </c>
+      <c r="D52" s="339"/>
       <c r="E52" s="341"/>
       <c r="F52" s="230"/>
       <c r="G52" s="230"/>
@@ -38629,16 +38636,18 @@
     </row>
     <row r="53" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="339" t="s">
-        <v>511</v>
+        <v>88</v>
       </c>
       <c r="B53" s="339" t="s">
         <v>444</v>
       </c>
       <c r="C53" s="339" t="s">
-        <v>548</v>
-      </c>
-      <c r="D53" s="339"/>
-      <c r="E53" s="341"/>
+        <v>458</v>
+      </c>
+      <c r="D53" s="339" t="s">
+        <v>457</v>
+      </c>
+      <c r="E53" s="430"/>
       <c r="F53" s="230"/>
       <c r="G53" s="230"/>
       <c r="H53" s="230"/>
@@ -38646,18 +38655,16 @@
       <c r="J53" s="230"/>
     </row>
     <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="339" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="339" t="s">
+      <c r="A54" s="230" t="s">
+        <v>512</v>
+      </c>
+      <c r="B54" s="230" t="s">
         <v>444</v>
       </c>
-      <c r="C54" s="339" t="s">
-        <v>458</v>
-      </c>
-      <c r="D54" s="339" t="s">
-        <v>457</v>
-      </c>
+      <c r="C54" s="230" t="s">
+        <v>549</v>
+      </c>
+      <c r="D54" s="430"/>
       <c r="E54" s="430"/>
       <c r="F54" s="230"/>
       <c r="G54" s="230"/>
@@ -38667,16 +38674,16 @@
     </row>
     <row r="55" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="230" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="B55" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C55" s="230" t="s">
-        <v>549</v>
-      </c>
-      <c r="D55" s="430"/>
-      <c r="E55" s="430"/>
+        <v>622</v>
+      </c>
+      <c r="D55" s="230"/>
+      <c r="E55" s="230"/>
       <c r="F55" s="230"/>
       <c r="G55" s="230"/>
       <c r="H55" s="230"/>
@@ -38685,15 +38692,17 @@
     </row>
     <row r="56" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="230" t="s">
-        <v>522</v>
+        <v>453</v>
       </c>
       <c r="B56" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C56" s="230" t="s">
-        <v>622</v>
-      </c>
-      <c r="D56" s="230"/>
+        <v>470</v>
+      </c>
+      <c r="D56" s="230" t="s">
+        <v>467</v>
+      </c>
       <c r="E56" s="230"/>
       <c r="F56" s="230"/>
       <c r="G56" s="230"/>
@@ -38703,17 +38712,15 @@
     </row>
     <row r="57" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="230" t="s">
-        <v>453</v>
+        <v>94</v>
       </c>
       <c r="B57" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C57" s="230" t="s">
-        <v>470</v>
-      </c>
-      <c r="D57" s="230" t="s">
-        <v>467</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D57" s="230"/>
       <c r="E57" s="230"/>
       <c r="F57" s="230"/>
       <c r="G57" s="230"/>
@@ -38723,7 +38730,7 @@
     </row>
     <row r="58" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="230" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B58" s="230" t="s">
         <v>444</v>
@@ -38741,13 +38748,13 @@
     </row>
     <row r="59" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="230" t="s">
-        <v>95</v>
+        <v>523</v>
       </c>
       <c r="B59" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C59" s="230" t="s">
-        <v>42</v>
+        <v>621</v>
       </c>
       <c r="D59" s="230"/>
       <c r="E59" s="230"/>
@@ -38759,13 +38766,13 @@
     </row>
     <row r="60" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="230" t="s">
-        <v>523</v>
+        <v>109</v>
       </c>
       <c r="B60" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C60" s="230" t="s">
-        <v>621</v>
+        <v>31</v>
       </c>
       <c r="D60" s="230"/>
       <c r="E60" s="230"/>
@@ -38777,7 +38784,7 @@
     </row>
     <row r="61" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="230" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B61" s="230" t="s">
         <v>444</v>
@@ -38785,7 +38792,7 @@
       <c r="C61" s="230" t="s">
         <v>31</v>
       </c>
-      <c r="D61" s="230"/>
+      <c r="D61" s="92"/>
       <c r="E61" s="230"/>
       <c r="F61" s="230"/>
       <c r="G61" s="230"/>
@@ -38795,35 +38802,37 @@
     </row>
     <row r="62" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="230" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B62" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C62" s="230" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="92"/>
+        <v>457</v>
+      </c>
+      <c r="D62" s="230" t="s">
+        <v>458</v>
+      </c>
       <c r="E62" s="230"/>
       <c r="F62" s="230"/>
       <c r="G62" s="230"/>
       <c r="H62" s="230"/>
       <c r="I62" s="230"/>
       <c r="J62" s="230"/>
+      <c r="L62" s="330"/>
+      <c r="M62" s="331"/>
     </row>
     <row r="63" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="230" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B63" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C63" s="230" t="s">
-        <v>457</v>
-      </c>
-      <c r="D63" s="230" t="s">
-        <v>458</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D63" s="230"/>
       <c r="E63" s="230"/>
       <c r="F63" s="230"/>
       <c r="G63" s="230"/>
@@ -38832,45 +38841,37 @@
       <c r="J63" s="230"/>
       <c r="L63" s="330"/>
       <c r="M63" s="331"/>
+      <c r="AB63" s="238" t="str">
+        <f>'Design HV &amp; WD'!A27</f>
+        <v>SB and SNPL</v>
+      </c>
     </row>
     <row r="64" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="230" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="B64" s="230" t="s">
         <v>444</v>
       </c>
       <c r="C64" s="230" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="230"/>
-      <c r="E64" s="230"/>
+        <v>458</v>
+      </c>
+      <c r="D64" s="230" t="s">
+        <v>463</v>
+      </c>
+      <c r="E64" s="430"/>
       <c r="F64" s="230"/>
       <c r="G64" s="230"/>
       <c r="H64" s="230"/>
       <c r="I64" s="230"/>
       <c r="J64" s="230"/>
-      <c r="L64" s="330"/>
-      <c r="M64" s="331"/>
-      <c r="AB64" s="238" t="str">
-        <f>'Design HV &amp; WD'!A27</f>
-        <v>SB and SNPL</v>
-      </c>
     </row>
     <row r="65" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="230" t="s">
-        <v>170</v>
-      </c>
-      <c r="B65" s="230" t="s">
-        <v>444</v>
-      </c>
-      <c r="C65" s="230" t="s">
-        <v>458</v>
-      </c>
-      <c r="D65" s="230" t="s">
-        <v>463</v>
-      </c>
-      <c r="E65" s="430"/>
+      <c r="A65" s="230"/>
+      <c r="B65" s="230"/>
+      <c r="C65" s="230"/>
+      <c r="D65" s="230"/>
+      <c r="E65" s="230"/>
       <c r="F65" s="230"/>
       <c r="G65" s="230"/>
       <c r="H65" s="230"/>
@@ -38888,15 +38889,17 @@
       <c r="H66" s="230"/>
       <c r="I66" s="230"/>
       <c r="J66" s="230"/>
+      <c r="L66" s="330"/>
+      <c r="M66" s="331"/>
     </row>
     <row r="67" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="230"/>
-      <c r="B67" s="230"/>
+      <c r="A67" s="339"/>
+      <c r="B67" s="339"/>
       <c r="C67" s="230"/>
       <c r="D67" s="230"/>
       <c r="E67" s="230"/>
       <c r="F67" s="230"/>
-      <c r="G67" s="230"/>
+      <c r="G67" s="331"/>
       <c r="H67" s="230"/>
       <c r="I67" s="230"/>
       <c r="J67" s="230"/>
@@ -38904,23 +38907,19 @@
       <c r="M67" s="331"/>
     </row>
     <row r="68" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="339"/>
-      <c r="B68" s="339"/>
-      <c r="C68" s="230"/>
+      <c r="A68" s="331"/>
+      <c r="B68" s="331"/>
+      <c r="C68" s="331"/>
       <c r="D68" s="230"/>
       <c r="E68" s="230"/>
       <c r="F68" s="230"/>
-      <c r="G68" s="331"/>
+      <c r="G68" s="230"/>
       <c r="H68" s="230"/>
       <c r="I68" s="230"/>
       <c r="J68" s="230"/>
-      <c r="L68" s="330"/>
-      <c r="M68" s="331"/>
     </row>
     <row r="69" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="331"/>
-      <c r="B69" s="331"/>
-      <c r="C69" s="331"/>
+      <c r="C69" s="230"/>
       <c r="D69" s="230"/>
       <c r="E69" s="230"/>
       <c r="F69" s="230"/>
@@ -38928,8 +38927,14 @@
       <c r="H69" s="230"/>
       <c r="I69" s="230"/>
       <c r="J69" s="230"/>
+      <c r="AB69" s="238" t="str">
+        <f>'Design HV &amp; WD'!A10</f>
+        <v>Gravel</v>
+      </c>
     </row>
     <row r="70" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="331"/>
+      <c r="B70" s="331"/>
       <c r="C70" s="230"/>
       <c r="D70" s="230"/>
       <c r="E70" s="230"/>
@@ -38938,17 +38943,13 @@
       <c r="H70" s="230"/>
       <c r="I70" s="230"/>
       <c r="J70" s="230"/>
-      <c r="AB70" s="238" t="str">
-        <f>'Design HV &amp; WD'!A10</f>
-        <v>Gravel</v>
-      </c>
     </row>
     <row r="71" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="331"/>
       <c r="B71" s="331"/>
       <c r="C71" s="230"/>
       <c r="D71" s="230"/>
-      <c r="E71" s="230"/>
+      <c r="E71" s="339"/>
       <c r="F71" s="230"/>
       <c r="G71" s="230"/>
       <c r="H71" s="230"/>
@@ -38960,7 +38961,7 @@
       <c r="B72" s="331"/>
       <c r="C72" s="230"/>
       <c r="D72" s="230"/>
-      <c r="E72" s="339"/>
+      <c r="E72" s="230"/>
       <c r="F72" s="230"/>
       <c r="G72" s="230"/>
       <c r="H72" s="230"/>
@@ -38968,8 +38969,8 @@
       <c r="J72" s="230"/>
     </row>
     <row r="73" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="331"/>
-      <c r="B73" s="331"/>
+      <c r="A73" s="230"/>
+      <c r="B73" s="230"/>
       <c r="C73" s="230"/>
       <c r="D73" s="230"/>
       <c r="E73" s="230"/>
@@ -38978,6 +38979,8 @@
       <c r="H73" s="230"/>
       <c r="I73" s="230"/>
       <c r="J73" s="230"/>
+      <c r="L73" s="330"/>
+      <c r="M73" s="331"/>
     </row>
     <row r="74" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="230"/>
@@ -38990,13 +38993,9 @@
       <c r="H74" s="230"/>
       <c r="I74" s="230"/>
       <c r="J74" s="230"/>
-      <c r="L74" s="330"/>
-      <c r="M74" s="331"/>
     </row>
     <row r="75" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="230"/>
-      <c r="B75" s="230"/>
-      <c r="C75" s="230"/>
+      <c r="C75" s="331"/>
       <c r="D75" s="230"/>
       <c r="E75" s="230"/>
       <c r="F75" s="230"/>
@@ -39006,7 +39005,9 @@
       <c r="J75" s="230"/>
     </row>
     <row r="76" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C76" s="331"/>
+      <c r="A76" s="230"/>
+      <c r="B76" s="230"/>
+      <c r="C76" s="230"/>
       <c r="D76" s="230"/>
       <c r="E76" s="230"/>
       <c r="F76" s="230"/>
@@ -39052,62 +39053,62 @@
       <c r="J79" s="230"/>
     </row>
     <row r="80" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="230"/>
-      <c r="B80" s="230"/>
-      <c r="C80" s="230"/>
-      <c r="D80" s="230"/>
+      <c r="A80" s="341"/>
+      <c r="B80" s="341"/>
+      <c r="C80" s="341"/>
+      <c r="D80" s="331"/>
       <c r="E80" s="230"/>
       <c r="F80" s="230"/>
       <c r="G80" s="230"/>
       <c r="H80" s="230"/>
       <c r="I80" s="230"/>
       <c r="J80" s="230"/>
+      <c r="AB80" s="238" t="e">
+        <f>'Design HV &amp; WD'!#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="81" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="341"/>
-      <c r="B81" s="341"/>
-      <c r="C81" s="341"/>
-      <c r="D81" s="331"/>
-      <c r="E81" s="230"/>
-      <c r="F81" s="230"/>
+      <c r="A81" s="230"/>
+      <c r="B81" s="230"/>
+      <c r="C81" s="230"/>
+      <c r="D81" s="230"/>
+      <c r="E81" s="331"/>
+      <c r="F81" s="331"/>
       <c r="G81" s="230"/>
       <c r="H81" s="230"/>
       <c r="I81" s="230"/>
       <c r="J81" s="230"/>
-      <c r="AB81" s="238" t="e">
-        <f>'Design HV &amp; WD'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="230"/>
-      <c r="B82" s="230"/>
-      <c r="C82" s="230"/>
-      <c r="D82" s="230"/>
-      <c r="E82" s="331"/>
-      <c r="F82" s="331"/>
-      <c r="G82" s="230"/>
-      <c r="H82" s="230"/>
-      <c r="I82" s="230"/>
-      <c r="J82" s="230"/>
-      <c r="AB82" s="238" t="str">
+      <c r="AB81" s="238" t="str">
         <f>'Design HV &amp; WD'!A9</f>
         <v>SFLS</v>
       </c>
     </row>
+    <row r="82" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="331"/>
+      <c r="B82" s="331"/>
+      <c r="C82" s="331"/>
+      <c r="D82" s="230"/>
+      <c r="E82" s="230"/>
+      <c r="F82" s="230"/>
+      <c r="G82" s="331"/>
+      <c r="H82" s="331"/>
+      <c r="I82" s="331"/>
+      <c r="J82" s="230"/>
+    </row>
     <row r="83" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="331"/>
-      <c r="B83" s="331"/>
-      <c r="C83" s="331"/>
       <c r="D83" s="230"/>
       <c r="E83" s="230"/>
       <c r="F83" s="230"/>
-      <c r="G83" s="331"/>
-      <c r="H83" s="331"/>
-      <c r="I83" s="331"/>
+      <c r="G83" s="230"/>
+      <c r="H83" s="230"/>
+      <c r="I83" s="230"/>
       <c r="J83" s="230"/>
     </row>
     <row r="84" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="230"/>
+      <c r="B84" s="230"/>
+      <c r="C84" s="230"/>
       <c r="D84" s="230"/>
       <c r="E84" s="230"/>
       <c r="F84" s="230"/>
@@ -39129,10 +39130,6 @@
       <c r="J85" s="230"/>
     </row>
     <row r="86" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="230"/>
-      <c r="B86" s="230"/>
-      <c r="C86" s="230"/>
-      <c r="D86" s="230"/>
       <c r="E86" s="230"/>
       <c r="F86" s="230"/>
       <c r="G86" s="230"/>
@@ -39141,25 +39138,40 @@
       <c r="J86" s="230"/>
     </row>
     <row r="87" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E87" s="230"/>
-      <c r="F87" s="230"/>
-      <c r="G87" s="230"/>
-      <c r="H87" s="230"/>
-      <c r="I87" s="230"/>
-      <c r="J87" s="230"/>
+      <c r="A87" s="155" t="s">
+        <v>550</v>
+      </c>
+      <c r="B87" s="155"/>
+      <c r="C87" s="155" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="88" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="155" t="s">
-        <v>550</v>
-      </c>
-      <c r="B88" s="155"/>
-      <c r="C88" s="155" t="s">
-        <v>445</v>
+      <c r="A88" s="331" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" s="230" t="s">
+        <v>441</v>
+      </c>
+      <c r="C88" s="230">
+        <v>1</v>
+      </c>
+      <c r="D88" s="230">
+        <v>2</v>
+      </c>
+      <c r="E88" s="238">
+        <v>3</v>
+      </c>
+      <c r="F88" s="356">
+        <v>4</v>
+      </c>
+      <c r="G88" s="356">
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="331" t="s">
-        <v>35</v>
+      <c r="A89" s="230" t="s">
+        <v>516</v>
       </c>
       <c r="B89" s="230" t="s">
         <v>441</v>
@@ -39173,10 +39185,10 @@
       <c r="E89" s="238">
         <v>3</v>
       </c>
-      <c r="F89" s="356">
+      <c r="F89" s="516">
         <v>4</v>
       </c>
-      <c r="G89" s="356">
+      <c r="G89" s="516">
         <v>5</v>
       </c>
     </row>
@@ -40010,10 +40022,10 @@
     <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState ref="A89:G115">
-    <sortCondition ref="A89:A115"/>
+  <sortState ref="A88:G115">
+    <sortCondition ref="A88:A115"/>
   </sortState>
-  <conditionalFormatting sqref="A13:J13 F14:J14 A14:D14 A34:J48 H49:J49 A75 A89:B93 C126:G127 C119:G124 D69 A74:D74 E69:J75 C70:D73 E51:J53 E56:J60 D83:D84 D95 C89:D94 E84:J87 A85:D86 E90:G115 A96:D115 E68:F68 A67:D68 E64:J64 E83:F83 A82:D82 E81:F81 A77:D78 E77:F79 C80:E80 B79:D79 E76 D75:D76 E66:E67 B64:D66 A63:E63 A62:G62 E61 A50:D54 F89:G89 A17:J17 A15:C16 E15:J16 F54:J55 A56:D61 A55:C55">
+  <conditionalFormatting sqref="A13:J13 F14:J14 A14:D14 A33:J47 H48:J48 A74 A88:B93 C126:G127 C119:G124 D68 A73:D73 E68:J74 C69:D72 E50:J52 E55:J59 D82:D83 D95 C88:D94 E83:J86 A84:D85 E90:G115 A96:D115 E67:F67 A66:D67 E63:J63 E82:F82 A81:D81 E80:F80 A76:D77 E76:F78 C79:E79 B78:D78 E75 D74:D75 E65:E66 B63:D65 A62:E62 A61:G61 E60 A49:D53 F88:G89 A16:J16 E15:J15 F53:J54 A55:D60 A54:C54 A15:C15 A89:C89">
     <cfRule type="expression" dxfId="46" priority="134">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
@@ -40048,32 +40060,32 @@
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29 J83 I29:J29 C81 A18 D18:J18 A31:A33 I12:J12 H68:J68 A21:B28 C21:J27 A80:B81 A79 F65:J67 A64:A66 F61:J63 A30:J30 A114 E50:J50 A10:J11 D31:J31 F32:J33 C32:D33 F80 F76 G76:J82 A19:C20 E19:J20">
+  <conditionalFormatting sqref="A28 J82 I28:J28 C80 A17 D17:J17 A30:A32 I12:J12 H67:J67 A20:B27 C20:J26 A79:B80 A78 F64:J66 A63:A65 F60:J62 A29:J29 A114 E49:J49 A10:J11 D30:J30 F31:J32 C31:D32 F79 F75 G75:J81 A18:C19 E18:J19">
     <cfRule type="expression" dxfId="39" priority="20">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
+  <conditionalFormatting sqref="B17:C17">
     <cfRule type="expression" dxfId="38" priority="19">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29 D29:H29">
+  <conditionalFormatting sqref="B28 D28:H28">
     <cfRule type="expression" dxfId="37" priority="18">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="36" priority="17">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:C31">
+  <conditionalFormatting sqref="B30:C30">
     <cfRule type="expression" dxfId="35" priority="16">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B33">
+  <conditionalFormatting sqref="B31:B32">
     <cfRule type="expression" dxfId="34" priority="15">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
@@ -40083,13 +40095,8 @@
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B75:C75">
+  <conditionalFormatting sqref="B74:C74">
     <cfRule type="expression" dxfId="32" priority="5">
-      <formula>MOD(ROW(), 2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="31" priority="2">
       <formula>MOD(ROW(), 2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40099,10 +40106,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B119:B129 B82 B10:B11 B13:B48 B77:B80 B74:B75 B103:B115 B50:B68" xr:uid="{8D1D524A-C617-AC40-8D5B-96059B1CB9AC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B119:B129 B81 B10:B11 B76:B79 B73:B74 B103:B115 B49:B67 B89 B13:B15 B16:B47" xr:uid="{8D1D524A-C617-AC40-8D5B-96059B1CB9AC}">
       <formula1>"not, only"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B85:B86 B89:B94" xr:uid="{4EEC21E0-40C6-EA41-881A-9C235CF911B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B84:B85 B88:B94" xr:uid="{4EEC21E0-40C6-EA41-881A-9C235CF911B0}">
       <formula1>"not, only"</formula1>
     </dataValidation>
   </dataValidations>
@@ -40118,8 +40125,8 @@
   </sheetPr>
   <dimension ref="A1:Z263"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40189,14 +40196,14 @@
         <v>11</v>
       </c>
       <c r="I2" s="360"/>
-      <c r="J2" s="435" t="s">
+      <c r="J2" s="434" t="s">
         <v>503</v>
       </c>
-      <c r="K2" s="436"/>
-      <c r="L2" s="436"/>
-      <c r="M2" s="436"/>
-      <c r="N2" s="436"/>
-      <c r="O2" s="436"/>
+      <c r="K2" s="435"/>
+      <c r="L2" s="435"/>
+      <c r="M2" s="435"/>
+      <c r="N2" s="435"/>
+      <c r="O2" s="435"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="412" t="s">
@@ -40224,12 +40231,12 @@
         <v>11</v>
       </c>
       <c r="I3" s="360"/>
-      <c r="J3" s="436"/>
-      <c r="K3" s="436"/>
-      <c r="L3" s="436"/>
-      <c r="M3" s="436"/>
-      <c r="N3" s="436"/>
-      <c r="O3" s="436"/>
+      <c r="J3" s="435"/>
+      <c r="K3" s="435"/>
+      <c r="L3" s="435"/>
+      <c r="M3" s="435"/>
+      <c r="N3" s="435"/>
+      <c r="O3" s="435"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="239" t="s">
@@ -40257,12 +40264,12 @@
         <v>11</v>
       </c>
       <c r="I4" s="360"/>
-      <c r="J4" s="436"/>
-      <c r="K4" s="436"/>
-      <c r="L4" s="436"/>
-      <c r="M4" s="436"/>
-      <c r="N4" s="436"/>
-      <c r="O4" s="436"/>
+      <c r="J4" s="435"/>
+      <c r="K4" s="435"/>
+      <c r="L4" s="435"/>
+      <c r="M4" s="435"/>
+      <c r="N4" s="435"/>
+      <c r="O4" s="435"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="238" t="s">
@@ -40498,8 +40505,10 @@
         <v>11</v>
       </c>
       <c r="I11" s="360"/>
-      <c r="J11" s="413"/>
-      <c r="K11" s="413"/>
+      <c r="J11" s="518"/>
+      <c r="K11" s="413" t="s">
+        <v>624</v>
+      </c>
       <c r="L11" s="413"/>
       <c r="M11" s="413"/>
       <c r="N11" s="413"/>
@@ -40640,7 +40649,7 @@
       </c>
       <c r="I16" s="360"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="412" t="s">
         <v>39</v>
       </c>
@@ -40667,7 +40676,7 @@
       </c>
       <c r="I17" s="360"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="335" t="s">
         <v>40</v>
       </c>
@@ -40694,7 +40703,7 @@
       </c>
       <c r="I18" s="360"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="412" t="s">
         <v>40</v>
       </c>
@@ -40721,7 +40730,7 @@
       </c>
       <c r="I19" s="360"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="335" t="s">
         <v>41</v>
       </c>
@@ -40748,7 +40757,7 @@
       </c>
       <c r="I20" s="360"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="333" t="s">
         <v>43</v>
       </c>
@@ -40775,7 +40784,7 @@
       </c>
       <c r="I21" s="360"/>
     </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="412" t="s">
         <v>45</v>
       </c>
@@ -40802,7 +40811,7 @@
       </c>
       <c r="I22" s="360"/>
     </row>
-    <row r="23" spans="1:9" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="237" t="s">
         <v>45</v>
       </c>
@@ -40829,7 +40838,7 @@
       </c>
       <c r="I23" s="360"/>
     </row>
-    <row r="24" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="237" t="s">
         <v>504</v>
       </c>
@@ -40856,7 +40865,7 @@
       </c>
       <c r="I24" s="360"/>
     </row>
-    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="238" t="s">
         <v>504</v>
       </c>
@@ -40882,35 +40891,39 @@
         <v>4.66</v>
       </c>
       <c r="I25" s="360"/>
-    </row>
-    <row r="26" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="L25" s="356"/>
+      <c r="M25" s="356"/>
+      <c r="N25" s="356"/>
+      <c r="O25" s="356"/>
+    </row>
+    <row r="26" spans="1:15" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="238" t="s">
         <v>516</v>
       </c>
       <c r="B26" s="367" t="s">
         <v>617</v>
       </c>
-      <c r="C26" s="405">
-        <v>0</v>
-      </c>
-      <c r="D26" s="405">
-        <v>3.6480243166666666E-3</v>
-      </c>
-      <c r="E26" s="405">
-        <v>4.4604244955585862E-2</v>
-      </c>
-      <c r="F26" s="405">
-        <v>0.20342634008944738</v>
-      </c>
-      <c r="G26" s="405">
-        <v>3.9634540783578566E-3</v>
+      <c r="C26" s="517">
+        <v>0</v>
+      </c>
+      <c r="D26" s="517">
+        <v>5.742821473158552E-2</v>
+      </c>
+      <c r="E26" s="517">
+        <v>0.32084893882646692</v>
+      </c>
+      <c r="F26" s="517">
+        <v>0.52933832709113615</v>
+      </c>
+      <c r="G26" s="517">
+        <v>3.7453183520599251E-3</v>
       </c>
       <c r="H26" s="384">
         <v>6</v>
       </c>
       <c r="I26" s="360"/>
     </row>
-    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="238" t="s">
         <v>516</v>
       </c>
@@ -40937,7 +40950,7 @@
       </c>
       <c r="I27" s="360"/>
     </row>
-    <row r="28" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28" s="412" t="s">
         <v>47</v>
       </c>
@@ -40964,7 +40977,7 @@
       </c>
       <c r="I28" s="360"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="238" t="s">
         <v>517</v>
       </c>
@@ -40991,7 +41004,7 @@
       </c>
       <c r="I29" s="360"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="333" t="s">
         <v>48</v>
       </c>
@@ -41018,7 +41031,7 @@
       </c>
       <c r="I30" s="360"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="412" t="s">
         <v>48</v>
       </c>
@@ -41045,7 +41058,7 @@
       </c>
       <c r="I31" s="360"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="238" t="s">
         <v>518</v>
       </c>
@@ -47177,7 +47190,7 @@
   </sheetPr>
   <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
@@ -47197,18 +47210,18 @@
     </row>
     <row r="2" spans="1:28" s="239" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="342"/>
-      <c r="D2" s="437" t="s">
+      <c r="D2" s="436" t="s">
         <v>277</v>
       </c>
-      <c r="E2" s="438"/>
-      <c r="F2" s="438"/>
-      <c r="G2" s="438"/>
-      <c r="H2" s="438"/>
+      <c r="E2" s="437"/>
+      <c r="F2" s="437"/>
+      <c r="G2" s="437"/>
+      <c r="H2" s="437"/>
       <c r="I2" s="241"/>
-      <c r="S2" s="441" t="s">
+      <c r="S2" s="440" t="s">
         <v>278</v>
       </c>
-      <c r="T2" s="441"/>
+      <c r="T2" s="440"/>
     </row>
     <row r="3" spans="1:28" s="239" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="140" t="s">
@@ -48226,11 +48239,11 @@
       <c r="J26" s="237"/>
       <c r="K26"/>
       <c r="L26"/>
-      <c r="U26" s="439"/>
-      <c r="V26" s="440"/>
-      <c r="W26" s="440"/>
-      <c r="X26" s="440"/>
-      <c r="Y26" s="440"/>
+      <c r="U26" s="438"/>
+      <c r="V26" s="439"/>
+      <c r="W26" s="439"/>
+      <c r="X26" s="439"/>
+      <c r="Y26" s="439"/>
       <c r="Z26" s="389"/>
     </row>
     <row r="27" spans="1:26" s="239" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -50710,25 +50723,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="446" t="s">
+      <c r="A3" s="445" t="s">
         <v>307</v>
       </c>
-      <c r="B3" s="444" t="s">
+      <c r="B3" s="443" t="s">
         <v>321</v>
       </c>
-      <c r="C3" s="444" t="s">
+      <c r="C3" s="443" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="444" t="s">
+      <c r="D3" s="443" t="s">
         <v>323</v>
       </c>
-      <c r="E3" s="444" t="s">
+      <c r="E3" s="443" t="s">
         <v>324</v>
       </c>
-      <c r="F3" s="444" t="s">
+      <c r="F3" s="443" t="s">
         <v>325</v>
       </c>
-      <c r="G3" s="444" t="s">
+      <c r="G3" s="443" t="s">
         <v>326</v>
       </c>
       <c r="J3" s="108" t="s">
@@ -50741,13 +50754,13 @@
       <c r="O3" s="108"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="447"/>
-      <c r="B4" s="445"/>
-      <c r="C4" s="445"/>
-      <c r="D4" s="445"/>
-      <c r="E4" s="445"/>
-      <c r="F4" s="445"/>
-      <c r="G4" s="445"/>
+      <c r="A4" s="446"/>
+      <c r="B4" s="444"/>
+      <c r="C4" s="444"/>
+      <c r="D4" s="444"/>
+      <c r="E4" s="444"/>
+      <c r="F4" s="444"/>
+      <c r="G4" s="444"/>
       <c r="J4" s="113" t="s">
         <v>15</v>
       </c>
@@ -51019,15 +51032,15 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="450" t="s">
+      <c r="A16" s="449" t="s">
         <v>328</v>
       </c>
-      <c r="B16" s="451"/>
-      <c r="C16" s="451"/>
-      <c r="D16" s="451"/>
-      <c r="E16" s="451"/>
-      <c r="F16" s="451"/>
-      <c r="G16" s="451"/>
+      <c r="B16" s="450"/>
+      <c r="C16" s="450"/>
+      <c r="D16" s="450"/>
+      <c r="E16" s="450"/>
+      <c r="F16" s="450"/>
+      <c r="G16" s="450"/>
       <c r="K16" s="59"/>
       <c r="L16" s="59"/>
       <c r="M16" s="59"/>
@@ -51371,10 +51384,10 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="448" t="s">
+      <c r="A28" s="447" t="s">
         <v>336</v>
       </c>
-      <c r="B28" s="449"/>
+      <c r="B28" s="448"/>
       <c r="C28" s="209">
         <f>SUM(C18:C27)</f>
         <v>1421.9080000000004</v>
@@ -51397,15 +51410,15 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="450" t="s">
+      <c r="A29" s="449" t="s">
         <v>337</v>
       </c>
-      <c r="B29" s="451"/>
-      <c r="C29" s="451"/>
-      <c r="D29" s="451"/>
-      <c r="E29" s="451"/>
-      <c r="F29" s="451"/>
-      <c r="G29" s="451"/>
+      <c r="B29" s="450"/>
+      <c r="C29" s="450"/>
+      <c r="D29" s="450"/>
+      <c r="E29" s="450"/>
+      <c r="F29" s="450"/>
+      <c r="G29" s="450"/>
     </row>
     <row r="30" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="98"/>
@@ -51777,15 +51790,15 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="442" t="s">
+      <c r="A43" s="441" t="s">
         <v>346</v>
       </c>
-      <c r="B43" s="443"/>
-      <c r="C43" s="443"/>
-      <c r="D43" s="443"/>
-      <c r="E43" s="443"/>
-      <c r="F43" s="443"/>
-      <c r="G43" s="443"/>
+      <c r="B43" s="442"/>
+      <c r="C43" s="442"/>
+      <c r="D43" s="442"/>
+      <c r="E43" s="442"/>
+      <c r="F43" s="442"/>
+      <c r="G43" s="442"/>
     </row>
     <row r="44" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="98"/>

</xml_diff>

<commit_message>
checkout create separate optimize file for project-based optimization
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D78085-0474-D347-A8F9-5E07B72B30F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D00EB0-20ED-194E-8038-857FDBB2EBCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="1140" windowWidth="23640" windowHeight="17540" activeTab="1" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
+    <workbookView xWindow="7960" yWindow="1140" windowWidth="23640" windowHeight="17540" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -4711,77 +4711,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4802,6 +4741,12 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4816,6 +4761,82 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -4877,27 +4898,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8158,7 +8158,7 @@
   </sheetPr>
   <dimension ref="A1:CP191"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
@@ -17676,16 +17676,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="453" t="s">
+      <c r="A1" s="476" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="454"/>
+      <c r="B1" s="477"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="455" t="s">
+      <c r="A2" s="478" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="456"/>
+      <c r="B2" s="479"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="X3" s="239" t="s">
@@ -17693,33 +17693,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="463" t="s">
+      <c r="A4" s="483" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="464"/>
+      <c r="B4" s="484"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="467" t="s">
+      <c r="D4" s="487" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="457" t="s">
+      <c r="E4" s="480" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="458"/>
-      <c r="G4" s="458"/>
-      <c r="H4" s="458"/>
-      <c r="I4" s="458"/>
-      <c r="J4" s="458"/>
-      <c r="K4" s="458"/>
-      <c r="L4" s="458"/>
-      <c r="M4" s="458"/>
-      <c r="N4" s="458"/>
-      <c r="O4" s="458"/>
-      <c r="P4" s="458"/>
-      <c r="Q4" s="458"/>
-      <c r="R4" s="458"/>
-      <c r="S4" s="458"/>
-      <c r="T4" s="458"/>
-      <c r="U4" s="459"/>
+      <c r="F4" s="481"/>
+      <c r="G4" s="481"/>
+      <c r="H4" s="481"/>
+      <c r="I4" s="481"/>
+      <c r="J4" s="481"/>
+      <c r="K4" s="481"/>
+      <c r="L4" s="481"/>
+      <c r="M4" s="481"/>
+      <c r="N4" s="481"/>
+      <c r="O4" s="481"/>
+      <c r="P4" s="481"/>
+      <c r="Q4" s="481"/>
+      <c r="R4" s="481"/>
+      <c r="S4" s="481"/>
+      <c r="T4" s="481"/>
+      <c r="U4" s="482"/>
       <c r="Y4" s="239">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -17786,12 +17786,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="465"/>
-      <c r="B5" s="466"/>
+      <c r="A5" s="485"/>
+      <c r="B5" s="486"/>
       <c r="C5" s="68" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="468"/>
+      <c r="D5" s="488"/>
       <c r="E5" s="69">
         <f>'Step Cost Analysis'!E5</f>
         <v>2020</v>
@@ -17929,10 +17929,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="469" t="s">
+      <c r="A6" s="455" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="470"/>
+      <c r="B6" s="456"/>
       <c r="C6" s="160">
         <v>10</v>
       </c>
@@ -18450,12 +18450,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="460" t="s">
+      <c r="A12" s="470" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="461"/>
-      <c r="C12" s="461"/>
-      <c r="D12" s="462"/>
+      <c r="B12" s="471"/>
+      <c r="C12" s="471"/>
+      <c r="D12" s="472"/>
       <c r="E12" s="279">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -18590,12 +18590,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="460" t="s">
+      <c r="A13" s="470" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="461"/>
-      <c r="C13" s="461"/>
-      <c r="D13" s="462"/>
+      <c r="B13" s="471"/>
+      <c r="C13" s="471"/>
+      <c r="D13" s="472"/>
       <c r="E13" s="279"/>
       <c r="F13" s="279"/>
       <c r="G13" s="279"/>
@@ -18688,10 +18688,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="469" t="s">
+      <c r="A14" s="455" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="470"/>
+      <c r="B14" s="456"/>
       <c r="C14" s="162">
         <v>10</v>
       </c>
@@ -19206,12 +19206,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="460" t="s">
+      <c r="A20" s="470" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="461"/>
-      <c r="C20" s="461"/>
-      <c r="D20" s="462"/>
+      <c r="B20" s="471"/>
+      <c r="C20" s="471"/>
+      <c r="D20" s="472"/>
       <c r="E20" s="279">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -19282,12 +19282,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="460" t="s">
+      <c r="A21" s="470" t="s">
         <v>196</v>
       </c>
-      <c r="B21" s="461"/>
-      <c r="C21" s="461"/>
-      <c r="D21" s="462"/>
+      <c r="B21" s="471"/>
+      <c r="C21" s="471"/>
+      <c r="D21" s="472"/>
       <c r="E21" s="279"/>
       <c r="F21" s="279"/>
       <c r="G21" s="279"/>
@@ -19313,10 +19313,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="469" t="s">
+      <c r="A22" s="455" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="470"/>
+      <c r="B22" s="456"/>
       <c r="C22" s="160">
         <v>10</v>
       </c>
@@ -19563,12 +19563,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="460" t="s">
+      <c r="A28" s="470" t="s">
         <v>198</v>
       </c>
-      <c r="B28" s="461"/>
-      <c r="C28" s="461"/>
-      <c r="D28" s="462"/>
+      <c r="B28" s="471"/>
+      <c r="C28" s="471"/>
+      <c r="D28" s="472"/>
       <c r="E28" s="279">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -19639,12 +19639,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="460" t="s">
+      <c r="A29" s="470" t="s">
         <v>199</v>
       </c>
-      <c r="B29" s="461"/>
-      <c r="C29" s="461"/>
-      <c r="D29" s="462"/>
+      <c r="B29" s="471"/>
+      <c r="C29" s="471"/>
+      <c r="D29" s="472"/>
       <c r="E29" s="279"/>
       <c r="F29" s="279"/>
       <c r="G29" s="279"/>
@@ -19670,10 +19670,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="469" t="s">
+      <c r="A30" s="455" t="s">
         <v>200</v>
       </c>
-      <c r="B30" s="470"/>
+      <c r="B30" s="456"/>
       <c r="C30" s="160">
         <v>10</v>
       </c>
@@ -19920,12 +19920,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="460" t="s">
+      <c r="A36" s="470" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="461"/>
-      <c r="C36" s="461"/>
-      <c r="D36" s="462"/>
+      <c r="B36" s="471"/>
+      <c r="C36" s="471"/>
+      <c r="D36" s="472"/>
       <c r="E36" s="279">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -19996,12 +19996,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="460" t="s">
+      <c r="A37" s="470" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="461"/>
-      <c r="C37" s="461"/>
-      <c r="D37" s="462"/>
+      <c r="B37" s="471"/>
+      <c r="C37" s="471"/>
+      <c r="D37" s="472"/>
       <c r="E37" s="279"/>
       <c r="F37" s="279"/>
       <c r="G37" s="279"/>
@@ -20027,10 +20027,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="469" t="s">
+      <c r="A38" s="455" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="470"/>
+      <c r="B38" s="456"/>
       <c r="C38" s="160">
         <v>10</v>
       </c>
@@ -20277,12 +20277,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="460" t="s">
+      <c r="A44" s="470" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="461"/>
-      <c r="C44" s="461"/>
-      <c r="D44" s="462"/>
+      <c r="B44" s="471"/>
+      <c r="C44" s="471"/>
+      <c r="D44" s="472"/>
       <c r="E44" s="279">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -20353,12 +20353,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="460" t="s">
+      <c r="A45" s="470" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="461"/>
-      <c r="C45" s="461"/>
-      <c r="D45" s="462"/>
+      <c r="B45" s="471"/>
+      <c r="C45" s="471"/>
+      <c r="D45" s="472"/>
       <c r="E45" s="279"/>
       <c r="F45" s="279"/>
       <c r="G45" s="279"/>
@@ -20384,11 +20384,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="478" t="s">
+      <c r="A46" s="457" t="s">
         <v>206</v>
       </c>
-      <c r="B46" s="479"/>
-      <c r="C46" s="480"/>
+      <c r="B46" s="458"/>
+      <c r="C46" s="459"/>
       <c r="D46" s="170"/>
       <c r="E46" s="287">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -20461,12 +20461,12 @@
       <c r="V46" s="240"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="484" t="s">
+      <c r="A47" s="465" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="485"/>
-      <c r="C47" s="485"/>
-      <c r="D47" s="486"/>
+      <c r="B47" s="466"/>
+      <c r="C47" s="466"/>
+      <c r="D47" s="467"/>
       <c r="E47" s="288">
         <f>E46</f>
         <v>1500000</v>
@@ -20537,7 +20537,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A48" s="171"/>
       <c r="B48" s="171"/>
-      <c r="C48" s="487" t="s">
+      <c r="C48" s="468" t="s">
         <v>208</v>
       </c>
       <c r="D48" s="172">
@@ -20612,7 +20612,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A49" s="171"/>
-      <c r="C49" s="488"/>
+      <c r="C49" s="469"/>
       <c r="D49" s="242">
         <v>37</v>
       </c>
@@ -20683,7 +20683,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A50" s="171"/>
-      <c r="C50" s="488"/>
+      <c r="C50" s="469"/>
       <c r="D50" s="242">
         <v>30</v>
       </c>
@@ -20754,7 +20754,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A51" s="171"/>
-      <c r="C51" s="488"/>
+      <c r="C51" s="469"/>
       <c r="D51" s="242">
         <v>41</v>
       </c>
@@ -20824,38 +20824,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="481" t="s">
+      <c r="A52" s="460" t="s">
         <v>209</v>
       </c>
-      <c r="B52" s="482"/>
-      <c r="C52" s="482"/>
-      <c r="D52" s="482"/>
-      <c r="E52" s="482"/>
-      <c r="F52" s="482"/>
-      <c r="G52" s="482"/>
-      <c r="H52" s="482"/>
-      <c r="I52" s="482"/>
-      <c r="J52" s="482"/>
-      <c r="K52" s="482"/>
-      <c r="L52" s="482"/>
-      <c r="M52" s="482"/>
-      <c r="N52" s="482"/>
-      <c r="O52" s="482"/>
-      <c r="P52" s="482"/>
-      <c r="Q52" s="482"/>
-      <c r="R52" s="482"/>
-      <c r="S52" s="482"/>
-      <c r="T52" s="482"/>
-      <c r="U52" s="482"/>
-      <c r="V52" s="482"/>
-      <c r="W52" s="483"/>
+      <c r="B52" s="461"/>
+      <c r="C52" s="461"/>
+      <c r="D52" s="461"/>
+      <c r="E52" s="461"/>
+      <c r="F52" s="461"/>
+      <c r="G52" s="461"/>
+      <c r="H52" s="461"/>
+      <c r="I52" s="461"/>
+      <c r="J52" s="461"/>
+      <c r="K52" s="461"/>
+      <c r="L52" s="461"/>
+      <c r="M52" s="461"/>
+      <c r="N52" s="461"/>
+      <c r="O52" s="461"/>
+      <c r="P52" s="461"/>
+      <c r="Q52" s="461"/>
+      <c r="R52" s="461"/>
+      <c r="S52" s="461"/>
+      <c r="T52" s="461"/>
+      <c r="U52" s="461"/>
+      <c r="V52" s="461"/>
+      <c r="W52" s="462"/>
       <c r="X52" s="240"/>
     </row>
     <row r="53" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="473" t="s">
+      <c r="A53" s="463" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="474"/>
+      <c r="B53" s="464"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -21032,10 +21032,10 @@
       <c r="X57" s="240"/>
     </row>
     <row r="58" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="471" t="s">
+      <c r="A58" s="453" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="472"/>
+      <c r="B58" s="454"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -21217,10 +21217,10 @@
       <c r="X62" s="240"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="471" t="s">
+      <c r="A63" s="453" t="s">
         <v>213</v>
       </c>
-      <c r="B63" s="472"/>
+      <c r="B63" s="454"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -21410,10 +21410,10 @@
       <c r="X67" s="240"/>
     </row>
     <row r="68" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="471" t="s">
+      <c r="A68" s="453" t="s">
         <v>214</v>
       </c>
-      <c r="B68" s="472"/>
+      <c r="B68" s="454"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -21591,10 +21591,10 @@
       <c r="X72" s="240"/>
     </row>
     <row r="73" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="471" t="s">
+      <c r="A73" s="453" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="472"/>
+      <c r="B73" s="454"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -21820,10 +21820,10 @@
       <c r="X77" s="240"/>
     </row>
     <row r="78" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="471" t="s">
+      <c r="A78" s="453" t="s">
         <v>217</v>
       </c>
-      <c r="B78" s="472"/>
+      <c r="B78" s="454"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -21995,10 +21995,10 @@
       <c r="X82" s="240"/>
     </row>
     <row r="83" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="471" t="s">
+      <c r="A83" s="453" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="472"/>
+      <c r="B83" s="454"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -22170,10 +22170,10 @@
       <c r="X87" s="240"/>
     </row>
     <row r="88" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="471" t="s">
+      <c r="A88" s="453" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="472"/>
+      <c r="B88" s="454"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -22345,10 +22345,10 @@
       <c r="X92" s="240"/>
     </row>
     <row r="93" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="471" t="s">
+      <c r="A93" s="453" t="s">
         <v>222</v>
       </c>
-      <c r="B93" s="472"/>
+      <c r="B93" s="454"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -22550,10 +22550,10 @@
       <c r="X97" s="240"/>
     </row>
     <row r="98" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="471" t="s">
+      <c r="A98" s="453" t="s">
         <v>224</v>
       </c>
-      <c r="B98" s="472"/>
+      <c r="B98" s="454"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -22745,10 +22745,10 @@
       <c r="X102" s="240"/>
     </row>
     <row r="103" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="471" t="s">
+      <c r="A103" s="453" t="s">
         <v>226</v>
       </c>
-      <c r="B103" s="472"/>
+      <c r="B103" s="454"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -22950,10 +22950,10 @@
       <c r="X107" s="240"/>
     </row>
     <row r="108" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="471" t="s">
+      <c r="A108" s="453" t="s">
         <v>227</v>
       </c>
-      <c r="B108" s="472"/>
+      <c r="B108" s="454"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -23155,10 +23155,10 @@
       <c r="X112" s="240"/>
     </row>
     <row r="113" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="471" t="s">
+      <c r="A113" s="453" t="s">
         <v>228</v>
       </c>
-      <c r="B113" s="472"/>
+      <c r="B113" s="454"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -23320,10 +23320,10 @@
       <c r="X117" s="240"/>
     </row>
     <row r="118" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="471" t="s">
+      <c r="A118" s="453" t="s">
         <v>229</v>
       </c>
-      <c r="B118" s="472"/>
+      <c r="B118" s="454"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -23525,10 +23525,10 @@
       <c r="X122" s="240"/>
     </row>
     <row r="123" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="471" t="s">
+      <c r="A123" s="453" t="s">
         <v>230</v>
       </c>
-      <c r="B123" s="472"/>
+      <c r="B123" s="454"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -23730,10 +23730,10 @@
       <c r="X127" s="240"/>
     </row>
     <row r="128" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="471" t="s">
+      <c r="A128" s="453" t="s">
         <v>231</v>
       </c>
-      <c r="B128" s="472"/>
+      <c r="B128" s="454"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -23935,10 +23935,10 @@
       <c r="X132" s="240"/>
     </row>
     <row r="133" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="471" t="s">
+      <c r="A133" s="453" t="s">
         <v>232</v>
       </c>
-      <c r="B133" s="472"/>
+      <c r="B133" s="454"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -24140,10 +24140,10 @@
       <c r="X137" s="240"/>
     </row>
     <row r="138" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="471" t="s">
+      <c r="A138" s="453" t="s">
         <v>233</v>
       </c>
-      <c r="B138" s="472"/>
+      <c r="B138" s="454"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -24353,10 +24353,10 @@
       <c r="X142" s="240"/>
     </row>
     <row r="143" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="471" t="s">
+      <c r="A143" s="453" t="s">
         <v>237</v>
       </c>
-      <c r="B143" s="472"/>
+      <c r="B143" s="454"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -24449,10 +24449,10 @@
       <c r="X144" s="240"/>
     </row>
     <row r="145" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="473" t="s">
+      <c r="A145" s="463" t="s">
         <v>239</v>
       </c>
-      <c r="B145" s="474"/>
+      <c r="B145" s="464"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -24525,10 +24525,10 @@
       <c r="X146" s="240"/>
     </row>
     <row r="147" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="473" t="s">
+      <c r="A147" s="463" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="474"/>
+      <c r="B147" s="464"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -24626,10 +24626,10 @@
       <c r="X148" s="240"/>
     </row>
     <row r="149" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="473" t="s">
+      <c r="A149" s="463" t="s">
         <v>241</v>
       </c>
-      <c r="B149" s="474"/>
+      <c r="B149" s="464"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -24751,12 +24751,12 @@
       <c r="X151" s="240"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="475" t="s">
+      <c r="A152" s="473" t="s">
         <v>242</v>
       </c>
-      <c r="B152" s="476"/>
-      <c r="C152" s="476"/>
-      <c r="D152" s="477"/>
+      <c r="B152" s="474"/>
+      <c r="C152" s="474"/>
+      <c r="D152" s="475"/>
       <c r="E152" s="311">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -25368,6 +25368,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -25384,37 +25415,6 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -25493,69 +25493,69 @@
       <c r="BZ1" s="186"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="453" t="s">
+      <c r="A2" s="476" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="489"/>
-      <c r="C2" s="490"/>
-      <c r="D2" s="492" t="s">
+      <c r="B2" s="496"/>
+      <c r="C2" s="497"/>
+      <c r="D2" s="499" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="493"/>
-      <c r="F2" s="493"/>
-      <c r="G2" s="493"/>
-      <c r="H2" s="493"/>
-      <c r="I2" s="493"/>
-      <c r="J2" s="493"/>
-      <c r="K2" s="493"/>
-      <c r="L2" s="493"/>
-      <c r="M2" s="493"/>
-      <c r="N2" s="493"/>
-      <c r="O2" s="493"/>
-      <c r="P2" s="493"/>
-      <c r="Q2" s="493"/>
-      <c r="R2" s="493"/>
-      <c r="S2" s="493"/>
-      <c r="T2" s="493"/>
+      <c r="E2" s="500"/>
+      <c r="F2" s="500"/>
+      <c r="G2" s="500"/>
+      <c r="H2" s="500"/>
+      <c r="I2" s="500"/>
+      <c r="J2" s="500"/>
+      <c r="K2" s="500"/>
+      <c r="L2" s="500"/>
+      <c r="M2" s="500"/>
+      <c r="N2" s="500"/>
+      <c r="O2" s="500"/>
+      <c r="P2" s="500"/>
+      <c r="Q2" s="500"/>
+      <c r="R2" s="500"/>
+      <c r="S2" s="500"/>
+      <c r="T2" s="500"/>
       <c r="AA2" s="131"/>
       <c r="BY2" s="186"/>
       <c r="BZ2" s="186"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="455" t="s">
+      <c r="A3" s="478" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="489"/>
-      <c r="C3" s="490"/>
+      <c r="B3" s="496"/>
+      <c r="C3" s="497"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="494" t="s">
+      <c r="F3" s="501" t="s">
         <v>352</v>
       </c>
-      <c r="G3" s="495"/>
-      <c r="H3" s="496" t="s">
+      <c r="G3" s="502"/>
+      <c r="H3" s="503" t="s">
         <v>353</v>
       </c>
-      <c r="I3" s="496"/>
-      <c r="J3" s="497"/>
-      <c r="K3" s="498" t="s">
+      <c r="I3" s="503"/>
+      <c r="J3" s="504"/>
+      <c r="K3" s="505" t="s">
         <v>354</v>
       </c>
-      <c r="L3" s="499"/>
-      <c r="M3" s="500"/>
-      <c r="N3" s="497" t="s">
+      <c r="L3" s="506"/>
+      <c r="M3" s="507"/>
+      <c r="N3" s="504" t="s">
         <v>355</v>
       </c>
-      <c r="O3" s="501"/>
-      <c r="P3" s="502"/>
-      <c r="Q3" s="503" t="s">
+      <c r="O3" s="508"/>
+      <c r="P3" s="509"/>
+      <c r="Q3" s="510" t="s">
         <v>356</v>
       </c>
-      <c r="R3" s="504"/>
-      <c r="S3" s="505" t="s">
+      <c r="R3" s="511"/>
+      <c r="S3" s="512" t="s">
         <v>357</v>
       </c>
-      <c r="T3" s="506"/>
+      <c r="T3" s="513"/>
       <c r="AA3" s="132"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -25720,7 +25720,7 @@
       <c r="AC6" s="133"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="511" t="str">
+      <c r="C7" s="490" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -25728,81 +25728,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="514"/>
-      <c r="E7" s="512"/>
-      <c r="F7" s="514" t="s">
+      <c r="D7" s="491"/>
+      <c r="E7" s="492"/>
+      <c r="F7" s="491" t="s">
         <v>380</v>
       </c>
-      <c r="G7" s="514"/>
-      <c r="H7" s="512"/>
-      <c r="I7" s="515" t="str">
+      <c r="G7" s="491"/>
+      <c r="H7" s="492"/>
+      <c r="I7" s="493" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$2620.741)</v>
       </c>
-      <c r="J7" s="516"/>
-      <c r="K7" s="516"/>
-      <c r="L7" s="516"/>
-      <c r="M7" s="516"/>
-      <c r="N7" s="516"/>
-      <c r="O7" s="516"/>
-      <c r="P7" s="516"/>
-      <c r="Q7" s="516"/>
-      <c r="R7" s="517"/>
-      <c r="S7" s="511" t="str">
+      <c r="J7" s="494"/>
+      <c r="K7" s="494"/>
+      <c r="L7" s="494"/>
+      <c r="M7" s="494"/>
+      <c r="N7" s="494"/>
+      <c r="O7" s="494"/>
+      <c r="P7" s="494"/>
+      <c r="Q7" s="494"/>
+      <c r="R7" s="495"/>
+      <c r="S7" s="490" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$319.295)</v>
       </c>
-      <c r="T7" s="514"/>
-      <c r="U7" s="514"/>
-      <c r="V7" s="514"/>
-      <c r="W7" s="514"/>
-      <c r="X7" s="512"/>
-      <c r="Y7" s="511" t="s">
+      <c r="T7" s="491"/>
+      <c r="U7" s="491"/>
+      <c r="V7" s="491"/>
+      <c r="W7" s="491"/>
+      <c r="X7" s="492"/>
+      <c r="Y7" s="490" t="s">
         <v>381</v>
       </c>
-      <c r="Z7" s="512"/>
+      <c r="Z7" s="492"/>
       <c r="AA7" s="134"/>
-      <c r="AH7" s="507" t="s">
+      <c r="AH7" s="514" t="s">
         <v>382</v>
       </c>
-      <c r="AI7" s="508"/>
+      <c r="AI7" s="515"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="509" t="s">
+      <c r="AK7" s="516" t="s">
         <v>383</v>
       </c>
       <c r="AL7" s="452"/>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="508"/>
-      <c r="AP7" s="510" t="s">
+      <c r="AN7" s="515"/>
+      <c r="AP7" s="517" t="s">
         <v>384</v>
       </c>
-      <c r="AQ7" s="459"/>
-      <c r="AS7" s="491" t="s">
+      <c r="AQ7" s="482"/>
+      <c r="AS7" s="498" t="s">
         <v>385</v>
       </c>
-      <c r="AT7" s="458"/>
-      <c r="AU7" s="458"/>
-      <c r="AV7" s="458"/>
-      <c r="AW7" s="458"/>
-      <c r="AX7" s="458"/>
-      <c r="AY7" s="458"/>
-      <c r="AZ7" s="458"/>
-      <c r="BA7" s="458"/>
-      <c r="BB7" s="459"/>
-      <c r="BD7" s="510" t="s">
+      <c r="AT7" s="481"/>
+      <c r="AU7" s="481"/>
+      <c r="AV7" s="481"/>
+      <c r="AW7" s="481"/>
+      <c r="AX7" s="481"/>
+      <c r="AY7" s="481"/>
+      <c r="AZ7" s="481"/>
+      <c r="BA7" s="481"/>
+      <c r="BB7" s="482"/>
+      <c r="BD7" s="517" t="s">
         <v>386</v>
       </c>
-      <c r="BE7" s="459"/>
+      <c r="BE7" s="482"/>
       <c r="BF7" s="186"/>
-      <c r="BG7" s="491" t="s">
+      <c r="BG7" s="498" t="s">
         <v>387</v>
       </c>
-      <c r="BH7" s="458"/>
-      <c r="BI7" s="458"/>
+      <c r="BH7" s="481"/>
+      <c r="BI7" s="481"/>
       <c r="BY7" s="186"/>
       <c r="BZ7" s="186"/>
     </row>
@@ -35747,17 +35747,17 @@
       <c r="BZ52" s="186"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="513"/>
-      <c r="D53" s="513"/>
-      <c r="E53" s="513"/>
-      <c r="F53" s="513"/>
-      <c r="G53" s="513"/>
-      <c r="H53" s="513"/>
-      <c r="I53" s="513"/>
-      <c r="J53" s="513"/>
-      <c r="K53" s="513"/>
-      <c r="L53" s="513"/>
-      <c r="M53" s="513"/>
+      <c r="C53" s="489"/>
+      <c r="D53" s="489"/>
+      <c r="E53" s="489"/>
+      <c r="F53" s="489"/>
+      <c r="G53" s="489"/>
+      <c r="H53" s="489"/>
+      <c r="I53" s="489"/>
+      <c r="J53" s="489"/>
+      <c r="K53" s="489"/>
+      <c r="L53" s="489"/>
+      <c r="M53" s="489"/>
       <c r="AC53" s="136" t="s">
         <v>436</v>
       </c>
@@ -35896,11 +35896,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -35917,6 +35912,11 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -35952,8 +35952,8 @@
   </sheetPr>
   <dimension ref="A1:Q221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36172,7 +36172,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="109">
-        <v>1.28</v>
+        <v>0.9</v>
       </c>
       <c r="C8" s="116" t="s">
         <v>249</v>
@@ -36196,7 +36196,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="109">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="C9" s="116" t="s">
         <v>250</v>
@@ -36220,7 +36220,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="109">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="C10" s="116" t="s">
         <v>251</v>
@@ -36244,7 +36244,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="109">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="C11" s="116" t="s">
         <v>252</v>
@@ -36268,7 +36268,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="109">
-        <v>1.23</v>
+        <v>0.9</v>
       </c>
       <c r="C12" s="239" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
Status on 03-11-19 optimization run
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD.xlsx
+++ b/MP LAUNCHPAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D0B377-07A6-2A4C-9E77-ED046A6C5B3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E4AF88-96D8-5A4D-9D37-D1BA12E37858}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44580" yWindow="460" windowWidth="28040" windowHeight="21140" activeTab="3" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28040" windowHeight="17540" activeTab="2" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="606">
   <si>
     <t>Scenario</t>
   </si>
@@ -4672,16 +4672,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4702,12 +4763,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4722,82 +4777,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -4859,6 +4838,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -17650,16 +17650,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="475" t="s">
+      <c r="A1" s="452" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="476"/>
+      <c r="B1" s="453"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="477" t="s">
+      <c r="A2" s="454" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="478"/>
+      <c r="B2" s="455"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="X3" s="239" t="s">
@@ -17667,33 +17667,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="482" t="s">
+      <c r="A4" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="483"/>
+      <c r="B4" s="463"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="486" t="s">
+      <c r="D4" s="466" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="479" t="s">
+      <c r="E4" s="456" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="480"/>
-      <c r="G4" s="480"/>
-      <c r="H4" s="480"/>
-      <c r="I4" s="480"/>
-      <c r="J4" s="480"/>
-      <c r="K4" s="480"/>
-      <c r="L4" s="480"/>
-      <c r="M4" s="480"/>
-      <c r="N4" s="480"/>
-      <c r="O4" s="480"/>
-      <c r="P4" s="480"/>
-      <c r="Q4" s="480"/>
-      <c r="R4" s="480"/>
-      <c r="S4" s="480"/>
-      <c r="T4" s="480"/>
-      <c r="U4" s="481"/>
+      <c r="F4" s="457"/>
+      <c r="G4" s="457"/>
+      <c r="H4" s="457"/>
+      <c r="I4" s="457"/>
+      <c r="J4" s="457"/>
+      <c r="K4" s="457"/>
+      <c r="L4" s="457"/>
+      <c r="M4" s="457"/>
+      <c r="N4" s="457"/>
+      <c r="O4" s="457"/>
+      <c r="P4" s="457"/>
+      <c r="Q4" s="457"/>
+      <c r="R4" s="457"/>
+      <c r="S4" s="457"/>
+      <c r="T4" s="457"/>
+      <c r="U4" s="458"/>
       <c r="Y4" s="239">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -17760,12 +17760,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="484"/>
-      <c r="B5" s="485"/>
+      <c r="A5" s="464"/>
+      <c r="B5" s="465"/>
       <c r="C5" s="68" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="487"/>
+      <c r="D5" s="467"/>
       <c r="E5" s="69">
         <f>'Step Cost Analysis'!E5</f>
         <v>2020</v>
@@ -17903,10 +17903,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="454" t="s">
+      <c r="A6" s="468" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="455"/>
+      <c r="B6" s="469"/>
       <c r="C6" s="160">
         <v>10</v>
       </c>
@@ -18424,12 +18424,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="469" t="s">
+      <c r="A12" s="459" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="470"/>
-      <c r="C12" s="470"/>
-      <c r="D12" s="471"/>
+      <c r="B12" s="460"/>
+      <c r="C12" s="460"/>
+      <c r="D12" s="461"/>
       <c r="E12" s="279">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -18564,12 +18564,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="469" t="s">
+      <c r="A13" s="459" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="470"/>
-      <c r="C13" s="470"/>
-      <c r="D13" s="471"/>
+      <c r="B13" s="460"/>
+      <c r="C13" s="460"/>
+      <c r="D13" s="461"/>
       <c r="E13" s="279"/>
       <c r="F13" s="279"/>
       <c r="G13" s="279"/>
@@ -18662,10 +18662,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="454" t="s">
+      <c r="A14" s="468" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="455"/>
+      <c r="B14" s="469"/>
       <c r="C14" s="162">
         <v>10</v>
       </c>
@@ -19180,12 +19180,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="469" t="s">
+      <c r="A20" s="459" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="470"/>
-      <c r="C20" s="470"/>
-      <c r="D20" s="471"/>
+      <c r="B20" s="460"/>
+      <c r="C20" s="460"/>
+      <c r="D20" s="461"/>
       <c r="E20" s="279">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -19256,12 +19256,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="469" t="s">
+      <c r="A21" s="459" t="s">
         <v>196</v>
       </c>
-      <c r="B21" s="470"/>
-      <c r="C21" s="470"/>
-      <c r="D21" s="471"/>
+      <c r="B21" s="460"/>
+      <c r="C21" s="460"/>
+      <c r="D21" s="461"/>
       <c r="E21" s="279"/>
       <c r="F21" s="279"/>
       <c r="G21" s="279"/>
@@ -19287,10 +19287,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="454" t="s">
+      <c r="A22" s="468" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="455"/>
+      <c r="B22" s="469"/>
       <c r="C22" s="160">
         <v>10</v>
       </c>
@@ -19537,12 +19537,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="469" t="s">
+      <c r="A28" s="459" t="s">
         <v>198</v>
       </c>
-      <c r="B28" s="470"/>
-      <c r="C28" s="470"/>
-      <c r="D28" s="471"/>
+      <c r="B28" s="460"/>
+      <c r="C28" s="460"/>
+      <c r="D28" s="461"/>
       <c r="E28" s="279">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -19613,12 +19613,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="469" t="s">
+      <c r="A29" s="459" t="s">
         <v>199</v>
       </c>
-      <c r="B29" s="470"/>
-      <c r="C29" s="470"/>
-      <c r="D29" s="471"/>
+      <c r="B29" s="460"/>
+      <c r="C29" s="460"/>
+      <c r="D29" s="461"/>
       <c r="E29" s="279"/>
       <c r="F29" s="279"/>
       <c r="G29" s="279"/>
@@ -19644,10 +19644,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="454" t="s">
+      <c r="A30" s="468" t="s">
         <v>200</v>
       </c>
-      <c r="B30" s="455"/>
+      <c r="B30" s="469"/>
       <c r="C30" s="160">
         <v>10</v>
       </c>
@@ -19894,12 +19894,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="469" t="s">
+      <c r="A36" s="459" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="470"/>
-      <c r="C36" s="470"/>
-      <c r="D36" s="471"/>
+      <c r="B36" s="460"/>
+      <c r="C36" s="460"/>
+      <c r="D36" s="461"/>
       <c r="E36" s="279">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -19970,12 +19970,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="469" t="s">
+      <c r="A37" s="459" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="470"/>
-      <c r="C37" s="470"/>
-      <c r="D37" s="471"/>
+      <c r="B37" s="460"/>
+      <c r="C37" s="460"/>
+      <c r="D37" s="461"/>
       <c r="E37" s="279"/>
       <c r="F37" s="279"/>
       <c r="G37" s="279"/>
@@ -20001,10 +20001,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="454" t="s">
+      <c r="A38" s="468" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="455"/>
+      <c r="B38" s="469"/>
       <c r="C38" s="160">
         <v>10</v>
       </c>
@@ -20251,12 +20251,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="469" t="s">
+      <c r="A44" s="459" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="470"/>
-      <c r="C44" s="470"/>
-      <c r="D44" s="471"/>
+      <c r="B44" s="460"/>
+      <c r="C44" s="460"/>
+      <c r="D44" s="461"/>
       <c r="E44" s="279">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -20327,12 +20327,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="469" t="s">
+      <c r="A45" s="459" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="470"/>
-      <c r="C45" s="470"/>
-      <c r="D45" s="471"/>
+      <c r="B45" s="460"/>
+      <c r="C45" s="460"/>
+      <c r="D45" s="461"/>
       <c r="E45" s="279"/>
       <c r="F45" s="279"/>
       <c r="G45" s="279"/>
@@ -20358,11 +20358,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="456" t="s">
+      <c r="A46" s="477" t="s">
         <v>206</v>
       </c>
-      <c r="B46" s="457"/>
-      <c r="C46" s="458"/>
+      <c r="B46" s="478"/>
+      <c r="C46" s="479"/>
       <c r="D46" s="170"/>
       <c r="E46" s="287">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -20435,12 +20435,12 @@
       <c r="V46" s="240"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="464" t="s">
+      <c r="A47" s="483" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="465"/>
-      <c r="C47" s="465"/>
-      <c r="D47" s="466"/>
+      <c r="B47" s="484"/>
+      <c r="C47" s="484"/>
+      <c r="D47" s="485"/>
       <c r="E47" s="288">
         <f>E46</f>
         <v>1500000</v>
@@ -20511,7 +20511,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A48" s="171"/>
       <c r="B48" s="171"/>
-      <c r="C48" s="467" t="s">
+      <c r="C48" s="486" t="s">
         <v>208</v>
       </c>
       <c r="D48" s="172">
@@ -20586,7 +20586,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A49" s="171"/>
-      <c r="C49" s="468"/>
+      <c r="C49" s="487"/>
       <c r="D49" s="242">
         <v>37</v>
       </c>
@@ -20657,7 +20657,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A50" s="171"/>
-      <c r="C50" s="468"/>
+      <c r="C50" s="487"/>
       <c r="D50" s="242">
         <v>30</v>
       </c>
@@ -20728,7 +20728,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A51" s="171"/>
-      <c r="C51" s="468"/>
+      <c r="C51" s="487"/>
       <c r="D51" s="242">
         <v>41</v>
       </c>
@@ -20798,38 +20798,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="459" t="s">
+      <c r="A52" s="480" t="s">
         <v>209</v>
       </c>
-      <c r="B52" s="460"/>
-      <c r="C52" s="460"/>
-      <c r="D52" s="460"/>
-      <c r="E52" s="460"/>
-      <c r="F52" s="460"/>
-      <c r="G52" s="460"/>
-      <c r="H52" s="460"/>
-      <c r="I52" s="460"/>
-      <c r="J52" s="460"/>
-      <c r="K52" s="460"/>
-      <c r="L52" s="460"/>
-      <c r="M52" s="460"/>
-      <c r="N52" s="460"/>
-      <c r="O52" s="460"/>
-      <c r="P52" s="460"/>
-      <c r="Q52" s="460"/>
-      <c r="R52" s="460"/>
-      <c r="S52" s="460"/>
-      <c r="T52" s="460"/>
-      <c r="U52" s="460"/>
-      <c r="V52" s="460"/>
-      <c r="W52" s="461"/>
+      <c r="B52" s="481"/>
+      <c r="C52" s="481"/>
+      <c r="D52" s="481"/>
+      <c r="E52" s="481"/>
+      <c r="F52" s="481"/>
+      <c r="G52" s="481"/>
+      <c r="H52" s="481"/>
+      <c r="I52" s="481"/>
+      <c r="J52" s="481"/>
+      <c r="K52" s="481"/>
+      <c r="L52" s="481"/>
+      <c r="M52" s="481"/>
+      <c r="N52" s="481"/>
+      <c r="O52" s="481"/>
+      <c r="P52" s="481"/>
+      <c r="Q52" s="481"/>
+      <c r="R52" s="481"/>
+      <c r="S52" s="481"/>
+      <c r="T52" s="481"/>
+      <c r="U52" s="481"/>
+      <c r="V52" s="481"/>
+      <c r="W52" s="482"/>
       <c r="X52" s="240"/>
     </row>
     <row r="53" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="462" t="s">
+      <c r="A53" s="472" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="463"/>
+      <c r="B53" s="473"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -21006,10 +21006,10 @@
       <c r="X57" s="240"/>
     </row>
     <row r="58" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="452" t="s">
+      <c r="A58" s="470" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="453"/>
+      <c r="B58" s="471"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -21191,10 +21191,10 @@
       <c r="X62" s="240"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="452" t="s">
+      <c r="A63" s="470" t="s">
         <v>213</v>
       </c>
-      <c r="B63" s="453"/>
+      <c r="B63" s="471"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -21384,10 +21384,10 @@
       <c r="X67" s="240"/>
     </row>
     <row r="68" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="452" t="s">
+      <c r="A68" s="470" t="s">
         <v>214</v>
       </c>
-      <c r="B68" s="453"/>
+      <c r="B68" s="471"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -21565,10 +21565,10 @@
       <c r="X72" s="240"/>
     </row>
     <row r="73" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="452" t="s">
+      <c r="A73" s="470" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="453"/>
+      <c r="B73" s="471"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -21794,10 +21794,10 @@
       <c r="X77" s="240"/>
     </row>
     <row r="78" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="452" t="s">
+      <c r="A78" s="470" t="s">
         <v>217</v>
       </c>
-      <c r="B78" s="453"/>
+      <c r="B78" s="471"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -21969,10 +21969,10 @@
       <c r="X82" s="240"/>
     </row>
     <row r="83" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="452" t="s">
+      <c r="A83" s="470" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="453"/>
+      <c r="B83" s="471"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -22144,10 +22144,10 @@
       <c r="X87" s="240"/>
     </row>
     <row r="88" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="452" t="s">
+      <c r="A88" s="470" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="453"/>
+      <c r="B88" s="471"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -22319,10 +22319,10 @@
       <c r="X92" s="240"/>
     </row>
     <row r="93" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="452" t="s">
+      <c r="A93" s="470" t="s">
         <v>222</v>
       </c>
-      <c r="B93" s="453"/>
+      <c r="B93" s="471"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -22524,10 +22524,10 @@
       <c r="X97" s="240"/>
     </row>
     <row r="98" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="452" t="s">
+      <c r="A98" s="470" t="s">
         <v>224</v>
       </c>
-      <c r="B98" s="453"/>
+      <c r="B98" s="471"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -22719,10 +22719,10 @@
       <c r="X102" s="240"/>
     </row>
     <row r="103" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="452" t="s">
+      <c r="A103" s="470" t="s">
         <v>226</v>
       </c>
-      <c r="B103" s="453"/>
+      <c r="B103" s="471"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -22924,10 +22924,10 @@
       <c r="X107" s="240"/>
     </row>
     <row r="108" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="452" t="s">
+      <c r="A108" s="470" t="s">
         <v>227</v>
       </c>
-      <c r="B108" s="453"/>
+      <c r="B108" s="471"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -23129,10 +23129,10 @@
       <c r="X112" s="240"/>
     </row>
     <row r="113" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="452" t="s">
+      <c r="A113" s="470" t="s">
         <v>228</v>
       </c>
-      <c r="B113" s="453"/>
+      <c r="B113" s="471"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -23294,10 +23294,10 @@
       <c r="X117" s="240"/>
     </row>
     <row r="118" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="452" t="s">
+      <c r="A118" s="470" t="s">
         <v>229</v>
       </c>
-      <c r="B118" s="453"/>
+      <c r="B118" s="471"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -23499,10 +23499,10 @@
       <c r="X122" s="240"/>
     </row>
     <row r="123" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="452" t="s">
+      <c r="A123" s="470" t="s">
         <v>230</v>
       </c>
-      <c r="B123" s="453"/>
+      <c r="B123" s="471"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -23704,10 +23704,10 @@
       <c r="X127" s="240"/>
     </row>
     <row r="128" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="452" t="s">
+      <c r="A128" s="470" t="s">
         <v>231</v>
       </c>
-      <c r="B128" s="453"/>
+      <c r="B128" s="471"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -23909,10 +23909,10 @@
       <c r="X132" s="240"/>
     </row>
     <row r="133" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="452" t="s">
+      <c r="A133" s="470" t="s">
         <v>232</v>
       </c>
-      <c r="B133" s="453"/>
+      <c r="B133" s="471"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -24114,10 +24114,10 @@
       <c r="X137" s="240"/>
     </row>
     <row r="138" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="452" t="s">
+      <c r="A138" s="470" t="s">
         <v>233</v>
       </c>
-      <c r="B138" s="453"/>
+      <c r="B138" s="471"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -24327,10 +24327,10 @@
       <c r="X142" s="240"/>
     </row>
     <row r="143" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="452" t="s">
+      <c r="A143" s="470" t="s">
         <v>237</v>
       </c>
-      <c r="B143" s="453"/>
+      <c r="B143" s="471"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -24423,10 +24423,10 @@
       <c r="X144" s="240"/>
     </row>
     <row r="145" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="462" t="s">
+      <c r="A145" s="472" t="s">
         <v>239</v>
       </c>
-      <c r="B145" s="463"/>
+      <c r="B145" s="473"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -24499,10 +24499,10 @@
       <c r="X146" s="240"/>
     </row>
     <row r="147" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="462" t="s">
+      <c r="A147" s="472" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="463"/>
+      <c r="B147" s="473"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -24600,10 +24600,10 @@
       <c r="X148" s="240"/>
     </row>
     <row r="149" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="462" t="s">
+      <c r="A149" s="472" t="s">
         <v>241</v>
       </c>
-      <c r="B149" s="463"/>
+      <c r="B149" s="473"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -24725,12 +24725,12 @@
       <c r="X151" s="240"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="472" t="s">
+      <c r="A152" s="474" t="s">
         <v>242</v>
       </c>
-      <c r="B152" s="473"/>
-      <c r="C152" s="473"/>
-      <c r="D152" s="474"/>
+      <c r="B152" s="475"/>
+      <c r="C152" s="475"/>
+      <c r="D152" s="476"/>
       <c r="E152" s="311">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -25342,37 +25342,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -25389,6 +25358,37 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -25467,69 +25467,69 @@
       <c r="BZ1" s="186"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="475" t="s">
+      <c r="A2" s="452" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="495"/>
-      <c r="C2" s="496"/>
-      <c r="D2" s="498" t="s">
+      <c r="B2" s="488"/>
+      <c r="C2" s="489"/>
+      <c r="D2" s="491" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="499"/>
-      <c r="F2" s="499"/>
-      <c r="G2" s="499"/>
-      <c r="H2" s="499"/>
-      <c r="I2" s="499"/>
-      <c r="J2" s="499"/>
-      <c r="K2" s="499"/>
-      <c r="L2" s="499"/>
-      <c r="M2" s="499"/>
-      <c r="N2" s="499"/>
-      <c r="O2" s="499"/>
-      <c r="P2" s="499"/>
-      <c r="Q2" s="499"/>
-      <c r="R2" s="499"/>
-      <c r="S2" s="499"/>
-      <c r="T2" s="499"/>
+      <c r="E2" s="492"/>
+      <c r="F2" s="492"/>
+      <c r="G2" s="492"/>
+      <c r="H2" s="492"/>
+      <c r="I2" s="492"/>
+      <c r="J2" s="492"/>
+      <c r="K2" s="492"/>
+      <c r="L2" s="492"/>
+      <c r="M2" s="492"/>
+      <c r="N2" s="492"/>
+      <c r="O2" s="492"/>
+      <c r="P2" s="492"/>
+      <c r="Q2" s="492"/>
+      <c r="R2" s="492"/>
+      <c r="S2" s="492"/>
+      <c r="T2" s="492"/>
       <c r="AA2" s="131"/>
       <c r="BY2" s="186"/>
       <c r="BZ2" s="186"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477" t="s">
+      <c r="A3" s="454" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="495"/>
-      <c r="C3" s="496"/>
+      <c r="B3" s="488"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="500" t="s">
+      <c r="F3" s="493" t="s">
         <v>352</v>
       </c>
-      <c r="G3" s="501"/>
-      <c r="H3" s="502" t="s">
+      <c r="G3" s="494"/>
+      <c r="H3" s="495" t="s">
         <v>353</v>
       </c>
-      <c r="I3" s="502"/>
-      <c r="J3" s="503"/>
-      <c r="K3" s="504" t="s">
+      <c r="I3" s="495"/>
+      <c r="J3" s="496"/>
+      <c r="K3" s="497" t="s">
         <v>354</v>
       </c>
-      <c r="L3" s="505"/>
-      <c r="M3" s="506"/>
-      <c r="N3" s="503" t="s">
+      <c r="L3" s="498"/>
+      <c r="M3" s="499"/>
+      <c r="N3" s="496" t="s">
         <v>355</v>
       </c>
-      <c r="O3" s="507"/>
-      <c r="P3" s="508"/>
-      <c r="Q3" s="509" t="s">
+      <c r="O3" s="500"/>
+      <c r="P3" s="501"/>
+      <c r="Q3" s="502" t="s">
         <v>356</v>
       </c>
-      <c r="R3" s="510"/>
-      <c r="S3" s="511" t="s">
+      <c r="R3" s="503"/>
+      <c r="S3" s="504" t="s">
         <v>357</v>
       </c>
-      <c r="T3" s="512"/>
+      <c r="T3" s="505"/>
       <c r="AA3" s="132"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -25694,7 +25694,7 @@
       <c r="AC6" s="133"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="489" t="str">
+      <c r="C7" s="510" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -25702,81 +25702,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="490"/>
-      <c r="E7" s="491"/>
-      <c r="F7" s="490" t="s">
+      <c r="D7" s="513"/>
+      <c r="E7" s="511"/>
+      <c r="F7" s="513" t="s">
         <v>380</v>
       </c>
-      <c r="G7" s="490"/>
-      <c r="H7" s="491"/>
-      <c r="I7" s="492" t="str">
+      <c r="G7" s="513"/>
+      <c r="H7" s="511"/>
+      <c r="I7" s="514" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$2620.741)</v>
       </c>
-      <c r="J7" s="493"/>
-      <c r="K7" s="493"/>
-      <c r="L7" s="493"/>
-      <c r="M7" s="493"/>
-      <c r="N7" s="493"/>
-      <c r="O7" s="493"/>
-      <c r="P7" s="493"/>
-      <c r="Q7" s="493"/>
-      <c r="R7" s="494"/>
-      <c r="S7" s="489" t="str">
+      <c r="J7" s="515"/>
+      <c r="K7" s="515"/>
+      <c r="L7" s="515"/>
+      <c r="M7" s="515"/>
+      <c r="N7" s="515"/>
+      <c r="O7" s="515"/>
+      <c r="P7" s="515"/>
+      <c r="Q7" s="515"/>
+      <c r="R7" s="516"/>
+      <c r="S7" s="510" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$319.295)</v>
       </c>
-      <c r="T7" s="490"/>
-      <c r="U7" s="490"/>
-      <c r="V7" s="490"/>
-      <c r="W7" s="490"/>
-      <c r="X7" s="491"/>
-      <c r="Y7" s="489" t="s">
+      <c r="T7" s="513"/>
+      <c r="U7" s="513"/>
+      <c r="V7" s="513"/>
+      <c r="W7" s="513"/>
+      <c r="X7" s="511"/>
+      <c r="Y7" s="510" t="s">
         <v>381</v>
       </c>
-      <c r="Z7" s="491"/>
+      <c r="Z7" s="511"/>
       <c r="AA7" s="134"/>
-      <c r="AH7" s="513" t="s">
+      <c r="AH7" s="506" t="s">
         <v>382</v>
       </c>
-      <c r="AI7" s="514"/>
+      <c r="AI7" s="507"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="515" t="s">
+      <c r="AK7" s="508" t="s">
         <v>383</v>
       </c>
       <c r="AL7" s="451"/>
       <c r="AM7" s="451"/>
-      <c r="AN7" s="514"/>
-      <c r="AP7" s="516" t="s">
+      <c r="AN7" s="507"/>
+      <c r="AP7" s="509" t="s">
         <v>384</v>
       </c>
-      <c r="AQ7" s="481"/>
-      <c r="AS7" s="497" t="s">
+      <c r="AQ7" s="458"/>
+      <c r="AS7" s="490" t="s">
         <v>385</v>
       </c>
-      <c r="AT7" s="480"/>
-      <c r="AU7" s="480"/>
-      <c r="AV7" s="480"/>
-      <c r="AW7" s="480"/>
-      <c r="AX7" s="480"/>
-      <c r="AY7" s="480"/>
-      <c r="AZ7" s="480"/>
-      <c r="BA7" s="480"/>
-      <c r="BB7" s="481"/>
-      <c r="BD7" s="516" t="s">
+      <c r="AT7" s="457"/>
+      <c r="AU7" s="457"/>
+      <c r="AV7" s="457"/>
+      <c r="AW7" s="457"/>
+      <c r="AX7" s="457"/>
+      <c r="AY7" s="457"/>
+      <c r="AZ7" s="457"/>
+      <c r="BA7" s="457"/>
+      <c r="BB7" s="458"/>
+      <c r="BD7" s="509" t="s">
         <v>386</v>
       </c>
-      <c r="BE7" s="481"/>
+      <c r="BE7" s="458"/>
       <c r="BF7" s="186"/>
-      <c r="BG7" s="497" t="s">
+      <c r="BG7" s="490" t="s">
         <v>387</v>
       </c>
-      <c r="BH7" s="480"/>
-      <c r="BI7" s="480"/>
+      <c r="BH7" s="457"/>
+      <c r="BI7" s="457"/>
       <c r="BY7" s="186"/>
       <c r="BZ7" s="186"/>
     </row>
@@ -35721,17 +35721,17 @@
       <c r="BZ52" s="186"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="488"/>
-      <c r="D53" s="488"/>
-      <c r="E53" s="488"/>
-      <c r="F53" s="488"/>
-      <c r="G53" s="488"/>
-      <c r="H53" s="488"/>
-      <c r="I53" s="488"/>
-      <c r="J53" s="488"/>
-      <c r="K53" s="488"/>
-      <c r="L53" s="488"/>
-      <c r="M53" s="488"/>
+      <c r="C53" s="512"/>
+      <c r="D53" s="512"/>
+      <c r="E53" s="512"/>
+      <c r="F53" s="512"/>
+      <c r="G53" s="512"/>
+      <c r="H53" s="512"/>
+      <c r="I53" s="512"/>
+      <c r="J53" s="512"/>
+      <c r="K53" s="512"/>
+      <c r="L53" s="512"/>
+      <c r="M53" s="512"/>
       <c r="AC53" s="136" t="s">
         <v>436</v>
       </c>
@@ -35870,6 +35870,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -35886,11 +35891,6 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -37646,8 +37646,8 @@
   </sheetPr>
   <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38079,9 +38079,7 @@
       <c r="E26" s="230" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="230" t="s">
-        <v>46</v>
-      </c>
+      <c r="F26" s="230"/>
       <c r="G26" s="230"/>
       <c r="H26" s="230"/>
       <c r="I26" s="230"/>
@@ -40098,7 +40096,7 @@
   </sheetPr>
   <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>

</xml_diff>